<commit_message>
refactor: código refatorado + criação de template para envio no corpo do e-mail
</commit_message>
<xml_diff>
--- a/kabum_produtos.xlsx
+++ b/kabum_produtos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="571">
   <si>
     <t>Produto</t>
   </si>
@@ -226,7 +226,7 @@
     <t>Notebook Acer Aspire 3 Intel Core I3 11ª Gen, RAM 4GB, SSD 512GB, 15.6 Polegadas Full HD - Windows 11 Home</t>
   </si>
   <si>
-    <t>R$2229.9</t>
+    <t>R$2314.4</t>
   </si>
   <si>
     <t>Notebook LG UltraSlim Intel Core i5, 8GB RAM, SSD 256GB, 15.6" Full HD IPS Iris Xe, Windows 11 Home, Preto - 15U50Q-L</t>
@@ -436,9 +436,6 @@
     <t>Notebook vaio fe15 15.6 fhd i5-1135g7 8gb ssd 512gb windows 11 home cinza escuro - vjfe55f11x-b0211h&lt;br /&gt;&lt;br /&gt;  Mais desempenho&lt;br /&gt; Aumente sua produtividade e faça  multitarefas sem se preocupar. O novo vaio vem equipado com  processadores intel de 11º geração&lt;br /&gt;&lt;br /&gt;  Precisão nos detalhes&lt;br /&gt;  A tela full hd proporciona um visual mais imersivo  e com menos distrações para os olhos. Aproveite  todo o poder gráfico das novas gpu intel xe graphics e desfrute de toda qualidade de imagem,  seja num filme, numa edição de fotos ou em  qualquer outro visual&lt;br /&gt;&lt;br /&gt;  Leveza e autonomia combinados&lt;br /&gt; Tenha autonomia para sair de casa sem  preocupações, o novo vaio fe15 possui bateria de até 10 horas de duração, design  compacto, leve, pesando apenas 1,75 kg, e fino, com 19,8 mm&lt;br /&gt; O tempo de duração da bateria pode variar de acordo com o uso--&lt;br /&gt;&lt;br /&gt; A qualidade e privacidade que você precisa&lt;br /&gt; A webcam hd e os dois microfones digitais com noise cancellation surpreendem a todos na videoconferência. Não seja surpreendido com a invasão de privacidade, a nossa webcam shutter (bloqueador mecânico da câmera) te mantém sempre seguro&lt;br /&gt;&lt;br /&gt;  Comfort key e tecnologia ergolift&lt;br /&gt;  Com a tecnologia do teclado ergolift o notebook possui uma leve inclinação sendo mais confortável na hora de digitar, reduzindo o estresse do pulso e das mãos para usar à vontade. E não se preocupe, porque com o comfort key as teclas são maiores, possibilitando muito conforto na digitação além de ser robusto (teclado suporta até 10 milhões de ciclos)</t>
   </si>
   <si>
-    <t>R$2949.9</t>
-  </si>
-  <si>
     <t>Notebook Samsung Book Go, Snapdragon 7c, 4GB RAM, SSD 128GB, Tela 14 Polegadas Full HD, W11 Home, Cinza, Com Office 365 Personal - Np340xla-k03br</t>
   </si>
   <si>
@@ -1615,13 +1612,13 @@
     <t>R$1899.0</t>
   </si>
   <si>
-    <t>Notebook Acer A314, Intel Celeron N4500, 4GB, SSD 128GB, Tela 14 Full HD, Linux</t>
-  </si>
-  <si>
-    <t>&lt;strong&gt;notebook acer a314 intel celeron n4500&lt;/strong&gt;&lt;strong&gt;dando conta em grande estilo:&lt;/strong&gt;desenvolvido para não deixar você parar, o aspire 3 tem a tecnologia que acompanha seu estilo de vida. Equipado com o processador intel&amp;nbspceleron&amp;nbsp- n4500 serie n, estudar, trabalhar e se divertir ficam mais fácil.&lt;strong&gt;imagens impressionantes:&lt;/strong&gt;assistir vídeos, filmes e séries será como estar no cinema com a tela de 14&amp;nbspfhd (1920 x 1080). A tecnologia acer comfyview&amp;nbspotimiza o conforto, refletindo menos luz e garantindo uma visualização mais confortável.&lt;strong&gt;bateria que não te deixa na mão:&lt;/strong&gt;o aspire 3 foi feito para aguentar todas as necessidades do dia. Dependendo do uso, sua bateria pode durar até 8 horas*, permitindo que você complete todas as suas tarefas!&lt;strong&gt;o poder da conectividade:&lt;/strong&gt;com entrada hdmi, portas usb 2.0, usb 3.2 e ethernet (rj-45), você tem diversas opções para estar sempre conectado recebendo e distribuindo informação.&lt;strong&gt;especificações técnicas&lt;/strong&gt;:&lt;strong&gt;marca:&lt;/strong&gt; acer&lt;strong&gt;modelo:&lt;/strong&gt; a314&lt;strong&gt;processador:&lt;/strong&gt; intel celeron&amp;nbspn4500 (1.1ghz até2.80ghz, cache 4mb)&lt;strong&gt;memória:&lt;/strong&gt; 4gb&amp;nbspddr4 2933mhz (4 gb modulo + slot livre) ddr4-2933mhz&amp;nbspexpansível até 16 gb&lt;strong&gt;armazenamento:&lt;/strong&gt; ssd 128gbslot livre m.2 2280, compatível com unidades ssd pcie 3.0 nvme x2/x4 de até 1tb (não acompanha o produto).slot ocupado sata 3, compatível com hdd ou ssd sata 3 2.5&amp;rdquo de até 2tb (não acompanha o produto)&lt;strong&gt;sistema operacional:&lt;/strong&gt; linux&lt;strong&gt;tela:&lt;/strong&gt; 14&amp;nbspled full hd(1920x1080), antirreflexo&lt;strong&gt;placa de vídeo:&lt;/strong&gt;&amp;nbspintel&amp;nbspuhd graphics&lt;strong&gt;portas e slots:&lt;/strong&gt; entrada de energia| rj-45| hdmi 2.0| 2xusb 3.2| trava kensington| usb2.0| entrada padrão combo microfone e alto falante&lt;strong&gt;dimensão:&lt;/strong&gt; altura:&amp;nbsp2cm| largura: 33cm| profundidade: 24 cm| peso: 1,65kg&lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;notebook acer a314 intel celeron n4500 nx.awbal.001| entregas para todo o brasil</t>
-  </si>
-  <si>
-    <t>R$2015.0</t>
+    <t>Bateria Notebook Dell Ultrabook, 47wh, E7440, 7.6v - 34gkr</t>
+  </si>
+  <si>
+    <t>Bateria substituta notebook dell para notebook ultrabook e7440 tipo 34gkr.&lt;strong&gt;especificações técnicas:&lt;/strong&gt;capacidade: 47whvoltagem: 7.4vtipo: bateria de li-ionnúmero de células: 4&lt;strong&gt;códigos alternativos:j60j534gkr909h5g0g2m.&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>R$1093.9</t>
   </si>
   <si>
     <t>Notebook Soyo 14 Polegadas, Core I3 10°g, 8GB, 240GB, Windows 10 Pro</t>
@@ -1633,15 +1630,6 @@
     <t>R$2482.93</t>
   </si>
   <si>
-    <t>Bateria Notebook Dell Ultrabook, 47wh, E7440, 7.6v - 34gkr</t>
-  </si>
-  <si>
-    <t>Bateria substituta notebook dell para notebook ultrabook e7440 tipo 34gkr.&lt;strong&gt;especificações técnicas:&lt;/strong&gt;capacidade: 47whvoltagem: 7.4vtipo: bateria de li-ionnúmero de células: 4&lt;strong&gt;códigos alternativos:j60j534gkr909h5g0g2m.&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t>R$1093.9</t>
-  </si>
-  <si>
     <t>Usado - Notebook Lenovo Ideapad 3-15iml05, Intel Core I5-10210u, 8GB, SSD 256GB, Tela 15.6p, Linux - 82bss00200 - Seminovo</t>
   </si>
   <si>
@@ -1651,15 +1639,6 @@
     <t>R$2279.54</t>
   </si>
   <si>
-    <t>Notebook Soyo, 14 Polegadas, Intel Core I3 10, 8GB, 480GB, Windows 10</t>
-  </si>
-  <si>
-    <t>&lt;strong&gt;notebook 14´´ intel core i3 10°, 8gb, 480gb, windows 10, soyo&lt;/strong&gt;nós somos a everex, comprometidos com o desenvolvimento de produtos de alta tecnologia e qualidade para você!alto desempenho, com os processador intel® core™ i3-10110uos notebooks soyo, utilizam os processadores intel® core™ i3, que combinam desempenho, segurança e versatilidade em um design compacto e exclusivo.permite verificar e-mails, estudar, navegar nas redes sociais ou fazer streaming de música e filmes.plugue no seu monitor ou na tv, através de um cabo hdmi (não incluso).projetado para se adaptar ao escritório ou em casa.ajuste flexível: ultracompacto e moderno, se encaixa perfeitamente em qualquer ambiente de trabalho ou residencial.desempenho de alto nívelprocessamento mais avançado: processadores intel® core™ i3 de10° geração, para que sua rotina seja mais eficiente.&lt;strong&gt;memória ddr4:&lt;/strong&gt;oferece mais desempenho e tecnologia: realize várias tarefas ao mesmo tempo com mais eficiência, com memória ddr4.alcance +,todos os diasconecte-se de qualquer lugar: portátil e leve, com fonte de energia bivolt, wi-fi integrado e tecnologia de última geração,que oferece velocidades mais rápidas e melhor desempenho, onde quer que você decida trabalhar, estudar ou se divertir!&lt;strong&gt;especificaçoes técnicas:&lt;/strong&gt;marca:soyomodelo: notebook 14”tela: 14´´ high definition, alta resolução 1366x768bateria: íon de lítio 7.6v 6000mahprocessador: intel® core™ i3-10110umemória ram: 8gbarmazenamento: 480gb ssdsistema operacional:windows 10 professionaltipo de memória: sodimm ddr4rede:10/100/1000 mbpswi-fi: 802.11 ac / bluetooth® 4.2 - suporte para redes 2.4, 5 ghzfonte:bivolt (entrada: 100 - 240vac 60hz / saída: 19v 2.1a)unidade optica: n?o possuigarantia: 12 mesespeso: 1,5 kg.dimensões:20,5x223,4x332,5 mmhomologacão anatel:06609-17-10516&lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;marca:&lt;/strong&gt; soyo&lt;br&gt;&lt;strong&gt;sistema operacional:&lt;/strong&gt; windows 10 professional&lt;br&gt;&lt;strong&gt;modelo:&lt;/strong&gt; sonbci3cm848w&lt;br&gt;&lt;strong&gt;processador:&lt;/strong&gt; intel core i3-10110u&lt;br&gt;&lt;strong&gt;memória ram:&lt;/strong&gt; 8gb&lt;br&gt;&lt;strong&gt;gráficos:&lt;/strong&gt; 1366x768 (hd)&lt;br&gt;&lt;strong&gt;armazenamento:&lt;/strong&gt; 480gb ssd&lt;br&gt;&lt;strong&gt;unidade optica:&lt;/strong&gt; não&lt;br&gt;&lt;strong&gt;energia:&lt;/strong&gt; entrada: 100 - 240vac 60hz / saída: 19v 2.1a&lt;br&gt;&lt;strong&gt;wi-fi:&lt;/strong&gt; 802.11 ac / bluetooth® 4.2 - redes 2.4 e. 5 ghz&lt;br&gt;&lt;strong&gt;rede:&lt;/strong&gt; 10/100/1000 mbps&lt;br&gt;&lt;strong&gt;garantia:&lt;/strong&gt; 12 meses&lt;br&gt;&lt;strong&gt;tela:&lt;/strong&gt; 14´´ high definition&lt;br&gt;&lt;strong&gt;anatel:&lt;/strong&gt; 06609-17-10516</t>
-  </si>
-  <si>
-    <t>R$2595.79</t>
-  </si>
-  <si>
     <t>Usado - Notebook Lenovo Ideapad S145, Intel Core I5-1035g1, 4GB, 1TB, Tela 15.6p, Windows 10, Prata - 82dj0005br - Vitrine</t>
   </si>
   <si>
@@ -1687,6 +1666,90 @@
     <t>R$1809.99</t>
   </si>
   <si>
+    <t>Notebook Asus, Intel Dual Core, 4GB, 500hd, Tela 15,6 Polegadas,Windows 10 - X543na</t>
+  </si>
+  <si>
+    <t>O notebook asus vivobook x543na tem design clássico, com acabamento escovado em cinza escuro, superelegante e o melhor de tudo, tem apenas 1,9kg, perfeito para você que precisa sair e levar o computador, mas também quer tela grande para aumentar a produtividade.&lt;br /&gt;&lt;br /&gt;  com o asus vivobook x543, você não será mais um na multidão. Se o seu objetivo é relaxar, aproveite o sistema de som superpoderoso do asus vivobook x543na.&lt;br /&gt;&lt;br /&gt;  ele usa cada milímetro do seu chassis para reproduzir graves mais impactantes e sem ruídos. A caixa de ressonância de 19,4cc torna o som cristalino e incrivelmente realista.&lt;br /&gt;&lt;br /&gt;  se você já teve a experiência de digitar em um teclado pequeno, sabe que não é confortável, não é produtivo e é isso que te faz parar. Então, se o seu objetivo for trabalhar, o asus vivobook será seu parceiro incansável. Ele tem teclado completo, com teclas grandes e com curso de 1,8 milímetros, que é ideal para tornar a digitação ágil, precisa e confortável.&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  características: &lt;br /&gt;&lt;br /&gt;  modelo: x543na-gq342t&lt;br /&gt;&lt;br /&gt;  processador: intel® celeron dual core n3350 1,1 ghz, 2 mb cache.&lt;br /&gt;&lt;br /&gt;  memória ram: 4 gb (4 gb onboard + 0 gb offboard)&lt;br /&gt;&lt;br /&gt;  armazenamento: 500 gb sata 5400 rpm&lt;br /&gt;&lt;br /&gt;  tela: 15,60 led-backlit anti-glare&lt;br /&gt;&lt;br /&gt;  resolução da tela: 1366 x 768&lt;br /&gt;&lt;br /&gt;  placa de vídeo: intel® hd graphics 500&lt;br /&gt;&lt;br /&gt;  tela sensível ao toque: não&lt;br /&gt;&lt;br /&gt;  clock de memória: 1333 mhz&lt;br /&gt;&lt;br /&gt;  wi-fi: 802.11ac&lt;br /&gt;&lt;br /&gt;  teclado retro iluminado: não&lt;br /&gt;&lt;br /&gt;  câmera frontal: vga&lt;br /&gt;&lt;br /&gt;  bluetooth: bluetooth 4,1&lt;br /&gt;&lt;br /&gt;  cartão de memória; micro sd&lt;br /&gt;&lt;br /&gt;  áudio; built-in speaker built-in microphone áudio by icepower® sonic master.&lt;br /&gt;&lt;br /&gt;  saídas: 2x usb 2.0 1x usb 3.0 1x headphone-out  audio-in combo jack 1x hdmi 1x micro sd card reader&lt;br /&gt;&lt;br /&gt;  adaptador de energia: 45,00 w&lt;br /&gt;&lt;br /&gt;  bateria; 3 cells / 2200 mah&lt;br /&gt;&lt;br /&gt;  software: asus live update asus product registration program asus giftbox asus smart gesture asus splendid asus webstorage sync agent asus icesound&lt;br /&gt;&lt;br /&gt;  sistema operacional: windows 10 home&lt;br /&gt;&lt;br /&gt;  * a memória disponível para uso pode sofrer variações conforme versão do sistema operacional, apps, conteúdo e dados instalados.&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  dimensões: &lt;br /&gt;&lt;br /&gt;  altura: 25,2 cm&lt;br /&gt;&lt;br /&gt;  largura: 38,1 cm&lt;br /&gt;&lt;br /&gt;  profundidade: 2,72 cm&lt;br /&gt;&lt;br /&gt;  peso: 1,9 kg&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  garantia do fornecedor de 12 meses.</t>
+  </si>
+  <si>
+    <t>R$2305.99</t>
+  </si>
+  <si>
+    <t>Usado - Notebook HP Probook 640 G2, Intel Core I5-6300u, 8GB, SSD 256GB, Tela 14p, Windows 10 Pro - L8u43av8gb - Seminovo</t>
+  </si>
+  <si>
+    <t>Notebook HP Probook L8U43AV8GB, processador Intel Core i5 de sexta geração, memoria RAM de 8GB, armazenamento SSD de 256GB e sistema operacional Windows 10 Pro.&lt;br /&gt;&lt;br /&gt;Modelo/Referencia: L8U43AV#8GB&lt;br /&gt;&lt;br /&gt;Certificação: Recertificado&lt;br /&gt;&lt;br /&gt;Medalha: Prata&lt;br /&gt;&lt;br /&gt;FICHA TÉCNICA:&lt;br /&gt;&lt;br /&gt;Sistema operacional: Windows 10 &lt;br /&gt;&lt;br /&gt;Processador: Intel Core i5-6300U – Dual core (4 Threads)– frequência de (2.40 GHz até 3.0GHz) - 3 MB de cache&lt;br /&gt;&lt;br /&gt;Memoria: 8 GB RAM &lt;br /&gt;&lt;br /&gt;Armazenamento: 256 GB SSD &lt;br /&gt;&lt;br /&gt;Tela: 14” &lt;br /&gt;Conteúdo da embalagem: Notebook, Fonte carregadora do notebook&lt;br /&gt;&lt;br /&gt;Observação: O produto não acompanha manual de instruções&lt;br /&gt;&lt;br /&gt;Garantia: 3 meses&lt;br /&gt;&lt;br /&gt;ATENÇÃO: VOCÊ ESTÁ ADQUIRINDO UM PRODUTO RECERTIFICADO!!!! &lt;br /&gt;&lt;br /&gt;&lt;br /&gt;O produto não acompanha caixa original, manual ou qualquer outro acessório. Apenas fonte de alimentação do notebook&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;Entenda o que é um produto recertificado:&lt;br /&gt;&lt;br /&gt;É um produto que volta do mercado disponível para venda nas mesmas condições de um produto novo, com suas funcionalidades e características originais. O produto passa por um rigoroso processo de análise onde todas as suas funcionalidades são testadas e o produto liberado para venda. &lt;br /&gt;&lt;br /&gt;O produto recertificado é classificado em medalhas de acordo com o estado estético e superficial do produto, sendo: OURO, PRATA E BRONZE.&lt;br /&gt; &lt;br /&gt;Recertificado Prata: Produto tem características similares ao Ouro, pode apresentar mínimos riscos quase imperceptíveis. &lt;br /&gt;&lt;br /&gt;Atenção: O Saldão da Informática não enviará fotos reais dos produtos para os clientes, como também não reservaremos produtos. As imagens exibidas são meramente ilustrativas.</t>
+  </si>
+  <si>
+    <t>Usado - Notebook Lenovo Ideapad S145, Intel Core I5-1035g1, 4GB, 1TB, Tela 15.6p, Windows 10 - 82dj0005br - Seminovo</t>
+  </si>
+  <si>
+    <t>Notebook Lenovo IdeaPad S145 82DJ0005BR, na cor prata, processador de 10º geração Intel Core i5-1035G1 de 1.00GHz até 3.60GHz, memória RAM de 4GB DDR4, HD de 1TB, tela de 15.6 polegadas e sistema operacional Windows 10.&lt;br /&gt;&lt;br /&gt;Modelo/Referencia: S145-15IIL-82DJ0005BR&lt;br /&gt;&lt;br /&gt;Certificação: Recertificado&lt;br /&gt;&lt;br /&gt;Medalha: Prata&lt;br /&gt;&lt;br /&gt;FICHA TÉCNICA:&lt;br /&gt;&lt;br /&gt;Sistema operacional: Windows 10 Home &lt;br /&gt;&lt;br /&gt;Processador: Intel Core i5-1035G1– Quad Care ( 8 Threads)- Frequência: 1.00GHz até 3.60GHz – 6 MB de Cache. &lt;br /&gt;&lt;br /&gt;Memoria: 4 GB RAM – DDR4- 2666MHz &lt;br /&gt;&lt;br /&gt;Armazenamento: 1 TB&lt;br /&gt;&lt;br /&gt;Tela: 15.6” (1366x768)&lt;br /&gt;&lt;br /&gt;Placa Gráfica: Intel UHD Graphics G1– Integrada &lt;br /&gt;&lt;br /&gt;Conectividade: Bluetooth 5.0– WiFi 802.11ac&lt;br /&gt;&lt;br /&gt;Teclado: Teclado português Brasil (ABNT) – teclado independente numérico&lt;br /&gt; &lt;br /&gt;Observação: Este produto não possui leitor de CD/DVD&lt;br /&gt;&lt;br /&gt;Entrada: Entrada para fonte de alimentação, 1x USB 2.0, 2x USB 3.1 ,1x HDMI, Leitor de cartões 4 em 1 (SD, SDHC, SDXC, MMC).&lt;br /&gt;&lt;br /&gt;Conteúdo da embalagem: Notebook, Fonte carregadora do notebook&lt;br /&gt;&lt;br /&gt;Observação: O produto não acompanha manual de instruções&lt;br /&gt;&lt;br /&gt;Garantia: 3 meses&lt;br /&gt;&lt;br /&gt;ATENÇÃO: VOCÊ ESTÁ ADQUIRINDO UM PRODUTO RECERTIFICADO!!!! &lt;br /&gt;&lt;br /&gt;O produto não acompanha caixa original, manual ou qualquer outro acessório. Apenas fonte de alimentação do notebook&lt;br /&gt;&lt;br /&gt;Entenda o que é um produto recertificado:&lt;br /&gt;&lt;br /&gt;É um produto que volta do mercado disponível para venda nas mesmas condições de um produto novo, com suas funcionalidades e características originais. O produto passa por um rigoroso processo de análise onde todas as suas funcionalidades são testadas e o produto liberado para venda. &lt;br /&gt;&lt;br /&gt;O produto recertificado é classificado em medalhas de acordo com o estado estético e superficial do produto, sendo: OURO, PRATA E BRONZE.&lt;br /&gt;&lt;br /&gt;Recertificado Prata: Produto tem características similares ao Ouro, pode apresentar mínimos riscos quase imperceptíveis. &lt;br /&gt;&lt;br /&gt;Atenção: O Saldão da Informática não enviará fotos reais dos produtos para os clientes, como também não reservaremos produtos. As imagens exibidas são meramente ilustrativas.</t>
+  </si>
+  <si>
+    <t>USADO: Notebook Lenovo Ideapad 3 Core I3 10110u, 4GB RAM, SSD 256GB, Windows 10 Pro</t>
+  </si>
+  <si>
+    <t>A voke oferece ao mercado a venda de computadores, notebooks, monitores, smartphones e tablets seminovos das marcas líderes do mercado com o objetivo de levar tecnologia e preço acessível. Bem vindos ao futuro da tecnologia!         informações principais:&lt;br&gt;- marca: lenovo&lt;br&gt;- sku: p004297-v1&lt;br&gt;- modelo: ideapad 3    - processador: intel core i3 10110u&lt;br&gt;- núcleos: 2&lt;br&gt;- threads: 4&lt;br&gt;- clock base: 2.10ghz&lt;br&gt;- clock turbo: 4.10ghz&lt;br&gt;- cache: 4mb&lt;br&gt;- tecnologia hyper-threading&lt;br&gt;- arquitetura comet lake&lt;br&gt;- fabricação em 10nm&lt;br&gt;&lt;br&gt;- placa gráfica: intel uhd graphics&lt;br&gt;- memória placa gráfica: 2gb&lt;br&gt;- suporte a directx 12&lt;br&gt;- suporte a opengl 4.5&lt;br&gt;- suporte a opencl 3.0&lt;br&gt;- suporte a api vulkan&lt;br&gt;- intel clear video hd, intel quick sync video, intel wireless display (widi)    - memória ram: 4gb&lt;br&gt;- tipo: ddr4&lt;br&gt;- clock: 2666mhz&lt;br&gt;- slots de memória: 1x dimm (expansível até 12gb)    - armazenamento: ssd 256gb    - sistema operacional: windows 10 pro    - tamanho da tela: 15,6´´&lt;br&gt;- tipo de tela: lcd&lt;br&gt;- revestimento anti-reflexo&lt;br&gt;- resolução da tela: 1280x720    - conexões:&lt;br&gt;- 1x usb 2.0&lt;br&gt;- 1x usb 3.0&lt;br&gt;- 1x hdmi&lt;br&gt;- 1x porta p3    - mais informações: consulte ficha técnica do anuncio ou entre em contato         - multímidia:&lt;br&gt;- alto falantes,&lt;br&gt;- microfone,&lt;br&gt;- entrada fone de ouvido,&lt;br&gt;- entrada microfone,&lt;br&gt;- webcam hd.         itens testados:&lt;br&gt;- teclado,&lt;br&gt;- tela,&lt;br&gt;- fonte,&lt;br&gt;- entradas,&lt;br&gt;- memória.         conteúdo da embalagem:&lt;br&gt;- 1x notebook&lt;br&gt;- 1x fonte (original ou genérica),&lt;br&gt;- não acompanha manual de instruções         obs sobre a bateria:&lt;br&gt;a autonomia da bateria poderá variar dependendo da configuração, dos aplicativos carregados, das configurações de energia e dos recursos utilizados. Os equipamentos podem trazer baterias proprio ou genéricas, testadas e revisadas por nossa equipe técnica. Ressaltamos que a bateria poderá não apresentar a mesma vida útil de um produto fechado.         sobre o produto:&lt;br&gt;- produto seminovo,&lt;br&gt;- acompanha nota fiscal,&lt;br&gt;- imagens ilustrativas,&lt;br&gt;- testado, configurado e higienizado,&lt;br&gt;- enviado nas embalagens da voke garantindo a proteção do produto,&lt;br&gt;- a voke não envia/comercializa produtos com tela quebrada e botões quebrados,&lt;br&gt;- as imagens são meramente ilustrativas. Podem ocorrer variação de formato, tamanho, cor e condição de uso.&lt;br&gt;- não nos responsabilizamos por sistema operacional, podendo existir ou não possibilidade de atualização.&lt;br&gt;- item sujeito a alteração. Para recursos como entrada de cd room, memória e informações adicionais não descritos no anuncio por favor entre em contato para confirmação         garantia:&lt;br&gt;****6 meses de garantia diretamente com a nossa loja voke***   &lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;memória ram:&lt;/strong&gt; 4gb&lt;br&gt;&lt;strong&gt;special price from date:&lt;/strong&gt; 2022-11-16 00:00:00&lt;br&gt;&lt;strong&gt;conectividade:&lt;/strong&gt; wifi&lt;br&gt;&lt;strong&gt;tipo de teclado:&lt;/strong&gt; abnt2&lt;br&gt;&lt;strong&gt;código anatel:&lt;/strong&gt; 041361904423&lt;br&gt;&lt;strong&gt;garantia:&lt;/strong&gt; 6 meses&lt;br&gt;&lt;strong&gt;estado:&lt;/strong&gt; seminovo&lt;br&gt;&lt;strong&gt;ean:&lt;/strong&gt; 7895145747247&lt;br&gt;&lt;strong&gt;tamanho da tela:&lt;/strong&gt; 15,6´´&lt;br&gt;&lt;strong&gt;memória interna:&lt;/strong&gt; 256gb&lt;br&gt;&lt;strong&gt;condição:&lt;/strong&gt; muito bom&lt;br&gt;&lt;strong&gt;correios height:&lt;/strong&gt; 27&lt;br&gt;&lt;strong&gt;modelo:&lt;/strong&gt; ideapad 3&lt;br&gt;&lt;strong&gt;conteúdo da embalagem:&lt;/strong&gt; 1x notebook1x fonte de energia&lt;br&gt;&lt;strong&gt;correios width:&lt;/strong&gt; 27&lt;br&gt;&lt;strong&gt;processador:&lt;/strong&gt; intel core i3 10110u&lt;br&gt;&lt;strong&gt;sistema operacional:&lt;/strong&gt; windows 10 pro&lt;br&gt;&lt;strong&gt;categories:&lt;/strong&gt; [2, 493, 494, 495, 496, 498, 500, 502, 504, 506, 531, 539]</t>
+  </si>
+  <si>
+    <t>USADO: Notebook Hp Probook 640 G2 Core I5 6300u, 4GB RAM, SSD 120GB - Windows 10 Pro</t>
+  </si>
+  <si>
+    <t>Bem vindos ao futuro da tecnologia - agasus agora é voke. Da união entre agasus e microcity, nos tornamos voke.&lt;br&gt;a voke oferece ao mercado a venda de computadores, notebooks, monitores, smartphones e tablets seminovos das marcas líderes do mercado com o objetivo de levar tecnologia e preço acessível.         informações principais:&lt;br&gt;- marca: hp&lt;br&gt;- sku: p004169-v1&lt;br&gt;- modelo: probook 640 g2&lt;br&gt;- processador: intel core i5 6300u&lt;br&gt;- placa gráfica: intel hd graphics 520&lt;br&gt;- memória ram: 4gb&lt;br&gt;- disco rígido: ssd 256gb&lt;br&gt;- sistema operacional: windows 10 pro &lt;br&gt;- tamanho da tela: 14 polegadas&lt;br&gt;- tela: antireflexo&lt;br&gt;- resolução da tela: 1366x768 pixels&lt;br&gt;- conexões: vga/displayport/bluetooth 4.1/usb 3.0/ethernet&lt;br&gt;- mais informações: consulte ficha técnica do anuncio ou entre em contato         multimídia:&lt;br&gt;- alto falantes,&lt;br&gt;- microfone,&lt;br&gt;- entrada fone de ouvido,&lt;br&gt;- entrada microfone,&lt;br&gt;- webcam hd 720p.         unidades opticas:&lt;br&gt;- sata 9,5 mm fixa&lt;br&gt;- unidade dvd-rom&lt;br&gt;- dvd+/-rw supermulti dl&lt;br&gt;- blu-ray rom dvd+/-rw supermulti dl&lt;br&gt;- economizador de peso         itens testados:&lt;br&gt;- teclado,&lt;br&gt;- tela,&lt;br&gt;- fonte,&lt;br&gt;- entradas,&lt;br&gt;- memória.         conteúdo da embalagem:&lt;br&gt;- 1x notebook&lt;br&gt;- 1x fonte (original ou genérica),&lt;br&gt;- não acompanha manual de instruções         &lt;br&gt;obs sobre a bateria:&lt;br&gt;a autonomia da bateria poderá variar dependendo da configuração, dos aplicativos carregados, das configurações de energia e dos recursos utilizados. Os equipamentos podem trazer baterias proprio ou genéricas, testadas e revisadas por nossa equipe técnica. Ressaltamos que a bateria poderá não apresentar a mesma vida útil de um produto fechado.         sobre o produto:&lt;br&gt;- produto seminovo,&lt;br&gt;- acompanha nota fiscal,&lt;br&gt;- imagens ilustrativas,&lt;br&gt;- testado, configurado e higienizado,&lt;br&gt;- enviado nas embalagens da agasus garantindo a proteção do produto,&lt;br&gt;- a agasus não envia/comercializa produtos com tela quebrada e botões quebrados,&lt;br&gt;- as imagens são meramente ilustrativas. Podem ocorrer variação de formato, tamanho, cor e condição de uso.&lt;br&gt;- não nos responsabilizamos por sistema operacional, podendo existir ou não possibilidade de atualização.&lt;br&gt;- item sujeito a alteração. Para recursos como entrada de cd room, memória e informações adicionais não descritos no anuncio por favor entre em contato para confirmação         garantia:&lt;br&gt;****6 meses de garantia diretamente com a nossa loja voke***   &lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;conteúdo da embalagem:&lt;/strong&gt; 1x notebook 1x fonte&lt;br&gt;&lt;strong&gt;special price from date:&lt;/strong&gt; 2022-10-03 00:00:00&lt;br&gt;&lt;strong&gt;ean:&lt;/strong&gt; 7895145742525&lt;br&gt;&lt;strong&gt;correios height:&lt;/strong&gt; 27&lt;br&gt;&lt;strong&gt;correios width:&lt;/strong&gt; 27&lt;br&gt;&lt;strong&gt;modelo:&lt;/strong&gt; probook 640 g2&lt;br&gt;&lt;strong&gt;sistema operacional:&lt;/strong&gt; windows 10 pro&lt;br&gt;&lt;strong&gt;processador:&lt;/strong&gt; intel core i5&lt;br&gt;&lt;strong&gt;conectividade:&lt;/strong&gt; wifi&lt;br&gt;&lt;strong&gt;memória ram:&lt;/strong&gt; 4gb&lt;br&gt;&lt;strong&gt;código anatel:&lt;/strong&gt; 026071502198&lt;br&gt;&lt;strong&gt;garantia:&lt;/strong&gt; 6 meses&lt;br&gt;&lt;strong&gt;tipo de teclado:&lt;/strong&gt; abnt2&lt;br&gt;&lt;strong&gt;condição:&lt;/strong&gt; muito bom&lt;br&gt;&lt;strong&gt;tamanho da tela:&lt;/strong&gt; 14´´&lt;br&gt;&lt;strong&gt;estado:&lt;/strong&gt; seminovo&lt;br&gt;&lt;strong&gt;categories:&lt;/strong&gt; [2, 493, 494, 495, 496, 498, 499, 500, 502, 515, 539, 506, 792]&lt;br&gt;&lt;strong&gt;memória interna:&lt;/strong&gt; 256gb</t>
+  </si>
+  <si>
+    <t>R$1749.0</t>
+  </si>
+  <si>
+    <t>Notebook Asus Vivobook, Intel Core I3-1220p 3.3GHz, 4GB, SSD 256GB, Intel UHD Graphics, Tela 15.6 LED Full HD, Windows 11 Home, Prata Metálico - X1502za-Ej1764w</t>
+  </si>
+  <si>
+    <t>O asus vivobook 15 &amp;eacute, o seu companheiro di&amp;aacute,rio que est&amp;aacute, sempre pronto para a a&amp;ccedil,&amp;atilde,o, seja no escrit&amp;oacute,rio ou em casa. Capaz de encarar as tarefas mais exigentes, este vivobook vem equipado com at&amp;eacute, o mais recente processador intel core i3-1220p de 12&amp;ordf, gera&amp;ccedil,&amp;atilde,o, significativamente mais r&amp;aacute,pido do que a gera&amp;ccedil,&amp;atilde,o anterior. E com 4gb de mem&amp;oacute,ria ram e 256gb de armazenamento ssd, &amp;eacute, capaz de ir al&amp;eacute,m e entregar toda a produtividade que voc&amp;ecirc, necessita.part number: 90nb0vx2-m02jh0sku asus: x1502za-ej1764wean code: 7898573299463c&amp;oacute,digo de homologa&amp;ccedil,&amp;atilde,o anatel: 06446-16-04076processador intel core i3 1220p 3,3 ghz, 12 mb cachemem&amp;oacute,ria ram: 4 gb (4 gb onboard + 0 gb offboard)armazenamento: 256 gb ssd pcie g3x2tela 15,60´´ led-backlit anti-glareresolu&amp;ccedil,&amp;atilde,o da tela: 1920 x 1080placa de v&amp;iacute,deo: intel uhd graphicsgarantia: 12 mesestela sens&amp;iacute,vel ao toque: n&amp;atilde,oclock de mem&amp;oacute,ria: 3200 mhzwi-fi 5tipo da placa de v&amp;iacute,deo: integradateclado retro iluminado: n&amp;atilde,oc&amp;acirc,mera frontal: hdbluetooth 5,1cart&amp;atilde,o de mem&amp;oacute,ria: n&amp;atilde,o&amp;aacute,udio:sonicmasteralto-falantes embutidosmicrofone embutidosa&amp;iacute,das:1x hdmi 1.41x 3.5mm combo audio jack1x dc-in1x usb 2.0 type-a1x usb 3.2 gen 1 type-c2x usb 3.2 gen 1 type-aadaptador de energia65,00 wbateria3 cells / 4000 mahsistema operacional windows 11 homecaracter&amp;iacute,sticas:especifica&amp;ccedil,&amp;otilde,es militares us mil-std 810hprote&amp;ccedil,&amp;atilde,o antibacterianatampa de privacidade para a webcampeso do produto: 1,7 kgdimens&amp;otilde,es: 35,97 cm x 23,25 cm x 1,99 ~ 1,99 cm&lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;tela:&lt;/strong&gt; 15,60´´ led-backlit anti-glare&lt;br&gt;&lt;strong&gt;wi-fi:&lt;/strong&gt; wi-fi 5(802.11ac) (dual band) 1*1 + bluetooth® 5.1&lt;br&gt;&lt;strong&gt;saídas:&lt;/strong&gt; 1x hdmi 1.41x 3.5mm combo audio jack1x dc-in1x usb 2.0 type-a1x usb 3.2 gen 1 type-c2x usb 3.2 gen 1 type-a&lt;br&gt;&lt;strong&gt;sku asus:&lt;/strong&gt; x1502za-ej1764w&lt;br&gt;&lt;strong&gt;clock de memória:&lt;/strong&gt; 3200 mhz&lt;br&gt;&lt;strong&gt;ean code:&lt;/strong&gt; 7898573299463&lt;br&gt;&lt;strong&gt;tela sensível ao toque:&lt;/strong&gt; não&lt;br&gt;&lt;strong&gt;câmera frontal:&lt;/strong&gt; hd&lt;br&gt;&lt;strong&gt;cartão de memória:&lt;/strong&gt; não&lt;br&gt;&lt;strong&gt;bateria:&lt;/strong&gt; 3 cells / 4000 mah&lt;br&gt;&lt;strong&gt;garantia:&lt;/strong&gt; 12 meses&lt;br&gt;&lt;strong&gt;adaptador de energia:&lt;/strong&gt; 65,00 w.&lt;br&gt;&lt;strong&gt;bluetooth:&lt;/strong&gt; bluetooth 5,1&lt;br&gt;&lt;strong&gt;áudio:&lt;/strong&gt; sonicmasteralto-falantes embutidosmicrofone embutido&lt;br&gt;&lt;strong&gt;teclado retro iluminado:&lt;/strong&gt; não&lt;br&gt;&lt;strong&gt;sistema operacional:&lt;/strong&gt; windows 11 home&lt;br&gt;&lt;strong&gt;armazenamento:&lt;/strong&gt; 256 gb ssd pcie g3x2&lt;br&gt;&lt;strong&gt;peso do produto:&lt;/strong&gt; 1,7 kg&lt;br&gt;&lt;strong&gt;resolução da tela:&lt;/strong&gt; 1920 x. 1080&lt;br&gt;&lt;strong&gt;software:&lt;/strong&gt; system diagnosisbattery health charging fan profilesplendidtru2lifefunction key lockwifi smartconnect link to myasustaskfirstlive updateasus intelligent performance technologyai noise cancelingmyasusscreenxpertglidex&lt;br&gt;&lt;strong&gt;dimensões:&lt;/strong&gt; 35,97 cm x. 23,25 cm x. 1,99 ~. 1,99 cm&lt;br&gt;&lt;strong&gt;características:&lt;/strong&gt; especificações militares us mil-std 810hproteção antibacterianatampa de privacidade para a. Webcam&lt;br&gt;&lt;strong&gt;placa de vídeo:&lt;/strong&gt; intel® uhd graphics&lt;br&gt;&lt;strong&gt;memória ram:&lt;/strong&gt; 4 gb (4 gb onboard + 0 gb offboard)&lt;br&gt;&lt;strong&gt;cor:&lt;/strong&gt; prata metálico&lt;br&gt;&lt;strong&gt;processador:&lt;/strong&gt; intel® core™ i3 1220p 3,3 ghz, 12 mb cache&lt;br&gt;&lt;strong&gt;codigo de homologação anatel:&lt;/strong&gt; 06446-16-04076</t>
+  </si>
+  <si>
+    <t>R$2948.21</t>
+  </si>
+  <si>
+    <t>R$2348.13</t>
+  </si>
+  <si>
+    <t>Notebook Ultra Multilaser, Core I5 8Gb, 1Tb, 14.1'' Polegadas, Windows 10 - Ub531</t>
+  </si>
+  <si>
+    <t>Notebook Ultra conta com Windows 10 Home, para quem busca mais performance para realizar suas tarefas. O desempenho notável do Notebook Ultra é possível graças ao processador Intel Core i5, e o Windows 10 Home. Ideal para tarefas do dia a dia e navegação na internet.   Além disso ele vem com: 1TB HDD e 8GB de RAM. Para mais espaço. Design leve e fino, com tela HD e imagens mais nítidas.</t>
+  </si>
+  <si>
+    <t>R$2518.9</t>
+  </si>
+  <si>
+    <t>Notebook Asus Vivobook Go E1504fa, AMD Ryzen 5 7520u, 8GB RAM, 256GB SSD, Windows 11, Tela 15,6 Polegadas, FULL HD, Black - Nj825w</t>
+  </si>
+  <si>
+    <t>&amp;eacute, leve. &amp;eacute, compacto. &amp;eacute, o asus vivobook go 15. Projetado para torn&amp;aacute,-lo produtivo e mant&amp;ecirc,-lo entretido onde quer que voc&amp;ecirc, v&amp;aacute,! Com processador amd ryzen 5 7520u de excelente desempenho, 8gb de mem&amp;oacute,ria ram lpddr51 e 256 gb de ssd2 , ele &amp;eacute, perfeito para seu dia a dia. Ainda conta com uma dobradi&amp;ccedil,a plana de 180&amp;deg,, tampa f&amp;iacute,sica protetora na webcam e muitos recursos de design bem pensados &amp;mdash, incluindo uma tela de 15 polegadas antirreflexo full hd &amp;mdash, tudo para que voc&amp;ecirc, v&amp;aacute, al&amp;eacute,m!part number: 90nb0zr2-m01by0sku asus: e1504fa-nj825wean code: 7898573299647c&amp;oacute,digo de homologa&amp;ccedil,&amp;atilde,o anatel: 06446-16-04076processador amd ryzen 5 7520u 2,8 ghz, 4 mb cachemem&amp;oacute,ria ram: 8 gb (8 gb onboard + 0 gb offboard)armazenamento: 256 gb ssd pcie g3x2tela 15,60´´ led-backlit anti-glareresolu&amp;ccedil,&amp;atilde,o da tela: 1920x1080placa de v&amp;iacute,deo: amd radeon graphicsgarantia: 12 mesestela sens&amp;iacute,vel ao toque: n&amp;atilde,oclock de mem&amp;oacute,ria: 5500 mhzwi-fi 5(802.11ac) (dual band) 1*1 + bluetooth 5.1tipo da placa de v&amp;iacute,deo: integradateclado retro iluminado: n&amp;atilde,oc&amp;acirc,mera frontal: hdbluetooth 5,1cart&amp;atilde,o de mem&amp;oacute,ria: n&amp;atilde,oaudio:sonicmasteralto-falantes embutidosmicrofone embutidosaidas:1x usb 2.0 type-a1x usb 3.2 gen 1 type-a1x usb 3.2 gen 1 type-c1x hdmi 1.41x 3.5mm combo audio jack1x dc-inadaptador de energia 45,00 wbateria 3 cells / 4000 mahsistema operacional windows 11 homecaracter&amp;iacute,sticas:especifica&amp;ccedil,&amp;otilde,es militares us mil-std 810htampa de privacidade para a webcampeso do produto: 1,63 kgdimens&amp;otilde,es: 36,03 cm x 23,25 cm x 1,79 ~ 1,79 cm&lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;software:&lt;/strong&gt; system diagnosisbattery health chargingfan profilesplendidfunction key lockwifi smartconnect link to myasustaskfirstlive updateai noise canceling&lt;br&gt;&lt;strong&gt;clock de memória:&lt;/strong&gt; 5500 mhz&lt;br&gt;&lt;strong&gt;adaptador de energia:&lt;/strong&gt; 45,00 w.&lt;br&gt;&lt;strong&gt;teclado retro iluminado:&lt;/strong&gt; não&lt;br&gt;&lt;strong&gt;tela sensível ao toque:&lt;/strong&gt; não&lt;br&gt;&lt;strong&gt;saídas:&lt;/strong&gt; 1x usb 2.0 type-a1x usb 3.2 gen 1 type-a1x usb 3.2 gen 1 type-c1x hdmi 1.41x 3.5mm combo audio jack1x dc-in&lt;br&gt;&lt;strong&gt;dimensões:&lt;/strong&gt; 36,03 cm x. 23,25 cm x. 1,79 ~. 1,79 cm&lt;br&gt;&lt;strong&gt;código de homologação anatel:&lt;/strong&gt; 06446-16-04076&lt;br&gt;&lt;strong&gt;câmera frontal:&lt;/strong&gt; hd&lt;br&gt;&lt;strong&gt;áudio:&lt;/strong&gt; sonicmasteralto-falantes embutidosmicrofone embutido&lt;br&gt;&lt;strong&gt;bluetooth:&lt;/strong&gt; bluetooth 5,1&lt;br&gt;&lt;strong&gt;sku asus:&lt;/strong&gt; e1504fa-nj825w&lt;br&gt;&lt;strong&gt;wi-fi:&lt;/strong&gt; wi-fi 5(802.11ac) (dual band) 1*1 + bluetooth® 5.1&lt;br&gt;&lt;strong&gt;ean code:&lt;/strong&gt; 7898573299647&lt;br&gt;&lt;strong&gt;bateria:&lt;/strong&gt; 3 cells / 4000 mah&lt;br&gt;&lt;strong&gt;garantia:&lt;/strong&gt; 12 meses&lt;br&gt;&lt;strong&gt;sistema operacional:&lt;/strong&gt; windows 11 home&lt;br&gt;&lt;strong&gt;cor:&lt;/strong&gt; preto&lt;br&gt;&lt;strong&gt;memória ram:&lt;/strong&gt; 8 gb (8 gb onboard + 0 gb offboard)&lt;br&gt;&lt;strong&gt;processador:&lt;/strong&gt; amd ryzen™ 5 7520u 2,8 ghz, 4 mb cache&lt;br&gt;&lt;strong&gt;armazenamento:&lt;/strong&gt; 256 gb ssd pcie g3x2&lt;br&gt;&lt;strong&gt;tela:&lt;/strong&gt; 15,60´´ led-backlit anti-glare&lt;br&gt;&lt;strong&gt;peso do produto:&lt;/strong&gt; 1,63 kg&lt;br&gt;&lt;strong&gt;resolução da tela:&lt;/strong&gt; 1920x1080&lt;br&gt;&lt;strong&gt;cartão de memória:&lt;/strong&gt; não&lt;br&gt;&lt;strong&gt;placa de vídeo:&lt;/strong&gt; amd radeon™ graphics&lt;br&gt;&lt;strong&gt;características:&lt;/strong&gt; especificações militares us mil-std 810htampa de privacidade para a. Webcam&lt;br&gt;&lt;strong&gt;manufacturer:&lt;/strong&gt; asus&lt;br&gt;&lt;strong&gt;mfrpartnumber:&lt;/strong&gt; e1504fa-nj825w&lt;br&gt;&lt;strong&gt;harddrivesize:&lt;/strong&gt; 256 gb ssd pcie g3x2&lt;br&gt;&lt;strong&gt;operatingsystem:&lt;/strong&gt; windows 11 home&lt;br&gt;&lt;strong&gt;processorbrand:&lt;/strong&gt; amd&lt;br&gt;&lt;strong&gt;processorspeed:&lt;/strong&gt; 2,8 ghz&lt;br&gt;&lt;strong&gt;ramsize:&lt;/strong&gt; 8 gb</t>
+  </si>
+  <si>
+    <t>Notebook Ultra Linux Intel I3, 256GB, 8GB RAM, 14,1 Polegadas, FULL HD,Preto - Ul151lx</t>
+  </si>
+  <si>
+    <t>Notebook ultra linux intel i3 256gb 8gb ram 14,1 pol. Full hd preto - ul151lx&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  notebook ultra, vem com linux, para você aproveitar ao máximo todos os recursos disponíveis. &lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  com ssd m.2 de 256gb de armazenamento. Muito mais espaço para seus vídeos, músicas e fotos ou que é mais essencial para você.&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  conta com 8gb de ram para você ter mais velocidade no recebimento de informações, tela de 14.1 hd para você ter imagens nítidas e vivas para uma experiência completa e surpreendente. Desenvolvida com bateria de longa duração, processador  intel core i3 de décima geração com alta velocidade e desempenho, da produtividade ao entretenimento, com o armazenamento de alta performance você terá muito mais rapidez no acesso a seus arquivos. Possui design ultraleve e superfino para você levar em qualquer lugar, transferência rápida de arquivos pelo usb 3.0 e usb tipo c.&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  ficha técnica&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  marca: ultra&lt;br /&gt;&lt;br /&gt;  modelo: notebook ultra linux intel i3 256gb 8gb ram 14,1 pol. Full hd preto - ul151lx&lt;br /&gt;&lt;br /&gt;  cor: preto&lt;br /&gt;&lt;br /&gt;  tela: 14,1 pol&lt;br /&gt;&lt;br /&gt;  sistema operacional: linux&lt;br /&gt;&lt;br /&gt;  processador: intel core i3&lt;br /&gt;&lt;br /&gt;  conexão: usb, bluetooth, p2sd&lt;br /&gt;&lt;br /&gt;  memória ram: 8gb&lt;br /&gt;&lt;br /&gt;  armazenamento: ssd m.2 de 256gb&lt;br /&gt;&lt;br /&gt;  câmera principal: 1mp&lt;br /&gt;&lt;br /&gt;  bateria: 4500mah 11,1v, 50whr carregador ac/dc bi-volt (110v-240v-50hz-60hz) com cabo de alimentação elétrica padrão brasileiro nbr14136:2002&lt;br /&gt;&lt;br /&gt;  áudio: hd áudio com controladora de som integrada a placa-mãe amplificada 2x alto-falantes 1w&lt;br /&gt;&lt;br /&gt;  entradas: 1x usb 3.0 gen 1, 1x usb 2.0, 1x usb type-c, 1x hdmi, 1xdc-in, 1x áudio combo, 1x rj45 ethernet, 1x microsd card reader&lt;br /&gt;&lt;br /&gt;  dimensões (lxaxc): 37 x 9 x 43cm&lt;br /&gt;&lt;br /&gt;  peso: 3500g&lt;br /&gt;&lt;br /&gt;  certificado anatel: 02143-18-04423&lt;br /&gt;&lt;br /&gt;  garantia: 1 ano&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  imagens meramente ilustrativas.</t>
+  </si>
+  <si>
+    <t>Notebook Ultra Intel Core I3, 8GB, SSD 256GB M.2, Tela 14.1 Full HD, Windows 11 Pro, Preto - Ul151l</t>
+  </si>
+  <si>
+    <t>Notebook ultra windows 11 pro intel i3 256gb 8gb ram 14,1 pol. Full hd preto - ul151l&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  notebook ultra, vem com o windows 11 pro, para você aproveitar ao máximo todos os recursos disponíveis. &lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  com ssd m.2 de 256gb de armazenamento. Muito mais espaço para seus vídeos, músicas e fotos ou que é mais essencial para você.&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  conta com 8gb de ram para você ter mais velocidade no recebimento de informações, tela de 14.1 hd para você ter imagens nítidas e vivas para uma experiência completa e surpreendente.&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  desenvolvida com bateria de longa duração, processador intel core i3 de décima geração com alta velocidade e desempenho, da produtividade ao entretenimento, com o armazenamento de alta performance você terá muito mais rapidez no acesso a seus arquivos. Possui design ultraleve e superfino para você levar em qualquer lugar, transferência rápida de arquivos pelo usb 3.0 e usb tipo c.&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  ficha técnica&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  marca: ultra&lt;br /&gt;&lt;br /&gt;  modelo: notebook ultra windows 11 pro intel i3 256gb 8gb ram 14,1 pol. Full hd preto - ul151l&lt;br /&gt;&lt;br /&gt;  cor: preto&lt;br /&gt;&lt;br /&gt;  tela: 14,1 polegadas&lt;br /&gt;&lt;br /&gt;  resolução: 1366 x 768&lt;br /&gt;&lt;br /&gt;  memória ram: 8gb ddr &lt;br /&gt;&lt;br /&gt;  memória interna: 256gb ssd&lt;br /&gt;&lt;br /&gt;  processador: intel core i3&lt;br /&gt;&lt;br /&gt;  sistema operacional: windows 11 pro &lt;br /&gt;&lt;br /&gt;  bateria: 4000 mah&lt;br /&gt;&lt;br /&gt;  áudio: hd com controladora de som integrada a placa mãe amplificada&lt;br /&gt;&lt;br /&gt;  portas: 1x usb 3.0, 1x usb 2.0, 1x usb tipo c, 1x áudio combo (microfone/fone) jack, 1x rj, 1x micro sd, 1x hdmi, 1x dc&lt;br /&gt;&lt;br /&gt;  teclado: padrão abnt2&lt;br /&gt;&lt;br /&gt;  câmera: frontal hd 1m&lt;br /&gt;&lt;br /&gt;  microfone: 2x d-mic integrados a câmera&lt;br /&gt;&lt;br /&gt;  dimensões (lxaxc): 32,26 x 2,08 x 22,35 cm&lt;br /&gt;&lt;br /&gt;  peso: 1,510kg&lt;br /&gt;&lt;br /&gt;  anatel: 02143-18-04423&lt;br /&gt;&lt;br /&gt;  garantia: 1 ano&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  imagens meramente ilustrativas.</t>
+  </si>
+  <si>
+    <t>R$2456.9</t>
+  </si>
+  <si>
+    <t>Notebook Positivo Vision C14, Intel Celeron Dual Core, 8GB, SSD 240GB, Tela 14 HD, Linux, Lumina Bar, Cinza</t>
+  </si>
+  <si>
+    <t>Descubra a nova linha de notebooks positivo vision, perfeito para todas as suas atividades diárias! Desenvolvido com foco em praticidade, ele é ideal para tarefas leves como planilhas, edição de texto e navegação na web. Além disso, você poderá desfrutar de videochamadas com sua câmera de alta definição. Suporta softwares de ensino e ferramentas básicas de trabalho, o positivo vision garante que você esteja sempre pronto para alcançar seus objetivos. Não perca tempo, experimente o poder da nova linha positivo vision e eleve suas atividades diárias a um novo nível de eficiência. &lt;br /&gt;&lt;br /&gt;A positivo tecnologia inova no mercado ao lançar a primeira linha de notebooks do mundo com a tecnologia lumina bar, oferecendo uma experiência superior aos usuários. Os notebooks possuem barras de led com ajuste de 3 níveis de intensidade, proporcionando uma iluminação ideal para a webcam, resultando em uma captura de imagem excepcional mesmo em ambientes com pouca iluminação. Tecla link exclusiva para conectar o celular ao notebook de uma forma mais simples. Sincronização de fotos, salvamento de imagens com facilidade, visualização de mensagens sms, status da bateria, entre outras funcionalidades com apenas um toque. &lt;br /&gt;&lt;br /&gt;Além disso, as teclas serigrafadas são um destaque adicional. Com letras nítidas e visíveis, projetadas para facilitar a digitação e auxiliar você em todas as suas tarefas diárias. Agora você pode digitar com confiança, mesmo em ambientes com pouca luz. Para acompanhar seu estilo de vida em movimento, o dispositivo é alimentado por uma bateria de longa duração, com uma média de 7 horas* de autonomia. Isso o torna ideal para atividades fora de casa, como levar para a escola ou faculdade, permitindo que você trabalhe ou estude sem se preocupar em encontrar uma tomada. Afinal, o vision c14 é leve, fino e portátil, pesando apenas 1,4 kg e espessura de 18,7 mm. Isso significa que você pode levá-lo para qualquer lugar com facilidade.</t>
+  </si>
+  <si>
     <t>Notebook Positivo Motion C, Intel Celeron, Dual-Core, 4GB, SSD 120GB, 14'' LED - Windows 11</t>
   </si>
   <si>
@@ -1696,100 +1759,22 @@
     <t>R$2173.99</t>
   </si>
   <si>
-    <t>Notebook Asus, Intel Dual Core, 4GB, 500hd, Tela 15,6 Polegadas,Windows 10 - X543na</t>
-  </si>
-  <si>
-    <t>O notebook asus vivobook x543na tem design clássico, com acabamento escovado em cinza escuro, superelegante e o melhor de tudo, tem apenas 1,9kg, perfeito para você que precisa sair e levar o computador, mas também quer tela grande para aumentar a produtividade.&lt;br /&gt;&lt;br /&gt;  com o asus vivobook x543, você não será mais um na multidão. Se o seu objetivo é relaxar, aproveite o sistema de som superpoderoso do asus vivobook x543na.&lt;br /&gt;&lt;br /&gt;  ele usa cada milímetro do seu chassis para reproduzir graves mais impactantes e sem ruídos. A caixa de ressonância de 19,4cc torna o som cristalino e incrivelmente realista.&lt;br /&gt;&lt;br /&gt;  se você já teve a experiência de digitar em um teclado pequeno, sabe que não é confortável, não é produtivo e é isso que te faz parar. Então, se o seu objetivo for trabalhar, o asus vivobook será seu parceiro incansável. Ele tem teclado completo, com teclas grandes e com curso de 1,8 milímetros, que é ideal para tornar a digitação ágil, precisa e confortável.&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  características: &lt;br /&gt;&lt;br /&gt;  modelo: x543na-gq342t&lt;br /&gt;&lt;br /&gt;  processador: intel® celeron dual core n3350 1,1 ghz, 2 mb cache.&lt;br /&gt;&lt;br /&gt;  memória ram: 4 gb (4 gb onboard + 0 gb offboard)&lt;br /&gt;&lt;br /&gt;  armazenamento: 500 gb sata 5400 rpm&lt;br /&gt;&lt;br /&gt;  tela: 15,60 led-backlit anti-glare&lt;br /&gt;&lt;br /&gt;  resolução da tela: 1366 x 768&lt;br /&gt;&lt;br /&gt;  placa de vídeo: intel® hd graphics 500&lt;br /&gt;&lt;br /&gt;  tela sensível ao toque: não&lt;br /&gt;&lt;br /&gt;  clock de memória: 1333 mhz&lt;br /&gt;&lt;br /&gt;  wi-fi: 802.11ac&lt;br /&gt;&lt;br /&gt;  teclado retro iluminado: não&lt;br /&gt;&lt;br /&gt;  câmera frontal: vga&lt;br /&gt;&lt;br /&gt;  bluetooth: bluetooth 4,1&lt;br /&gt;&lt;br /&gt;  cartão de memória; micro sd&lt;br /&gt;&lt;br /&gt;  áudio; built-in speaker built-in microphone áudio by icepower® sonic master.&lt;br /&gt;&lt;br /&gt;  saídas: 2x usb 2.0 1x usb 3.0 1x headphone-out  audio-in combo jack 1x hdmi 1x micro sd card reader&lt;br /&gt;&lt;br /&gt;  adaptador de energia: 45,00 w&lt;br /&gt;&lt;br /&gt;  bateria; 3 cells / 2200 mah&lt;br /&gt;&lt;br /&gt;  software: asus live update asus product registration program asus giftbox asus smart gesture asus splendid asus webstorage sync agent asus icesound&lt;br /&gt;&lt;br /&gt;  sistema operacional: windows 10 home&lt;br /&gt;&lt;br /&gt;  * a memória disponível para uso pode sofrer variações conforme versão do sistema operacional, apps, conteúdo e dados instalados.&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  dimensões: &lt;br /&gt;&lt;br /&gt;  altura: 25,2 cm&lt;br /&gt;&lt;br /&gt;  largura: 38,1 cm&lt;br /&gt;&lt;br /&gt;  profundidade: 2,72 cm&lt;br /&gt;&lt;br /&gt;  peso: 1,9 kg&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  garantia do fornecedor de 12 meses.</t>
-  </si>
-  <si>
-    <t>R$2305.99</t>
-  </si>
-  <si>
-    <t>Usado - Notebook HP Probook 640 G2, Intel Core I5-6300u, 8GB, SSD 256GB, Tela 14p, Windows 10 Pro - L8u43av8gb - Seminovo</t>
-  </si>
-  <si>
-    <t>Notebook HP Probook L8U43AV8GB, processador Intel Core i5 de sexta geração, memoria RAM de 8GB, armazenamento SSD de 256GB e sistema operacional Windows 10 Pro.&lt;br /&gt;&lt;br /&gt;Modelo/Referencia: L8U43AV#8GB&lt;br /&gt;&lt;br /&gt;Certificação: Recertificado&lt;br /&gt;&lt;br /&gt;Medalha: Prata&lt;br /&gt;&lt;br /&gt;FICHA TÉCNICA:&lt;br /&gt;&lt;br /&gt;Sistema operacional: Windows 10 &lt;br /&gt;&lt;br /&gt;Processador: Intel Core i5-6300U – Dual core (4 Threads)– frequência de (2.40 GHz até 3.0GHz) - 3 MB de cache&lt;br /&gt;&lt;br /&gt;Memoria: 8 GB RAM &lt;br /&gt;&lt;br /&gt;Armazenamento: 256 GB SSD &lt;br /&gt;&lt;br /&gt;Tela: 14” &lt;br /&gt;Conteúdo da embalagem: Notebook, Fonte carregadora do notebook&lt;br /&gt;&lt;br /&gt;Observação: O produto não acompanha manual de instruções&lt;br /&gt;&lt;br /&gt;Garantia: 3 meses&lt;br /&gt;&lt;br /&gt;ATENÇÃO: VOCÊ ESTÁ ADQUIRINDO UM PRODUTO RECERTIFICADO!!!! &lt;br /&gt;&lt;br /&gt;&lt;br /&gt;O produto não acompanha caixa original, manual ou qualquer outro acessório. Apenas fonte de alimentação do notebook&lt;br /&gt;&lt;br /&gt;&lt;br /&gt;Entenda o que é um produto recertificado:&lt;br /&gt;&lt;br /&gt;É um produto que volta do mercado disponível para venda nas mesmas condições de um produto novo, com suas funcionalidades e características originais. O produto passa por um rigoroso processo de análise onde todas as suas funcionalidades são testadas e o produto liberado para venda. &lt;br /&gt;&lt;br /&gt;O produto recertificado é classificado em medalhas de acordo com o estado estético e superficial do produto, sendo: OURO, PRATA E BRONZE.&lt;br /&gt; &lt;br /&gt;Recertificado Prata: Produto tem características similares ao Ouro, pode apresentar mínimos riscos quase imperceptíveis. &lt;br /&gt;&lt;br /&gt;Atenção: O Saldão da Informática não enviará fotos reais dos produtos para os clientes, como também não reservaremos produtos. As imagens exibidas são meramente ilustrativas.</t>
-  </si>
-  <si>
-    <t>Usado - Notebook Lenovo Ideapad S145, Intel Core I5-1035g1, 4GB, 1TB, Tela 15.6p, Windows 10 - 82dj0005br - Seminovo</t>
-  </si>
-  <si>
-    <t>Notebook Lenovo IdeaPad S145 82DJ0005BR, na cor prata, processador de 10º geração Intel Core i5-1035G1 de 1.00GHz até 3.60GHz, memória RAM de 4GB DDR4, HD de 1TB, tela de 15.6 polegadas e sistema operacional Windows 10.&lt;br /&gt;&lt;br /&gt;Modelo/Referencia: S145-15IIL-82DJ0005BR&lt;br /&gt;&lt;br /&gt;Certificação: Recertificado&lt;br /&gt;&lt;br /&gt;Medalha: Prata&lt;br /&gt;&lt;br /&gt;FICHA TÉCNICA:&lt;br /&gt;&lt;br /&gt;Sistema operacional: Windows 10 Home &lt;br /&gt;&lt;br /&gt;Processador: Intel Core i5-1035G1– Quad Care ( 8 Threads)- Frequência: 1.00GHz até 3.60GHz – 6 MB de Cache. &lt;br /&gt;&lt;br /&gt;Memoria: 4 GB RAM – DDR4- 2666MHz &lt;br /&gt;&lt;br /&gt;Armazenamento: 1 TB&lt;br /&gt;&lt;br /&gt;Tela: 15.6” (1366x768)&lt;br /&gt;&lt;br /&gt;Placa Gráfica: Intel UHD Graphics G1– Integrada &lt;br /&gt;&lt;br /&gt;Conectividade: Bluetooth 5.0– WiFi 802.11ac&lt;br /&gt;&lt;br /&gt;Teclado: Teclado português Brasil (ABNT) – teclado independente numérico&lt;br /&gt; &lt;br /&gt;Observação: Este produto não possui leitor de CD/DVD&lt;br /&gt;&lt;br /&gt;Entrada: Entrada para fonte de alimentação, 1x USB 2.0, 2x USB 3.1 ,1x HDMI, Leitor de cartões 4 em 1 (SD, SDHC, SDXC, MMC).&lt;br /&gt;&lt;br /&gt;Conteúdo da embalagem: Notebook, Fonte carregadora do notebook&lt;br /&gt;&lt;br /&gt;Observação: O produto não acompanha manual de instruções&lt;br /&gt;&lt;br /&gt;Garantia: 3 meses&lt;br /&gt;&lt;br /&gt;ATENÇÃO: VOCÊ ESTÁ ADQUIRINDO UM PRODUTO RECERTIFICADO!!!! &lt;br /&gt;&lt;br /&gt;O produto não acompanha caixa original, manual ou qualquer outro acessório. Apenas fonte de alimentação do notebook&lt;br /&gt;&lt;br /&gt;Entenda o que é um produto recertificado:&lt;br /&gt;&lt;br /&gt;É um produto que volta do mercado disponível para venda nas mesmas condições de um produto novo, com suas funcionalidades e características originais. O produto passa por um rigoroso processo de análise onde todas as suas funcionalidades são testadas e o produto liberado para venda. &lt;br /&gt;&lt;br /&gt;O produto recertificado é classificado em medalhas de acordo com o estado estético e superficial do produto, sendo: OURO, PRATA E BRONZE.&lt;br /&gt;&lt;br /&gt;Recertificado Prata: Produto tem características similares ao Ouro, pode apresentar mínimos riscos quase imperceptíveis. &lt;br /&gt;&lt;br /&gt;Atenção: O Saldão da Informática não enviará fotos reais dos produtos para os clientes, como também não reservaremos produtos. As imagens exibidas são meramente ilustrativas.</t>
-  </si>
-  <si>
-    <t>USADO: Notebook Lenovo Ideapad 3 Core I3 10110u, 4GB RAM, SSD 256GB, Windows 10 Pro</t>
-  </si>
-  <si>
-    <t>A voke oferece ao mercado a venda de computadores, notebooks, monitores, smartphones e tablets seminovos das marcas líderes do mercado com o objetivo de levar tecnologia e preço acessível. Bem vindos ao futuro da tecnologia!         informações principais:&lt;br&gt;- marca: lenovo&lt;br&gt;- sku: p004297-v1&lt;br&gt;- modelo: ideapad 3    - processador: intel core i3 10110u&lt;br&gt;- núcleos: 2&lt;br&gt;- threads: 4&lt;br&gt;- clock base: 2.10ghz&lt;br&gt;- clock turbo: 4.10ghz&lt;br&gt;- cache: 4mb&lt;br&gt;- tecnologia hyper-threading&lt;br&gt;- arquitetura comet lake&lt;br&gt;- fabricação em 10nm&lt;br&gt;&lt;br&gt;- placa gráfica: intel uhd graphics&lt;br&gt;- memória placa gráfica: 2gb&lt;br&gt;- suporte a directx 12&lt;br&gt;- suporte a opengl 4.5&lt;br&gt;- suporte a opencl 3.0&lt;br&gt;- suporte a api vulkan&lt;br&gt;- intel clear video hd, intel quick sync video, intel wireless display (widi)    - memória ram: 4gb&lt;br&gt;- tipo: ddr4&lt;br&gt;- clock: 2666mhz&lt;br&gt;- slots de memória: 1x dimm (expansível até 12gb)    - armazenamento: ssd 256gb    - sistema operacional: windows 10 pro    - tamanho da tela: 15,6´´&lt;br&gt;- tipo de tela: lcd&lt;br&gt;- revestimento anti-reflexo&lt;br&gt;- resolução da tela: 1280x720    - conexões:&lt;br&gt;- 1x usb 2.0&lt;br&gt;- 1x usb 3.0&lt;br&gt;- 1x hdmi&lt;br&gt;- 1x porta p3    - mais informações: consulte ficha técnica do anuncio ou entre em contato         - multímidia:&lt;br&gt;- alto falantes,&lt;br&gt;- microfone,&lt;br&gt;- entrada fone de ouvido,&lt;br&gt;- entrada microfone,&lt;br&gt;- webcam hd.         itens testados:&lt;br&gt;- teclado,&lt;br&gt;- tela,&lt;br&gt;- fonte,&lt;br&gt;- entradas,&lt;br&gt;- memória.         conteúdo da embalagem:&lt;br&gt;- 1x notebook&lt;br&gt;- 1x fonte (original ou genérica),&lt;br&gt;- não acompanha manual de instruções         obs sobre a bateria:&lt;br&gt;a autonomia da bateria poderá variar dependendo da configuração, dos aplicativos carregados, das configurações de energia e dos recursos utilizados. Os equipamentos podem trazer baterias proprio ou genéricas, testadas e revisadas por nossa equipe técnica. Ressaltamos que a bateria poderá não apresentar a mesma vida útil de um produto fechado.         sobre o produto:&lt;br&gt;- produto seminovo,&lt;br&gt;- acompanha nota fiscal,&lt;br&gt;- imagens ilustrativas,&lt;br&gt;- testado, configurado e higienizado,&lt;br&gt;- enviado nas embalagens da voke garantindo a proteção do produto,&lt;br&gt;- a voke não envia/comercializa produtos com tela quebrada e botões quebrados,&lt;br&gt;- as imagens são meramente ilustrativas. Podem ocorrer variação de formato, tamanho, cor e condição de uso.&lt;br&gt;- não nos responsabilizamos por sistema operacional, podendo existir ou não possibilidade de atualização.&lt;br&gt;- item sujeito a alteração. Para recursos como entrada de cd room, memória e informações adicionais não descritos no anuncio por favor entre em contato para confirmação         garantia:&lt;br&gt;****6 meses de garantia diretamente com a nossa loja voke***   &lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;memória ram:&lt;/strong&gt; 4gb&lt;br&gt;&lt;strong&gt;special price from date:&lt;/strong&gt; 2022-11-16 00:00:00&lt;br&gt;&lt;strong&gt;conectividade:&lt;/strong&gt; wifi&lt;br&gt;&lt;strong&gt;tipo de teclado:&lt;/strong&gt; abnt2&lt;br&gt;&lt;strong&gt;código anatel:&lt;/strong&gt; 041361904423&lt;br&gt;&lt;strong&gt;garantia:&lt;/strong&gt; 6 meses&lt;br&gt;&lt;strong&gt;estado:&lt;/strong&gt; seminovo&lt;br&gt;&lt;strong&gt;ean:&lt;/strong&gt; 7895145747247&lt;br&gt;&lt;strong&gt;tamanho da tela:&lt;/strong&gt; 15,6´´&lt;br&gt;&lt;strong&gt;memória interna:&lt;/strong&gt; 256gb&lt;br&gt;&lt;strong&gt;condição:&lt;/strong&gt; muito bom&lt;br&gt;&lt;strong&gt;correios height:&lt;/strong&gt; 27&lt;br&gt;&lt;strong&gt;modelo:&lt;/strong&gt; ideapad 3&lt;br&gt;&lt;strong&gt;conteúdo da embalagem:&lt;/strong&gt; 1x notebook1x fonte de energia&lt;br&gt;&lt;strong&gt;correios width:&lt;/strong&gt; 27&lt;br&gt;&lt;strong&gt;processador:&lt;/strong&gt; intel core i3 10110u&lt;br&gt;&lt;strong&gt;sistema operacional:&lt;/strong&gt; windows 10 pro&lt;br&gt;&lt;strong&gt;categories:&lt;/strong&gt; [2, 493, 494, 495, 496, 498, 500, 502, 504, 506, 531, 539]</t>
-  </si>
-  <si>
-    <t>USADO: Notebook Hp Probook 640 G2 Core I5 6300u, 4GB RAM, SSD 120GB - Windows 10 Pro</t>
-  </si>
-  <si>
-    <t>Bem vindos ao futuro da tecnologia - agasus agora é voke. Da união entre agasus e microcity, nos tornamos voke.&lt;br&gt;a voke oferece ao mercado a venda de computadores, notebooks, monitores, smartphones e tablets seminovos das marcas líderes do mercado com o objetivo de levar tecnologia e preço acessível.         informações principais:&lt;br&gt;- marca: hp&lt;br&gt;- sku: p004169-v1&lt;br&gt;- modelo: probook 640 g2&lt;br&gt;- processador: intel core i5 6300u&lt;br&gt;- placa gráfica: intel hd graphics 520&lt;br&gt;- memória ram: 4gb&lt;br&gt;- disco rígido: ssd 256gb&lt;br&gt;- sistema operacional: windows 10 pro &lt;br&gt;- tamanho da tela: 14 polegadas&lt;br&gt;- tela: antireflexo&lt;br&gt;- resolução da tela: 1366x768 pixels&lt;br&gt;- conexões: vga/displayport/bluetooth 4.1/usb 3.0/ethernet&lt;br&gt;- mais informações: consulte ficha técnica do anuncio ou entre em contato         multimídia:&lt;br&gt;- alto falantes,&lt;br&gt;- microfone,&lt;br&gt;- entrada fone de ouvido,&lt;br&gt;- entrada microfone,&lt;br&gt;- webcam hd 720p.         unidades opticas:&lt;br&gt;- sata 9,5 mm fixa&lt;br&gt;- unidade dvd-rom&lt;br&gt;- dvd+/-rw supermulti dl&lt;br&gt;- blu-ray rom dvd+/-rw supermulti dl&lt;br&gt;- economizador de peso         itens testados:&lt;br&gt;- teclado,&lt;br&gt;- tela,&lt;br&gt;- fonte,&lt;br&gt;- entradas,&lt;br&gt;- memória.         conteúdo da embalagem:&lt;br&gt;- 1x notebook&lt;br&gt;- 1x fonte (original ou genérica),&lt;br&gt;- não acompanha manual de instruções         &lt;br&gt;obs sobre a bateria:&lt;br&gt;a autonomia da bateria poderá variar dependendo da configuração, dos aplicativos carregados, das configurações de energia e dos recursos utilizados. Os equipamentos podem trazer baterias proprio ou genéricas, testadas e revisadas por nossa equipe técnica. Ressaltamos que a bateria poderá não apresentar a mesma vida útil de um produto fechado.         sobre o produto:&lt;br&gt;- produto seminovo,&lt;br&gt;- acompanha nota fiscal,&lt;br&gt;- imagens ilustrativas,&lt;br&gt;- testado, configurado e higienizado,&lt;br&gt;- enviado nas embalagens da agasus garantindo a proteção do produto,&lt;br&gt;- a agasus não envia/comercializa produtos com tela quebrada e botões quebrados,&lt;br&gt;- as imagens são meramente ilustrativas. Podem ocorrer variação de formato, tamanho, cor e condição de uso.&lt;br&gt;- não nos responsabilizamos por sistema operacional, podendo existir ou não possibilidade de atualização.&lt;br&gt;- item sujeito a alteração. Para recursos como entrada de cd room, memória e informações adicionais não descritos no anuncio por favor entre em contato para confirmação         garantia:&lt;br&gt;****6 meses de garantia diretamente com a nossa loja voke***   &lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;conteúdo da embalagem:&lt;/strong&gt; 1x notebook 1x fonte&lt;br&gt;&lt;strong&gt;special price from date:&lt;/strong&gt; 2022-10-03 00:00:00&lt;br&gt;&lt;strong&gt;ean:&lt;/strong&gt; 7895145742525&lt;br&gt;&lt;strong&gt;correios height:&lt;/strong&gt; 27&lt;br&gt;&lt;strong&gt;correios width:&lt;/strong&gt; 27&lt;br&gt;&lt;strong&gt;modelo:&lt;/strong&gt; probook 640 g2&lt;br&gt;&lt;strong&gt;sistema operacional:&lt;/strong&gt; windows 10 pro&lt;br&gt;&lt;strong&gt;processador:&lt;/strong&gt; intel core i5&lt;br&gt;&lt;strong&gt;conectividade:&lt;/strong&gt; wifi&lt;br&gt;&lt;strong&gt;memória ram:&lt;/strong&gt; 4gb&lt;br&gt;&lt;strong&gt;código anatel:&lt;/strong&gt; 026071502198&lt;br&gt;&lt;strong&gt;garantia:&lt;/strong&gt; 6 meses&lt;br&gt;&lt;strong&gt;tipo de teclado:&lt;/strong&gt; abnt2&lt;br&gt;&lt;strong&gt;condição:&lt;/strong&gt; muito bom&lt;br&gt;&lt;strong&gt;tamanho da tela:&lt;/strong&gt; 14´´&lt;br&gt;&lt;strong&gt;estado:&lt;/strong&gt; seminovo&lt;br&gt;&lt;strong&gt;categories:&lt;/strong&gt; [2, 493, 494, 495, 496, 498, 499, 500, 502, 515, 539, 506, 792]&lt;br&gt;&lt;strong&gt;memória interna:&lt;/strong&gt; 256gb</t>
-  </si>
-  <si>
-    <t>R$1749.0</t>
-  </si>
-  <si>
-    <t>Notebook Lenovo Ideapad 1 R3-7320u, 8GB, 256GB, SSD, Windows 11</t>
-  </si>
-  <si>
-    <t>Esecifica&amp;ccedil,&amp;otilde,es:marca: lenovonome do produto: ideapad 1nome do modelo: ideapad 1 15amn7part number: 82x50000brcor: cloud greycategoria: notebooksegmento: ultrafinoprocessador: amd ryzen 3 7320u (cores / threads) quadcore / 8 threads (cache) 2mb l2 / 4mb l3 (clock) 2.4ghz (4.1ghz max turbo)mem&amp;oacute,ria ram: 8gb 5500mhzdetalhe mem&amp;oacute,ria ram: 8gb soldado lpddr5-5500m&amp;aacute,xima expans&amp;atilde,o da mem&amp;oacute,ria: mem&amp;oacute,ria m&amp;aacute,xima 8gb soldado lpddr5-5500armazenamento (ssd): ssd de 256gb pcie nvme m.2m&amp;aacute,xima expans&amp;atilde,o de armazenamento: um slot, at&amp;eacute, 1tb m.2 2242 ssdchipset: amd socplaca de v&amp;iacute,deo: integrada amd radeon? 610m graphicssistema operacional: windows 11tela: 15.6´´resolu&amp;ccedil,&amp;atilde,o de tela: hd (1366x768) antirreflexoformato de tela: 16:9 widescreenbrilho da tela: 220 nitstipo de painel: tnabertura de tela: 169&amp;deg,wi-fi: wifi 2x2 accamera: hd-720p com privacidademicrofone: microfone tipo dual arraybluetooth: bluetooth 5.0audio (alto-falantes): alto-falantes com certifica&amp;ccedil,&amp;atilde,o dolby&amp;reg, audio? (2 x 1.5w)audio (porta combo para headset/headphone): 1usb (3.2) gen 1: 1usb (2.0): 1usb tipo c (3.2 gen1): 1leitor de cart&amp;otilde,es: leitor de cart&amp;otilde,es 4 em 1 (sd, sdhc, sdxc, mmc)sa&amp;iacute,da hdmi ( 1.4b): 1ptp touchpad: 1teclado padr&amp;atilde,o brasileiro: 1teclado num&amp;eacute,rico: 1bateria: 3 c&amp;eacute,lulas 42whbateria remov&amp;iacute,vel: n&amp;atilde,oadaptador ac: 65wdimens&amp;otilde,es produto aprox. Largura: 360.2 mmdimens&amp;otilde,es produto aprox. Profundidade: 236 mmdimens&amp;otilde,es produto aprox. Altura: 17.9 mmpeso produto aprox. : 1.58 kgdimens&amp;otilde,es embalagem aprox. Largura: 533 mmdimens&amp;otilde,es embalagem aprox. Profundidade: 333 mmdimens&amp;otilde,es embalagem aprox. Altura: 74 mmpeso embalagem aprox.: 2.42 kg&lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;infadicional:&lt;/strong&gt; notebook lenovo ideapad 1 r3-7320u 8gb 256gb ssd windows 11 home 15,6</t>
-  </si>
-  <si>
-    <t>Notebook Asus Vivobook, Intel Core I3-1220p 3.3GHz, 4GB, SSD 256GB, Intel UHD Graphics, Tela 15.6 LED Full HD, Windows 11 Home, Prata Metálico - X1502za-Ej1764w</t>
-  </si>
-  <si>
-    <t>O asus vivobook 15 &amp;eacute, o seu companheiro di&amp;aacute,rio que est&amp;aacute, sempre pronto para a a&amp;ccedil,&amp;atilde,o, seja no escrit&amp;oacute,rio ou em casa. Capaz de encarar as tarefas mais exigentes, este vivobook vem equipado com at&amp;eacute, o mais recente processador intel core i3-1220p de 12&amp;ordf, gera&amp;ccedil,&amp;atilde,o, significativamente mais r&amp;aacute,pido do que a gera&amp;ccedil,&amp;atilde,o anterior. E com 4gb de mem&amp;oacute,ria ram e 256gb de armazenamento ssd, &amp;eacute, capaz de ir al&amp;eacute,m e entregar toda a produtividade que voc&amp;ecirc, necessita.part number: 90nb0vx2-m02jh0sku asus: x1502za-ej1764wean code: 7898573299463c&amp;oacute,digo de homologa&amp;ccedil,&amp;atilde,o anatel: 06446-16-04076processador intel core i3 1220p 3,3 ghz, 12 mb cachemem&amp;oacute,ria ram: 4 gb (4 gb onboard + 0 gb offboard)armazenamento: 256 gb ssd pcie g3x2tela 15,60´´ led-backlit anti-glareresolu&amp;ccedil,&amp;atilde,o da tela: 1920 x 1080placa de v&amp;iacute,deo: intel uhd graphicsgarantia: 12 mesestela sens&amp;iacute,vel ao toque: n&amp;atilde,oclock de mem&amp;oacute,ria: 3200 mhzwi-fi 5tipo da placa de v&amp;iacute,deo: integradateclado retro iluminado: n&amp;atilde,oc&amp;acirc,mera frontal: hdbluetooth 5,1cart&amp;atilde,o de mem&amp;oacute,ria: n&amp;atilde,o&amp;aacute,udio:sonicmasteralto-falantes embutidosmicrofone embutidosa&amp;iacute,das:1x hdmi 1.41x 3.5mm combo audio jack1x dc-in1x usb 2.0 type-a1x usb 3.2 gen 1 type-c2x usb 3.2 gen 1 type-aadaptador de energia65,00 wbateria3 cells / 4000 mahsistema operacional windows 11 homecaracter&amp;iacute,sticas:especifica&amp;ccedil,&amp;otilde,es militares us mil-std 810hprote&amp;ccedil,&amp;atilde,o antibacterianatampa de privacidade para a webcampeso do produto: 1,7 kgdimens&amp;otilde,es: 35,97 cm x 23,25 cm x 1,99 ~ 1,99 cm&lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;tela:&lt;/strong&gt; 15,60´´ led-backlit anti-glare&lt;br&gt;&lt;strong&gt;wi-fi:&lt;/strong&gt; wi-fi 5(802.11ac) (dual band) 1*1 + bluetooth® 5.1&lt;br&gt;&lt;strong&gt;saídas:&lt;/strong&gt; 1x hdmi 1.41x 3.5mm combo audio jack1x dc-in1x usb 2.0 type-a1x usb 3.2 gen 1 type-c2x usb 3.2 gen 1 type-a&lt;br&gt;&lt;strong&gt;sku asus:&lt;/strong&gt; x1502za-ej1764w&lt;br&gt;&lt;strong&gt;clock de memória:&lt;/strong&gt; 3200 mhz&lt;br&gt;&lt;strong&gt;ean code:&lt;/strong&gt; 7898573299463&lt;br&gt;&lt;strong&gt;tela sensível ao toque:&lt;/strong&gt; não&lt;br&gt;&lt;strong&gt;câmera frontal:&lt;/strong&gt; hd&lt;br&gt;&lt;strong&gt;cartão de memória:&lt;/strong&gt; não&lt;br&gt;&lt;strong&gt;bateria:&lt;/strong&gt; 3 cells / 4000 mah&lt;br&gt;&lt;strong&gt;garantia:&lt;/strong&gt; 12 meses&lt;br&gt;&lt;strong&gt;adaptador de energia:&lt;/strong&gt; 65,00 w.&lt;br&gt;&lt;strong&gt;bluetooth:&lt;/strong&gt; bluetooth 5,1&lt;br&gt;&lt;strong&gt;áudio:&lt;/strong&gt; sonicmasteralto-falantes embutidosmicrofone embutido&lt;br&gt;&lt;strong&gt;teclado retro iluminado:&lt;/strong&gt; não&lt;br&gt;&lt;strong&gt;sistema operacional:&lt;/strong&gt; windows 11 home&lt;br&gt;&lt;strong&gt;armazenamento:&lt;/strong&gt; 256 gb ssd pcie g3x2&lt;br&gt;&lt;strong&gt;peso do produto:&lt;/strong&gt; 1,7 kg&lt;br&gt;&lt;strong&gt;resolução da tela:&lt;/strong&gt; 1920 x. 1080&lt;br&gt;&lt;strong&gt;software:&lt;/strong&gt; system diagnosisbattery health charging fan profilesplendidtru2lifefunction key lockwifi smartconnect link to myasustaskfirstlive updateasus intelligent performance technologyai noise cancelingmyasusscreenxpertglidex&lt;br&gt;&lt;strong&gt;dimensões:&lt;/strong&gt; 35,97 cm x. 23,25 cm x. 1,99 ~. 1,99 cm&lt;br&gt;&lt;strong&gt;características:&lt;/strong&gt; especificações militares us mil-std 810hproteção antibacterianatampa de privacidade para a. Webcam&lt;br&gt;&lt;strong&gt;placa de vídeo:&lt;/strong&gt; intel® uhd graphics&lt;br&gt;&lt;strong&gt;memória ram:&lt;/strong&gt; 4 gb (4 gb onboard + 0 gb offboard)&lt;br&gt;&lt;strong&gt;cor:&lt;/strong&gt; prata metálico&lt;br&gt;&lt;strong&gt;processador:&lt;/strong&gt; intel® core™ i3 1220p 3,3 ghz, 12 mb cache&lt;br&gt;&lt;strong&gt;codigo de homologação anatel:&lt;/strong&gt; 06446-16-04076</t>
-  </si>
-  <si>
-    <t>R$2948.21</t>
-  </si>
-  <si>
-    <t>R$2348.13</t>
-  </si>
-  <si>
-    <t>Notebook Positivo Vision C14, Intel Celeron Dual Core, 8GB, SSD 240GB, Tela 14 HD, Linux, Lumina Bar, Cinza</t>
-  </si>
-  <si>
-    <t>Descubra a nova linha de notebooks positivo vision, perfeito para todas as suas atividades diárias! Desenvolvido com foco em praticidade, ele é ideal para tarefas leves como planilhas, edição de texto e navegação na web. Além disso, você poderá desfrutar de videochamadas com sua câmera de alta definição. Suporta softwares de ensino e ferramentas básicas de trabalho, o positivo vision garante que você esteja sempre pronto para alcançar seus objetivos. Não perca tempo, experimente o poder da nova linha positivo vision e eleve suas atividades diárias a um novo nível de eficiência. &lt;br /&gt;&lt;br /&gt;A positivo tecnologia inova no mercado ao lançar a primeira linha de notebooks do mundo com a tecnologia lumina bar, oferecendo uma experiência superior aos usuários. Os notebooks possuem barras de led com ajuste de 3 níveis de intensidade, proporcionando uma iluminação ideal para a webcam, resultando em uma captura de imagem excepcional mesmo em ambientes com pouca iluminação. Tecla link exclusiva para conectar o celular ao notebook de uma forma mais simples. Sincronização de fotos, salvamento de imagens com facilidade, visualização de mensagens sms, status da bateria, entre outras funcionalidades com apenas um toque. &lt;br /&gt;&lt;br /&gt;Além disso, as teclas serigrafadas são um destaque adicional. Com letras nítidas e visíveis, projetadas para facilitar a digitação e auxiliar você em todas as suas tarefas diárias. Agora você pode digitar com confiança, mesmo em ambientes com pouca luz. Para acompanhar seu estilo de vida em movimento, o dispositivo é alimentado por uma bateria de longa duração, com uma média de 7 horas* de autonomia. Isso o torna ideal para atividades fora de casa, como levar para a escola ou faculdade, permitindo que você trabalhe ou estude sem se preocupar em encontrar uma tomada. Afinal, o vision c14 é leve, fino e portátil, pesando apenas 1,4 kg e espessura de 18,7 mm. Isso significa que você pode levá-lo para qualquer lugar com facilidade.</t>
-  </si>
-  <si>
-    <t>Notebook Asus Vivobook Go E1504fa, AMD Ryzen 5 7520u, 8GB RAM, 256GB SSD, Windows 11, Tela 15,6 Polegadas, FULL HD, Black - Nj825w</t>
-  </si>
-  <si>
-    <t>&amp;eacute, leve. &amp;eacute, compacto. &amp;eacute, o asus vivobook go 15. Projetado para torn&amp;aacute,-lo produtivo e mant&amp;ecirc,-lo entretido onde quer que voc&amp;ecirc, v&amp;aacute,! Com processador amd ryzen 5 7520u de excelente desempenho, 8gb de mem&amp;oacute,ria ram lpddr51 e 256 gb de ssd2 , ele &amp;eacute, perfeito para seu dia a dia. Ainda conta com uma dobradi&amp;ccedil,a plana de 180&amp;deg,, tampa f&amp;iacute,sica protetora na webcam e muitos recursos de design bem pensados &amp;mdash, incluindo uma tela de 15 polegadas antirreflexo full hd &amp;mdash, tudo para que voc&amp;ecirc, v&amp;aacute, al&amp;eacute,m!part number: 90nb0zr2-m01by0sku asus: e1504fa-nj825wean code: 7898573299647c&amp;oacute,digo de homologa&amp;ccedil,&amp;atilde,o anatel: 06446-16-04076processador amd ryzen 5 7520u 2,8 ghz, 4 mb cachemem&amp;oacute,ria ram: 8 gb (8 gb onboard + 0 gb offboard)armazenamento: 256 gb ssd pcie g3x2tela 15,60´´ led-backlit anti-glareresolu&amp;ccedil,&amp;atilde,o da tela: 1920x1080placa de v&amp;iacute,deo: amd radeon graphicsgarantia: 12 mesestela sens&amp;iacute,vel ao toque: n&amp;atilde,oclock de mem&amp;oacute,ria: 5500 mhzwi-fi 5(802.11ac) (dual band) 1*1 + bluetooth 5.1tipo da placa de v&amp;iacute,deo: integradateclado retro iluminado: n&amp;atilde,oc&amp;acirc,mera frontal: hdbluetooth 5,1cart&amp;atilde,o de mem&amp;oacute,ria: n&amp;atilde,oaudio:sonicmasteralto-falantes embutidosmicrofone embutidosaidas:1x usb 2.0 type-a1x usb 3.2 gen 1 type-a1x usb 3.2 gen 1 type-c1x hdmi 1.41x 3.5mm combo audio jack1x dc-inadaptador de energia 45,00 wbateria 3 cells / 4000 mahsistema operacional windows 11 homecaracter&amp;iacute,sticas:especifica&amp;ccedil,&amp;otilde,es militares us mil-std 810htampa de privacidade para a webcampeso do produto: 1,63 kgdimens&amp;otilde,es: 36,03 cm x 23,25 cm x 1,79 ~ 1,79 cm&lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;software:&lt;/strong&gt; system diagnosisbattery health chargingfan profilesplendidfunction key lockwifi smartconnect link to myasustaskfirstlive updateai noise canceling&lt;br&gt;&lt;strong&gt;clock de memória:&lt;/strong&gt; 5500 mhz&lt;br&gt;&lt;strong&gt;adaptador de energia:&lt;/strong&gt; 45,00 w.&lt;br&gt;&lt;strong&gt;teclado retro iluminado:&lt;/strong&gt; não&lt;br&gt;&lt;strong&gt;tela sensível ao toque:&lt;/strong&gt; não&lt;br&gt;&lt;strong&gt;saídas:&lt;/strong&gt; 1x usb 2.0 type-a1x usb 3.2 gen 1 type-a1x usb 3.2 gen 1 type-c1x hdmi 1.41x 3.5mm combo audio jack1x dc-in&lt;br&gt;&lt;strong&gt;dimensões:&lt;/strong&gt; 36,03 cm x. 23,25 cm x. 1,79 ~. 1,79 cm&lt;br&gt;&lt;strong&gt;código de homologação anatel:&lt;/strong&gt; 06446-16-04076&lt;br&gt;&lt;strong&gt;câmera frontal:&lt;/strong&gt; hd&lt;br&gt;&lt;strong&gt;áudio:&lt;/strong&gt; sonicmasteralto-falantes embutidosmicrofone embutido&lt;br&gt;&lt;strong&gt;bluetooth:&lt;/strong&gt; bluetooth 5,1&lt;br&gt;&lt;strong&gt;sku asus:&lt;/strong&gt; e1504fa-nj825w&lt;br&gt;&lt;strong&gt;wi-fi:&lt;/strong&gt; wi-fi 5(802.11ac) (dual band) 1*1 + bluetooth® 5.1&lt;br&gt;&lt;strong&gt;ean code:&lt;/strong&gt; 7898573299647&lt;br&gt;&lt;strong&gt;bateria:&lt;/strong&gt; 3 cells / 4000 mah&lt;br&gt;&lt;strong&gt;garantia:&lt;/strong&gt; 12 meses&lt;br&gt;&lt;strong&gt;sistema operacional:&lt;/strong&gt; windows 11 home&lt;br&gt;&lt;strong&gt;cor:&lt;/strong&gt; preto&lt;br&gt;&lt;strong&gt;memória ram:&lt;/strong&gt; 8 gb (8 gb onboard + 0 gb offboard)&lt;br&gt;&lt;strong&gt;processador:&lt;/strong&gt; amd ryzen™ 5 7520u 2,8 ghz, 4 mb cache&lt;br&gt;&lt;strong&gt;armazenamento:&lt;/strong&gt; 256 gb ssd pcie g3x2&lt;br&gt;&lt;strong&gt;tela:&lt;/strong&gt; 15,60´´ led-backlit anti-glare&lt;br&gt;&lt;strong&gt;peso do produto:&lt;/strong&gt; 1,63 kg&lt;br&gt;&lt;strong&gt;resolução da tela:&lt;/strong&gt; 1920x1080&lt;br&gt;&lt;strong&gt;cartão de memória:&lt;/strong&gt; não&lt;br&gt;&lt;strong&gt;placa de vídeo:&lt;/strong&gt; amd radeon™ graphics&lt;br&gt;&lt;strong&gt;características:&lt;/strong&gt; especificações militares us mil-std 810htampa de privacidade para a. Webcam&lt;br&gt;&lt;strong&gt;manufacturer:&lt;/strong&gt; asus&lt;br&gt;&lt;strong&gt;mfrpartnumber:&lt;/strong&gt; e1504fa-nj825w&lt;br&gt;&lt;strong&gt;harddrivesize:&lt;/strong&gt; 256 gb ssd pcie g3x2&lt;br&gt;&lt;strong&gt;operatingsystem:&lt;/strong&gt; windows 11 home&lt;br&gt;&lt;strong&gt;processorbrand:&lt;/strong&gt; amd&lt;br&gt;&lt;strong&gt;processorspeed:&lt;/strong&gt; 2,8 ghz&lt;br&gt;&lt;strong&gt;ramsize:&lt;/strong&gt; 8 gb</t>
-  </si>
-  <si>
-    <t>Notebook Ultra Linux Intel I3, 256GB, 8GB RAM, 14,1 Polegadas, FULL HD,Preto - Ul151lx</t>
-  </si>
-  <si>
-    <t>Notebook ultra linux intel i3 256gb 8gb ram 14,1 pol. Full hd preto - ul151lx&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  notebook ultra, vem com linux, para você aproveitar ao máximo todos os recursos disponíveis. &lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  com ssd m.2 de 256gb de armazenamento. Muito mais espaço para seus vídeos, músicas e fotos ou que é mais essencial para você.&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  conta com 8gb de ram para você ter mais velocidade no recebimento de informações, tela de 14.1 hd para você ter imagens nítidas e vivas para uma experiência completa e surpreendente. Desenvolvida com bateria de longa duração, processador  intel core i3 de décima geração com alta velocidade e desempenho, da produtividade ao entretenimento, com o armazenamento de alta performance você terá muito mais rapidez no acesso a seus arquivos. Possui design ultraleve e superfino para você levar em qualquer lugar, transferência rápida de arquivos pelo usb 3.0 e usb tipo c.&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  ficha técnica&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  marca: ultra&lt;br /&gt;&lt;br /&gt;  modelo: notebook ultra linux intel i3 256gb 8gb ram 14,1 pol. Full hd preto - ul151lx&lt;br /&gt;&lt;br /&gt;  cor: preto&lt;br /&gt;&lt;br /&gt;  tela: 14,1 pol&lt;br /&gt;&lt;br /&gt;  sistema operacional: linux&lt;br /&gt;&lt;br /&gt;  processador: intel core i3&lt;br /&gt;&lt;br /&gt;  conexão: usb, bluetooth, p2sd&lt;br /&gt;&lt;br /&gt;  memória ram: 8gb&lt;br /&gt;&lt;br /&gt;  armazenamento: ssd m.2 de 256gb&lt;br /&gt;&lt;br /&gt;  câmera principal: 1mp&lt;br /&gt;&lt;br /&gt;  bateria: 4500mah 11,1v, 50whr carregador ac/dc bi-volt (110v-240v-50hz-60hz) com cabo de alimentação elétrica padrão brasileiro nbr14136:2002&lt;br /&gt;&lt;br /&gt;  áudio: hd áudio com controladora de som integrada a placa-mãe amplificada 2x alto-falantes 1w&lt;br /&gt;&lt;br /&gt;  entradas: 1x usb 3.0 gen 1, 1x usb 2.0, 1x usb type-c, 1x hdmi, 1xdc-in, 1x áudio combo, 1x rj45 ethernet, 1x microsd card reader&lt;br /&gt;&lt;br /&gt;  dimensões (lxaxc): 37 x 9 x 43cm&lt;br /&gt;&lt;br /&gt;  peso: 3500g&lt;br /&gt;&lt;br /&gt;  certificado anatel: 02143-18-04423&lt;br /&gt;&lt;br /&gt;  garantia: 1 ano&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  imagens meramente ilustrativas.</t>
-  </si>
-  <si>
-    <t>Notebook Ultra Intel Core I3, 8GB, SSD 256GB M.2, Tela 14.1 Full HD, Windows 11 Pro, Preto - Ul151l</t>
-  </si>
-  <si>
-    <t>Notebook ultra windows 11 pro intel i3 256gb 8gb ram 14,1 pol. Full hd preto - ul151l&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  notebook ultra, vem com o windows 11 pro, para você aproveitar ao máximo todos os recursos disponíveis. &lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  com ssd m.2 de 256gb de armazenamento. Muito mais espaço para seus vídeos, músicas e fotos ou que é mais essencial para você.&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  conta com 8gb de ram para você ter mais velocidade no recebimento de informações, tela de 14.1 hd para você ter imagens nítidas e vivas para uma experiência completa e surpreendente.&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  desenvolvida com bateria de longa duração, processador intel core i3 de décima geração com alta velocidade e desempenho, da produtividade ao entretenimento, com o armazenamento de alta performance você terá muito mais rapidez no acesso a seus arquivos. Possui design ultraleve e superfino para você levar em qualquer lugar, transferência rápida de arquivos pelo usb 3.0 e usb tipo c.&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  ficha técnica&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  marca: ultra&lt;br /&gt;&lt;br /&gt;  modelo: notebook ultra windows 11 pro intel i3 256gb 8gb ram 14,1 pol. Full hd preto - ul151l&lt;br /&gt;&lt;br /&gt;  cor: preto&lt;br /&gt;&lt;br /&gt;  tela: 14,1 polegadas&lt;br /&gt;&lt;br /&gt;  resolução: 1366 x 768&lt;br /&gt;&lt;br /&gt;  memória ram: 8gb ddr &lt;br /&gt;&lt;br /&gt;  memória interna: 256gb ssd&lt;br /&gt;&lt;br /&gt;  processador: intel core i3&lt;br /&gt;&lt;br /&gt;  sistema operacional: windows 11 pro &lt;br /&gt;&lt;br /&gt;  bateria: 4000 mah&lt;br /&gt;&lt;br /&gt;  áudio: hd com controladora de som integrada a placa mãe amplificada&lt;br /&gt;&lt;br /&gt;  portas: 1x usb 3.0, 1x usb 2.0, 1x usb tipo c, 1x áudio combo (microfone/fone) jack, 1x rj, 1x micro sd, 1x hdmi, 1x dc&lt;br /&gt;&lt;br /&gt;  teclado: padrão abnt2&lt;br /&gt;&lt;br /&gt;  câmera: frontal hd 1m&lt;br /&gt;&lt;br /&gt;  microfone: 2x d-mic integrados a câmera&lt;br /&gt;&lt;br /&gt;  dimensões (lxaxc): 32,26 x 2,08 x 22,35 cm&lt;br /&gt;&lt;br /&gt;  peso: 1,510kg&lt;br /&gt;&lt;br /&gt;  anatel: 02143-18-04423&lt;br /&gt;&lt;br /&gt;  garantia: 1 ano&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  imagens meramente ilustrativas.</t>
-  </si>
-  <si>
-    <t>R$2456.9</t>
-  </si>
-  <si>
-    <t>Notebook Positivo, 4GB, 64GB, Windows 11 Office - 3002497, Tela 14''  Cinza - Cel-n4020</t>
-  </si>
-  <si>
-    <t>O Notebook Positivo Motion C - 464D apresenta um design fino, elegante e compacto os novos Notebooks da Positivo disponibilizam o máximo em entretenimento e diversão! Com processador Intel Celeron o Notebook Positivo Motion C apresenta um baixo consumo de energia. Trabalhe e divirta-se o dia todo, sem precisar estar conectado a tomada, graças à bateria com mais de 7 horas de duração.</t>
-  </si>
-  <si>
-    <t>Tela 14 Polegadas Led Slim Notebook, 30 Pinos 1366x768</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;tela substituta 14" em led para notebook com resolução 1366x768 e conector de 30 pinos do canto direito inferior.&lt;br /&gt;&lt;br /&gt;&lt;strong&gt;especificações técnicas:&lt;br /&gt;&lt;br /&gt;&lt;/strong&gt;modelo nt140whm-n43&lt;br /&gt;tamanho: 14.0 pol&lt;br /&gt;formato padrão: wxga&lt;br /&gt;tipo de aparelho: notebook&lt;br /&gt;resolução 1366x768&lt;br /&gt;pinos conector 30 pinos&lt;br /&gt;posição conector direito inferior&lt;br /&gt;&lt;br /&gt;&lt;strong&gt;códigos alternativos: b140xtn07.2&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>R$1133.95</t>
+    <t>Tampa Superior Com Teclado Para Notebook Hp Modelo 840 G8, Padrão Abnt Português - M36312-201</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;tampa superior com teclado para uso em notebook hp modelo 840 g8 padrão abnt português.&lt;br /&gt;&lt;br /&gt;&lt;strong&gt;especificações técnicas:&lt;/strong&gt; &lt;br /&gt;&lt;br /&gt;código: m36312-201&lt;br /&gt;marca: hp&lt;br /&gt;padrão: abnt2&lt;br /&gt;&lt;br /&gt;&lt;strong&gt;modelos compatíveis:&lt;/strong&gt; hp elitebook 840 g8 i5. &lt;br /&gt;&lt;br /&gt;&lt;br /&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>R$2260.56</t>
+  </si>
+  <si>
+    <t>Notebook Dell Inspiron 3511 Core I3-1115g4, 4GB RAM, SSD 256GB, Tela 15,6 Polegadas Led HD - Windows 11 Home</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;notebook dell inspiron 3511&amp;nbspa velocidade de que você precisa:&lt;/strong&gt;&amp;nbspum desempenho responsivo e silencioso, contando com opções de configuração que incluem processadores intel&amp;nbspcore&amp;nbspde 11ª geração e armazenamento ssd pci-e.&lt;strong&gt;perfeito para você:&lt;/strong&gt;&amp;nbsptenha um teclado expansivo com keypad numérico, teclas 6,4% maiores e um touchpad espaçoso que facilita a sua navegação.&lt;strong&gt;design pensado para seu dia a dia:&lt;/strong&gt;&amp;nbsptrabalhe confortavelmente graças a uma dobradiça de elevação que ergue seu notebook em um ângulo ergonômico, proporcionando um ângulo de digitação mais confortável.&lt;strong&gt;agradável aos olhos:&lt;/strong&gt;&amp;nbspas soluções de software low blue light do dell comfortview ajudam a reduzir as emissões nocivas de luz azul e otimizam o conforto ocular.&lt;strong&gt;há mais para ver:&lt;/strong&gt;&amp;nbspveja mais detalhes na tela em um notebook de 15,6&amp;quot full hd com bordas estreitas em três lados e tenha uma experiência de visualização mais imersiva.&lt;strong&gt;uma preocupação comum:&lt;/strong&gt;&amp;nbspprojetado para resistir ao uso regular, com pequenos pés de borracha e amortecedores na dobradiça que impedem a derrapagem e dão mais estabilidade em superfícies duras.&lt;strong&gt;especificações técnicas:&lt;/strong&gt;&lt;strong&gt;processador:&lt;/strong&gt; 11ª geração intel&amp;nbspcore&amp;nbspi3-1115g4 (2-core, cache de 6mb, até 4.1ghz)&lt;strong&gt;sistema operacional:&lt;/strong&gt; windows 11 home, português&lt;strong&gt;placa de vídeo:&amp;nbsp&lt;/strong&gt;intel&amp;nbspuhd com memória gráfica compartilhada&lt;strong&gt;tela:&amp;nbsp&lt;/strong&gt;full hd de 15.6&amp;quot (1920 x 1080) wva&lt;strong&gt;memória:&amp;nbsp&lt;/strong&gt;4gb ddr4 (1x4gb) 2666mhz expansível até 16gb (2 slots sodimm)&lt;strong&gt;armazenamento:&amp;nbsp&lt;/strong&gt;ssd de 256gb pcie nvme m.2&lt;strong&gt;cor:&amp;nbsp&lt;/strong&gt;apollo - preto carbono&amp;nbsp&amp;nbsp&lt;strong&gt;assistência técnica:&amp;nbsp&lt;/strong&gt;1 ano de garantia básica via correios&lt;strong&gt;teclado:&amp;nbsp&lt;/strong&gt;teclado padrão em português, com leitor de impressão digital (compatível apenas com windows)&lt;strong&gt;portas:&amp;nbsp&lt;/strong&gt;2 portas usb 3.2 de 1ª geração | 1 porta usb 2.0 | 1 conector de áudio&amp;nbsp| 1porta hdmi 1.4 |1 slot m.2 2230 para placa de wifi e bluetooth | 1 slot m.2 2230/2280 para unidade de estado sólido (ssd)/intel optane (não possui slot sata) | 1 slot de cartão sd&lt;strong&gt;câmera:&amp;nbsp&lt;/strong&gt;câmera hd de 720p a 30 fps com microfone único integrado&amp;nbsp&lt;strong&gt;áudio e alto-falantes:&amp;nbsp&lt;/strong&gt;alto-falantes estéreo, 2 de 2 w = 4 w no total&lt;strong&gt;wireless:&amp;nbsp&lt;/strong&gt;802.11ac 1x1 wi-fi, placa de rede wireless com bluetooth&lt;strong&gt;bateria principal:&amp;nbsp&lt;/strong&gt;bateria de 4 células e 54wh (integrada)&lt;strong&gt;energia:&amp;nbsp&lt;/strong&gt;adaptador ca 65 watts (bivolt)&lt;strong&gt;altura: &lt;/strong&gt;1,75 cm a 1,90 cm |&lt;strong&gt; largura:&lt;/strong&gt; 35,85 cm | &lt;strong&gt;profundidade:&lt;/strong&gt; 23,56 cm | &lt;strong&gt;peso:&lt;/strong&gt; 1,85 kg&lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;notebook dell inspiron 3511 core i3-1115g4 | entregas para todo o brasil</t>
+  </si>
+  <si>
+    <t>R$2855.0</t>
   </si>
   <si>
     <t>Fonte Ac Adapter Hp, 65wm, USB-C, 20v, 1.8m - L32392-001</t>
@@ -1831,93 +1816,99 @@
     <t>Atenção ! Equipamento de mostruário.&lt;br /&gt;&lt;br /&gt;notebook custo beneficio, top de excelente marca,&lt;br /&gt;perfeito para diversas atividades do dia a dia,&lt;br /&gt;com ssd para aumentar sua velocidade.&lt;br /&gt;Possui garantia e nota fiscal, e ao realizar a compra enviamos o produto junto de seu carregador.&lt;br /&gt;&lt;br /&gt;caso tenha duvidas, pergunte no campo abaixo e responderemos em até 24h.  &lt;br /&gt;caso queira falar diretamente conosco, envie uma mensagem em nosso whatsapp oficial, pesquise nossa loja &lt;br /&gt;na internet imperiums informática e tire suas duvidas.  &lt;br /&gt;&lt;br /&gt;caso tenha duvidas, pergunte no campo de perguntas abaixo.&lt;br /&gt;&lt;br /&gt;modelo: hp elitebook notebook 840 g1&lt;br /&gt;processador: i5-4300u&lt;br /&gt;memoria ram: 8gb ram&lt;br /&gt;armazenamento: 480gb ssd&lt;br /&gt;tela: 14 polegadas hd+&lt;br /&gt;wifi e bluetooth&lt;br /&gt;windows 10 pró&lt;br /&gt;&lt;br /&gt;garantia do vendedor: 3 meses</t>
   </si>
   <si>
+    <t>Usado - Notebook Lenovo Ideapad 330, Intel Celeron N4000, 4GB, 500GB, Tela 15.6p, Linux - 81fns00000 - Seminovo</t>
+  </si>
+  <si>
+    <t>Notebook Lenovo Ideapad 330 81FNS00000, cor prata, processador Intel Celeron N4000 de 1.10GHz até 2.60GHz, memória RAM de 4GB DDR4, HD 500GB, tela de 15.6 polegadas e sistema operacional Linux&lt;br /&gt;Modelo/Referencia: 330-15IGM81FNS00000&lt;br /&gt;&lt;br /&gt;Certificação: Recertificado&lt;br /&gt;&lt;br /&gt;Medalha: Ouro&lt;br /&gt;&lt;br /&gt;FICHA TÉCNICA:&lt;br /&gt;&lt;br /&gt;Sistema operacional: Linux.&lt;br /&gt;&lt;br /&gt;Processador: Intel Celeron N4000– Dual Care ( 2Threads)- Frequência: 1.10GHz até 2.60GHz – 4 MB de Cache. &lt;br /&gt;&lt;br /&gt;Memoria: 4 GB RAM &lt;br /&gt; &lt;br /&gt;Armazenamento: 1 TB&lt;br /&gt;&lt;br /&gt;Tela: 15.6”&lt;br /&gt;&lt;br /&gt;Conteúdo da embalagem: Notebook, Fonte carregadora do notebook&lt;br /&gt;&lt;br /&gt;Observação: O produto não acompanha manual de instruções&lt;br /&gt;&lt;br /&gt;Garantia: 3 meses&lt;br /&gt;&lt;br /&gt;ATENÇÃO: VOCÊ ESTÁ ADQUIRINDO UM PRODUTO RECERTIFICADO!!!! &lt;br /&gt;&lt;br /&gt;O produto acompanha a caixa original de fábrica, não acompanha manual de instruções ou qualquer outro acessório&lt;br /&gt;&lt;br /&gt;Entenda o que é um produto recertificado:&lt;br /&gt;&lt;br /&gt;É um produto que volta do mercado disponível para venda nas mesmas condições de um produto novo, com suas funcionalidades e características originais. O produto passa por um rigoroso processo de análise onde todas as suas funcionalidades são testadas e o produto liberado para venda. &lt;br /&gt;&lt;br /&gt;O produto recertificado é classificado em medalhas de acordo com o estado estético e superficial do produto, sendo: OURO, PRATA E BRONZE.&lt;br /&gt;&lt;br /&gt;Recertificado Prata: Produto tem características similares ao Ouro, pode apresentar mínimos riscos quase imperceptíveis.&lt;br /&gt; &lt;br /&gt;Atenção: O Saldão da Informática não enviará fotos reais dos produtos para os clientes, como também não reservaremos produtos. As imagens exibidas são meramente ilustrativas.</t>
+  </si>
+  <si>
     <t>Notebook Intel Core I5, Tela 15.6” Full HD Ips, 8GB, 480 SSD E Windows 10 - Everex</t>
   </si>
   <si>
     <t>Notebook Intel Core I5, Tela 15.6” Full HD Ips, 8GB, 480 SSD E Windows 10 Pro - Everex</t>
   </si>
   <si>
+    <t>Notebook Asus Vivobook 15 X1500ea, Intel Pentium Gold 7505, 4 GB RAM, 128GB, SSD Windows 11, Tela 15,6 Polegadas, FULL HD</t>
+  </si>
+  <si>
+    <t>Seja para trabalho ou lazer, o asus vivobook 15 &amp;eacute, um notebook que oferece desempenho, praticidade e &amp;oacute,timos visuais. Sua tela nanoedge com bordas extremamente finas possui revestimento fosco antirreflexivo para uma experi&amp;ecirc,ncia verdadeiramente envolvente. Equipado com processador intel pentium gold e placa de v&amp;iacute,deo intel uhd graphics, o asus vivobook 15 &amp;eacute, superfino, leve e ainda conta com uma bateria de longa dura&amp;ccedil,&amp;atilde,o de 37 wh, o que o torna perfeito para sua utiliza&amp;ccedil,&amp;atilde,o di&amp;aacute,ria.part number: 90nb0ty6-m04nx0sku asus: x1500ea-ej4239wsean code: 7898573299449c&amp;oacute,digo de homologa&amp;ccedil,ao anatel: 00915-18-04423processador intel pentium gold 7505 2 ghz, 4 mb cachemem&amp;oacute,ria ram: 4 gb (4 gb onboard + 0 gb offboard)armazenamento: 128 gb ssdtela 15,60´´ led-backlit tft lcd anti-glareresolu&amp;ccedil,&amp;atilde,o da tela: 1920x1080placa de v&amp;iacute,deo: intel uhd graphicsgarantia 12 mesestela sens&amp;iacute,vel ao toque: n&amp;atilde,oclock de mem&amp;oacute,ria 2400 mhzwi-fi 5placa de v&amp;iacute,deo integradac&amp;acirc,mera frontal: vgabluetooth 5,1cart&amp;atilde,o de mem&amp;oacute,ria: n&amp;atilde,o&amp;aacute,udio:sonicmasteraudio by icepowerbuilt-in speakerbuilt-in microphonesa&amp;iacute,das:1x 3.5mm combo audio jack1x hdmi 1.41x usb 3.2 gen 1 type-a1x usb 3.2 gen 1 type-c2x usb 2.0 type-aadaptador de energia 45,00 wbateria 2 cells / 3300 mahmicrosoft 365 personal por 1 ano inclu&amp;iacute,do (necess&amp;aacute,rio ativar em at&amp;eacute, 6 meses ap&amp;oacute,s a ativa&amp;ccedil,&amp;atilde,o do windows)sistema operacional: windows 11 homecaracter&amp;iacute,sticas:tela nanoedgecarregamento r&amp;aacute,pido da bateriasecurity lockpeso do produto: 1,8 kgdimens&amp;otilde,es: 36 cm x 23,5 cm x 1,99 cm&lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;sku asus:&lt;/strong&gt; x1500ea-ej4239ws&lt;br&gt;&lt;strong&gt;bluetooth:&lt;/strong&gt; bluetooth 5,1&lt;br&gt;&lt;strong&gt;câmera frontal:&lt;/strong&gt; vga&lt;br&gt;&lt;strong&gt;garantia:&lt;/strong&gt; 12 meses&lt;br&gt;&lt;strong&gt;placa de vídeo:&lt;/strong&gt; intel® uhd graphics&lt;br&gt;&lt;strong&gt;ean code:&lt;/strong&gt; 7898573299449&lt;br&gt;&lt;strong&gt;cor:&lt;/strong&gt; prata metálico&lt;br&gt;&lt;strong&gt;peso do produto:&lt;/strong&gt; 1,8 kg&lt;br&gt;&lt;strong&gt;resolução da tela:&lt;/strong&gt; 1920x1080&lt;br&gt;&lt;strong&gt;dimensões:&lt;/strong&gt; 36 cm x. 23,5 cm x. 1,99 ~. 1,99 cm&lt;br&gt;&lt;strong&gt;características:&lt;/strong&gt; tela nanoedgecarregamento rápido da bateriasecurity lock&lt;br&gt;&lt;strong&gt;software:&lt;/strong&gt; wi-fi smartconnect system diagnosis battery health chargingfan mode splendid tru2life function key lock wifiroamingoptimizationlink to myasus&lt;br&gt;&lt;strong&gt;clock de memória:&lt;/strong&gt; 2400 mhz&lt;br&gt;&lt;strong&gt;tela sensível ao toque:&lt;/strong&gt; não&lt;br&gt;&lt;strong&gt;sistema operacional:&lt;/strong&gt; windows 11 home&lt;br&gt;&lt;strong&gt;bateria:&lt;/strong&gt; 2 cells / 3300 mah&lt;br&gt;&lt;strong&gt;saídas:&lt;/strong&gt; 1x 3.5mm combo audio jack1x hdmi 1.41x usb 3.2 gen 1 type-a1x usb 3.2 gen 1 type-c2x usb 2.0 type-a&lt;br&gt;&lt;strong&gt;código de homologação anatel:&lt;/strong&gt; 00915-18-04423&lt;br&gt;&lt;strong&gt;adaptador de energia:&lt;/strong&gt; 45,00 w.&lt;br&gt;&lt;strong&gt;cartão de memória:&lt;/strong&gt; não&lt;br&gt;&lt;strong&gt;armazenamento:&lt;/strong&gt; 128 gb ssd&lt;br&gt;&lt;strong&gt;wi-fi:&lt;/strong&gt; wi-fi 5(802.11ac) (dual band) 1*1 + bluetooth® 5.1&lt;br&gt;&lt;strong&gt;tela:&lt;/strong&gt; 15,60´´ led-backlit tft lcd anti-glare&lt;br&gt;&lt;strong&gt;áudio:&lt;/strong&gt; sonicmasteraudio by icepower®built-in speakerbuilt-in microphone&lt;br&gt;&lt;strong&gt;processador:&lt;/strong&gt; intel® pentium gold 7505 2 ghz, 4 mb cache&lt;br&gt;&lt;strong&gt;memória ram:&lt;/strong&gt; 4 gb (4 gb onboard + 0 gb offboard)</t>
+  </si>
+  <si>
+    <t>Notebook Lenovo Ideapad 3i Celeron 4gb 500gb Linux 15.6´´ Prata</t>
+  </si>
+  <si>
+    <t>Notebook Lenovo IdeaPad 3i Celeron 4GB 500GB Linux 15.6´´ PrataLenovo IdeaPad 3i possui design leve e compacto. Com tela antirreflexo de 15.6´´ para mais conforto visual. Notebook ideal para todos os momentos. Conta com WiFi AC ultrarrá,pido e teclado numé,rico para trabalhar com mais agilidade nas suas planilhas. Possibilidade de utilizar o armazenamento de forma hí,brida e ganhar muito mais agilidade e produtividade no seu dia a dia. Com o slot disponí,vel, você, tem a opç,ã,o de adicionar um SSD NVMe M.2 para ter mais seguranç,a ao armazenar seus dados.CONECTIVIDADEBluetooth SimUSB (2.0) 1Leitor de Cartõ,es 4 em 1 (SD, SDHC, SDXC, MMC)USB (3.2) 2..</t>
+  </si>
+  <si>
+    <t>R$2935.9</t>
+  </si>
+  <si>
+    <t>Notebook Positivo Motion, Intel Cel-n4020, 4GB, SSD 240GB, Tela 14p LED HD, Linux, Cinza - 3002635</t>
+  </si>
+  <si>
+    <t>Processador intel® celeron® dual core 1,10 ghz com frequência de burst de até 2,80 ghz, 4mb cache, 2 núcleos, 2 threads &lt;br /&gt;fabricante do processador intel® &lt;br /&gt;linha do processador celeron® dual core &lt;br /&gt;modelo do processador n4020 &lt;br /&gt;geração do processador não se aplica &lt;br /&gt;arquitetura do processador 64 bitschipset da cpu não se aplica &lt;br /&gt;soquete da cpu fcbga1090 &lt;br /&gt;cache 4mb &lt;br /&gt;quantidade de núcleos 2 &lt;br /&gt;quantidade de threads 2 &lt;br /&gt;velocidade / frequência máxima do processador burst de até 2.80 ghz &lt;br /&gt;velocidade / frequência mínima do processador 1.10 ghz &lt;br /&gt;placa de vídeo processamento de vídeo integrado intel® graphics &lt;br /&gt;suporte microsoft® directx® e opengl &lt;br /&gt;modelo de placa de vídeo processamento de vídeo integrado intel® uhd 600 graphics &lt;br /&gt;marca do chipset de vídeo intel® &lt;br /&gt;tipo / interface de placa de vídeo integrada &lt;br /&gt;saída hdmi &lt;br /&gt;memória de placa de vídeo não se aplica &lt;br /&gt;barramento da memória de vídeo ddr4 &lt;br /&gt;placa mãe fabricante placa mãe positivo tecnologia &lt;br /&gt;marca do chipset da placa mãe intel® &lt;br /&gt;áudio áudio de alta definição (hd áudio), microfone e alto -falantes estéreo embutidos &lt;br /&gt;modos de som stereo &lt;br /&gt;memória 4gb (ddr4 onboard) &lt;br /&gt;memória ram 4gb &lt;br /&gt;tipo da memória ram ddr4 &lt;br /&gt;chip on board &lt;br /&gt;velocidade / clock da memória ram 2133mt/s &lt;br /&gt;barramento / tecnologia da memória ram ddr4 &lt;br /&gt;slot de memória disponível não se aplica &lt;br /&gt;quantidade de slots de memória ram não se aplica &lt;br /&gt;capacidade máxima de memória ram não se aplica &lt;br /&gt;memória optane não se aplica &lt;br /&gt;armazenamento tecnologia de armazenamento ssd &lt;br /&gt;armazenamento / tamanho do hd não se aplica &lt;br /&gt;armazenamento / tamanho do ssd 240gb &lt;br /&gt;armazenamento / tamanho do ufs não se aplica &lt;br /&gt;armazenamento / tamanho do emmc não se aplica &lt;br /&gt;velocidade de leitura do hd não se aplica &lt;br /&gt;velocidade de leitura do ssd 400mb/s &lt;br /&gt;velocidade de leitura do ufs não se aplica &lt;br /&gt;velocidade de leitura do emmc não se aplica &lt;br /&gt;quantidade de slots de armazenamento não se aplicacapacidade de expansão de armazenamento não se aplica &lt;br /&gt;tela 14.1\", led hd, widescreen, 1366 x 768, 16:9, antirreflexiv</t>
+  </si>
+  <si>
+    <t>R$2579.04</t>
+  </si>
+  <si>
+    <t>Notebook Concórdia C3115, Intel Core I3-1115g4, 8GB, SSD 512GB, Tela 15.6 HD, Linux</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;notebook concórdia c3115 i3 1115g4 8gb ssd 512gb tela 15,6&amp;quot hd linux&amp;nbsp &amp;nbsp&lt;/strong&gt;apresentamos o mais recente lançamento no mundo dos notebooks: o modelo que combina versatilidade, confiabilidade, modernidade e tecnologia&amp;nbspde&amp;nbspponta! &lt;strong&gt;notebook concórdia c3115.&lt;/strong&gt; com recursos adaptáveis ao seu estilo de vida, oferecendo alta qualidade, durabilidade e desempenho consistente. Sua aparência elegante com resolução hd e recursos avançados é o combo perfeito para tornar a experiência digital a mais&amp;nbspexcepcional.</t>
+  </si>
+  <si>
+    <t>R$2839.0</t>
+  </si>
+  <si>
+    <t>Usado - Notebook Lenovo Thinkpad T480 Core I5 8350u, 8GB RAM, SSD 256GB, Windows 10 Pro</t>
+  </si>
+  <si>
+    <t>A agasus oferece ao mercado a comercialização de computadores, notebooks, servidores, monitores, smartphones e periféricos seminovos das marcas líderes com o objetivo de levar tecnologia e preço acessível a todos os seus clientes.          informações principais:    - marca: lenovo       - sku: p003680-v1    - modelo: thinkpad t480    - marca processador: intel    - placa gráfica: uhd graphics 620    -  linha processador: core i5 8350ugº    - memória ram: 8gb    - capacidade hd: 500gb    - sistema operativo: windows     - versão do sistema operacional: 10 pro    - tamanho da tela: 14”    -  resolução da tela: ?1920 x 1080 pixels    - tipo de bateria: íon de lítio    - mais informações: consulte ficha técnica do anuncio ou entre em contato         itens testados:    - teclado,    - webcam,    - audio (microfone, saída, entrada de fone),    - fonte,    - tela,    - rede cabeada e wi-fi,    - portas usb,    - saidas de vídeo,    - slots de memória e hd.         conteúdo da embalagem:    - 1x notebook     - 1x fonte (original ou genérica),    - não acompanha manual de instruções         obs sobre a bateria:    a autonomia da bateria poderá variar dependendo da configuração, dos aplicativos carregados, das configurações de energia e dos recursos utilizados. Os equipamentos podem trazer baterias proprio ou genéricas, testadas e revisadas por nossa equipe técnica. Ressaltamos que a bateria poderá não apresentar a mesma vida útil de um produto fechado.         garantia:     ****6 meses de garantia diretamente com a nossa loja agasus***   &lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;conteúdo da embalagem:&lt;/strong&gt; 1x notebook1x fonte (original ou genérica),&lt;br&gt;&lt;strong&gt;processador:&lt;/strong&gt; intel core i5 8350u&lt;br&gt;&lt;strong&gt;código anatel:&lt;/strong&gt; 010430802198&lt;br&gt;&lt;strong&gt;garantia:&lt;/strong&gt; 6 meses&lt;br&gt;&lt;strong&gt;conectividade:&lt;/strong&gt; wifi&lt;br&gt;&lt;strong&gt;memória ram:&lt;/strong&gt; 8gb&lt;br&gt;&lt;strong&gt;modelo:&lt;/strong&gt; thinkpad t480&lt;br&gt;&lt;strong&gt;ean:&lt;/strong&gt; 0192330094382&lt;br&gt;&lt;strong&gt;correios width:&lt;/strong&gt; 48&lt;br&gt;&lt;strong&gt;categories:&lt;/strong&gt; [493, 494, 495, 496, 498, 499, 500, 501, 502, 504, 2, 539]&lt;br&gt;&lt;strong&gt;tipo de teclado:&lt;/strong&gt; abnt&lt;br&gt;&lt;strong&gt;estado:&lt;/strong&gt; seminovo&lt;br&gt;&lt;strong&gt;special price from date:&lt;/strong&gt; 2022-01-06 00:00:00&lt;br&gt;&lt;strong&gt;condição:&lt;/strong&gt; muito bom&lt;br&gt;&lt;strong&gt;tamanho da tela:&lt;/strong&gt; 14´´&lt;br&gt;&lt;strong&gt;correios height:&lt;/strong&gt; 27&lt;br&gt;&lt;strong&gt;sistema operacional:&lt;/strong&gt; windows 10 pro&lt;br&gt;&lt;strong&gt;memória interna:&lt;/strong&gt; 256gb</t>
+  </si>
+  <si>
+    <t>Usado - Notebook Acer Aspire 5 A514-54-52ty, Intel Core I5-1135g7, 8GB, SSD 256GB, Tela 14 Polegadas, Windows 10 - Seminovo</t>
+  </si>
+  <si>
+    <t>Notebook Acer Aspire 5 A514-54-52Ty, processador de 11º geração Intel Core i5-1135G7 de 2.40GHz até 4.20GHz, memória RAM de 8GB DDR4, SSD de 256GB, tela de 14 polegadas e sistema operacional Windows 10&lt;br /&gt;&lt;br /&gt;Modelo/Referencia: A514-54-52Ty&lt;br /&gt;&lt;br /&gt;Certificação: Recertificado&lt;br /&gt;&lt;br /&gt;Medalha: Bronze&lt;br /&gt;&lt;br /&gt;FICHA TÉCNICA:&lt;br /&gt;Sistema operacional: Windows 11 home 64- bits&lt;br /&gt;&lt;br /&gt;Processador: Intel Core i5– 1135G7- Quad Core (8 threads) – Frequência: até 4.20 GHz - 8 MB Intel de SmartCache &lt;br /&gt;&lt;br /&gt;Memoria: 8 GB RAM DDR4 (4GB Soldada + 4GB Módulo) - DDR4-2666MHz – Expansível até 20GB&lt;br /&gt;&lt;br /&gt;Armazenamento: 256 GB SSD PCIe 3.0 x4 NVMe (M.2 2280)&lt;br /&gt;&lt;br /&gt;Tela: 14” IPS FHD (1920 x 1080)&lt;br /&gt;&lt;br /&gt;Placa Gráfica: Intel Iris Xe Graphics com memória compartilhada com a memória RAM&lt;br /&gt; &lt;br /&gt;Conectividade: Bluetooth 5.0 - Suporte a redes com frequência (2.4 GHz e 5 GHz) – Wireless LAN 802.11a/b/g/n/ac&lt;br /&gt;&lt;br /&gt;Teclado: português do Brasil (ABNT2) – Multi-gestual com dois botões- Teclado numérico independente&lt;br /&gt;&lt;br /&gt;Observação: Este produto não possui leitor de CD/DVD&lt;br /&gt;&lt;br /&gt;Upgrades: Slot ocupado M.2 2280, compatível com unidades SSD PCIe 3.0 NVMe x2/x4 de até 512 GB - Slot livre SATA 3, compatível com HDD ou SSD SATA 3 2.5” de até 2TB&lt;br /&gt;&lt;br /&gt;Entrada: Entrada para fonte de alimentação, Porta Ethernet (RJ-45), 2x portas USB 3.2 Gen 1 (5 Gbps), Entrada combo para alto falante e fone de ouvido, Porta USB Type-C® 3.2 Gen 1 (5 Gbps), Porta USB 2.0, Porta HDMI®2.0&lt;br /&gt;&lt;br /&gt;Conteúdo da embalagem: Notebook, Fonte carregadora do notebook&lt;br /&gt;&lt;br /&gt;Observação: O produto não acompanha manual de instruções&lt;br /&gt;&lt;br /&gt;Garantia: 3 meses&lt;br /&gt;&lt;br /&gt;ATENÇÃO: VOCÊ ESTÁ ADQUIRINDO UM PRODUTO RECERTIFICADO!!!! &lt;br /&gt;&lt;br /&gt;O produto acompanha a caixa original de fábrica, não acompanha manual de instruções ou qualquer outro acessório &lt;br /&gt;&lt;br /&gt;Entenda o que é um produto recertificado:&lt;br /&gt;&lt;br /&gt;É um produto que volta do mercado disponível para venda nas mesmas condições de um produto novo, com suas funcionalidades e características originais. O produto passa por um rigoroso processo de análise onde todas as suas funcionalidades são testadas e o produto liberado para venda. &lt;br /&gt;&lt;br /&gt;O produto recertificado é classificado em medalhas de acordo com o estado estético e superficial do produto, sendo: OURO, PRATA E BRONZE.&lt;br /&gt;&lt;br /&gt;Recertificado Ouro: Produto está em ótimas condições estéticas, similar a um produto novo. &lt;br /&gt;&lt;br /&gt;Recertificado Prata: Produto tem características similares ao Ouro, pode apresentar mínimos riscos quase imperceptíveis. &lt;br /&gt;&lt;br /&gt;Recertificado Bronze: Produto possuí riscos visíveis (nenhum risco apresentado é na tela do produto). Estes riscos não alteram o funcionamento do equipamento.&lt;br /&gt;&lt;br /&gt;Atenção: O Saldão da Informática não enviará fotos reais dos produtos para os clientes, como também não reservaremos produtos. As imagens exibidas são meramente ilustrativas.</t>
+  </si>
+  <si>
+    <t>R$2665.56</t>
+  </si>
+  <si>
+    <t>Notebook Lenovo Ideapad 3 15itl6, Intel I3-1115G4, 8GB, SSD 256GB, Tela de 15.6 Polegadas FULLHD, Windows 11 Home</t>
+  </si>
+  <si>
+    <t>Notebook lenovo ideapad 3 15itl6 15.6 fhd/ i3-1115g4/ 8gb/ 256gb ssd/ win 11 home&lt;br&gt;&lt;br&gt;armazenamento : ssd&lt;br&gt;cor : cinza artico&lt;br&gt;memoria : 8gb ddr4 3200&lt;br&gt;memoria maxima : 128gb&lt;br&gt;processador : i3-1115g4&lt;br&gt;rj 45 : nao&lt;br&gt;ssd : 256gb m.2 pcie nvme&lt;br&gt;tela : 15.6 full hd antirreflexo&lt;br&gt;garantia com o fabricante : 01 ano&lt;br&gt;precisa de pilhas ou baterias : sim&lt;br&gt;as pilhas ou baterias estao inclusas : sim&lt;br&gt;tipo de bateria ou pilha : lithium ion&lt;br&gt;dimensao da embalagem a / p / l : 19.9mm / 236.5mm / 359.2mm&lt;br&gt;ean : 197532097674&lt;br&gt;anatel : 05788-17-04423&lt;br&gt;ncm : 84713019&lt;br&gt;peso do produto com embalagem : 1.65kg&lt;br&gt;part number: 82md0010br&lt;br&gt;modelo: ideapad 3 15itl6&lt;br&gt;garantia com o seller: 7 dia/dias&lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;armazenamento:&lt;/strong&gt; ssd&lt;br&gt;&lt;strong&gt;cor:&lt;/strong&gt; cinza a?rtico&lt;br&gt;&lt;strong&gt;memoria:&lt;/strong&gt; 8gb ddr4 3200&lt;br&gt;&lt;strong&gt;memoria maxima:&lt;/strong&gt; 128gb&lt;br&gt;&lt;strong&gt;processador:&lt;/strong&gt; i3 1115g4&lt;br&gt;&lt;strong&gt;rj 45:&lt;/strong&gt; na?o&lt;br&gt;&lt;strong&gt;ssd:&lt;/strong&gt; 256gb m.2 pcie nvme&lt;br&gt;&lt;strong&gt;tela:&lt;/strong&gt; 15.6 full hd antirreflexo&lt;br&gt;&lt;strong&gt;garantia com o. Fabricante:&lt;/strong&gt; 01 ano&lt;br&gt;&lt;strong&gt;precisa de pilhas ou baterias?:&lt;/strong&gt; sim&lt;br&gt;&lt;strong&gt;as pilhas ou baterias estao inclusas?:&lt;/strong&gt; sim&lt;br&gt;&lt;strong&gt;tipo de bateria ou pilha:&lt;/strong&gt; lithium ion&lt;br&gt;&lt;strong&gt;dimensao da embalagem a. / p. / l.:&lt;/strong&gt; 19.9mm / 236.5mm / 359.2mm&lt;br&gt;&lt;strong&gt;ean:&lt;/strong&gt; 197532097674&lt;br&gt;&lt;strong&gt;anatel:&lt;/strong&gt; 05788 17 04423&lt;br&gt;&lt;strong&gt;ncm:&lt;/strong&gt; 84713019&lt;br&gt;&lt;strong&gt;peso do produto com embalagem:&lt;/strong&gt; 1.65kg&lt;br&gt;&lt;strong&gt;garantia com o. Seller::&lt;/strong&gt; 7 dia/dias&lt;br&gt;&lt;strong&gt;part number:&lt;/strong&gt; 82md0010br</t>
+  </si>
+  <si>
+    <t>R$2893.12</t>
+  </si>
+  <si>
+    <t>Notebook Positivo Vision C15, Intel Celeron, 4GB, SSD 240GB, Tela Lumina 15 HD, Linux, Cinza</t>
+  </si>
+  <si>
+    <t>Notebook positivo vision c15 intel® celeron® linux 4gb 240gb ssd lumina bar 15” hd - cinzadescubra a nova linha de notebooks positivo vision, perfeito para todas as suas atividades diárias! Desenvolvido com foco em praticidade, ele é ideal para tarefas leves como planilhas, edição de texto e navegação na web. Além disso, você poderá desfrutar de vídeo chamadas com sua câmera de alta definição. Suporta softwares de ensino e ferramentas básicas de trabalho, o positivo vision c15 garante que você esteja sempre pronto para alcançar seus objetivos. Não perca tempo, experimente o poder da nova linha positivo vision e eleve suas atividades diárias a um novo nível de eficiência.quem confia na qualidade do seu produto oferece garantia ampliada. O positivo vision c15 conta com 2 anos de garantia de fábrica.a positivo tecnologia inova no mercado ao lançar a primeira linha de notebooks do mundo com a tecnologia lumina bar, oferecendo uma experiência superior aos usuários. Os notebooks possuem barras de led com ajuste de 3 níveis de intensidade, proporcionando uma iluminação ideal para a webcam, resultando em uma captura de imagem excepcional mesmo em ambientes com pouca iluminação.tecla link exclusiva para conectar o celular ao notebook de uma forma mais simples. Sincronização de fotos, salvamento de imagens com facilidade, visualização de mensagens sms, status da bateria, entre outras funcionalidades com apenas um toque.mais agilidade com o smart touch, composto por 3 botões na lateral do vision c15 para você criar atalhos com os aplicativos que mais usa. Escolha o que cada um vai abrir para aumentar a agilidade das suas tarefas.além disso, as teclas serigrafadas são um destaque adicional. Com letras nítidas e visíveis, projetadas para facilitar a digitação e auxiliar você em todas as suas tarefas diárias. Agora você pode digitar com confiança, mesmo em ambientes com pouca luz.para acompanhar seu estilo de vida em movimento, o notebook é alimentado por uma bateria de longa duração, com uma média de 8 horas* de autonomia. Isso o torna ideal para atividades fora de casa, como levar para a escola ou faculdade, permitindo que você trabalhe ou estude sem se preocupar em encontrar uma tomada. Afinal, o vision c é leve, fino e portátil, pesando apenas 1,7 kg e espessura de 19,9 mm. Isso significa que você pode levá-lo para qualquer lugar com facilidade.&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>R$1439.0</t>
+  </si>
+  <si>
+    <t>Notebook Soyo Intel Dual Core N4020, 8GB DDR4, SSD 240GB, Tela 14.1 HD, Windows 10 Pro</t>
+  </si>
+  <si>
+    <t>Notebook soyo - processadores intel® dual core n4020 - ddr4nós somos a everex, comprometidos com o desenvolvimento de produtos de alta tecnologia e qualidade para você!alto desempenho, com os processadores intel® dual core n4020.os notebooks soyo, utilizam os processadores intel® dual core, que combinam desempenho, segurança e versatilidade em um design compacto e exclusivo.permite verificar e-mails, estudar, navegar nas redes sociais ou fazer streaming de música e filmes.plugue no seu monitor ou na tv, através de um cabo hdmi (não incluso).projetado para se adaptar ao escritório ou residência.ajuste flexível: ultracompacto e moderno, se encaixa perfeitamente em qualquer ambiente de trabalho ou residencial.desempenho de alto nívelprocessamento mais avançado: processadores intel® dual core de última geração, para que sua rotina seja mais eficiente.memória ddr4oferece mais desempenho e tecnologia: realize várias tarefas ao mesmo tempo com mais eficiência, com memória ddr4.alcance +,todos os diasconecte-se de qualquer lugar: portátil e leve, com fonte de energia bivolt, wi-fi integrado e tecnologia de última geração, que oferece velocidades mais rápidas e melhor desempenho, onde quer que você decida trabalhar, estudar ou se divertir!especificaçoes técnicas:marca:soyomodelo: notebook 14.1”tela: 14.1´´ high definition, alta resolução 1366x768bateria: íon de lítio 7.6v 5000mah / 38whprocessador: intel® dual core n4020memória ram: permite utilizar até 2 slots de 8gb cadasistema operacional:windows 10 professionaltipo de memória:sodimm ddr4expansão de memória:16 gbrede:10/100/1000 mbpswi-fi:802.11a/b/g/n/acfonte:bivolt 100-240v ac - 60hx / saída: 12vdc 2a 24wunidade optica: n?o possuigarantia: 12 mesespeso: 1,8 kg.dimensões: 18,9 x 33,26 x 22,35 cm( produto) (axlxc)homologacão: anatel&lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;notebook 14´1 soyo:&lt;/strong&gt; notebook&lt;br&gt;&lt;strong&gt;portatil:&lt;/strong&gt; 1,8 kg&lt;br&gt;&lt;strong&gt;windows:&lt;/strong&gt; 10 pro - soyofessional&lt;br&gt;&lt;strong&gt;memoria:&lt;/strong&gt; ddr4&lt;br&gt;&lt;strong&gt;tela:&lt;/strong&gt; 14.1´´ high definition resolução 1366x768&lt;br&gt;&lt;strong&gt;cor:&lt;/strong&gt; cinza</t>
+  </si>
+  <si>
+    <t>R$1818.31</t>
+  </si>
+  <si>
     <t>Usado - Notebook Lenovo Ideapad S145, AMD Ryzen 5-3500u, 8GB, 1TB, Tela 15.6p, Windows 10 - 81v70004br - Seminovo</t>
   </si>
   <si>
     <t>Notebook Lenovo Ideapad S145-81V70004BR, cor prata, processador AMD Ryzen 5-3500U de 2.1GHz até 3.7GHz, memória RAM de 8GB DDR4, HD de 1TB, tela de 15.6 polegadas e sistema operacional Windows 10.&lt;br /&gt;&lt;br /&gt;Modelo/Referencia: S145-15API-81V70004BR&lt;br /&gt;&lt;br /&gt;Certificação: Recertificado&lt;br /&gt;&lt;br /&gt;Medalha: Bronze&lt;br /&gt;&lt;br /&gt;FICHA TÉCNICA:&lt;br /&gt;&lt;br /&gt;Sistema operacional: Windows 10 &lt;br /&gt;&lt;br /&gt;Processador: AMD Ryzen 5 3500U– Quad Care ( 8 Threads)- Frequência: 2.1GHz até 3.7GHz– 4 MB de Cache. &lt;br /&gt;&lt;br /&gt;Memoria: 8 GB RAM DDR4- 2400MHz&lt;br /&gt;&lt;br /&gt;Armazenamento: 1 TB&lt;br /&gt;&lt;br /&gt;Tela: 15.6” (1366x768)&lt;br /&gt;&lt;br /&gt;Placa Gráfica: Radeon RX Vega 8 Graphics - Integrada &lt;br /&gt;&lt;br /&gt;Conectividade: Bluetooth 4.2 – WiFi 1x1 802.11 AC&lt;br /&gt;&lt;br /&gt;Teclado: Teclado português Brasil (ABNT) – teclado independente numérico &lt;br /&gt;&lt;br /&gt;Observação: Este produto não possui leitor de CD/DVD&lt;br /&gt;&lt;br /&gt;Entrada: Entrada para fonte de alimentação, 1x USB 2.0, 2x USB 3.1Gen 1 , 1x HDMI, Leitor de cartões 4 em 1 (SD, SDHC, SDXC, MMC).&lt;br /&gt;&lt;br /&gt;Conteúdo da embalagem: Notebook, Fonte carregadora do notebook&lt;br /&gt;&lt;br /&gt;Observação: O produto não acompanha manual de instruções&lt;br /&gt;&lt;br /&gt;Garantia: 3 meses&lt;br /&gt;&lt;br /&gt;ATENÇÃO: VOCÊ ESTÁ ADQUIRINDO UM PRODUTO RECERTIFICADO!!!! &lt;br /&gt;&lt;br /&gt;O produto não acompanha caixa original, manual ou qualquer outro acessório. Apenas fonte de alimentação do notebook&lt;br /&gt;&lt;br /&gt;Entenda o que é um produto recertificado:&lt;br /&gt;&lt;br /&gt;É um produto que volta do mercado disponível para venda nas mesmas condições de um produto novo, com suas funcionalidades e características originais. O produto passa por um rigoroso processo de análise onde todas as suas funcionalidades são testadas e o produto liberado para venda. &lt;br /&gt;&lt;br /&gt;O produto recertificado é classificado em medalhas de acordo com o estado estético e superficial do produto, sendo: OURO, PRATA E BRONZE.&lt;br /&gt;&lt;br /&gt;Recertificado Bronze: Produto possuí riscos visíveis (nenhum risco apresentado é na tela do produto). Estes riscos não alteram o funcionamento do equipamento.&lt;br /&gt;&lt;br /&gt;Atenção: O Saldão da Informática não enviará fotos reais dos produtos para os clientes, como também não reservaremos produtos. As imagens exibidas são meramente ilustrativas.</t>
   </si>
   <si>
-    <t>Notebook Lenovo Ideapad 3i Celeron 4gb 500gb Linux 15.6´´ Prata</t>
-  </si>
-  <si>
-    <t>Notebook Lenovo IdeaPad 3i Celeron 4GB 500GB Linux 15.6´´ PrataLenovo IdeaPad 3i possui design leve e compacto. Com tela antirreflexo de 15.6´´ para mais conforto visual. Notebook ideal para todos os momentos. Conta com WiFi AC ultrarrá,pido e teclado numé,rico para trabalhar com mais agilidade nas suas planilhas. Possibilidade de utilizar o armazenamento de forma hí,brida e ganhar muito mais agilidade e produtividade no seu dia a dia. Com o slot disponí,vel, você, tem a opç,ã,o de adicionar um SSD NVMe M.2 para ter mais seguranç,a ao armazenar seus dados.CONECTIVIDADEBluetooth SimUSB (2.0) 1Leitor de Cartõ,es 4 em 1 (SD, SDHC, SDXC, MMC)USB (3.2) 2..</t>
-  </si>
-  <si>
-    <t>R$2935.9</t>
-  </si>
-  <si>
-    <t>Notebook Concórdia C3115, Intel Core I3-1115g4, 8GB, SSD 256GB, Tela 15.6 HD, Linux</t>
-  </si>
-  <si>
-    <t>&lt;strong&gt;notebook concórdia c3115 i3 1115g4 8gb ssd 256gb tela 15,6&amp;quot hd&amp;nbsplinux ?&amp;nbsp&lt;/strong&gt;??????apresentamos o mais recente lançamento no mundo dos notebooks: o modelo que combina versatilidade, confiabilidade, modernidade e tecnologia&amp;nbspde&amp;nbspponta! &lt;strong&gt;notebook concórdia c3115.&lt;/strong&gt; com recursos adaptáveis ao seu estilo de vida, oferecendo alta qualidade, durabilidade e desempenho consistente. Sua aparência elegante com resolução hd e recursos avançados é o combo perfeito para tornar a experiência digital a mais&amp;nbspexcepcional.</t>
-  </si>
-  <si>
-    <t>R$2781.0</t>
-  </si>
-  <si>
-    <t>Usado - Notebook Acer Aspire 5, Intel Core I3-1115g4, 8GB, SSD 512GB, Tela 14 Full HD, Windows 10 - A514-54-37m1 - Vitrine</t>
-  </si>
-  <si>
-    <t>ATENÇÃO: VOCÊ ESTÁ ADQUIRINDO UM PRODUTO RECERTIFICADO!!!! &lt;br /&gt;&lt;br /&gt;O produto acompanha a caixa original de fábrica, não acompanha manual de instruções ou qualquer outro acessório  &lt;br /&gt;&lt;br /&gt;Entenda o que é um produto recertificado:&lt;br /&gt;&lt;br /&gt;É um produto que volta do mercado disponível para venda nas mesmas condições de um produto novo, com suas funcionalidades e características originais. O produto passa por um rigoroso processo de análise onde todas as suas funcionalidades são testadas e o produto liberado para venda. &lt;br /&gt;O produto recertificado é classificado em medalhas de acordo com o estado estético e superficial do produto, sendo: OURO, PRATA E BRONZE.&lt;br /&gt;&lt;br /&gt;Recertificado Ouro: Produto está em ótimas condições estéticas, similar a um produto novo.&lt;br /&gt;&lt;br /&gt;Atenção: O Saldão da Informática não enviará fotos reais dos produtos para os clientes, como também não reservaremos produtos. As imagens exibidas são meramente ilustrativas.&lt;br /&gt;&lt;br /&gt;Notebook Acer Aspire 5 A514-54-37M1, cor dourado, processador de 11º geração Intel Core i3-1115G4 de 3.00GHz até 4.10GHz, memória RAM de 8GB DDR4, SSD de 512GB, tela de 14 polegadas e sistema operacional Windows 10&lt;br /&gt;&lt;br /&gt;Modelo/Referencia: A514-54-37M1&lt;br /&gt;&lt;br /&gt;Certificação: Recertificado&lt;br /&gt;&lt;br /&gt;Medalha: Ouro&lt;br /&gt;&lt;br /&gt;FICHA TÉCNICA:&lt;br /&gt;&lt;br /&gt;Sistema operacional: Windows 10 Home 64-bits&lt;br /&gt;&lt;br /&gt;Processador: Intel Core i3-1115G4  - Dual Core (4 Threads) - Frequência: até 4.10 GHz - 6 MB  Smart Cache&lt;br /&gt;&lt;br /&gt;Memoria: 8 GB RAM (4 GB Soldada + 4 GB Módulo) - DDR4-2666 Mhz - Expansível até 20 GB&lt;br /&gt;&lt;br /&gt;Armazenamento: 512 GB SDD PCIe 3.0 x4 NVMe (M.2 2280)&lt;br /&gt;&lt;br /&gt;Tela: 14” IPS FHD (1920 x 1080)&lt;br /&gt;&lt;br /&gt;Gráfico: Intel UHD Graphics&lt;br /&gt;&lt;br /&gt;Conectividade: Bluetooth 5.0 - Suporte a redes com frequência de (2.4 GHz e 5 GHz) - Wireless IEE 802.11a/b/g/n/ac&lt;br /&gt;&lt;br /&gt;Teclado: português do Brasil (ABNT2)&lt;br /&gt;&lt;br /&gt;Observação: Este produto não possui leitor de CD/DVD&lt;br /&gt;&lt;br /&gt;Upgrades: Slot livre SATA 3, compatível com HDD ou SSD SATA 3 2.5” de até 2TB&lt;br /&gt;&lt;br /&gt;Entrada: Entrada para fonte de alimentação, Porta (RJ-45), Porta HDMI 2.0, 2x Portas USB 3.2 Gen 1 (5 Gbps), Porta USB Type-C 3.2 Gen 1 (5 Gbps), Porta USB 2.0&lt;br /&gt;&lt;br /&gt;Conteúdo da embalagem: Notebook, Fonte carregadora do notebook&lt;br /&gt;&lt;br /&gt;Observação: O produto não acompanha manual de instruções&lt;br /&gt;&lt;br /&gt;Garantia: 3 meses</t>
-  </si>
-  <si>
-    <t>R$2665.56</t>
-  </si>
-  <si>
-    <t>Notebook Concórdia C3115, Intel Core I3-1115g4, 8GB, SSD 512GB, Tela 15.6 HD, Linux</t>
-  </si>
-  <si>
-    <t>&lt;strong&gt;notebook concórdia c3115 i3 1115g4 8gb ssd 512gb tela 15,6&amp;quot hd linux&amp;nbsp &amp;nbsp&lt;/strong&gt;apresentamos o mais recente lançamento no mundo dos notebooks: o modelo que combina versatilidade, confiabilidade, modernidade e tecnologia&amp;nbspde&amp;nbspponta! &lt;strong&gt;notebook concórdia c3115.&lt;/strong&gt; com recursos adaptáveis ao seu estilo de vida, oferecendo alta qualidade, durabilidade e desempenho consistente. Sua aparência elegante com resolução hd e recursos avançados é o combo perfeito para tornar a experiência digital a mais&amp;nbspexcepcional.</t>
-  </si>
-  <si>
-    <t>R$2839.0</t>
-  </si>
-  <si>
-    <t>Usado - Notebook Lenovo Thinkpad T480 Core I5 8350u, 8GB RAM, SSD 256GB, Windows 10 Pro</t>
-  </si>
-  <si>
-    <t>A agasus oferece ao mercado a comercialização de computadores, notebooks, servidores, monitores, smartphones e periféricos seminovos das marcas líderes com o objetivo de levar tecnologia e preço acessível a todos os seus clientes.          informações principais:    - marca: lenovo       - sku: p003680-v1    - modelo: thinkpad t480    - marca processador: intel    - placa gráfica: uhd graphics 620    -  linha processador: core i5 8350ugº    - memória ram: 8gb    - capacidade hd: 500gb    - sistema operativo: windows     - versão do sistema operacional: 10 pro    - tamanho da tela: 14”    -  resolução da tela: ?1920 x 1080 pixels    - tipo de bateria: íon de lítio    - mais informações: consulte ficha técnica do anuncio ou entre em contato         itens testados:    - teclado,    - webcam,    - audio (microfone, saída, entrada de fone),    - fonte,    - tela,    - rede cabeada e wi-fi,    - portas usb,    - saidas de vídeo,    - slots de memória e hd.         conteúdo da embalagem:    - 1x notebook     - 1x fonte (original ou genérica),    - não acompanha manual de instruções         obs sobre a bateria:    a autonomia da bateria poderá variar dependendo da configuração, dos aplicativos carregados, das configurações de energia e dos recursos utilizados. Os equipamentos podem trazer baterias proprio ou genéricas, testadas e revisadas por nossa equipe técnica. Ressaltamos que a bateria poderá não apresentar a mesma vida útil de um produto fechado.         garantia:     ****6 meses de garantia diretamente com a nossa loja agasus***   &lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;conteúdo da embalagem:&lt;/strong&gt; 1x notebook1x fonte (original ou genérica),&lt;br&gt;&lt;strong&gt;processador:&lt;/strong&gt; intel core i5 8350u&lt;br&gt;&lt;strong&gt;código anatel:&lt;/strong&gt; 010430802198&lt;br&gt;&lt;strong&gt;garantia:&lt;/strong&gt; 6 meses&lt;br&gt;&lt;strong&gt;conectividade:&lt;/strong&gt; wifi&lt;br&gt;&lt;strong&gt;memória ram:&lt;/strong&gt; 8gb&lt;br&gt;&lt;strong&gt;modelo:&lt;/strong&gt; thinkpad t480&lt;br&gt;&lt;strong&gt;ean:&lt;/strong&gt; 0192330094382&lt;br&gt;&lt;strong&gt;correios width:&lt;/strong&gt; 48&lt;br&gt;&lt;strong&gt;categories:&lt;/strong&gt; [493, 494, 495, 496, 498, 499, 500, 501, 502, 504, 2, 539]&lt;br&gt;&lt;strong&gt;tipo de teclado:&lt;/strong&gt; abnt&lt;br&gt;&lt;strong&gt;estado:&lt;/strong&gt; seminovo&lt;br&gt;&lt;strong&gt;special price from date:&lt;/strong&gt; 2022-01-06 00:00:00&lt;br&gt;&lt;strong&gt;condição:&lt;/strong&gt; muito bom&lt;br&gt;&lt;strong&gt;tamanho da tela:&lt;/strong&gt; 14´´&lt;br&gt;&lt;strong&gt;correios height:&lt;/strong&gt; 27&lt;br&gt;&lt;strong&gt;sistema operacional:&lt;/strong&gt; windows 10 pro&lt;br&gt;&lt;strong&gt;memória interna:&lt;/strong&gt; 256gb</t>
-  </si>
-  <si>
-    <t>Usado - Notebook Acer Aspire 5 A514-54-52ty, Intel Core I5-1135g7, 8GB, SSD 256GB, Tela 14 Polegadas, Windows 10 - Seminovo</t>
-  </si>
-  <si>
-    <t>Notebook Acer Aspire 5 A514-54-52Ty, processador de 11º geração Intel Core i5-1135G7 de 2.40GHz até 4.20GHz, memória RAM de 8GB DDR4, SSD de 256GB, tela de 14 polegadas e sistema operacional Windows 10&lt;br /&gt;&lt;br /&gt;Modelo/Referencia: A514-54-52Ty&lt;br /&gt;&lt;br /&gt;Certificação: Recertificado&lt;br /&gt;&lt;br /&gt;Medalha: Bronze&lt;br /&gt;&lt;br /&gt;FICHA TÉCNICA:&lt;br /&gt;Sistema operacional: Windows 11 home 64- bits&lt;br /&gt;&lt;br /&gt;Processador: Intel Core i5– 1135G7- Quad Core (8 threads) – Frequência: até 4.20 GHz - 8 MB Intel de SmartCache &lt;br /&gt;&lt;br /&gt;Memoria: 8 GB RAM DDR4 (4GB Soldada + 4GB Módulo) - DDR4-2666MHz – Expansível até 20GB&lt;br /&gt;&lt;br /&gt;Armazenamento: 256 GB SSD PCIe 3.0 x4 NVMe (M.2 2280)&lt;br /&gt;&lt;br /&gt;Tela: 14” IPS FHD (1920 x 1080)&lt;br /&gt;&lt;br /&gt;Placa Gráfica: Intel Iris Xe Graphics com memória compartilhada com a memória RAM&lt;br /&gt; &lt;br /&gt;Conectividade: Bluetooth 5.0 - Suporte a redes com frequência (2.4 GHz e 5 GHz) – Wireless LAN 802.11a/b/g/n/ac&lt;br /&gt;&lt;br /&gt;Teclado: português do Brasil (ABNT2) – Multi-gestual com dois botões- Teclado numérico independente&lt;br /&gt;&lt;br /&gt;Observação: Este produto não possui leitor de CD/DVD&lt;br /&gt;&lt;br /&gt;Upgrades: Slot ocupado M.2 2280, compatível com unidades SSD PCIe 3.0 NVMe x2/x4 de até 512 GB - Slot livre SATA 3, compatível com HDD ou SSD SATA 3 2.5” de até 2TB&lt;br /&gt;&lt;br /&gt;Entrada: Entrada para fonte de alimentação, Porta Ethernet (RJ-45), 2x portas USB 3.2 Gen 1 (5 Gbps), Entrada combo para alto falante e fone de ouvido, Porta USB Type-C® 3.2 Gen 1 (5 Gbps), Porta USB 2.0, Porta HDMI®2.0&lt;br /&gt;&lt;br /&gt;Conteúdo da embalagem: Notebook, Fonte carregadora do notebook&lt;br /&gt;&lt;br /&gt;Observação: O produto não acompanha manual de instruções&lt;br /&gt;&lt;br /&gt;Garantia: 3 meses&lt;br /&gt;&lt;br /&gt;ATENÇÃO: VOCÊ ESTÁ ADQUIRINDO UM PRODUTO RECERTIFICADO!!!! &lt;br /&gt;&lt;br /&gt;O produto acompanha a caixa original de fábrica, não acompanha manual de instruções ou qualquer outro acessório &lt;br /&gt;&lt;br /&gt;Entenda o que é um produto recertificado:&lt;br /&gt;&lt;br /&gt;É um produto que volta do mercado disponível para venda nas mesmas condições de um produto novo, com suas funcionalidades e características originais. O produto passa por um rigoroso processo de análise onde todas as suas funcionalidades são testadas e o produto liberado para venda. &lt;br /&gt;&lt;br /&gt;O produto recertificado é classificado em medalhas de acordo com o estado estético e superficial do produto, sendo: OURO, PRATA E BRONZE.&lt;br /&gt;&lt;br /&gt;Recertificado Ouro: Produto está em ótimas condições estéticas, similar a um produto novo. &lt;br /&gt;&lt;br /&gt;Recertificado Prata: Produto tem características similares ao Ouro, pode apresentar mínimos riscos quase imperceptíveis. &lt;br /&gt;&lt;br /&gt;Recertificado Bronze: Produto possuí riscos visíveis (nenhum risco apresentado é na tela do produto). Estes riscos não alteram o funcionamento do equipamento.&lt;br /&gt;&lt;br /&gt;Atenção: O Saldão da Informática não enviará fotos reais dos produtos para os clientes, como também não reservaremos produtos. As imagens exibidas são meramente ilustrativas.</t>
-  </si>
-  <si>
-    <t>Notebook Lenovo Ideapad 3 15itl6, Intel I3-1115G4, 8GB, SSD 256GB, Tela de 15.6 Polegadas FULLHD, Windows 11 Home</t>
-  </si>
-  <si>
-    <t>Notebook lenovo ideapad 3 15itl6 15.6 fhd/ i3-1115g4/ 8gb/ 256gb ssd/ win 11 home&lt;br&gt;&lt;br&gt;armazenamento : ssd&lt;br&gt;cor : cinza artico&lt;br&gt;memoria : 8gb ddr4 3200&lt;br&gt;memoria maxima : 128gb&lt;br&gt;processador : i3-1115g4&lt;br&gt;rj 45 : nao&lt;br&gt;ssd : 256gb m.2 pcie nvme&lt;br&gt;tela : 15.6 full hd antirreflexo&lt;br&gt;garantia com o fabricante : 01 ano&lt;br&gt;precisa de pilhas ou baterias : sim&lt;br&gt;as pilhas ou baterias estao inclusas : sim&lt;br&gt;tipo de bateria ou pilha : lithium ion&lt;br&gt;dimensao da embalagem a / p / l : 19.9mm / 236.5mm / 359.2mm&lt;br&gt;ean : 197532097674&lt;br&gt;anatel : 05788-17-04423&lt;br&gt;ncm : 84713019&lt;br&gt;peso do produto com embalagem : 1.65kg&lt;br&gt;part number: 82md0010br&lt;br&gt;modelo: ideapad 3 15itl6&lt;br&gt;garantia com o seller: 7 dia/dias&lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;armazenamento:&lt;/strong&gt; ssd&lt;br&gt;&lt;strong&gt;cor:&lt;/strong&gt; cinza a?rtico&lt;br&gt;&lt;strong&gt;memoria:&lt;/strong&gt; 8gb ddr4 3200&lt;br&gt;&lt;strong&gt;memoria maxima:&lt;/strong&gt; 128gb&lt;br&gt;&lt;strong&gt;processador:&lt;/strong&gt; i3 1115g4&lt;br&gt;&lt;strong&gt;rj 45:&lt;/strong&gt; na?o&lt;br&gt;&lt;strong&gt;ssd:&lt;/strong&gt; 256gb m.2 pcie nvme&lt;br&gt;&lt;strong&gt;tela:&lt;/strong&gt; 15.6 full hd antirreflexo&lt;br&gt;&lt;strong&gt;garantia com o. Fabricante:&lt;/strong&gt; 01 ano&lt;br&gt;&lt;strong&gt;precisa de pilhas ou baterias?:&lt;/strong&gt; sim&lt;br&gt;&lt;strong&gt;as pilhas ou baterias estao inclusas?:&lt;/strong&gt; sim&lt;br&gt;&lt;strong&gt;tipo de bateria ou pilha:&lt;/strong&gt; lithium ion&lt;br&gt;&lt;strong&gt;dimensao da embalagem a. / p. / l.:&lt;/strong&gt; 19.9mm / 236.5mm / 359.2mm&lt;br&gt;&lt;strong&gt;ean:&lt;/strong&gt; 197532097674&lt;br&gt;&lt;strong&gt;anatel:&lt;/strong&gt; 05788 17 04423&lt;br&gt;&lt;strong&gt;ncm:&lt;/strong&gt; 84713019&lt;br&gt;&lt;strong&gt;peso do produto com embalagem:&lt;/strong&gt; 1.65kg&lt;br&gt;&lt;strong&gt;garantia com o. Seller::&lt;/strong&gt; 7 dia/dias&lt;br&gt;&lt;strong&gt;part number:&lt;/strong&gt; 82md0010br</t>
-  </si>
-  <si>
-    <t>R$2893.12</t>
-  </si>
-  <si>
-    <t>Notebook Positivo Vision C15, Intel Celeron, 4GB, SSD 240GB, Tela Lumina 15 HD, Linux, Cinza</t>
-  </si>
-  <si>
-    <t>Notebook positivo vision c15 intel® celeron® linux 4gb 240gb ssd lumina bar 15” hd - cinzadescubra a nova linha de notebooks positivo vision, perfeito para todas as suas atividades diárias! Desenvolvido com foco em praticidade, ele é ideal para tarefas leves como planilhas, edição de texto e navegação na web. Além disso, você poderá desfrutar de vídeo chamadas com sua câmera de alta definição. Suporta softwares de ensino e ferramentas básicas de trabalho, o positivo vision c15 garante que você esteja sempre pronto para alcançar seus objetivos. Não perca tempo, experimente o poder da nova linha positivo vision e eleve suas atividades diárias a um novo nível de eficiência.quem confia na qualidade do seu produto oferece garantia ampliada. O positivo vision c15 conta com 2 anos de garantia de fábrica.a positivo tecnologia inova no mercado ao lançar a primeira linha de notebooks do mundo com a tecnologia lumina bar, oferecendo uma experiência superior aos usuários. Os notebooks possuem barras de led com ajuste de 3 níveis de intensidade, proporcionando uma iluminação ideal para a webcam, resultando em uma captura de imagem excepcional mesmo em ambientes com pouca iluminação.tecla link exclusiva para conectar o celular ao notebook de uma forma mais simples. Sincronização de fotos, salvamento de imagens com facilidade, visualização de mensagens sms, status da bateria, entre outras funcionalidades com apenas um toque.mais agilidade com o smart touch, composto por 3 botões na lateral do vision c15 para você criar atalhos com os aplicativos que mais usa. Escolha o que cada um vai abrir para aumentar a agilidade das suas tarefas.além disso, as teclas serigrafadas são um destaque adicional. Com letras nítidas e visíveis, projetadas para facilitar a digitação e auxiliar você em todas as suas tarefas diárias. Agora você pode digitar com confiança, mesmo em ambientes com pouca luz.para acompanhar seu estilo de vida em movimento, o notebook é alimentado por uma bateria de longa duração, com uma média de 8 horas* de autonomia. Isso o torna ideal para atividades fora de casa, como levar para a escola ou faculdade, permitindo que você trabalhe ou estude sem se preocupar em encontrar uma tomada. Afinal, o vision c é leve, fino e portátil, pesando apenas 1,7 kg e espessura de 19,9 mm. Isso significa que você pode levá-lo para qualquer lugar com facilidade.&lt;br&gt;</t>
-  </si>
-  <si>
-    <t>R$1439.0</t>
-  </si>
-  <si>
-    <t>Notebook Soyo Intel Dual Core N4020, 8GB DDR4, SSD 240GB, Tela 14.1 HD, Windows 10 Pro</t>
-  </si>
-  <si>
-    <t>Notebook soyo - processadores intel® dual core n4020 - ddr4nós somos a everex, comprometidos com o desenvolvimento de produtos de alta tecnologia e qualidade para você!alto desempenho, com os processadores intel® dual core n4020.os notebooks soyo, utilizam os processadores intel® dual core, que combinam desempenho, segurança e versatilidade em um design compacto e exclusivo.permite verificar e-mails, estudar, navegar nas redes sociais ou fazer streaming de música e filmes.plugue no seu monitor ou na tv, através de um cabo hdmi (não incluso).projetado para se adaptar ao escritório ou residência.ajuste flexível: ultracompacto e moderno, se encaixa perfeitamente em qualquer ambiente de trabalho ou residencial.desempenho de alto nívelprocessamento mais avançado: processadores intel® dual core de última geração, para que sua rotina seja mais eficiente.memória ddr4oferece mais desempenho e tecnologia: realize várias tarefas ao mesmo tempo com mais eficiência, com memória ddr4.alcance +,todos os diasconecte-se de qualquer lugar: portátil e leve, com fonte de energia bivolt, wi-fi integrado e tecnologia de última geração, que oferece velocidades mais rápidas e melhor desempenho, onde quer que você decida trabalhar, estudar ou se divertir!especificaçoes técnicas:marca:soyomodelo: notebook 14.1”tela: 14.1´´ high definition, alta resolução 1366x768bateria: íon de lítio 7.6v 5000mah / 38whprocessador: intel® dual core n4020memória ram: permite utilizar até 2 slots de 8gb cadasistema operacional:windows 10 professionaltipo de memória:sodimm ddr4expansão de memória:16 gbrede:10/100/1000 mbpswi-fi:802.11a/b/g/n/acfonte:bivolt 100-240v ac - 60hx / saída: 12vdc 2a 24wunidade optica: n?o possuigarantia: 12 mesespeso: 1,8 kg.dimensões: 18,9 x 33,26 x 22,35 cm( produto) (axlxc)homologacão: anatel&lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;notebook 14´1 soyo:&lt;/strong&gt; notebook&lt;br&gt;&lt;strong&gt;portatil:&lt;/strong&gt; 1,8 kg&lt;br&gt;&lt;strong&gt;windows:&lt;/strong&gt; 10 pro - soyofessional&lt;br&gt;&lt;strong&gt;memoria:&lt;/strong&gt; ddr4&lt;br&gt;&lt;strong&gt;tela:&lt;/strong&gt; 14.1´´ high definition resolução 1366x768&lt;br&gt;&lt;strong&gt;cor:&lt;/strong&gt; cinza</t>
-  </si>
-  <si>
-    <t>R$1818.31</t>
-  </si>
-  <si>
     <t>Compre Notebook M11w Prime 2 Em 1 Windows 11 Home E Ganhe Teclado + Mouse Sem Fio 2,4 Ghz 1600 Dpi Usb Preto  Tc202k</t>
   </si>
   <si>
@@ -1925,33 +1916,6 @@
   </si>
   <si>
     <t>R$1725.8</t>
-  </si>
-  <si>
-    <t>Notebook Positivo Vision C15 Intel Celeron Dual Core, 4GB RAM, 128GB Emmc, Tela 15 Polegadas HD, Lumina Bar - Cinza</t>
-  </si>
-  <si>
-    <t>Descrição &lt;br /&gt;tecla link &lt;br /&gt;tecla exclusiva para conectar o celular &lt;br /&gt;ao notebook de uma forma mais &lt;br /&gt;simples. Sincronização de fotos, &lt;br /&gt;transferência de imagens com facilidade, &lt;br /&gt;visualização de mensagens sms, status &lt;br /&gt;da bateria, entre outras funcionalidades &lt;br /&gt;com apenas um toque &lt;br /&gt;lumina bar &lt;br /&gt;a positivo inova no mercado ao lançar a &lt;br /&gt;primeira linha de notebooks do mundo com &lt;br /&gt;a tecnologia lumina bar, oferecendo uma &lt;br /&gt;experiência superior aos usuários. Esses &lt;br /&gt;notebooks possuem barras de led com &lt;br /&gt;ajuste de 3 níveis de intensidade, &lt;br /&gt;proporcionando uma iluminação ideal para a &lt;br /&gt;webcam, resultando em uma captura de &lt;br /&gt;imagem excepcional mesmo em ambientes &lt;br /&gt;com pouca iluminação. &lt;br /&gt;vision para qualquer lugar &lt;br /&gt;o design moderno com linhas mais &lt;br /&gt;retas e sutis. Produto com tela hd de &lt;br /&gt;15.6?? Combinada com a leveza do &lt;br /&gt;aparelho, somente 1,7kg e espessura &lt;br /&gt;de 19,9 mm. Fácil de levar na mochila &lt;br /&gt;ou na bolsa, acompanha para &lt;br /&gt;qualquer ambiente, lindo onde estiver. &lt;br /&gt;sistema fanless &lt;br /&gt;o positivo vision c 15 possui um &lt;br /&gt;sistema sem aquecimento e sem ruídos &lt;br /&gt;para um uso sem distrações. Tecnologia &lt;br /&gt;que faz com que as máquinas não &lt;br /&gt;precisem de ventoinhas para a &lt;br /&gt;refrigeração. &lt;br /&gt;armazenamento expansível com slot de ssd ou hd disponível &lt;br /&gt;caso precise de mais &lt;br /&gt;armazenamento, o positivo vision &lt;br /&gt;c15 conta com um slot disponível &lt;br /&gt;para um upgrade no seu &lt;br /&gt;notebook. &lt;br /&gt;smart touch &lt;br /&gt;o positivo vision c15 traz o exclusivo smart &lt;br /&gt;touch, que consiste em uma barra touch &lt;br /&gt;com 3 ícones retro-iluminados com funções &lt;br /&gt;customizáveis, através do software de &lt;br /&gt;customização integrado no produto, &lt;br /&gt;possibilitando mais liberdade ao usuário &lt;br /&gt;para criar acessos rápidos a aplicativos ou &lt;br /&gt;sites favoritos! &lt;br /&gt;especificações técnicas &lt;br /&gt;código de homologação anatel: 06446-16-04076 &lt;br /&gt;processador &lt;br /&gt;fabricante do processador: intel® &lt;br /&gt;linha do processador: celeron® dual core &lt;br /&gt;modelo do processador: n4020 &lt;br /&gt;arquitetura do processador :64 bits</t>
-  </si>
-  <si>
-    <t>R$1259.0</t>
-  </si>
-  <si>
-    <t>Notebook Lenovo Ideapad 1i I3-1215u, 4GB RAM, SSD 256GB Nvme, 15.6 polegadas, Windows 11, 82vy000tbr</t>
-  </si>
-  <si>
-    <t>O ideapad&amp;trade, 1i eleva sua categoria de notebooks com um processador intel&amp;reg, super eficiente de 12&amp;ordf, gera&amp;ccedil,&amp;atilde,o em um chassi fino e compacto de 17,9 mm que facilita a multitarefa enquanto aumenta a efici&amp;ecirc,ncia energ&amp;eacute,tica com at&amp;eacute, 11 horas de dura&amp;ccedil,&amp;atilde,o da bateria e carga r&amp;aacute,pida. Obtenha aproveitamento m&amp;aacute,ximo da tela com as molduras super estreitas, alto-falantes dolby audio&amp;trade, e flip to start para inicializa&amp;ccedil,&amp;atilde,o instant&amp;acirc,nea. Otimize sua experi&amp;ecirc,ncia de chamada de v&amp;iacute,deo com uma c&amp;acirc,mera de 1mp que vem com um obturador de privacidade para afastar os olhos curiosos e o cancelamento de ru&amp;iacute,do inteligente para cortar o ru&amp;iacute,do de fundo no seu microfone.dois alto-falantes dolby audio&amp;trade, tamb&amp;eacute,m transmitem &amp;aacute,udio rico e robusto. Com um processador intel&amp;reg, de 12&amp;ordf, gera&amp;ccedil,&amp;atilde,o em seu laptop, voc&amp;ecirc, pode, sem esfor&amp;ccedil,o, realizar multiplas tarefas simultaneamente, comunicar-se facilmente com amigos e familiares e levar todo o seu entretenimento favorito para onde for. Mantenha-se produtivo em qualquer lugar com uma longa vida &amp;uacute,til da bateria com apenas uma carga. Em seguida, recarregue sua bateria em 15 minutos com um r&amp;aacute,pido impulso de carga para us&amp;aacute,-lo por 2 horas. Sem wifi? N&amp;atilde,o se preocupe, com a op&amp;ccedil,&amp;atilde,o de armazenamento r&amp;aacute,pido ssd, voc&amp;ecirc, pode continuar acessando e editando arquivos offline.marca: lenovonome do produto: ideapad 1inome do modelo: ideapad 1 15iau7part number: 82vy000tbrcor: cloud greycategoria: notebooksegmento: ultrafinoprocessador: intel core i3-1215u (cores / threads) 6 cores / 8 threads (cache) 6mb (clock) 1.2ghz (4.4ghz max turbo)mem&amp;oacute,ria ram: 4gbdetalhe mem&amp;oacute,ria ram: 4gb soldado ddr4-3200barramento da mem&amp;oacute,ria: 3200mhzarmazenamento (ssd): ssd de 256gb pcie nvme m.2m&amp;aacute,xima expans&amp;atilde,o de armazenamento: um slot, at&amp;eacute, 1tb m.2 2242 ssd ou 512gb m.2 2280 ssdchipset: intel socplaca de v&amp;iacute,deo: intel uhd graphicssistema operacional: windows 11tela: 15.6´´resolu&amp;ccedil,&amp;atilde,o de tela: hd (1366 x 768) antirreflexoformato de tela: 16:9 widescreenbrilho da tela: 220 nitstipo de painel: tnabertura de tela: 169&amp;deg,wi-fi: wifi 2x2 acdrive &amp;oacute,ptico (leitor dvd): n&amp;atilde,ocamera: hd-720p com privacidademicrofone: microfone tipo dual arraybluetooth: bluetooth 5.0sintonizador de tv: n&amp;atilde,oaudio (alto-falantes): alto-falantes com certifica&amp;ccedil,&amp;atilde,o dolby&amp;reg, audio (2 x 1.5w)audio (porta combo para headset/headphone): 1usb (3.2) gen 1: 1usb (2.0): 1usb tipo c (3.2) gen 1: 1kensington lock: n&amp;atilde,oleitor de cart&amp;otilde,es: leitor de cart&amp;otilde,es 4 em 1 (sd, sdhc, sdxc, mmc)sa&amp;iacute,da hdmi ( 1.4b): 1sa&amp;iacute,da vga: n&amp;atilde,orj-45: n&amp;atilde,olan / rede: n&amp;atilde,oleitor de impress&amp;atilde,o digital: n&amp;atilde,optp touchpad: 1teclado padr&amp;atilde,o brasileiro: 1teclado backlit led: n&amp;atilde,oteclado num&amp;eacute,rico: 1bateria: 3 c&amp;eacute,lulas 42whbateria remov&amp;iacute,vel: n&amp;atilde,oadaptador ac: 65wdimens&amp;otilde,es produto aprox. Largura: 360.2 mmdimens&amp;otilde,es produto aprox. Profundidade: 236 mmdimens&amp;otilde,es produto aprox. Altura: 17.9mmpeso produto aprox.: 1.63 kgdimens&amp;otilde,es embalagem aprox. Largura: 533 mmdimens&amp;otilde,es embalagem aprox. Profundidade: 333 mmdimens&amp;otilde,es embalagem aprox. Altura: 74 mmpeso embalagem aprox.: 2.42 kg&lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;anatel:&lt;/strong&gt; 057881704423&lt;br&gt;&lt;strong&gt;processador:&lt;/strong&gt; core i3&lt;br&gt;&lt;strong&gt;marca do processador:&lt;/strong&gt; intel&lt;br&gt;&lt;strong&gt;nome do sistema operacional:&lt;/strong&gt; windows 11&lt;br&gt;&lt;strong&gt;memória ram:&lt;/strong&gt; 4gb&lt;br&gt;&lt;strong&gt;capacidade do ssd:&lt;/strong&gt; 256gb&lt;br&gt;&lt;strong&gt;tela:&lt;/strong&gt; 15.6´´ hd (1366 x. 768)&lt;br&gt;&lt;strong&gt;cor:&lt;/strong&gt; cloud grey</t>
-  </si>
-  <si>
-    <t>R$2854.0</t>
-  </si>
-  <si>
-    <t>Notebook Positivo C4128ei Celeron N3350, 4GB DDR4, SSD 480GB, Tela 14 Polegadas, HD Led, Windows 10 Pro</t>
-  </si>
-  <si>
-    <t>&lt;strong&gt;notebook positivo motion i341tbi&amp;nbspintel core i3-7100u.&lt;/strong&gt;o notebook positivo motion i tem design moderno e fino, ele disponibiliza o máximo em entretenimento e diversão! O positivo motion série i, é o notebook para quem deseja um equipamento elegante e funcional. O notebook positivo motion i conta com processador intel 7100u de baixo consumo de energia, intel graphics que faz sua experiência visual ser incrível em alta definição, a memória ddr4 traz mais performance e menor consumo de bateria, além de tudo, também tem aplicativos para escritório (editor de texto, planilha eletrônica, gerenciador de apresentações, editor de imagens e editor html) e antivírus grátis. Seu touchpad teve suas dimensões e funcionalidades atualizadas! Basta um simples gesto para ativar o teclado numérico. Seus filmes, músicas e vídeos favoritos estão ainda mais perto! O teclado conta com teclas de acesso rápido netflix*, deezer* e youtube, que são entretenimento garantido ao simples toque de um botão. Trabalhe e divirta-se o dia todo, sem precisar estar conectado a tomada, graças à bateria com mais de 5 horas de duração.&lt;strong&gt;especificações:&lt;/strong&gt;marca: positivomodelo: motion&amp;nbspi341tbipart number: 3011794, 3011873cor: cinza escurowebcam, com webcam coverprocessador:&amp;nbspintel core i3-7100u (3m de cache, 2,40 ghz)sistema operacional: windows 10 pro, 64bits em português brasilmemória:&amp;nbspram 4 gbtipo de memória: on-board ddr4armazenamento: hd 1tb 5400rpmleitor de cartões micro sd, suporta os padrões sdhc e sdxctela:&amp;nbsplcd 14&amp;#39&amp;nbspwidescreen led&amp;nbspresolução 1366 x 768 de alta definição (hd)vídeo:&amp;nbspprocessamento de vídeo integrado intel graphicsáudio:&amp;nbspáudio de alta definição (hd áudio) |&amp;nbspmicrofone e alto-falantes estéreo embutidosconectividade:&amp;nbsprede sem fio ieee 802.11 b/g/ntm |&amp;nbspbluetooth 4.0conexão:1x usb 3.1 gen 12x usb 2.0, 1x hdmi1x áudio (para microfone e fone de ouvido)1x dc-in (carregador)teclado:&amp;nbspportuguês-brasil (84 teclas + tecla power + 3 teclas de acesso rápido)mouse:&amp;nbsptipo touchpad, com toque múltiplo, 2 botões integrados e função de teclado numéricocarregador:&amp;nbsp100~240v automáticobateria:&amp;nbsp38wh - integradadimensões do produto (lxpxa): 32,9cm |&amp;nbsp21,5cm |&amp;nbsp1,9cm | peso: 1,6kg&lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;notebook positivo motion i341tbiintel core i3-7100u | entrega para todo o brasil</t>
-  </si>
-  <si>
-    <t>R$2322.0</t>
   </si>
   <si>
     <t>Notebook Multilaser Ultra, Intel Celeron, 4GB RAM, SSD 240GB, Tela 15.6 FULL HD, Windows 11 + Microsoft 365</t>
@@ -2307,7 +2271,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F223"/>
+  <dimension ref="A1:F215"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2725,32 +2689,32 @@
         <v>103</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" t="s">
         <v>105</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>106</v>
       </c>
-      <c r="C33" t="s">
+      <c r="E33" t="s">
         <v>107</v>
       </c>
-      <c r="E33" t="s">
-        <v>108</v>
-      </c>
       <c r="F33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34" t="s">
         <v>109</v>
-      </c>
-      <c r="B34" t="s">
-        <v>110</v>
       </c>
       <c r="C34" t="s">
         <v>29</v>
@@ -2758,21 +2722,21 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" t="s">
         <v>111</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>112</v>
-      </c>
-      <c r="C35" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" t="s">
         <v>114</v>
-      </c>
-      <c r="B36" t="s">
-        <v>115</v>
       </c>
       <c r="C36" t="s">
         <v>37</v>
@@ -2780,49 +2744,49 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" t="s">
         <v>116</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>117</v>
-      </c>
-      <c r="C37" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
+        <v>118</v>
+      </c>
+      <c r="B38" t="s">
         <v>119</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>120</v>
       </c>
-      <c r="C38" t="s">
+      <c r="E38" t="s">
         <v>121</v>
       </c>
-      <c r="E38" t="s">
-        <v>122</v>
-      </c>
       <c r="F38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
+        <v>122</v>
+      </c>
+      <c r="B39" t="s">
         <v>123</v>
       </c>
-      <c r="B39" t="s">
-        <v>124</v>
-      </c>
       <c r="C39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" t="s">
         <v>125</v>
-      </c>
-      <c r="B40" t="s">
-        <v>126</v>
       </c>
       <c r="C40" t="s">
         <v>33</v>
@@ -2830,27 +2794,27 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
+        <v>126</v>
+      </c>
+      <c r="B41" t="s">
         <v>127</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>128</v>
       </c>
-      <c r="C41" t="s">
+      <c r="E41" t="s">
         <v>129</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>130</v>
-      </c>
-      <c r="F41" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
+        <v>131</v>
+      </c>
+      <c r="B42" t="s">
         <v>132</v>
-      </c>
-      <c r="B42" t="s">
-        <v>133</v>
       </c>
       <c r="C42" t="s">
         <v>42</v>
@@ -2858,13 +2822,13 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
+        <v>133</v>
+      </c>
+      <c r="B43" t="s">
         <v>134</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>135</v>
-      </c>
-      <c r="C43" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2872,7 +2836,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C44" t="s">
         <v>33</v>
@@ -2880,93 +2844,93 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
+        <v>137</v>
+      </c>
+      <c r="B45" t="s">
         <v>138</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>139</v>
-      </c>
-      <c r="C45" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
+        <v>140</v>
+      </c>
+      <c r="B46" t="s">
         <v>141</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>142</v>
       </c>
-      <c r="C46" t="s">
+      <c r="E46" t="s">
         <v>143</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>144</v>
-      </c>
-      <c r="F46" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
+        <v>145</v>
+      </c>
+      <c r="B47" t="s">
         <v>146</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>147</v>
-      </c>
-      <c r="C47" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
+        <v>148</v>
+      </c>
+      <c r="B48" t="s">
         <v>149</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>150</v>
-      </c>
-      <c r="C48" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
+        <v>151</v>
+      </c>
+      <c r="B49" t="s">
         <v>152</v>
       </c>
-      <c r="B49" t="s">
-        <v>153</v>
-      </c>
       <c r="C49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
+        <v>153</v>
+      </c>
+      <c r="B50" t="s">
         <v>154</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>155</v>
-      </c>
-      <c r="C50" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
+        <v>156</v>
+      </c>
+      <c r="B51" t="s">
         <v>157</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>158</v>
-      </c>
-      <c r="C51" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
+        <v>159</v>
+      </c>
+      <c r="B52" t="s">
         <v>160</v>
-      </c>
-      <c r="B52" t="s">
-        <v>161</v>
       </c>
       <c r="C52" t="s">
         <v>29</v>
@@ -2974,10 +2938,10 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
+        <v>161</v>
+      </c>
+      <c r="B53" t="s">
         <v>162</v>
-      </c>
-      <c r="B53" t="s">
-        <v>163</v>
       </c>
       <c r="C53" t="s">
         <v>9</v>
@@ -2985,43 +2949,43 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
+        <v>163</v>
+      </c>
+      <c r="B54" t="s">
         <v>164</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>165</v>
-      </c>
-      <c r="C54" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
+        <v>166</v>
+      </c>
+      <c r="B55" t="s">
         <v>167</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>168</v>
-      </c>
-      <c r="C55" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
+        <v>169</v>
+      </c>
+      <c r="B56" t="s">
         <v>170</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>171</v>
-      </c>
-      <c r="C56" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
+        <v>172</v>
+      </c>
+      <c r="B57" t="s">
         <v>173</v>
-      </c>
-      <c r="B57" t="s">
-        <v>174</v>
       </c>
       <c r="C57" t="s">
         <v>33</v>
@@ -3029,54 +2993,54 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
+        <v>174</v>
+      </c>
+      <c r="B58" t="s">
         <v>175</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>176</v>
-      </c>
-      <c r="C58" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
+        <v>177</v>
+      </c>
+      <c r="B59" t="s">
         <v>178</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
         <v>179</v>
-      </c>
-      <c r="C59" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
+        <v>180</v>
+      </c>
+      <c r="B60" t="s">
         <v>181</v>
       </c>
-      <c r="B60" t="s">
-        <v>182</v>
-      </c>
       <c r="C60" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
+        <v>182</v>
+      </c>
+      <c r="B61" t="s">
         <v>183</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>184</v>
-      </c>
-      <c r="C61" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B62" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C62" t="s">
         <v>73</v>
@@ -3084,10 +3048,10 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
+        <v>186</v>
+      </c>
+      <c r="B63" t="s">
         <v>187</v>
-      </c>
-      <c r="B63" t="s">
-        <v>188</v>
       </c>
       <c r="C63" t="s">
         <v>83</v>
@@ -3095,186 +3059,186 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
+        <v>188</v>
+      </c>
+      <c r="B64" t="s">
         <v>189</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>190</v>
-      </c>
-      <c r="C64" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
+        <v>191</v>
+      </c>
+      <c r="B65" t="s">
         <v>192</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
         <v>193</v>
-      </c>
-      <c r="C65" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
+        <v>194</v>
+      </c>
+      <c r="B66" t="s">
         <v>195</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>196</v>
-      </c>
-      <c r="C66" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
+        <v>197</v>
+      </c>
+      <c r="B67" t="s">
         <v>198</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>199</v>
-      </c>
-      <c r="C67" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
+        <v>200</v>
+      </c>
+      <c r="B68" t="s">
         <v>201</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>202</v>
-      </c>
-      <c r="C68" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
+        <v>203</v>
+      </c>
+      <c r="B69" t="s">
         <v>204</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>205</v>
-      </c>
-      <c r="C69" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
+        <v>206</v>
+      </c>
+      <c r="B70" t="s">
         <v>207</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>208</v>
-      </c>
-      <c r="C70" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
+        <v>209</v>
+      </c>
+      <c r="B71" t="s">
         <v>210</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
         <v>211</v>
-      </c>
-      <c r="C71" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
+        <v>212</v>
+      </c>
+      <c r="B72" t="s">
         <v>213</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" t="s">
         <v>214</v>
-      </c>
-      <c r="C72" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
+        <v>215</v>
+      </c>
+      <c r="B73" t="s">
         <v>216</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
         <v>217</v>
-      </c>
-      <c r="C73" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
+        <v>218</v>
+      </c>
+      <c r="B74" t="s">
         <v>219</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" t="s">
         <v>220</v>
-      </c>
-      <c r="C74" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
+        <v>221</v>
+      </c>
+      <c r="B75" t="s">
         <v>222</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
         <v>223</v>
-      </c>
-      <c r="C75" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
+        <v>224</v>
+      </c>
+      <c r="B76" t="s">
         <v>225</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" t="s">
         <v>226</v>
-      </c>
-      <c r="C76" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
+        <v>227</v>
+      </c>
+      <c r="B77" t="s">
         <v>228</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" t="s">
         <v>229</v>
-      </c>
-      <c r="C77" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
+        <v>230</v>
+      </c>
+      <c r="B78" t="s">
         <v>231</v>
       </c>
-      <c r="B78" t="s">
-        <v>232</v>
-      </c>
       <c r="C78" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
+        <v>232</v>
+      </c>
+      <c r="B79" t="s">
         <v>233</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" t="s">
         <v>234</v>
-      </c>
-      <c r="C79" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B80" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C80" t="s">
         <v>33</v>
@@ -3282,54 +3246,54 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
+        <v>236</v>
+      </c>
+      <c r="B81" t="s">
         <v>237</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" t="s">
         <v>238</v>
-      </c>
-      <c r="C81" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
+        <v>239</v>
+      </c>
+      <c r="B82" t="s">
         <v>240</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" t="s">
         <v>241</v>
-      </c>
-      <c r="C82" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
+        <v>242</v>
+      </c>
+      <c r="B83" t="s">
         <v>243</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" t="s">
         <v>244</v>
-      </c>
-      <c r="C83" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
+        <v>245</v>
+      </c>
+      <c r="B84" t="s">
         <v>246</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" t="s">
         <v>247</v>
-      </c>
-      <c r="C84" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
+        <v>248</v>
+      </c>
+      <c r="B85" t="s">
         <v>249</v>
-      </c>
-      <c r="B85" t="s">
-        <v>250</v>
       </c>
       <c r="C85" t="s">
         <v>33</v>
@@ -3337,131 +3301,131 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
+        <v>250</v>
+      </c>
+      <c r="B86" t="s">
         <v>251</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" t="s">
         <v>252</v>
-      </c>
-      <c r="C86" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
+        <v>253</v>
+      </c>
+      <c r="B87" t="s">
         <v>254</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" t="s">
         <v>255</v>
-      </c>
-      <c r="C87" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
+        <v>256</v>
+      </c>
+      <c r="B88" t="s">
         <v>257</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" t="s">
         <v>258</v>
-      </c>
-      <c r="C88" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
+        <v>259</v>
+      </c>
+      <c r="B89" t="s">
         <v>260</v>
       </c>
-      <c r="B89" t="s">
-        <v>261</v>
-      </c>
       <c r="C89" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
+        <v>261</v>
+      </c>
+      <c r="B90" t="s">
         <v>262</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
         <v>263</v>
-      </c>
-      <c r="C90" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
+        <v>264</v>
+      </c>
+      <c r="B91" t="s">
         <v>265</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" t="s">
         <v>266</v>
-      </c>
-      <c r="C91" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
+        <v>267</v>
+      </c>
+      <c r="B92" t="s">
         <v>268</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
         <v>269</v>
-      </c>
-      <c r="C92" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B93" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C93" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
+        <v>271</v>
+      </c>
+      <c r="B94" t="s">
         <v>272</v>
       </c>
-      <c r="B94" t="s">
-        <v>273</v>
-      </c>
       <c r="C94" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
+        <v>273</v>
+      </c>
+      <c r="B95" t="s">
         <v>274</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" t="s">
         <v>275</v>
-      </c>
-      <c r="C95" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
+        <v>276</v>
+      </c>
+      <c r="B96" t="s">
         <v>277</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C96" t="s">
         <v>278</v>
-      </c>
-      <c r="C96" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
+        <v>279</v>
+      </c>
+      <c r="B97" t="s">
         <v>280</v>
-      </c>
-      <c r="B97" t="s">
-        <v>281</v>
       </c>
       <c r="C97" t="s">
         <v>37</v>
@@ -3469,137 +3433,137 @@
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
+        <v>281</v>
+      </c>
+      <c r="B98" t="s">
         <v>282</v>
       </c>
-      <c r="B98" t="s">
-        <v>283</v>
-      </c>
       <c r="C98" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="A99" t="s">
+        <v>283</v>
+      </c>
+      <c r="B99" t="s">
         <v>284</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" t="s">
         <v>285</v>
-      </c>
-      <c r="C99" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
+        <v>286</v>
+      </c>
+      <c r="B100" t="s">
         <v>287</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C100" t="s">
         <v>288</v>
       </c>
-      <c r="C100" t="s">
-        <v>289</v>
-      </c>
       <c r="E100" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F100" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B101" t="s">
         <v>67</v>
       </c>
       <c r="C101" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
+        <v>291</v>
+      </c>
+      <c r="B102" t="s">
         <v>292</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" t="s">
         <v>293</v>
-      </c>
-      <c r="C102" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" t="s">
+        <v>294</v>
+      </c>
+      <c r="B103" t="s">
         <v>295</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103" t="s">
         <v>296</v>
-      </c>
-      <c r="C103" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" t="s">
+        <v>297</v>
+      </c>
+      <c r="B104" t="s">
         <v>298</v>
       </c>
-      <c r="B104" t="s">
-        <v>299</v>
-      </c>
       <c r="C104" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" t="s">
+        <v>299</v>
+      </c>
+      <c r="B105" t="s">
+        <v>299</v>
+      </c>
+      <c r="C105" t="s">
         <v>300</v>
-      </c>
-      <c r="B105" t="s">
-        <v>300</v>
-      </c>
-      <c r="C105" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" t="s">
+        <v>301</v>
+      </c>
+      <c r="B106" t="s">
         <v>302</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C106" t="s">
         <v>303</v>
-      </c>
-      <c r="C106" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
+        <v>304</v>
+      </c>
+      <c r="B107" t="s">
         <v>305</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
         <v>306</v>
-      </c>
-      <c r="C107" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108" t="s">
+        <v>307</v>
+      </c>
+      <c r="B108" t="s">
         <v>308</v>
       </c>
-      <c r="B108" t="s">
+      <c r="C108" t="s">
         <v>309</v>
-      </c>
-      <c r="C108" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
+        <v>310</v>
+      </c>
+      <c r="B109" t="s">
         <v>311</v>
-      </c>
-      <c r="B109" t="s">
-        <v>312</v>
       </c>
       <c r="C109" t="s">
         <v>49</v>
@@ -3607,76 +3571,76 @@
     </row>
     <row r="110" spans="1:6">
       <c r="A110" t="s">
+        <v>312</v>
+      </c>
+      <c r="B110" t="s">
         <v>313</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C110" t="s">
         <v>314</v>
-      </c>
-      <c r="C110" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
+        <v>315</v>
+      </c>
+      <c r="B111" t="s">
         <v>316</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" t="s">
         <v>317</v>
-      </c>
-      <c r="C111" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
+        <v>318</v>
+      </c>
+      <c r="B112" t="s">
         <v>319</v>
       </c>
-      <c r="B112" t="s">
-        <v>320</v>
-      </c>
       <c r="C112" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
+        <v>320</v>
+      </c>
+      <c r="B113" t="s">
         <v>321</v>
       </c>
-      <c r="B113" t="s">
-        <v>322</v>
-      </c>
       <c r="C113" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
+        <v>322</v>
+      </c>
+      <c r="B114" t="s">
         <v>323</v>
       </c>
-      <c r="B114" t="s">
+      <c r="C114" t="s">
         <v>324</v>
-      </c>
-      <c r="C114" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
+        <v>325</v>
+      </c>
+      <c r="B115" t="s">
         <v>326</v>
       </c>
-      <c r="B115" t="s">
+      <c r="C115" t="s">
         <v>327</v>
-      </c>
-      <c r="C115" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
+        <v>328</v>
+      </c>
+      <c r="B116" t="s">
         <v>329</v>
-      </c>
-      <c r="B116" t="s">
-        <v>330</v>
       </c>
       <c r="C116" t="s">
         <v>46</v>
@@ -3684,65 +3648,65 @@
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
+        <v>330</v>
+      </c>
+      <c r="B117" t="s">
         <v>331</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C117" t="s">
         <v>332</v>
-      </c>
-      <c r="C117" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
+        <v>333</v>
+      </c>
+      <c r="B118" t="s">
         <v>334</v>
       </c>
-      <c r="B118" t="s">
+      <c r="C118" t="s">
         <v>335</v>
-      </c>
-      <c r="C118" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
+        <v>336</v>
+      </c>
+      <c r="B119" t="s">
         <v>337</v>
       </c>
-      <c r="B119" t="s">
+      <c r="C119" t="s">
         <v>338</v>
-      </c>
-      <c r="C119" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
+        <v>339</v>
+      </c>
+      <c r="B120" t="s">
         <v>340</v>
       </c>
-      <c r="B120" t="s">
-        <v>341</v>
-      </c>
       <c r="C120" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
+        <v>341</v>
+      </c>
+      <c r="B121" t="s">
         <v>342</v>
       </c>
-      <c r="B121" t="s">
+      <c r="C121" t="s">
         <v>343</v>
-      </c>
-      <c r="C121" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
+        <v>344</v>
+      </c>
+      <c r="B122" t="s">
         <v>345</v>
-      </c>
-      <c r="B122" t="s">
-        <v>346</v>
       </c>
       <c r="C122" t="s">
         <v>83</v>
@@ -3750,21 +3714,21 @@
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B123" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C123" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
+        <v>347</v>
+      </c>
+      <c r="B124" t="s">
         <v>348</v>
-      </c>
-      <c r="B124" t="s">
-        <v>349</v>
       </c>
       <c r="C124" t="s">
         <v>37</v>
@@ -3772,65 +3736,65 @@
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
+        <v>349</v>
+      </c>
+      <c r="B125" t="s">
         <v>350</v>
       </c>
-      <c r="B125" t="s">
+      <c r="C125" t="s">
         <v>351</v>
-      </c>
-      <c r="C125" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
+        <v>352</v>
+      </c>
+      <c r="B126" t="s">
         <v>353</v>
       </c>
-      <c r="B126" t="s">
+      <c r="C126" t="s">
         <v>354</v>
-      </c>
-      <c r="C126" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
+        <v>355</v>
+      </c>
+      <c r="B127" t="s">
         <v>356</v>
       </c>
-      <c r="B127" t="s">
+      <c r="C127" t="s">
         <v>357</v>
-      </c>
-      <c r="C127" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
+        <v>358</v>
+      </c>
+      <c r="B128" t="s">
         <v>359</v>
       </c>
-      <c r="B128" t="s">
+      <c r="C128" t="s">
         <v>360</v>
-      </c>
-      <c r="C128" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
+        <v>361</v>
+      </c>
+      <c r="B129" t="s">
         <v>362</v>
       </c>
-      <c r="B129" t="s">
+      <c r="C129" t="s">
         <v>363</v>
-      </c>
-      <c r="C129" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
+        <v>364</v>
+      </c>
+      <c r="B130" t="s">
         <v>365</v>
-      </c>
-      <c r="B130" t="s">
-        <v>366</v>
       </c>
       <c r="C130" t="s">
         <v>33</v>
@@ -3838,10 +3802,10 @@
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
+        <v>366</v>
+      </c>
+      <c r="B131" t="s">
         <v>367</v>
-      </c>
-      <c r="B131" t="s">
-        <v>368</v>
       </c>
       <c r="C131" t="s">
         <v>64</v>
@@ -3849,109 +3813,109 @@
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
+        <v>368</v>
+      </c>
+      <c r="B132" t="s">
+        <v>368</v>
+      </c>
+      <c r="C132" t="s">
         <v>369</v>
-      </c>
-      <c r="B132" t="s">
-        <v>369</v>
-      </c>
-      <c r="C132" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
+        <v>370</v>
+      </c>
+      <c r="B133" t="s">
         <v>371</v>
       </c>
-      <c r="B133" t="s">
-        <v>372</v>
-      </c>
       <c r="C133" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
+        <v>372</v>
+      </c>
+      <c r="B134" t="s">
         <v>373</v>
       </c>
-      <c r="B134" t="s">
+      <c r="C134" t="s">
         <v>374</v>
-      </c>
-      <c r="C134" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
+        <v>375</v>
+      </c>
+      <c r="B135" t="s">
         <v>376</v>
       </c>
-      <c r="B135" t="s">
+      <c r="C135" t="s">
         <v>377</v>
-      </c>
-      <c r="C135" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
+        <v>378</v>
+      </c>
+      <c r="B136" t="s">
         <v>379</v>
       </c>
-      <c r="B136" t="s">
+      <c r="C136" t="s">
         <v>380</v>
-      </c>
-      <c r="C136" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
+        <v>381</v>
+      </c>
+      <c r="B137" t="s">
         <v>382</v>
       </c>
-      <c r="B137" t="s">
+      <c r="C137" t="s">
         <v>383</v>
-      </c>
-      <c r="C137" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
+        <v>384</v>
+      </c>
+      <c r="B138" t="s">
         <v>385</v>
       </c>
-      <c r="B138" t="s">
+      <c r="C138" t="s">
         <v>386</v>
-      </c>
-      <c r="C138" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
+        <v>387</v>
+      </c>
+      <c r="B139" t="s">
         <v>388</v>
       </c>
-      <c r="B139" t="s">
+      <c r="C139" t="s">
         <v>389</v>
-      </c>
-      <c r="C139" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
+        <v>390</v>
+      </c>
+      <c r="B140" t="s">
         <v>391</v>
       </c>
-      <c r="B140" t="s">
+      <c r="C140" t="s">
         <v>392</v>
-      </c>
-      <c r="C140" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
+        <v>393</v>
+      </c>
+      <c r="B141" t="s">
         <v>394</v>
-      </c>
-      <c r="B141" t="s">
-        <v>395</v>
       </c>
       <c r="C141" t="s">
         <v>37</v>
@@ -3959,65 +3923,65 @@
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
+        <v>395</v>
+      </c>
+      <c r="B142" t="s">
         <v>396</v>
       </c>
-      <c r="B142" t="s">
+      <c r="C142" t="s">
         <v>397</v>
-      </c>
-      <c r="C142" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
+        <v>398</v>
+      </c>
+      <c r="B143" t="s">
         <v>399</v>
       </c>
-      <c r="B143" t="s">
+      <c r="C143" t="s">
         <v>400</v>
-      </c>
-      <c r="C143" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
+        <v>401</v>
+      </c>
+      <c r="B144" t="s">
         <v>402</v>
       </c>
-      <c r="B144" t="s">
+      <c r="C144" t="s">
         <v>403</v>
-      </c>
-      <c r="C144" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
+        <v>404</v>
+      </c>
+      <c r="B145" t="s">
         <v>405</v>
       </c>
-      <c r="B145" t="s">
+      <c r="C145" t="s">
         <v>406</v>
-      </c>
-      <c r="C145" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
+        <v>407</v>
+      </c>
+      <c r="B146" t="s">
         <v>408</v>
       </c>
-      <c r="B146" t="s">
+      <c r="C146" t="s">
         <v>409</v>
-      </c>
-      <c r="C146" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
+        <v>410</v>
+      </c>
+      <c r="B147" t="s">
         <v>411</v>
-      </c>
-      <c r="B147" t="s">
-        <v>412</v>
       </c>
       <c r="C147" t="s">
         <v>64</v>
@@ -4025,208 +3989,208 @@
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
+        <v>412</v>
+      </c>
+      <c r="B148" t="s">
+        <v>412</v>
+      </c>
+      <c r="C148" t="s">
         <v>413</v>
-      </c>
-      <c r="B148" t="s">
-        <v>413</v>
-      </c>
-      <c r="C148" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
+        <v>414</v>
+      </c>
+      <c r="B149" t="s">
+        <v>414</v>
+      </c>
+      <c r="C149" t="s">
         <v>415</v>
-      </c>
-      <c r="B149" t="s">
-        <v>415</v>
-      </c>
-      <c r="C149" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
+        <v>416</v>
+      </c>
+      <c r="B150" t="s">
+        <v>331</v>
+      </c>
+      <c r="C150" t="s">
         <v>417</v>
-      </c>
-      <c r="B150" t="s">
-        <v>332</v>
-      </c>
-      <c r="C150" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
+        <v>418</v>
+      </c>
+      <c r="B151" t="s">
         <v>419</v>
       </c>
-      <c r="B151" t="s">
+      <c r="C151" t="s">
         <v>420</v>
-      </c>
-      <c r="C151" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
+        <v>421</v>
+      </c>
+      <c r="B152" t="s">
         <v>422</v>
       </c>
-      <c r="B152" t="s">
-        <v>423</v>
-      </c>
       <c r="C152" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
+        <v>423</v>
+      </c>
+      <c r="B153" t="s">
         <v>424</v>
       </c>
-      <c r="B153" t="s">
+      <c r="C153" t="s">
         <v>425</v>
-      </c>
-      <c r="C153" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
+        <v>426</v>
+      </c>
+      <c r="B154" t="s">
         <v>427</v>
       </c>
-      <c r="B154" t="s">
+      <c r="C154" t="s">
         <v>428</v>
-      </c>
-      <c r="C154" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
+        <v>429</v>
+      </c>
+      <c r="B155" t="s">
         <v>430</v>
       </c>
-      <c r="B155" t="s">
+      <c r="C155" t="s">
         <v>431</v>
-      </c>
-      <c r="C155" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
+        <v>432</v>
+      </c>
+      <c r="B156" t="s">
         <v>433</v>
       </c>
-      <c r="B156" t="s">
+      <c r="C156" t="s">
         <v>434</v>
-      </c>
-      <c r="C156" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
+        <v>435</v>
+      </c>
+      <c r="B157" t="s">
         <v>436</v>
       </c>
-      <c r="B157" t="s">
+      <c r="C157" t="s">
         <v>437</v>
-      </c>
-      <c r="C157" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
+        <v>438</v>
+      </c>
+      <c r="B158" t="s">
         <v>439</v>
       </c>
-      <c r="B158" t="s">
+      <c r="C158" t="s">
         <v>440</v>
-      </c>
-      <c r="C158" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B159" t="s">
+        <v>441</v>
+      </c>
+      <c r="C159" t="s">
         <v>442</v>
-      </c>
-      <c r="C159" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
+        <v>443</v>
+      </c>
+      <c r="B160" t="s">
         <v>444</v>
       </c>
-      <c r="B160" t="s">
+      <c r="C160" t="s">
         <v>445</v>
-      </c>
-      <c r="C160" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
+        <v>446</v>
+      </c>
+      <c r="B161" t="s">
         <v>447</v>
       </c>
-      <c r="B161" t="s">
+      <c r="C161" t="s">
         <v>448</v>
-      </c>
-      <c r="C161" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
+        <v>449</v>
+      </c>
+      <c r="B162" t="s">
         <v>450</v>
       </c>
-      <c r="B162" t="s">
+      <c r="C162" t="s">
         <v>451</v>
-      </c>
-      <c r="C162" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
+        <v>452</v>
+      </c>
+      <c r="B163" t="s">
         <v>453</v>
       </c>
-      <c r="B163" t="s">
+      <c r="C163" t="s">
         <v>454</v>
-      </c>
-      <c r="C163" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
+        <v>455</v>
+      </c>
+      <c r="B164" t="s">
         <v>456</v>
       </c>
-      <c r="B164" t="s">
+      <c r="C164" t="s">
         <v>457</v>
-      </c>
-      <c r="C164" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
+        <v>458</v>
+      </c>
+      <c r="B165" t="s">
         <v>459</v>
       </c>
-      <c r="B165" t="s">
+      <c r="C165" t="s">
         <v>460</v>
-      </c>
-      <c r="C165" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
+        <v>461</v>
+      </c>
+      <c r="B166" t="s">
         <v>462</v>
-      </c>
-      <c r="B166" t="s">
-        <v>463</v>
       </c>
       <c r="C166" t="s">
         <v>73</v>
@@ -4234,178 +4198,190 @@
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
+        <v>463</v>
+      </c>
+      <c r="B167" t="s">
         <v>464</v>
       </c>
-      <c r="B167" t="s">
+      <c r="C167" t="s">
         <v>465</v>
-      </c>
-      <c r="C167" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
+        <v>466</v>
+      </c>
+      <c r="B168" t="s">
         <v>467</v>
       </c>
-      <c r="B168" t="s">
+      <c r="C168" t="s">
         <v>468</v>
-      </c>
-      <c r="C168" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
+        <v>469</v>
+      </c>
+      <c r="B169" t="s">
         <v>470</v>
       </c>
-      <c r="B169" t="s">
+      <c r="C169" t="s">
         <v>471</v>
-      </c>
-      <c r="C169" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
+        <v>472</v>
+      </c>
+      <c r="B170" t="s">
         <v>473</v>
       </c>
-      <c r="B170" t="s">
+      <c r="C170" t="s">
         <v>474</v>
-      </c>
-      <c r="C170" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
+        <v>475</v>
+      </c>
+      <c r="B171" t="s">
         <v>476</v>
       </c>
-      <c r="B171" t="s">
+      <c r="C171" t="s">
         <v>477</v>
-      </c>
-      <c r="C171" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
+        <v>478</v>
+      </c>
+      <c r="B172" t="s">
         <v>479</v>
       </c>
-      <c r="B172" t="s">
+      <c r="C172" t="s">
         <v>480</v>
-      </c>
-      <c r="C172" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
+        <v>481</v>
+      </c>
+      <c r="B173" t="s">
         <v>482</v>
       </c>
-      <c r="B173" t="s">
+      <c r="C173" t="s">
         <v>483</v>
-      </c>
-      <c r="C173" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
+        <v>484</v>
+      </c>
+      <c r="B174" t="s">
         <v>485</v>
       </c>
-      <c r="B174" t="s">
+      <c r="C174" t="s">
         <v>486</v>
-      </c>
-      <c r="C174" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
+        <v>487</v>
+      </c>
+      <c r="B175" t="s">
         <v>488</v>
       </c>
-      <c r="B175" t="s">
-        <v>489</v>
-      </c>
       <c r="C175" t="s">
-        <v>490</v>
+        <v>97</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
+        <v>487</v>
+      </c>
+      <c r="B176" t="s">
         <v>488</v>
       </c>
-      <c r="B176" t="s">
-        <v>489</v>
-      </c>
       <c r="C176" t="s">
-        <v>490</v>
+        <v>97</v>
       </c>
     </row>
     <row r="177" spans="1:6">
       <c r="A177" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B177" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C177" t="s">
-        <v>493</v>
+        <v>155</v>
       </c>
     </row>
     <row r="178" spans="1:6">
       <c r="A178" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B178" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C178" t="s">
-        <v>496</v>
+        <v>223</v>
       </c>
     </row>
     <row r="179" spans="1:6">
       <c r="A179" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="B179" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="C179" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
     </row>
     <row r="180" spans="1:6">
       <c r="A180" t="s">
+        <v>496</v>
+      </c>
+      <c r="B180" t="s">
         <v>497</v>
       </c>
-      <c r="B180" t="s">
+      <c r="C180" t="s">
         <v>498</v>
       </c>
-      <c r="C180" t="s">
-        <v>97</v>
+      <c r="E180" t="s">
+        <v>64</v>
+      </c>
+      <c r="F180" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="181" spans="1:6">
       <c r="A181" t="s">
+        <v>496</v>
+      </c>
+      <c r="B181" t="s">
+        <v>497</v>
+      </c>
+      <c r="C181" t="s">
+        <v>498</v>
+      </c>
+      <c r="E181" t="s">
+        <v>64</v>
+      </c>
+      <c r="F181" t="s">
         <v>499</v>
-      </c>
-      <c r="B181" t="s">
-        <v>500</v>
-      </c>
-      <c r="C181" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="182" spans="1:6">
       <c r="A182" t="s">
+        <v>500</v>
+      </c>
+      <c r="B182" t="s">
         <v>501</v>
       </c>
-      <c r="B182" t="s">
+      <c r="C182" t="s">
         <v>502</v>
-      </c>
-      <c r="C182" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="183" spans="1:6">
@@ -4416,74 +4392,62 @@
         <v>504</v>
       </c>
       <c r="C183" t="s">
-        <v>505</v>
+        <v>33</v>
       </c>
     </row>
     <row r="184" spans="1:6">
       <c r="A184" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B184" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C184" t="s">
-        <v>156</v>
+        <v>502</v>
       </c>
     </row>
     <row r="185" spans="1:6">
       <c r="A185" t="s">
+        <v>505</v>
+      </c>
+      <c r="B185" t="s">
         <v>506</v>
       </c>
-      <c r="B185" t="s">
-        <v>507</v>
-      </c>
       <c r="C185" t="s">
-        <v>83</v>
+        <v>263</v>
       </c>
     </row>
     <row r="186" spans="1:6">
       <c r="A186" t="s">
+        <v>507</v>
+      </c>
+      <c r="B186" t="s">
         <v>508</v>
       </c>
-      <c r="B186" t="s">
+      <c r="C186" t="s">
         <v>509</v>
-      </c>
-      <c r="C186" t="s">
-        <v>510</v>
-      </c>
-      <c r="E186" t="s">
-        <v>64</v>
-      </c>
-      <c r="F186" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="187" spans="1:6">
       <c r="A187" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="B187" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
       <c r="C187" t="s">
-        <v>83</v>
+        <v>354</v>
       </c>
     </row>
     <row r="188" spans="1:6">
       <c r="A188" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
       <c r="B188" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="C188" t="s">
-        <v>510</v>
-      </c>
-      <c r="E188" t="s">
-        <v>64</v>
-      </c>
-      <c r="F188" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
     </row>
     <row r="189" spans="1:6">
@@ -4494,194 +4458,194 @@
         <v>513</v>
       </c>
       <c r="C189" t="s">
-        <v>355</v>
+        <v>514</v>
       </c>
     </row>
     <row r="190" spans="1:6">
       <c r="A190" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B190" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C190" t="s">
-        <v>33</v>
+        <v>517</v>
       </c>
     </row>
     <row r="191" spans="1:6">
       <c r="A191" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="B191" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="C191" t="s">
-        <v>264</v>
+        <v>520</v>
       </c>
     </row>
     <row r="192" spans="1:6">
       <c r="A192" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="B192" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
       <c r="C192" t="s">
-        <v>33</v>
+        <v>523</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>518</v>
+        <v>524</v>
       </c>
       <c r="B193" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="C193" t="s">
-        <v>520</v>
+        <v>526</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>521</v>
+        <v>527</v>
       </c>
       <c r="B194" t="s">
-        <v>522</v>
+        <v>528</v>
       </c>
       <c r="C194" t="s">
-        <v>355</v>
+        <v>529</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>521</v>
+        <v>530</v>
       </c>
       <c r="B195" t="s">
-        <v>522</v>
+        <v>531</v>
       </c>
       <c r="C195" t="s">
-        <v>355</v>
+        <v>29</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>523</v>
+        <v>532</v>
       </c>
       <c r="B196" t="s">
-        <v>524</v>
+        <v>533</v>
       </c>
       <c r="C196" t="s">
-        <v>525</v>
+        <v>49</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>526</v>
+        <v>534</v>
       </c>
       <c r="B197" t="s">
-        <v>527</v>
+        <v>535</v>
       </c>
       <c r="C197" t="s">
-        <v>528</v>
+        <v>226</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>529</v>
+        <v>536</v>
       </c>
       <c r="B198" t="s">
-        <v>530</v>
+        <v>537</v>
       </c>
       <c r="C198" t="s">
-        <v>531</v>
+        <v>369</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>532</v>
+        <v>538</v>
       </c>
       <c r="B199" t="s">
-        <v>533</v>
+        <v>539</v>
       </c>
       <c r="C199" t="s">
-        <v>534</v>
+        <v>42</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>535</v>
+        <v>540</v>
       </c>
       <c r="B200" t="s">
-        <v>536</v>
+        <v>541</v>
       </c>
       <c r="C200" t="s">
-        <v>29</v>
+        <v>542</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="B201" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="C201" t="s">
-        <v>49</v>
+        <v>542</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B202" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C202" t="s">
-        <v>370</v>
+        <v>542</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="B203" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="C203" t="s">
-        <v>297</v>
+        <v>545</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>541</v>
+        <v>546</v>
       </c>
       <c r="B204" t="s">
-        <v>542</v>
+        <v>547</v>
       </c>
       <c r="C204" t="s">
-        <v>297</v>
+        <v>548</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>539</v>
+        <v>549</v>
       </c>
       <c r="B205" t="s">
-        <v>540</v>
+        <v>550</v>
       </c>
       <c r="C205" t="s">
-        <v>370</v>
+        <v>190</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>543</v>
+        <v>551</v>
       </c>
       <c r="B206" t="s">
-        <v>544</v>
+        <v>552</v>
       </c>
       <c r="C206" t="s">
-        <v>545</v>
+        <v>553</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -4697,178 +4661,90 @@
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>549</v>
+        <v>554</v>
       </c>
       <c r="B208" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="C208" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="B209" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="C209" t="s">
-        <v>554</v>
+        <v>190</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="B210" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="C210" t="s">
-        <v>191</v>
+        <v>559</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="B211" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="C211" t="s">
-        <v>551</v>
+        <v>562</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>552</v>
+        <v>560</v>
       </c>
       <c r="B212" t="s">
-        <v>553</v>
+        <v>561</v>
       </c>
       <c r="C212" t="s">
-        <v>554</v>
+        <v>562</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" t="s">
-        <v>557</v>
+        <v>563</v>
       </c>
       <c r="B213" t="s">
-        <v>558</v>
+        <v>564</v>
       </c>
       <c r="C213" t="s">
-        <v>551</v>
+        <v>296</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>559</v>
+        <v>565</v>
       </c>
       <c r="B214" t="s">
-        <v>560</v>
+        <v>566</v>
       </c>
       <c r="C214" t="s">
-        <v>561</v>
+        <v>567</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>562</v>
+        <v>568</v>
       </c>
       <c r="B215" t="s">
-        <v>563</v>
+        <v>569</v>
       </c>
       <c r="C215" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3">
-      <c r="A216" t="s">
-        <v>565</v>
-      </c>
-      <c r="B216" t="s">
-        <v>566</v>
-      </c>
-      <c r="C216" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3">
-      <c r="A217" t="s">
-        <v>568</v>
-      </c>
-      <c r="B217" t="s">
-        <v>569</v>
-      </c>
-      <c r="C217" t="s">
         <v>570</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3">
-      <c r="A218" t="s">
-        <v>571</v>
-      </c>
-      <c r="B218" t="s">
-        <v>572</v>
-      </c>
-      <c r="C218" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3">
-      <c r="A219" t="s">
-        <v>571</v>
-      </c>
-      <c r="B219" t="s">
-        <v>572</v>
-      </c>
-      <c r="C219" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3">
-      <c r="A220" t="s">
-        <v>574</v>
-      </c>
-      <c r="B220" t="s">
-        <v>575</v>
-      </c>
-      <c r="C220" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3">
-      <c r="A221" t="s">
-        <v>577</v>
-      </c>
-      <c r="B221" t="s">
-        <v>578</v>
-      </c>
-      <c r="C221" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3">
-      <c r="A222" t="s">
-        <v>577</v>
-      </c>
-      <c r="B222" t="s">
-        <v>578</v>
-      </c>
-      <c r="C222" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3">
-      <c r="A223" t="s">
-        <v>580</v>
-      </c>
-      <c r="B223" t="s">
-        <v>581</v>
-      </c>
-      <c r="C223" t="s">
-        <v>582</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: iniciando desenvolvimento dos templates
</commit_message>
<xml_diff>
--- a/kabum_produtos.xlsx
+++ b/kabum_produtos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="295">
   <si>
     <t>Produto</t>
   </si>
@@ -73,12 +73,6 @@
 &lt;p&gt;Sa&amp;iacute;da full HD (1920 X 1080) de 120Hz no PS5 &amp;amp; Xbox Series X/S&lt;/p&gt;</t>
   </si>
   <si>
-    <t>Monitor Concórdia Gamer Curvo 27'', Led Full, Hd, 165hz, Freesync - Cz270f</t>
-  </si>
-  <si>
-    <t>&lt;strong&gt;você na vantagem sempre!&amp;nbsp &amp;nbsp&amp;nbsp&lt;/strong&gt;o&amp;nbsp&lt;strong&gt;monitor concórdia gamer curvo cz270f 27&amp;quot led full hd 165hz freesync&lt;/strong&gt;&amp;nbspconta com resposta de 1ms e taxa de atualização de 165hz, permitindo a mais alta performance durante suas gameplays. Sua curvatura amplia o campo de visão relativo, concentrando toda a ação ao alcance dos olhos do usuário, sem perder resolução.&lt;strong&gt;monitor curvo&amp;nbsp &amp;nbsp&lt;/strong&gt;tenha mais imersão na sua gameplay com esse monitor curvo da concórdia. Observe seus adversários ainda mais de perto com essa imersão de 1500r de curvatura e um ângulo de visão de 178º.&lt;strong&gt;inclinável&amp;nbsp&lt;/strong&gt;ajuste de inclinação da tela de 5&amp;deg a 15&amp;deg. Ajuste seu monitor da maneira que quiser deixando sua visão ainda mais confortável e ampla!&lt;strong&gt;especificações:&lt;/strong&gt;&lt;strong&gt;tela:&lt;/strong&gt;painel: vaárea ativa: 596.736 &amp;times 335.664 mmângulo de visão: 178/178&amp;nbspcurvatura: r1500&amp;nbspresolução: 1920*1080165hzdot pitch: 0,3108cores do painel: 16.7m&amp;nbsp&amp;nbspbrilho(máximo): 250cd/m2tempo de resposta: 1ms&amp;nbspcontraste: 3000: 1taxa de heartz: 165hz&amp;nbsp &amp;nbsp&lt;strong&gt;conectividade:&amp;nbsp&lt;/strong&gt;hdmidisplayport 1.4dvientrada earphonedc (energia)&lt;strong&gt;alimentação:&lt;/strong&gt;tipo: adaptador externovoltagem: 12v/3.5aconsumo: 38w | stand by: 0.5w&amp;nbsp&lt;strong&gt;recursos do monitor:&lt;/strong&gt;- base de fácil desmontagem- freesync/g-sync&amp;nbsp&amp;nbsp- filtro de luz azul- flicker free- baixo consumo em modo stand by- overdriver&amp;nbsp- base fixa- sem bordas- auto falante interno: sim.- vesa: 100*100mm.&amp;nbsp&lt;strong&gt;acompanha:&lt;/strong&gt;&amp;nbspcabo displayport,&amp;nbspmanual do usuário e parafusos.&amp;nbsp&amp;nbsp&lt;strong&gt;dimensões da tela (cm)(axlxp):&lt;/strong&gt;&amp;nbsp36 | 61 | 4,5 | peso(kg): 4,734.&lt;strong&gt;dimensões da tela com base&amp;nbsp(cm)(axlxp)&lt;/strong&gt;: 43 | 61 | 17 | peso(kg): 4,734.&lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;monitor concórdia gamer curvo cz270f 27´´ led full hd 165hz freesync | entregue para todo o brasil |</t>
-  </si>
-  <si>
     <t>Monitor Gamer Asus TUF 31.5 LED 2K QHD, 165Hz, 1ms, HDMI e DisplayPort,  HDR, 120% sRGB, FreeSync Premium, Som Integrado, VESA - VG32VQ1B</t>
   </si>
   <si>
@@ -140,6 +134,12 @@
 &lt;h3&gt;Aproveite essa oportunidade e adquira seu Monitor Gamer no KaBuM!&lt;/h3&gt;</t>
   </si>
   <si>
+    <t>Monitor Gamer AOC Hero 27 Full HD, Wide, 144 Hz, 1ms, IPS, HDMI e VGA, G-Sync, Ajuste de Ângulo - 27G2/BK</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;O monitor AOC Hero 27 &amp;eacute; compat&amp;iacute;vel com a tecnologia G-Sync e entrega aos gamers uma experi&amp;ecirc;ncia lisa, r&amp;aacute;pida e responsiva em todos os jogos. Experimente uma jogabilidade impec&amp;aacute;vel com a taxa de atualiza&amp;ccedil;&amp;atilde;o de tela 144 Hz que garante imagens r&amp;aacute;pidas, suaves e movimentos n&amp;iacute;tidos, para nenhum detalhe passar despercebido.&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>Monitor Gamer Acer KG251Q Nitro 24.5" Full HD, 250Hz, 1ms, Displayport e HDMI, HDR10, FreeSync, Preto - UM.KX1AA.Z02</t>
   </si>
   <si>
@@ -155,12 +155,6 @@
 &lt;p&gt;&amp;Eacute; uma tecnologia de exibi&amp;ccedil;&amp;atilde;o que cria&lt;strong&gt; n&amp;iacute;veis mais profundos de contraste&lt;/strong&gt; em preto e branco, proporcionando uma imers&amp;atilde;o de n&amp;iacute;vel maior por meio da recria&amp;ccedil;&amp;atilde;o de imagem realista.&lt;/p&gt;
 &lt;p&gt;&amp;nbsp;&lt;/p&gt;
 &lt;h3&gt;Compre agora no KaBuM"&lt;/h3&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer AOC Hero 27 Full HD, Wide, 144 Hz, 1ms, IPS, HDMI e VGA, G-Sync, Ajuste de Ângulo - 27G2/BK</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;O monitor AOC Hero 27 &amp;eacute; compat&amp;iacute;vel com a tecnologia G-Sync e entrega aos gamers uma experi&amp;ecirc;ncia lisa, r&amp;aacute;pida e responsiva em todos os jogos. Experimente uma jogabilidade impec&amp;aacute;vel com a taxa de atualiza&amp;ccedil;&amp;atilde;o de tela 144 Hz que garante imagens r&amp;aacute;pidas, suaves e movimentos n&amp;iacute;tidos, para nenhum detalhe passar despercebido.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Monitor Gamer AOC Legend 27' LED, Curvo, 240 Hz, Full HD, 0.5ms, FreeSync Premium, 120% sRGB, HDMI/DisplayPort - C27G2ZE</t>
@@ -192,12 +186,6 @@
 &lt;h3 style="text-align: justify;"&gt;Compre agora no KaBuM!&lt;/h3&gt;</t>
   </si>
   <si>
-    <t>Monitor Gamer AOC Hero 23.8 Full HD, Wide, 144 Hz, 1ms, FreeSync, HDMI e DisplayPort, IPS, Ajuste de Altura - 24G2/BK</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;O monitor Gamer AOC Hero &amp;eacute; compat&amp;iacute;vel com a tecnologia G-Sync e entrega aos gamers uma experi&amp;ecirc;ncia lisa, r&amp;aacute;pida e responsiva em todos os jogos. Experimente uma jogabilidade impec&amp;aacute;vel com a taxa de atualiza&amp;ccedil;&amp;atilde;o de tela 144 Hz que garante imagens r&amp;aacute;pidas, suaves e movimentos n&amp;iacute;tidos, para nenhum detalhe passar despercebido.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>Monitor Gamer LG UltraGear 24 Full HD, 144Hz, 1ms, IPS, HDMI e DisplayPort, 99% sRGB, HDR, FreeSync Premium, VESA - 24GN60R-B.AWZM</t>
   </si>
   <si>
@@ -208,6 +196,12 @@
 &lt;h2&gt;&lt;br /&gt;HDR10 com sRGB 99% (T&amp;iacute;p.)&lt;/h2&gt;
 &lt;p&gt;Este monitor suporta HDR10 com sRGB 99% (Tip.) permitindo uma imers&amp;atilde;o visual realista com contraste e cores de grande riqueza. Independentemente do campo de batalha, poder&amp;aacute; ajudar os jogadores a ver as cores dram&amp;aacute;ticas pretendidas pelos criadores do jogo.&lt;br /&gt;Com a tecnologia FreeSync Premium, os jogadores podem experimentar movimentos fluidos e cont&amp;iacute;nuos em jogos de alta resolu&amp;ccedil;&amp;atilde;o e em ritmo acelerado. Ele virtualmente minimiza a trepida&amp;ccedil;&amp;atilde;o e a trepida&amp;ccedil;&amp;atilde;o da tela.&lt;/p&gt;
 &lt;h3&gt;&lt;br /&gt;Monitor Gamer &amp;eacute; no KaBuM!&lt;/h3&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer AOC Hero 23.8 Full HD, Wide, 144 Hz, 1ms, FreeSync, HDMI e DisplayPort, IPS, Ajuste de Altura - 24G2/BK</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;O monitor Gamer AOC Hero &amp;eacute; compat&amp;iacute;vel com a tecnologia G-Sync e entrega aos gamers uma experi&amp;ecirc;ncia lisa, r&amp;aacute;pida e responsiva em todos os jogos. Experimente uma jogabilidade impec&amp;aacute;vel com a taxa de atualiza&amp;ccedil;&amp;atilde;o de tela 144 Hz que garante imagens r&amp;aacute;pidas, suaves e movimentos n&amp;iacute;tidos, para nenhum detalhe passar despercebido.&lt;/p&gt;</t>
   </si>
   <si>
     <t>Monitor Gamer AOC Viper 27 Full HD, 165Hz, 1ms, IPS, HDMI e DisplayPort, FreeSync - 27G2SE</t>
@@ -293,6 +287,15 @@
     <t>Monitor Gamer Samsung Odyssey G32A 27" Preto LS27AG320NLXZD &lt;br /&gt;Resolução FHD e painel IPS. Agora você pode ver os jogos como nunca antes. O painel IPS oferece cores claras e um amplo ângulo de visão de 178º para maior clareza a partir de qualquer posição. Com mais pixels e maior profundidade, os jogos estão mais próximos da realidade do que nunca. Compatível com Nvidia G-Sync. Jogabilidade fácil e sem esforço. A compatibilidade G-Sync mantém a placa de vídeo e o painel sincronizados para eliminar cortes, atraso de tela e rasgos de imagem. Cenas de jogo rápidas e complexas são estáveis e sem repetições com AMD FreeSync Premium aumentando sua vantagem competitiva.</t>
   </si>
   <si>
+    <t>Monitor Gamer Samsung Odyssey G4 25 IPS Full HD, 240Hz, 1ms, HDMI e DisplayPort,  99% sRGB, HDR, FreeSync Premium  - LS25BG400ELXZD</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Monitor Gamer Samsung Odyssey G4 25 IPS Full HD&lt;/h2&gt;
+&lt;p&gt;Resolu&amp;ccedil;&amp;atilde;o FHD e painel IPS. Agora voc&amp;ecirc; pode ver os jogos como nunca antes. O painel IPS oferece cores claras e um amplo &amp;acirc;ngulo de vis&amp;atilde;o de 178&amp;ordm; para maior clareza a partir de qualquer posi&amp;ccedil;&amp;atilde;o. Com mais pixels e maior profundidade, os jogos est&amp;atilde;o mais pr&amp;oacute;ximos da realidade do que nunca.&lt;br /&gt;240Hz de taxa de atualiza&amp;ccedil;&amp;atilde;o &amp;amp; 1ms de tempo de resposta. Velocidade nas cenas. A taxa de atualiza&amp;ccedil;&amp;atilde;o de 240Hz elimina o atraso para uma jogabilidade emocionante com a&amp;ccedil;&amp;atilde;o ultra-suave. Ataque os inimigos assim que os v&amp;ecirc;-los com um tempo de resposta de 1ms e quadros sem borr&amp;atilde;o.&lt;/p&gt;
+&lt;h2&gt;&lt;br /&gt;Foco sem nunca quebrar o fluxo&lt;/h2&gt;
+&lt;p&gt;Compat&amp;iacute;vel com Nvidia G-Sync. Jogabilidade f&amp;aacute;cil e sem esfor&amp;ccedil;o. A compatibilidade G-Sync mant&amp;eacute;m a placa de v&amp;iacute;deo e o painel sincronizados para eliminar cortes, atraso de tela e rasgos de imagem. Cenas de jogo r&amp;aacute;pidas e complexas s&amp;atilde;o est&amp;aacute;veis e sem repeti&amp;ccedil;&amp;otilde;es com AMD FreeSync Premium aumentando sua vantagem competitiva.&lt;br /&gt;Auto Source Switch+ Ligue e jogue instantaneamente. Com o Auto Source Switch+, seu monitor detecta quando os dispositivos conectados s&amp;atilde;o ligados e muda instantaneamente para o novo sinal de fonte. Isto o ajuda a chegar mais r&amp;aacute;pido &amp;agrave; a&amp;ccedil;&amp;atilde;o do jogo sem passar por v&amp;aacute;rias fontes de entrada.&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>Monitor Gamer Gigabyte 27 Curvo, Full HD, HDMI/DisplayPort, FreeSync, 165Hz, 1ms, Altura Ajustável - G27FC-A-SA</t>
   </si>
   <si>
@@ -395,6 +398,26 @@
 &lt;h3&gt;Aproveite essa oportunidade e adquira seu Monitor Gamer Acer no KaBuM!&lt;/h3&gt;</t>
   </si>
   <si>
+    <t>Monitor Gamer Husky Hailstorm 31.5' LED, Curvo, 165 Hz, Full HD, 1ms, Adaptive Sync, HDMI/DisplayPort, Ajuste de Ângulo - HGMT002</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Monitor Gamer Husky Hailstorm 31.5' LED, Curvo, 165 Hz, Full HD, 1ms, Adaptive Sync, HDMI/DisplayPort, Ajuste de &amp;Acirc;ngulo&amp;nbsp;&lt;/h2&gt;
+&lt;h2&gt;&amp;nbsp;&lt;/h2&gt;
+&lt;h3&gt;Esteja um passo &amp;agrave; frente!&amp;nbsp;&lt;/h3&gt;
+&lt;p&gt;O Monitor Husky Hail Storm conta com resposta de 1ms e taxa de atualiza&amp;ccedil;&amp;atilde;o de &lt;strong&gt;165Hz&lt;/strong&gt;, permitindo a mais alta performance durante suas gameplays. Sua &lt;strong&gt;curvatura&lt;/strong&gt; amplia o campo de vis&amp;atilde;o relativo, concentrando toda a a&amp;ccedil;&amp;atilde;o ao alcance dos olhos do usu&amp;aacute;rio, sem perder resolu&amp;ccedil;&amp;atilde;o.&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Melhor Entrega de Imagens para sua Gameplay&lt;/h3&gt;
+&lt;p&gt;Compat&amp;iacute;vel com a tecnologia &lt;strong&gt;Adaptive Sync&lt;/strong&gt;, permite a sincroniza&amp;ccedil;&amp;atilde;o dos frames da placa de v&amp;iacute;deo, decretando o fim do input lag, bem como do tearing.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Conectividade&lt;/h3&gt;
+&lt;p&gt;O monitor Husky Hailstorm acompanha um cabo &lt;strong&gt;DisplayPort&lt;/strong&gt; que garante a melhor qualidade de imagem para seu jogo. Al&amp;eacute;m da conex&amp;atilde;o DP, o monitor ainda possui duas conex&amp;otilde;es &lt;strong&gt;HDMI&lt;/strong&gt; e uma &lt;strong&gt;conex&amp;atilde;o P2&lt;/strong&gt; para ouvir seu jogo diretamente do seu monitor.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Maior Ergonomia e Conforto para Uso Prolongado&amp;nbsp;&amp;nbsp;&lt;/h3&gt;
+&lt;p&gt;O Husky Hailstorm possui ajuste de &lt;strong&gt;inclina&amp;ccedil;&amp;atilde;o de 5&amp;deg; a 15&amp;deg;&lt;/strong&gt; que se ajusta ergonomicamente para o seu uso. O monitor tamb&amp;eacute;m conta com &lt;strong&gt;Redu&amp;ccedil;&amp;atilde;o de Luz Azul&lt;/strong&gt;, se tornando uma &amp;oacute;tima op&amp;ccedil;&amp;atilde;o para Gameplays prolongadas.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Seu Monitor Husky voc&amp;ecirc; encontra aqui no KaBuM!&lt;/h3&gt;</t>
+  </si>
+  <si>
     <t>Monitor Gamer AOC Sniper 27' IPS, Wide, 75 Hz, Full HD, 1ms, Adaptive Sync, 98% sRGB, HDMI/VGA, Ajuste de Ângulo - 27G2HE5</t>
   </si>
   <si>
@@ -468,12 +491,6 @@
 &lt;h3&gt;Compre j&amp;aacute; o seu no KaBuM&lt;/h3&gt;</t>
   </si>
   <si>
-    <t>Monitor Gamer Lg Ultragear 27 Polegadas,FULL  HdD144hz 1ms Ips, HDMI e Displayport</t>
-  </si>
-  <si>
-    <t>Monitor gamer lg ultragear, 27 full hd 144hz 1ms ips hdmi e displayport hdr 10 99% srgb, freesync premium vesa - 27gn65r o monitor gamer lg ultragear 27gn65r é uma opção de alta performance desenvolvida para atender às demandas dos jogadores mais exigentes. Com uma tela de 27 polegadas em resolução full hd (1920 x 1080), esse monitor oferece uma experiência visual imersiva com imagens nítidas e detalhadas. A velocidade é uma das principais características desse monitor, com um tempo de resposta ultra-rápido de 1ms (gtg), o que significa que as transições de cores são praticamente instantâneas, eliminando o efeito de arrasto nas imagens durante os jogos mais rápidos e intensos. Além disso, a taxa de atualização de 144hz proporciona uma jogabilidade mais fluida, permitindo que os jogadores vejam o próximo quadro rapidamente e tenham uma experiência de jogo mais suave. O painel ips do monitor garante ângulos de visão amplos e cores vibrantes, com suporte para 99% do espaço de cores srgb e tecnologia hdr10. Isso resulta em imagens mais realistas e ricas em detalhes, criando uma experiência de visualização imersiva para jogos, filmes e conteúdos em geral. O monitor gamer lg ultragear 27gn65r também é compatível com a tecnologia amd freesync premium e nvidia g-sync, que ajudam a eliminar o screen tearing e o stuttering durante os jogos, sincronizando a taxa de atualização do monitor com a taxa de quadros da placa gráfica para uma jogabilidade mais suave e sem interrupções. O design eletrizante e moderno do monitor complementa perfeitamente o setup gamer, enquanto a compatibilidade vesa permite a instalação em suportes ou braços para maior versatilidade. Se você busca uma experiência de jogo de alta performance com imagens fluidas, cores vívidas e tempos de resposta rápidos, o monitor gamer lg ultragear 27gn65r é uma escolha excelente para elevar seu entretenimento e desempenho nos jogos.   especificações: - marca: lg - modelo: 27gn65r     características: tela: - cor: preto - tamanho: 27” - tipo de tela: ips - ângulo de visão: 178º / 178º - resolução máxima: full hd (1920 x 1080) - brilho: 300 cd/m² - contraste: 1000:01 - tempo de resposta: 1ms (gtg) - taxa de atualização: 144hz - gama de cores: srgb 99% (típ.) - profundidade de cores (nº de cores): 16,7m - distância entre pixels: 0,3108 x 0,3108 mm - tratamento de tela: antirreflexivo   entradas e saídas: - hdmi: sim (v2.0) - displayport: sim (v1.4) - saída de fone de ouvido: sim   energia: - consumo de energia: 32w (típ.) - fonte: adaptador externo   ajustes: - ajustes de posição: inclinação, altura, pivô - tamanho da furação: 100 x 100 mm   recursos: - hdr: hdr10 - flicker safe: sim - amd freesync: freesync premium - nvidia g-sync: sim - modo leitura: sim - onscreen control: sim - motion blur reduction: sim - crosshair: sim - dynamic action sync: sim - black stabilizer: sim - plug &amp; play: sim</t>
-  </si>
-  <si>
     <t>Monitor Gamer Gigabyte, 27 Full HD, 180Hz, 1ms, DisplayPort e HDMI, 108% sRGB, HDR, Adaptive-Sync - GS27FC SA</t>
   </si>
   <si>
@@ -489,6 +506,12 @@
 &lt;p&gt;GS27FC pode exibir &lt;strong&gt;16,7 milh&amp;otilde;es de cores&lt;/strong&gt; e possui uma taxa de contraste de &lt;strong&gt;3000:1&lt;/strong&gt;. Ele permite que voc&amp;ecirc; desfrute de uma experi&amp;ecirc;ncia de jogo fluente com cores reais e vibrantes. O GS27FC est&amp;aacute; pronto para &lt;strong&gt;HDR&lt;/strong&gt;, o que desperta interesse em uma ampla gama de aplica&amp;ccedil;&amp;otilde;es, incluindo jogos, entretenimento cinematogr&amp;aacute;fico e cria&amp;ccedil;&amp;atilde;o de conte&amp;uacute;do multim&amp;iacute;dia.&lt;/p&gt;
 &lt;p&gt;&amp;nbsp;&lt;/p&gt;
 &lt;h3&gt;Compre j&amp;aacute; o seu no KaBuM!&lt;/h3&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Lg Ultragear 27 Polegadas,FULL  HdD144hz 1ms Ips, HDMI e Displayport</t>
+  </si>
+  <si>
+    <t>Monitor gamer lg ultragear, 27 full hd 144hz 1ms ips hdmi e displayport hdr 10 99% srgb, freesync premium vesa - 27gn65r o monitor gamer lg ultragear 27gn65r é uma opção de alta performance desenvolvida para atender às demandas dos jogadores mais exigentes. Com uma tela de 27 polegadas em resolução full hd (1920 x 1080), esse monitor oferece uma experiência visual imersiva com imagens nítidas e detalhadas. A velocidade é uma das principais características desse monitor, com um tempo de resposta ultra-rápido de 1ms (gtg), o que significa que as transições de cores são praticamente instantâneas, eliminando o efeito de arrasto nas imagens durante os jogos mais rápidos e intensos. Além disso, a taxa de atualização de 144hz proporciona uma jogabilidade mais fluida, permitindo que os jogadores vejam o próximo quadro rapidamente e tenham uma experiência de jogo mais suave. O painel ips do monitor garante ângulos de visão amplos e cores vibrantes, com suporte para 99% do espaço de cores srgb e tecnologia hdr10. Isso resulta em imagens mais realistas e ricas em detalhes, criando uma experiência de visualização imersiva para jogos, filmes e conteúdos em geral. O monitor gamer lg ultragear 27gn65r também é compatível com a tecnologia amd freesync premium e nvidia g-sync, que ajudam a eliminar o screen tearing e o stuttering durante os jogos, sincronizando a taxa de atualização do monitor com a taxa de quadros da placa gráfica para uma jogabilidade mais suave e sem interrupções. O design eletrizante e moderno do monitor complementa perfeitamente o setup gamer, enquanto a compatibilidade vesa permite a instalação em suportes ou braços para maior versatilidade. Se você busca uma experiência de jogo de alta performance com imagens fluidas, cores vívidas e tempos de resposta rápidos, o monitor gamer lg ultragear 27gn65r é uma escolha excelente para elevar seu entretenimento e desempenho nos jogos.   especificações: - marca: lg - modelo: 27gn65r     características: tela: - cor: preto - tamanho: 27” - tipo de tela: ips - ângulo de visão: 178º / 178º - resolução máxima: full hd (1920 x 1080) - brilho: 300 cd/m² - contraste: 1000:01 - tempo de resposta: 1ms (gtg) - taxa de atualização: 144hz - gama de cores: srgb 99% (típ.) - profundidade de cores (nº de cores): 16,7m - distância entre pixels: 0,3108 x 0,3108 mm - tratamento de tela: antirreflexivo   entradas e saídas: - hdmi: sim (v2.0) - displayport: sim (v1.4) - saída de fone de ouvido: sim   energia: - consumo de energia: 32w (típ.) - fonte: adaptador externo   ajustes: - ajustes de posição: inclinação, altura, pivô - tamanho da furação: 100 x 100 mm   recursos: - hdr: hdr10 - flicker safe: sim - amd freesync: freesync premium - nvidia g-sync: sim - modo leitura: sim - onscreen control: sim - motion blur reduction: sim - crosshair: sim - dynamic action sync: sim - black stabilizer: sim - plug &amp; play: sim</t>
   </si>
   <si>
     <t>Monitor Gamer AOC 27 2K QHD, 155hz, 1ms, HDMI e DisplayPort, FreeSync Premium, 121.5% sRGB, VESA - Q27G2</t>
@@ -511,6 +534,12 @@
     <t>Uma velocidade ultrarrápida de 240Hz e 1ms permite que os jogadores vejam o próximo quadro rapidamente e fazem com que a imagem apareça suavemente. Os jogadores podem responder rapidamente aos oponentes e mirar no alvo facilmente.</t>
   </si>
   <si>
+    <t>Monitor Concórdia Gamer Curvo Cz270f200 27'' LED FULL HD, 200hz, 1ms, HDMI, DP, DVI</t>
+  </si>
+  <si>
+    <t>o monitor concórdia gamer curvo 27" 200hz entrega aos gamers uma experiência lisa, rápida e responsiva em todos os jogos. Experimente uma jogabilidade impecável com a taxa de atualização de tela 200 hz que garante imagens rápidas, suaves e movimentos nítidos, para nenhum detalhe passar despercebido. Com tela de 27", ultrarrápido e cheio de ótimos recursos para todos os tipos de jogos, a partir de agora seus momentos serão ainda mais insanos e sua experiência, impecável.conectividadehdmi: sim v1.4display port v1.2: sim acompanha cabo v1.2dvi: simphone: sim</t>
+  </si>
+  <si>
     <t>Monitor Gamer Acer Nitro Edo, 27 Polegadas, Full HD, 1MS, Curvo, VA, 180Hz, - Ed270r-S3biip</t>
   </si>
   <si>
@@ -566,12 +595,6 @@
 &lt;h3&gt;Aproveite essa oportunidade e adquira seu Monitor Gamer Curvo no KaBuM!&lt;/h3&gt;</t>
   </si>
   <si>
-    <t>Monitor Concórdia Gamer Curvo Cz270f200 27'' LED FULL HD, 200hz, 1ms, HDMI, DP, DVI</t>
-  </si>
-  <si>
-    <t>o monitor concórdia gamer curvo 27" 200hz entrega aos gamers uma experiência lisa, rápida e responsiva em todos os jogos. Experimente uma jogabilidade impecável com a taxa de atualização de tela 200 hz que garante imagens rápidas, suaves e movimentos nítidos, para nenhum detalhe passar despercebido. Com tela de 27", ultrarrápido e cheio de ótimos recursos para todos os tipos de jogos, a partir de agora seus momentos serão ainda mais insanos e sua experiência, impecável.conectividadehdmi: sim v1.4display port v1.2: sim acompanha cabo v1.2dvi: simphone: sim</t>
-  </si>
-  <si>
     <t>Monitor Gamer Acer Nitro 31.5p Curvo, Full HD, 165Hz - Ed320qr S3biipx</t>
   </si>
   <si>
@@ -678,16 +701,16 @@
 &lt;p dir="ltr"&gt;Jogue todos os seus jogos no primeiro n&amp;iacute;vel, afinal voc&amp;ecirc; est&amp;aacute; adquirindo um super monitor. Todos os m&amp;iacute;nimos detalhes foram pensados no desenvolvimento deste produto.&lt;/p&gt;</t>
   </si>
   <si>
+    <t>Monitor Gamer Acer Nitro Qg270, 27 Polegadas, Full Hd, 180hz, 1ms Freesync</t>
+  </si>
+  <si>
+    <t>Monitor gamer acer nitro qg270 27 polegadas full hd 180hz 1ms freesync  &lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  com o monitor gamer nitro qg270 27 polegadas da acer você conseguirá jogar com muito mais clareza e foco! Ele conta com uma alta taxa de atualização de até 180hz e visual response boost (vrb) de até 1 ms. Além disso, o design zeroframe praticamente elimina as bordas e garante a sua imersão no jogo.&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  confira as principais características do nitro qg270 27 polegadas:&lt;br /&gt;&lt;br /&gt;  tela de 27 polegadas full hd: o nitro qg270 entrega imagens mais nítidas, levando sua experiência visual e seu foco no jogo para um novo nível.&lt;br /&gt;&lt;br /&gt;  design zeroframe: monitor com tela led va e design zeroframe, que praticamente elimina as bordas para que você tenha uma verdadeira imersão no jogo.&lt;br /&gt;&lt;br /&gt;  taxa de atualização de até 180hz: esse monitor conta com uma alta taxa de atualização de até 180hz. Prepare-se para ver imagens mais suaves, sem rastros e sem rasgos.&lt;br /&gt;&lt;br /&gt;  tecnologia hdr10: a tela cria níveis mais profundos de contraste preto e branco. Conte com mais imersão no jogo por meio da recriação de imagens realistas.&lt;br /&gt;&lt;br /&gt;  visual response boost (vrb) de até 1 ms: o monitor reduz borrões, efeitos fantasmas e manchas nas imagens. Além disso, elimina o desfoque em objetos em movimento rápido.&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  características:&lt;br /&gt;&lt;br /&gt;  marca: acer&lt;br /&gt;&lt;br /&gt;  modelo: nitro qg270&lt;br /&gt;&lt;br /&gt;  tecnologias: hdr10, md freesync premium, acervision care, flicker-less, low dimming, bluelightshield, acer display widget, game mode, adaptative contrast management&lt;br /&gt;&lt;br /&gt;  cor: preto&lt;br /&gt;&lt;br /&gt;  resolução de tela: full hd 1920 x 1080 180 hz&lt;br /&gt;&lt;br /&gt;  conexão: 1x hdmi (2.0) e 1x displayport(1.4)&lt;br /&gt;&lt;br /&gt;  brilho: 300 nits&lt;br /&gt;&lt;br /&gt;  tempo de resposta: 1 ms vrb visual response boost&lt;br /&gt;&lt;br /&gt;  contraste: 3000:1&lt;br /&gt;&lt;br /&gt;  atualização: até 180 hz&lt;br /&gt;&lt;br /&gt;  interfaces/portas: 1x hdmi(2.0), 1x displayport(1.4), 1x saída de áudio e entrada de alimentação&lt;br /&gt;&lt;br /&gt;  inclinação: -5 graus a 15 graus (aproximadamente)&lt;br /&gt;&lt;br /&gt;  cores: 16.7 milhões&lt;br /&gt;&lt;br /&gt;  ângulo de visão: 178 graus esquerda / direita e 178 graus cima / baixo&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  itens inclusos:&lt;br /&gt;&lt;br /&gt;  monitor&lt;br /&gt;&lt;br /&gt;  suportes&lt;br /&gt;&lt;br /&gt;  manual em português&lt;br /&gt;&lt;br /&gt;  termo de garantia&lt;br /&gt;&lt;br /&gt;  1x cabo de energia&lt;br /&gt;&lt;br /&gt;  1x cabo hdmi&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  garantia: 12 meses (diretamente com a fabricante)</t>
+  </si>
+  <si>
     <t>Monitor Gamer LG 23.8" Full HD, 144Hz, 1Ms, HDMI, DP, IPS, HDR Freesync - 24GN600-B</t>
   </si>
   <si>
     <t>Monitor Gamer LG 23,8 Full HD 144Hz 1MS HDMI DP IPS HDR Freesync 24GN600-B&lt;br /&gt;&lt;br /&gt;PROJETADO PARA VELOCIDADE INCRÍVEL&lt;br /&gt;Com IPS de 1ms comparável à velocidade TN, fornecendo a imagem residual minimizada e um tempo de resposta rápido, permite que você desfrute de um desempenho de jogo totalmente novo.&lt;br /&gt;&lt;br /&gt;MOVIMENTO DE JOGO FLUIDO&lt;br /&gt;Uma velocidade ultra-rápida de 144 Hz permite que os jogadores vejam o próximo quadro rapidamente e faz com que a imagem apareça suavemente. Os jogadores podem responder rapidamente aos oponentes e mirar no alvo facilmente.&lt;br /&gt;&lt;br /&gt;SINTA O COMBATE REAL COM CORES VERDADEIRAS&lt;br /&gt;Este monitor suporta HDR10 com sRGB 99 (Typ.) Permitindo imersão visual realista com cores ricas e contraste. Independentemente do campo de batalha, pode ajudar os jogadores a ver todas as cores dramáticas que os desenvolvedores do jogo pretendiam.&lt;br /&gt;&lt;br /&gt;REAJA MAIS RÁPIDO AOS OPONENTES&lt;br /&gt;Minimize o atraso de entrada com Dynamic Action Sync para que os jogadores possam capturar cada momento em tempo real.&lt;br /&gt;&lt;br /&gt;ATAQUE PRIMEIRO NO ESCURO&lt;br /&gt;Os jogadores podem evitar que os atiradores se escondam nos lugares mais escuros e escapar rapidamente das situações quando o flash explode.</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Acer Nitro Qg270, 27 Polegadas, Full Hd, 180hz, 1ms Freesync</t>
-  </si>
-  <si>
-    <t>Monitor gamer acer nitro qg270 27 polegadas full hd 180hz 1ms freesync  &lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  com o monitor gamer nitro qg270 27 polegadas da acer você conseguirá jogar com muito mais clareza e foco! Ele conta com uma alta taxa de atualização de até 180hz e visual response boost (vrb) de até 1 ms. Além disso, o design zeroframe praticamente elimina as bordas e garante a sua imersão no jogo.&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  confira as principais características do nitro qg270 27 polegadas:&lt;br /&gt;&lt;br /&gt;  tela de 27 polegadas full hd: o nitro qg270 entrega imagens mais nítidas, levando sua experiência visual e seu foco no jogo para um novo nível.&lt;br /&gt;&lt;br /&gt;  design zeroframe: monitor com tela led va e design zeroframe, que praticamente elimina as bordas para que você tenha uma verdadeira imersão no jogo.&lt;br /&gt;&lt;br /&gt;  taxa de atualização de até 180hz: esse monitor conta com uma alta taxa de atualização de até 180hz. Prepare-se para ver imagens mais suaves, sem rastros e sem rasgos.&lt;br /&gt;&lt;br /&gt;  tecnologia hdr10: a tela cria níveis mais profundos de contraste preto e branco. Conte com mais imersão no jogo por meio da recriação de imagens realistas.&lt;br /&gt;&lt;br /&gt;  visual response boost (vrb) de até 1 ms: o monitor reduz borrões, efeitos fantasmas e manchas nas imagens. Além disso, elimina o desfoque em objetos em movimento rápido.&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  características:&lt;br /&gt;&lt;br /&gt;  marca: acer&lt;br /&gt;&lt;br /&gt;  modelo: nitro qg270&lt;br /&gt;&lt;br /&gt;  tecnologias: hdr10, md freesync premium, acervision care, flicker-less, low dimming, bluelightshield, acer display widget, game mode, adaptative contrast management&lt;br /&gt;&lt;br /&gt;  cor: preto&lt;br /&gt;&lt;br /&gt;  resolução de tela: full hd 1920 x 1080 180 hz&lt;br /&gt;&lt;br /&gt;  conexão: 1x hdmi (2.0) e 1x displayport(1.4)&lt;br /&gt;&lt;br /&gt;  brilho: 300 nits&lt;br /&gt;&lt;br /&gt;  tempo de resposta: 1 ms vrb visual response boost&lt;br /&gt;&lt;br /&gt;  contraste: 3000:1&lt;br /&gt;&lt;br /&gt;  atualização: até 180 hz&lt;br /&gt;&lt;br /&gt;  interfaces/portas: 1x hdmi(2.0), 1x displayport(1.4), 1x saída de áudio e entrada de alimentação&lt;br /&gt;&lt;br /&gt;  inclinação: -5 graus a 15 graus (aproximadamente)&lt;br /&gt;&lt;br /&gt;  cores: 16.7 milhões&lt;br /&gt;&lt;br /&gt;  ângulo de visão: 178 graus esquerda / direita e 178 graus cima / baixo&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  itens inclusos:&lt;br /&gt;&lt;br /&gt;  monitor&lt;br /&gt;&lt;br /&gt;  suportes&lt;br /&gt;&lt;br /&gt;  manual em português&lt;br /&gt;&lt;br /&gt;  termo de garantia&lt;br /&gt;&lt;br /&gt;  1x cabo de energia&lt;br /&gt;&lt;br /&gt;  1x cabo hdmi&lt;br /&gt;&lt;br /&gt;  &lt;br /&gt;&lt;br /&gt;  garantia: 12 meses (diretamente com a fabricante)</t>
   </si>
   <si>
     <t>Monitor Gamer Cooler Master 23.8 Full HD, 144 Hz, 0.5ms, HDMI e DisplayPort, DCI-P3 de 90%, HDR - CMI-GM238-FFS-BR</t>
@@ -742,6 +765,12 @@
     <t>Desfrute de uma incrível qualidade de imagem com o monitor LG e se surpreenda com o HDR10. A alta gama de cores e com resolução 4k é facilmente superior quando comparado a monitores convencionais. Com a tecnologia AMD Radeon FreeSync você aproveitará ainda mais das imagens do Monitor LG, eliminando os cortes e repetições de imagem..</t>
   </si>
   <si>
+    <t>Monitor Gamer Redragon Pearl, 23.6 Polegadas, 165hz, Curvo, LED, FHD, HDMI - Gm24g3c</t>
+  </si>
+  <si>
+    <t>Características:&lt;br /&gt; - marca: redragon&lt;br /&gt; - modelo: gm24g3c&lt;br /&gt; especificações:&lt;br /&gt; - cor: preto&lt;br /&gt; - alta taxa de atualização até 144hz auxiliando na fluidez da gameplay.&lt;br /&gt; - design elegante e minimalista para se integrar a qualquer setup.&lt;br /&gt; - tecnologia freesync integrada para eliminar as quebras de imagem.&lt;br /&gt; - diversas opções de conexões de vídeo para maior praticidade e versatilidade.&lt;br /&gt; - tamanho: 23,6”&lt;br /&gt; - resolução: 1920 x 1080&lt;br /&gt; - tipo de painel: csot&lt;br /&gt; - taxa de atualização: 165 hz&lt;br /&gt; - número de cores: 16.7 m&lt;br /&gt; - brilho máximo: 250cd/m2 (typical)&lt;br /&gt; - taxa de contraste: 3000:1&lt;br /&gt; - conectividade: hdmi 1.4 x 2, dp x1, 1x 3.5mm áudio.&lt;br /&gt; - power range: 100-240v 50/60hz&lt;br /&gt; - peso bruto(g): 4750&lt;br /&gt; - peso liquido(g): 3450&lt;br /&gt; conteúdo da embalagem:&lt;br /&gt; - monitor gamer redragon</t>
+  </si>
+  <si>
     <t>Monitor Gamer Cooler Master 27 Full HD, 165 Hz, 0.5ms, HDMI e DisplayPort, DCI-P3 90%, HDR - CMI-GM27-FFS-BR</t>
   </si>
   <si>
@@ -768,13 +797,31 @@
     <t>O Monitor Kaizen traz um novo significado para a palavra imersão, a sua tela IPS Full HD proporciona realismo total para a sua jogatina. Tenha uma jogabilidade fluida com uma taxa de atualização de 144Hz, sem rastros e sem o efeito Ghosting. A tela de 27" FHD do Warrior Kaizen garante uma imersão total em seus games. Aproveite ao máximo a qualidade de imagem em alta resolução. Seu painel IPS garante maior fidelidade de cores e qualidade de imagem em seus jogos. A tecnologia FreeSync sincroniza os quadros gerados pela placa gráfica (GPU) com a taxa de atualização do monitor. Isso garante que eles fiquem sempre alinhados e proporcionem uma imagem fluida e sem cortes. Ele conta com um com tempo de resposta de 1ms, permitindo que você tenha a reação mais rápida para os seus desafios. Com iluminação RGB, seu setup gamer ainda melhor. Conta com base ajustável em altura e rotação com ajustes precisos e tempo de resposta ultra rápido para seus comandos. O monitor Warrior Kayzen se adapta perfeitamente ao seu setup.</t>
   </si>
   <si>
-    <t>Monitor Gamer Bluecase 24 Polegadas Full HD,  144HZ, 1ms, HDMI e DisplayPort, FreeSync - BM242GW</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Full HD 144Hz de atualização para melhores gráficos. Com 1 conector DisplayPort e 1 conector HDMI. &lt;br /&gt;&lt;br /&gt;TAXA DE ATUALIZAÇÃO   &lt;br /&gt;Uma taxa de atualização de 144Hz deixa a sua tela sem nenhum borrão, serrilhado ou "ghosting". FLICKER-FREE   A função Flicker-Free regula o brilho para diminuir o cansaço dos olhos durante os jogos. &lt;br /&gt;&lt;br /&gt;APENAS 1MS TEMPO DE RESPOSTA (GTG)   &lt;br /&gt;Melhor desempenho e experiência de jogo nas ações de rápido movimento. &lt;br /&gt;&lt;br /&gt;TECNOLOGIA AMD FREESYNC   &lt;br /&gt;O AMD FREESYNC faz a sincronização entre a taxa de atualização de seu monitor e a taxa de quadros de sua placa de vídeo eliminando imagens quebradas.</t>
-  </si>
-  <si>
     <t>Monitor Gamer Acer 23.8 Polegadas Full HD, 165Hz, 1ms, HDR, FreeSync, HDMI e DisplayPort - QG241Y</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Curvo Concórdia 31.5" QHD R1500, 165Hz, 1ms, HDMI/DisplayPort, FreeSync, Ajuste de Altura, Som Integrado, Preto - C315Q</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Monitor Conc&amp;oacute;rdia Gamer Curvo C315Q 31,5'' ,2K, WQHD, 165hz, 1ms, 2 HDMI, DP, Ajuste de Altura e Rota&amp;ccedil;&amp;atilde;o&lt;/h2&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Curvatura Imersiva de 31,5 Polegadas&lt;/h2&gt;
+&lt;p&gt;O painel WQHD (2560 X 1440) de 31,5 polegadas do Monitor Conc&amp;oacute;rdia Gamer Curvo C315Q oferece visuais impressionantes de todos os &amp;acirc;ngulos com uma curvatura de 1500R que garante que cada ponto seja igualmente visto aos seus olhos. Isso contribui para um maior conforto de visualiza&amp;ccedil;&amp;atilde;o - mesmo durante o uso prolongado - e permite que voc&amp;ecirc; aproveite um amplo &amp;acirc;ngulo de visualiza&amp;ccedil;&amp;atilde;o com menos distor&amp;ccedil;&amp;atilde;o e mudan&amp;ccedil;a de cor ao jogar e assistir filmes.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Taxa de Atualiza&amp;ccedil;&amp;atilde;o de 165Hz&lt;/h2&gt;
+&lt;p&gt;A taxa de atualiza&amp;ccedil;&amp;atilde;o do Monitor Conc&amp;oacute;rdia Gamer Curvo C315Q diminui o atraso e o desfoque de movimento para dar a voc&amp;ecirc; vantagem todos os tipos de jogos.&amp;nbsp; Essa taxa de atualiza&amp;ccedil;&amp;atilde;o ultrarr&amp;aacute;pida permite que voc&amp;ecirc; jogue com as configura&amp;ccedil;&amp;otilde;es visuais mais altas e reaja instantaneamente ao que est&amp;aacute; na tela - para que voc&amp;ecirc; obtenha o primeiro ataque.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Design Ergon&amp;ocirc;mico&lt;/h2&gt;
+&lt;p&gt;Com um suporte ergonomicamente projetado, o Monitor Conc&amp;oacute;rdia Gamer Curvo C315Q oferece inclina&amp;ccedil;&amp;atilde;o, rota&amp;ccedil;&amp;atilde;o e giro da tela de 180&amp;deg; para que voc&amp;ecirc; possa encontrar facilmente sua posi&amp;ccedil;&amp;atilde;o de visualiza&amp;ccedil;&amp;atilde;o ideal.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Cooler Master Ga271, 27 Polegadas, Wqhd, Va, Hdr10, 100hz, 1ms, Srgb</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;mergulhe no mundo dos jogos&lt;/strong&gt;&lt;br /&gt;o ga271 é um monitor wqhd com taxa de atualização de até 100 hz com suporte para adaptive sync. Com todos os recursos e especificações necessários, o ga271 é um monitor orientado para o valor que oferece desempenho excepcional em aplicações de jogos e de trabalho.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;encontre seu equilíbrio&lt;/strong&gt;&lt;br /&gt;o ga271 com um painel de 27" com resolução wqhd oferece visuais impressionantes para seus jogos e aplicativos relacionados ao trabalho. O ga271 pode ser seu monitor principal para lidar com planilhas durante o dia, bem como para jogar e desfrutar de entretenimento durante a noite.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;100hz + 1ms&lt;/strong&gt;&lt;br /&gt;o ga271 oferece uma taxa de atualização fluida de 100 hz com tempo de resposta de 1 ms, proporcionando imagens mais nítidas e responsivas para jogos, bem como para uso geral de produtividade.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;contraste mais profundo&lt;/strong&gt;&lt;br /&gt;o painel va do ga271 produz pretos mais profundos e escuros para um nível de contraste aprimorado, resultando em maior qualidade de imagem. Com uma relação de contraste de 4000:1, o painel va do ga271 é capaz de reproduzir um nível de contraste 4x superior ao de um painel ips padrão.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;sincronização adaptativa&lt;/strong&gt;&lt;br /&gt;ga271 vem com suporte adaptive sync, proporcionando uma experiência extra suave e sem interrupções em seus jogos. Ganhe uma vantagem competitiva sobre seus oponentes com menos manchas de movimento e visuais mais claros nos jogos que você joga.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;luz azul baixa e sem cintilação&lt;/strong&gt;&lt;br /&gt;ga271 não treme e possui um modo de luz azul baixa para proteger ainda mais seus olhos de emissões de luz azul potencialmente prejudiciais.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;pronto para hdr&lt;/strong&gt;&lt;br /&gt;o ga271 não é ótimo apenas para jogos, mas também para desfrutar de entretenimento, pois aceita entrada hdr, permitindo visualizar conteúdo com maiores detalhes e cores em comparação com um monitor tradicional.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;estética minimalista&lt;/strong&gt;&lt;br /&gt;ga271 segue o básico com um design prático com foco em uma estética minimalista. O design limpo certamente se encaixa perfeitamente em sua configuração de trabalho e lazer.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;opções de conectividade&lt;/strong&gt;&lt;br /&gt;conecte seus dispositivos às portas de e/s que consistem em: 1 x porta de exibição,  2 x hdmi 2.0, 1 x conector de fone de ouvido de 3,5 mm&lt;/p&gt;&lt;p&gt; &lt;/p&gt;&lt;p&gt;&lt;strong&gt;especificações:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;	&lt;li&gt;marca: cooler master&lt;/li&gt;	&lt;li&gt;modelo: cmi-ga271&lt;/li&gt;	&lt;li&gt;tipo de painel: série plana&lt;/li&gt;	&lt;li&gt;razão: 16:9&lt;/li&gt;	&lt;li&gt;tamanho da tela: 27"&lt;/li&gt;	&lt;li&gt;painel: va 1.07b&lt;/li&gt;	&lt;li&gt;resolução: 2k wqhd 2560x1440&lt;/li&gt;	&lt;li&gt;taxa de quadros: 100hz&lt;/li&gt;	&lt;li&gt;relação de contraste: 4000:1&lt;/li&gt;	&lt;li&gt;visão de angulo: 178°/178°&lt;/li&gt;	&lt;li&gt;brilho: 250 lêndeas&lt;/li&gt;	&lt;li&gt;gama de cores: srgb 95%&lt;/li&gt;	&lt;li&gt;entradas hdmi: 2&lt;/li&gt;	&lt;li&gt;entrada dp: 1&lt;/li&gt;	&lt;li&gt;tecnologia vrr: adaptive sync, faixa freesync: sim, faixa g-sync: sim&lt;/li&gt;	&lt;li&gt;tempo de resposta: 1ms (mprt) &lt;/li&gt;	&lt;li&gt;proteção de luz azul: sim &lt;/li&gt;	&lt;li&gt;consumo: 18w&lt;/li&gt;	&lt;li&gt;ajuste de inclinação: -5°~+20°&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Monitor 29 Lg 29wk500 - Tela Ips Full Hd Ultrawide Freesync - Modo Gamer - Screen Split 2.0 - 5ms</t>
   </si>
   <si>
     <t>Monitor Samsung Odyssey, 27pol., Full HD, 165Hz, 1MS, HDMI, Display Port, FreeSync</t>
@@ -789,18 +836,6 @@
     <t>Para você que é fanático por games, precisa ter equipamentos que leve você aos mais altos níveis de habilidade e jogabilidade. A Samsung apresenta o monitor gamer Odyssey G30 LS24BG300ELMZD de 24".
 Com resolução FHD, ele possui frequência de atualização de 144Hz atualiza as imagens da tela com mais frequência a cada segundo, permitindo uma jogabilidade mais suave que acompanha até mesmo os jogadores mais rápidos, painel VA, tempo de resposta de 1ms onde os pixels da tela respondem de maneira quase instantânea, permitindo que a ação rápida flua com precisão do mundo real. Seu desempenho na tela é tão rápido quanto seus próprios reflexos e conexões como 1 Display Port, EA Display Port Version: 1.2, 1 HDMI, EA HDMI Version: 1.4, HDCP Version (HDMI): 2.2, Headphone.
 E ainda, conta com várias características que te ajudam ainda mais como AMD FreeSync Premium que apresenta tecnologia de sincronização adaptativa que reduz atraso de tela, rasgos de imagem e a latência de entrada, assegurando assim que cada cena flua sem interrupções, ajuste de altura, design sem bordas em 3 lados que revela o espaço máximo para uma jogabilidade maior e mais ousada.</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Curvo Duex Dx 270zg, 27 Polegadas, FULL HD (1920x1080), 240hz, Preto</t>
-  </si>
-  <si>
-    <t>Marca: duex&lt;br /&gt;modelo: dx 270zg &lt;br /&gt;&lt;br /&gt;especificações: &lt;br /&gt;&lt;br /&gt;tamanho da tela: 27" &lt;br /&gt;área de display: 527.4 (h) x 296.4 (v) &lt;br /&gt;resolução: 1920x1080 (240hz) &lt;br /&gt;pixel pitch: 0.27mm &lt;br /&gt;ângulo de visão: h:178 / v:178 &lt;br /&gt;brilho: 250cd/m² &lt;br /&gt;tempo de resposta: 1ms &lt;br /&gt;número de cores: 16.7m &lt;br /&gt;&lt;br /&gt;conectores: &lt;br /&gt;2x hdmi &lt;br /&gt;1x displayport &lt;br /&gt;1x usb &lt;br /&gt;1x áudio &lt;br /&gt;&lt;br /&gt;conteúdo da caixa: &lt;br /&gt;monitor &lt;br /&gt;base&lt;br /&gt;cabo hdmi&lt;br /&gt;fonte de energia&lt;br /&gt;&lt;br /&gt;garantia: 365 dias</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Draxen 23.8'' resolução de 1920 x 1080 tempo de resposta de 1 MS 165HZ Full HD, Sem Borda</t>
-  </si>
-  <si>
-    <t>o monitor gamer draxen 165hz full hd é tudo o que você precisa para completar o seu setup. desenvolvido pensando no seu estilo de vida, oferecendo qualidade, desempenho e um design mais moderno do que nunca. a sua tela 23.8 lhe dará comodidade para estudar, trabalhar ou assistir sua série ou filme favoritos no seu tempo de lazer. além disso, sua alta resolução de 1920 x 1080 permite que você desfrute de momentos únicos graças a uma imagem nítida, cores realistas e contraste incrível. exibição de vídeo perfeita com tempo de resposta de 1 ms e mais de 16,7 milhões de cores que transformam as imagens em uma experiência muito fiel à realidade.&lt;br&gt;aprimore sua configuração com estilo. a furação padrão vesa 75x75 permite que você fixe o monitor em uma parede ou em um suporte.</t>
   </si>
   <si>
     <t>Monitor Gamer Bluecase, 27", 2.5k, 75hz, 5ms, Preto - BM2716GW</t>
@@ -818,539 +853,16 @@
 Além disso, ainda conta com HDR10, Flicker Safe, AMD FreeSync para maior fluídez durante seus jogos competitivos, Motion Blur Reduction, Crosshair, Dynamic Action Sync, Black Stabilizer, Plug &amp; Play, Modo Leitura e OnScreen Control. Ajuste de inclinação para adequar ao seu estilo de jogo e design de 3 lados praticamente sem bordas.</t>
   </si>
   <si>
-    <t>Monitor Cooler Master Ga271, 27 Polegadas, Wqhd, Va, Hdr10, 100hz, 1ms, Srgb</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;mergulhe no mundo dos jogos&lt;/strong&gt;&lt;br /&gt;o ga271 é um monitor wqhd com taxa de atualização de até 100 hz com suporte para adaptive sync. Com todos os recursos e especificações necessários, o ga271 é um monitor orientado para o valor que oferece desempenho excepcional em aplicações de jogos e de trabalho.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;encontre seu equilíbrio&lt;/strong&gt;&lt;br /&gt;o ga271 com um painel de 27" com resolução wqhd oferece visuais impressionantes para seus jogos e aplicativos relacionados ao trabalho. O ga271 pode ser seu monitor principal para lidar com planilhas durante o dia, bem como para jogar e desfrutar de entretenimento durante a noite.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;100hz + 1ms&lt;/strong&gt;&lt;br /&gt;o ga271 oferece uma taxa de atualização fluida de 100 hz com tempo de resposta de 1 ms, proporcionando imagens mais nítidas e responsivas para jogos, bem como para uso geral de produtividade.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;contraste mais profundo&lt;/strong&gt;&lt;br /&gt;o painel va do ga271 produz pretos mais profundos e escuros para um nível de contraste aprimorado, resultando em maior qualidade de imagem. Com uma relação de contraste de 4000:1, o painel va do ga271 é capaz de reproduzir um nível de contraste 4x superior ao de um painel ips padrão.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;sincronização adaptativa&lt;/strong&gt;&lt;br /&gt;ga271 vem com suporte adaptive sync, proporcionando uma experiência extra suave e sem interrupções em seus jogos. Ganhe uma vantagem competitiva sobre seus oponentes com menos manchas de movimento e visuais mais claros nos jogos que você joga.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;luz azul baixa e sem cintilação&lt;/strong&gt;&lt;br /&gt;ga271 não treme e possui um modo de luz azul baixa para proteger ainda mais seus olhos de emissões de luz azul potencialmente prejudiciais.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;pronto para hdr&lt;/strong&gt;&lt;br /&gt;o ga271 não é ótimo apenas para jogos, mas também para desfrutar de entretenimento, pois aceita entrada hdr, permitindo visualizar conteúdo com maiores detalhes e cores em comparação com um monitor tradicional.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;estética minimalista&lt;/strong&gt;&lt;br /&gt;ga271 segue o básico com um design prático com foco em uma estética minimalista. O design limpo certamente se encaixa perfeitamente em sua configuração de trabalho e lazer.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;opções de conectividade&lt;/strong&gt;&lt;br /&gt;conecte seus dispositivos às portas de e/s que consistem em: 1 x porta de exibição,  2 x hdmi 2.0, 1 x conector de fone de ouvido de 3,5 mm&lt;/p&gt;&lt;p&gt; &lt;/p&gt;&lt;p&gt;&lt;strong&gt;especificações:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;	&lt;li&gt;marca: cooler master&lt;/li&gt;	&lt;li&gt;modelo: cmi-ga271&lt;/li&gt;	&lt;li&gt;tipo de painel: série plana&lt;/li&gt;	&lt;li&gt;razão: 16:9&lt;/li&gt;	&lt;li&gt;tamanho da tela: 27"&lt;/li&gt;	&lt;li&gt;painel: va 1.07b&lt;/li&gt;	&lt;li&gt;resolução: 2k wqhd 2560x1440&lt;/li&gt;	&lt;li&gt;taxa de quadros: 100hz&lt;/li&gt;	&lt;li&gt;relação de contraste: 4000:1&lt;/li&gt;	&lt;li&gt;visão de angulo: 178°/178°&lt;/li&gt;	&lt;li&gt;brilho: 250 lêndeas&lt;/li&gt;	&lt;li&gt;gama de cores: srgb 95%&lt;/li&gt;	&lt;li&gt;entradas hdmi: 2&lt;/li&gt;	&lt;li&gt;entrada dp: 1&lt;/li&gt;	&lt;li&gt;tecnologia vrr: adaptive sync, faixa freesync: sim, faixa g-sync: sim&lt;/li&gt;	&lt;li&gt;tempo de resposta: 1ms (mprt) &lt;/li&gt;	&lt;li&gt;proteção de luz azul: sim &lt;/li&gt;	&lt;li&gt;consumo: 18w&lt;/li&gt;	&lt;li&gt;ajuste de inclinação: -5°~+20°&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>Monitor Gamer AOC Entusiasta Monitor 27 Polegadas, FULL HD, Wide, Ips, 1ms, 75hz, Adaptive G-sync</t>
   </si>
   <si>
     <t>Monitor Gamer AOC. Desenvolvidos para suportar todas as emoções dos jogos, o tempo de resposta de 1ms oferece alta velocidade, definição e muita suavidade em todos os movimentos. A avançada tecnologia Painel IPS esclarece automaticamente as áreas escuras do mundo do jogo, entregando mais cor, brilho e contraste, melhorando a visualização com amplos ângulos de visão. Game Mode, Esta função possui predefinições de fábrica para otimizar cada tipo de jogo. Assim, os níveis de gama preto, proporções de contraste e nitidez são instantaneamente calibrados</t>
   </si>
   <si>
-    <t>USADO: Monitor Gamer LG, Tela 29 Polegadas, 75Hz, 1ms, Dynamic Action Sync, AMD FreeSync - 29UM69G-B.AWZM - Bronze Recer</t>
-  </si>
-  <si>
-    <t>Monitor Gamer LG 29UM69G-B.AWZM, com tela de 29? polegadas com resolução Full HD (2560 x 1080), uma taxa de atualização de 75Hz, e um tempo de resposta de 1ms com tecnologia que todo gamer precisa como Dynamic action Sync e AMD FreeSync&lt;br /&gt;&lt;br /&gt;ATENÇÃO: este produto é RECERTIFICADO.&lt;br /&gt;Os eletrônicos são originais e acompanham Nota Fiscal. Os produtos passam por uma avaliação de qualidade rigorosa, que certifica as condições técnicas e estéticas do aparelho, categorizadas de acordo com os selos ouro, prata ou bronze. Você ainda conta com garantia de três meses contra problemas e pode fazer a devolução do produto em até sete dias.&lt;br /&gt;SAIBA O QUE É UM PRODUTO RECERTIFICADO (BRONZE)&lt;br /&gt;O produto recertificado em condições de fábrica é um produto que volta para o mercado, disponível para vendas, nas mesmas condições de um produto novo, com todas as funcionalidades e características originais, beneficiando o comprador e possibilitando economizar dinheiro na compra.&lt;br /&gt;O produto recertificado em condições de fábrica passa por um processo rigoroso de análise, onde todas as funcionalidades são testadas e após constatação de 100% de funcionamento o produto é liberado como recertificado.&lt;br /&gt;Depois de atingir 100% da certificação técnica de operação em suas funcionalidades, os produtos do Saldão da Informática são classificados em 3 certificações, de acordo com seu estado estético e superficial, sendo assim classificados como: Ouro, Prata e Bronze.&lt;br /&gt;Esse produto é recertificado Bronze: Produto têm alguns riscos. Estes riscos não alteram ao perfeito funcionamento do equipamento.</t>
-  </si>
-  <si>
-    <t>Monitor 27" LED/IPS Acer Gamer Ultra Fino, 75Hz, 1Ms, HDMI + VGA - SA270</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;Monitor Gamer Acer LCD 27 SA270 Bbix Full HD 75Hz 1ms IPS FreeSync HDMI Preto UM.HS0AA.B02&lt;/b&gt;&lt;br /&gt;&lt;br /&gt;NÃO PERCA NENHUM DETALHE DO SEU JOGO&lt;br /&gt;Veja tudo em alta definição com a resolução de 1920 x 1080 Full HD.&lt;br /&gt;E com as 27 da tela, seus jogos terão um campo de visão privilegiado.&lt;br /&gt;&lt;br /&gt;ENTRE NO UNIVERSO GAMER&lt;br /&gt;Garanta uma ótima performance de cor em seus jogos favoritos. O painel In Plane Switching (IPS) promove cores mais vibrantes e nítidas de qualquer ângulo, sem deixar rastros.&lt;br /&gt;&lt;br /&gt;ESTEJA PRONTO PARA JOGAR&lt;br /&gt;A taxa de atualização de 75Hz leva a renderização dos seus jogos a outro nível.&lt;br /&gt;E o tempo de resposta de 1ms acelera as transições e não trava durante a ação.</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Bluecase 23.6 Polegadas, Curvo, LED FULL HD, 180Hz, HDMI,VGA, Preto - Bm24ffd1gc</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;b&gt;monitor gamer full hd curvo led 23,6" bluecase 180hz hdmi vga preto - bm24ffd1gc&lt;/b&gt;&lt;/p&gt;&lt;p&gt;&lt;br /&gt;o monitor gamer bm24ffd1gc possui um tamanho de 23,6", proporcionando uma resolu&amp;ccedil;&amp;atilde;o m&amp;aacute;xima de 1920x1080 pixels full hd. Sua taxa de atualiza&amp;ccedil;&amp;atilde;o m&amp;aacute;xima &amp;eacute; de 180 hz atrav&amp;eacute;s das conex&amp;otilde;es hdmi e dp, oferece imagens mais suaves e fluidas.&amp;nbsp;equipado com ilumina&amp;ccedil;&amp;atilde;o led, o monitor possui um brilho de 300 cd/m&amp;sup2; e um contraste t&amp;iacute;pico de 4.000:1, resultando em cores vibrantes e imagens detalhadas. O monitor gamer bm24ffd1gc &amp;eacute; uma &amp;oacute;tima escolha para jogos, trabalho e entretenimento, proporcionando uma experi&amp;ecirc;ncia visual envolvente e de alta qualidade.&lt;/p&gt;&lt;p&gt;&lt;br /&gt;&lt;b&gt;caracter&amp;iacute;sticas monitor gamer led full hd bluecase 23,6" 180hz - preto&lt;/b&gt;&lt;br /&gt;- marca: bluecase&lt;br /&gt;- modelo: bm24ffd1gcbx&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Gigabyte 27 Full HD, 165Hz, 1ms, IPS, HDMI e DisplayPort, 130% sRGB, HDR, FreeSync, Altura Ajustável - G27F2BR</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;Monitor Gamer Gigabyte 27 Full HD&lt;/h2&gt;
-&lt;h2&gt;&amp;nbsp;&lt;/h2&gt;
-&lt;h2&gt;A &amp;Uacute;ltima Milha para o seu Sistema de Jogo&lt;/h2&gt;
-&lt;p&gt;Como um jogador invis&amp;iacute;vel, o monitor costuma ser subestimado. A verdade &amp;eacute; que os monitores se formam como um efeito sin&amp;eacute;rgico e trazem o melhor desempenho dos componentes do PC. Os monitores de jogos GIGABYTE oferecem &lt;strong&gt;as especifica&amp;ccedil;&amp;otilde;es e qualidade mais recentes&lt;/strong&gt;, os usu&amp;aacute;rios podem realmente desfrutar de um &lt;strong&gt;desempenho de alto n&amp;iacute;vel&lt;/strong&gt; sem a necessidade de extravag&amp;acirc;ncia.&lt;/p&gt;
-&lt;p&gt;Suporta tecnologia&amp;nbsp;&lt;strong&gt;Adaptive-Sync&lt;/strong&gt;&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Tempo de resposta MPRT de 1ms&lt;/h2&gt;
-&lt;p&gt;&lt;strong&gt;Tempo de resposta super r&amp;aacute;pido de 1ms&lt;/strong&gt;&amp;nbsp;para a experi&amp;ecirc;ncia de jogo mais suave de todos os tempos!&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;FHD com 165 Hz (OC 180 Hz)&lt;/h2&gt;
-&lt;p&gt;&lt;strong&gt;Alta resolu&amp;ccedil;&amp;atilde;o&lt;/strong&gt;&amp;nbsp;e taxa de atualiza&amp;ccedil;&amp;atilde;o r&amp;aacute;pida, oferecendo qualidade de exibi&amp;ccedil;&amp;atilde;o detalhada e experi&amp;ecirc;ncia de jogo fluida!&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;95% DCI-P3&lt;/h2&gt;
-&lt;p&gt;Fant&amp;aacute;stica&lt;strong&gt;&amp;nbsp;tela colorida e 130%&lt;/strong&gt;&amp;nbsp;DCI-P3 super ampla gama de cores.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Simples e Estiloso&lt;/h2&gt;
-&lt;p&gt;A&amp;nbsp;&lt;strong&gt;apar&amp;ecirc;ncia simplificada&lt;/strong&gt;&amp;nbsp;representa a simplicidade da filosofia de design da s&amp;eacute;rie de jogos GIGABYTE, &lt;strong&gt;suporte robusto e acabamento fosco&lt;/strong&gt; constru&amp;iacute;do para recursos funcionais e est&amp;eacute;ticos adicionando mais &amp;agrave;s caracter&amp;iacute;sticas.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;OSD Sidekick&lt;/h2&gt;
-&lt;p&gt;O GIGABYTE&amp;nbsp;&lt;strong&gt;OSD Sidekick&lt;/strong&gt;&amp;nbsp;permite que voc&amp;ecirc; defina as op&amp;ccedil;&amp;otilde;es de exibi&amp;ccedil;&amp;atilde;o com teclado e mouse, oferecendo a maneira mais &lt;strong&gt;f&amp;aacute;cil de ajustar&lt;/strong&gt; as configura&amp;ccedil;&amp;otilde;es do monitor.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Painel&lt;/h2&gt;
-&lt;p&gt;O painel revela suas&amp;nbsp;&lt;strong&gt;informa&amp;ccedil;&amp;otilde;es de hardware em tempo real&lt;/strong&gt;, incluindo&amp;nbsp;&lt;strong&gt;voltagens da CPU, velocidade do clock, temperaturas, etc.&lt;/strong&gt;&amp;nbsp;A melhor parte &amp;eacute; que n&amp;atilde;o ser&amp;aacute; bloqueado por nenhum jogo.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Equalizador Preto&lt;/h2&gt;
-&lt;p&gt;Esse recurso permite que voc&amp;ecirc; tenha mais&amp;nbsp;&lt;strong&gt;detalhes do lado escuro&lt;/strong&gt;&amp;nbsp;sem superexpor o lado claro ao mesmo tempo.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Atualiza&amp;ccedil;&amp;atilde;o autom&amp;aacute;tica&lt;/h2&gt;
-&lt;p&gt;Os usu&amp;aacute;rios podem &lt;strong&gt;desfrutar sem esfor&amp;ccedil;o da melhor experi&amp;ecirc;ncia de jogo&lt;/strong&gt; com recursos que a GIGABYTE continua a desenvolver e atualizar enquanto oferece&amp;nbsp;&lt;strong&gt;prote&amp;ccedil;&amp;atilde;o extra ao seu monitor&lt;/strong&gt;.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;&amp;Acirc;NGULO DE VIS&amp;Atilde;O PERFEITO&lt;/h2&gt;
-&lt;p&gt;O monitor Gaming GIGABYTE possui um suporte exclusivo projetado ergonomicamente para oferecer&amp;nbsp;&lt;strong&gt;ampla gama de ajustes de altura e inclina&amp;ccedil;&amp;atilde;o&lt;/strong&gt;.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Compre agora no KaBuM!&lt;/h3&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer KBM! GAMING MG330 31.5' Led, Curvo, 165 Hz, Full Hd, 1ms, Adaptive Sync, Hdmi/Displayport, Ajuste De Ângulo - KGMG33031PT</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;Monitor Gamer KBM! GAMING MG330 31.5' LED, Curvo, 165 Hz, Full HD, 1ms, Adaptive Sync, HDMI/DisplayPort, Ajuste de&amp;nbsp; ngulo - KGMG330&lt;/h2&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Esteja um passo &amp;agrave; frente!&lt;/h2&gt;
-&lt;p&gt;O Monitor Gamer KBM! GAMING MG330 conta com resposta de &lt;strong&gt;1ms&lt;/strong&gt; e taxa de atualiza&amp;ccedil;&amp;atilde;o de &lt;strong&gt;165Hz&lt;/strong&gt;, permitindo a mais alta performance durante suas gameplays. Sua curvatura amplia o campo de vis&amp;atilde;o relativo, concentrando toda a a&amp;ccedil;&amp;atilde;o ao alcance dos olhos do usu&amp;aacute;rio, sem perder resolu&amp;ccedil;&amp;atilde;o.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Melhor Entrega de Imagens para sua Gameplay&lt;/h2&gt;
-&lt;p&gt;Compat&amp;iacute;vel com a tecnologia &lt;strong&gt;Adaptive Sync&lt;/strong&gt;, permite a sincroniza&amp;ccedil;&amp;atilde;o dos frames da placa de v&amp;iacute;deo, decretando o fim do input lag, bem como do tearing.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Conectividade&lt;/h2&gt;
-&lt;p&gt;O Monitor Gamer KBM! GAMING MG330 acompanha um cabo &lt;strong&gt;DisplayPort&lt;/strong&gt; que garante a melhor qualidade de imagem para seu jogo. Al&amp;eacute;m da conex&amp;atilde;o DP, o monitor ainda possui duas conex&amp;otilde;es &lt;strong&gt;HDMI&lt;/strong&gt; e uma conex&amp;atilde;o &lt;strong&gt;P2&lt;/strong&gt; para ouvir seu jogo diretamente do seu monitor.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Maior Ergonomia e Conforto para Uso Prolongado&lt;/h2&gt;
-&lt;p&gt;O Monitor Gamer KBM! GAMING MG330 possui ajuste de inclina&amp;ccedil;&amp;atilde;o &lt;strong&gt;de 5&amp;deg; a 15&amp;deg;&lt;/strong&gt; que se ajusta ergonomicamente para o seu uso. O monitor tamb&amp;eacute;m conta com &lt;strong&gt;Redu&amp;ccedil;&amp;atilde;o de Luz Azul&lt;/strong&gt;, se tornando uma &amp;oacute;tima op&amp;ccedil;&amp;atilde;o para Gameplays prolongadas.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Seu Monitor KBM! GAMING voc&amp;ecirc; encontra aqui no KaBuM!&lt;/h3&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Redragon Pearl, 23.6 Polegadas, 165hz, Curvo, LED, FHD, HDMI - Gm24g3c</t>
-  </si>
-  <si>
-    <t>Características:&lt;br /&gt; - marca: redragon&lt;br /&gt; - modelo: gm24g3c&lt;br /&gt; especificações:&lt;br /&gt; - cor: preto&lt;br /&gt; - alta taxa de atualização até 144hz auxiliando na fluidez da gameplay.&lt;br /&gt; - design elegante e minimalista para se integrar a qualquer setup.&lt;br /&gt; - tecnologia freesync integrada para eliminar as quebras de imagem.&lt;br /&gt; - diversas opções de conexões de vídeo para maior praticidade e versatilidade.&lt;br /&gt; - tamanho: 23,6”&lt;br /&gt; - resolução: 1920 x 1080&lt;br /&gt; - tipo de painel: csot&lt;br /&gt; - taxa de atualização: 165 hz&lt;br /&gt; - número de cores: 16.7 m&lt;br /&gt; - brilho máximo: 250cd/m2 (typical)&lt;br /&gt; - taxa de contraste: 3000:1&lt;br /&gt; - conectividade: hdmi 1.4 x 2, dp x1, 1x 3.5mm áudio.&lt;br /&gt; - power range: 100-240v 50/60hz&lt;br /&gt; - peso bruto(g): 4750&lt;br /&gt; - peso liquido(g): 3450&lt;br /&gt; conteúdo da embalagem:&lt;br /&gt; - monitor gamer redragon</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Redragon Amber, Tela de 27 Polegadas FHD, 165HZ, Curvo, LED, HDMI, Preto - GM27H10C</t>
-  </si>
-  <si>
-    <t>Características:&lt;br /&gt; - marca: redragon&lt;br /&gt; - modelo: gm27h10c&lt;br /&gt; especificações:&lt;br /&gt; - cor: preto&lt;br /&gt; - tamanho: 27”&lt;br /&gt; - resolução: 1920 x 1080 16:9&lt;br /&gt; - tipo de painel: va&lt;br /&gt; - taxa de atualização: 165 hz&lt;br /&gt; - número de cores: 16.7 m&lt;br /&gt; - brilho máximo: 250cd/m2 (typical)&lt;br /&gt; - taxa de contraste: 3000:1&lt;br /&gt; - conectividade: dp x1, hdmi x2, dc in x1&lt;br /&gt; - power range: 100-240v 50/60hz&lt;br /&gt; - tempo de resposta: 1ms&lt;br /&gt; - peso bruto(g): 5960g&lt;br /&gt; - peso liquido(g): 4830g&lt;br /&gt; conteúdo da embalagem:&lt;br /&gt; - monitor gamer redragon</t>
-  </si>
-  <si>
-    <t>Monitor 29 Lg 29wk500 - Tela Ips Full Hd Ultrawide Freesync - Modo Gamer - Screen Split 2.0 - 5ms</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Curvo Concórdia 31.5" QHD R1500, 165Hz, 1ms, HDMI/DisplayPort, FreeSync, Ajuste de Altura, Som Integrado, Preto - C315Q</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;Monitor Conc&amp;oacute;rdia Gamer Curvo C315Q 31,5'' ,2K, WQHD, 165hz, 1ms, 2 HDMI, DP, Ajuste de Altura e Rota&amp;ccedil;&amp;atilde;o&lt;/h2&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Curvatura Imersiva de 31,5 Polegadas&lt;/h2&gt;
-&lt;p&gt;O painel WQHD (2560 X 1440) de 31,5 polegadas do Monitor Conc&amp;oacute;rdia Gamer Curvo C315Q oferece visuais impressionantes de todos os &amp;acirc;ngulos com uma curvatura de 1500R que garante que cada ponto seja igualmente visto aos seus olhos. Isso contribui para um maior conforto de visualiza&amp;ccedil;&amp;atilde;o - mesmo durante o uso prolongado - e permite que voc&amp;ecirc; aproveite um amplo &amp;acirc;ngulo de visualiza&amp;ccedil;&amp;atilde;o com menos distor&amp;ccedil;&amp;atilde;o e mudan&amp;ccedil;a de cor ao jogar e assistir filmes.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Taxa de Atualiza&amp;ccedil;&amp;atilde;o de 165Hz&lt;/h2&gt;
-&lt;p&gt;A taxa de atualiza&amp;ccedil;&amp;atilde;o do Monitor Conc&amp;oacute;rdia Gamer Curvo C315Q diminui o atraso e o desfoque de movimento para dar a voc&amp;ecirc; vantagem todos os tipos de jogos.&amp;nbsp; Essa taxa de atualiza&amp;ccedil;&amp;atilde;o ultrarr&amp;aacute;pida permite que voc&amp;ecirc; jogue com as configura&amp;ccedil;&amp;otilde;es visuais mais altas e reaja instantaneamente ao que est&amp;aacute; na tela - para que voc&amp;ecirc; obtenha o primeiro ataque.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Design Ergon&amp;ocirc;mico&lt;/h2&gt;
-&lt;p&gt;Com um suporte ergonomicamente projetado, o Monitor Conc&amp;oacute;rdia Gamer Curvo C315Q oferece inclina&amp;ccedil;&amp;atilde;o, rota&amp;ccedil;&amp;atilde;o e giro da tela de 180&amp;deg; para que voc&amp;ecirc; possa encontrar facilmente sua posi&amp;ccedil;&amp;atilde;o de visualiza&amp;ccedil;&amp;atilde;o ideal.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer HQ 27 Polegadas, FULL HD 144HZ A 240HZ 1MS HDMI Display Port, Curvo LED, Alto Falantes Iluminação RGB - Battle 27h240g</t>
-  </si>
-  <si>
-    <t>Monitor gamer hq battle&lt;br /&gt;&lt;br /&gt;A jogatina perfeita&lt;br /&gt;Com o monitor hq battle, os seus movimentos serão instantâneos e o seu tempo de reação ocorrerá em tempo real em qualquer tipo de jogo.&lt;br /&gt;Sem atrasos, você jogará com desempenho profissional.&lt;br /&gt;Graças a combinação de tempo de resposta ultrarápido + alta taxa de atualização, você sairá na frente dos seus oponentes:&lt;br /&gt;&lt;br /&gt;Tempo de resposta: 1ms&lt;br /&gt;Desempenho sem igual, imagens nítidas e sem espera. Enxergue toda a cena no milésimo de segundo em que ela acontece. Não desperdice nenhum movimento. O seu reflexo convertido em vitórias!&lt;br /&gt;&lt;br /&gt;Taxa de atualização: 240hz&lt;br /&gt;Nada de rastros nem imagens desfocadas. Tenha uma incrível vantagem sobre o seu adversário, principalmente em cenas rápidas. A altíssima taxa de atualização permitirá a você perceber cada sensível mudança no ambiente. E diferente dos demais modelos da linha battle, o 27h240g possui incríveis 240hz. É a garantia de uma experiência sublime.&lt;br /&gt;&lt;br /&gt;Amd freesync e nvidia g-sync&lt;br /&gt;E para completar o time, o monitor hq battle conta com as tecnologias amd freesync e nvidia g-sync. Incríveis ferramentas que impedem imagens serrilhadas e cortadas.&lt;br /&gt;Elas apresentam a tecnologia de sincronização adaptável, que reduz o travamento de tela, oscilação e atrasos.&lt;br /&gt;&lt;br /&gt;Enxergue no escuro&lt;br /&gt;Graças ao painel va utilizado nos monitores hq battle, você se dará bem em qualquer tipo de ambiente, mesmo em situações de baixa luminosidade.&lt;br /&gt;Encontre seus inimigos escondidos em qualquer lugar, mesmo os mais escuros.&lt;br /&gt;&lt;br /&gt;Mais sobre o painel va&lt;br /&gt;Quando falamos em tipo de painel para monitores gamer, existem três opções disponíveis no mercado.&lt;br /&gt;E por que a hq escolheu o tipo va para o monitor battle?&lt;br /&gt;A resposta é simples. Pois essa opção oferece a maior gama de vantagens para o jogador:&lt;br /&gt;1- ângulo de visão de 178x178 graus, enxergue bem em qualquer ângulo&lt;br /&gt;2- alto nível de contraste, imagens nítidas mesmo em cenas muito claras ou muito escuras&lt;br /&gt;3- tempo de resposta real de 1ms mprt&lt;br /&gt;4- cores vivas e nítidas&lt;br /&gt;5- permite as mais altas taxas de atualização&lt;br /&gt;&lt;br /&gt;Design único&lt;br /&gt;Além de todos os recursos apresentados, ainda temos o fato do monitor hq battle ter um visual sensacional.&lt;br /&gt;Desenvolvido com uma tela curva, isso já seria o bastante para deixar o seu setup gamer ainda mais moderno. Mas além disso, ele ainda possui a tecnologia ´´frameless´´, sem bordas, que garantirão a você uma imersão total. Aproveite 100% da tela.&lt;br /&gt;&lt;br /&gt;Conectividade e recursos&lt;br /&gt;Para garantir uma experiência perfeita, equipamos o battle com tudo o que você precisa.&lt;br /&gt;Dupla saída de vídeo hdmi e display port, além de uma conexão usb.&lt;br /&gt;E para deixar tudo ainda melhor, ele vem acompanhado com dois alto falantes surround e iluminação em rgb.</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Duex 24´ Full HD (1920x1080), 144Hz, Preto - Dx 240zg</t>
-  </si>
-  <si>
-    <t>Marca: duex&lt;br /&gt;modelo: dx 240zg &lt;br /&gt;&lt;br /&gt;especificações: &lt;br /&gt;&lt;br /&gt;tamanho da tela: 24" &lt;br /&gt;área de display: 527.4 (h) x 296.4 (v) &lt;br /&gt;resolução: 1920x1080 (144hz) &lt;br /&gt;pixel pitch: 0.27mm &lt;br /&gt;ângulo de visão: h:178 / v:178 &lt;br /&gt;brilho: 250cd/m² &lt;br /&gt;tempo de resposta: 1ms &lt;br /&gt;número de cores: 16.7m &lt;br /&gt;&lt;br /&gt;conectores: &lt;br /&gt;1x hdmi &lt;br /&gt;1x displayport &lt;br /&gt;1x usb &lt;br /&gt;1x saída de áudio &lt;br /&gt;&lt;br /&gt;conteúdo da caixa: &lt;br /&gt;monitor &lt;br /&gt;base &lt;br /&gt;cabo hdmi &lt;br /&gt;cabo displayport &lt;br /&gt;fonte de energia &lt;br /&gt;guia do usuário&lt;br /&gt;&lt;br /&gt;garantia: 365 dias</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Bluecase 27" 2.5K, 75Hz, HDMI / Displayport, Vesa - BM2713GW</t>
-  </si>
-  <si>
-    <t>Explore um nível superior de qualidade gráfica do seu gameplay com o monitor gamer Bluecase - BM2713GW   &lt;br /&gt;&lt;br /&gt;Esse monitor possui um painel TN ultrarrápido com frequência máxima de até 75 Hz e baixíssimo tempo de resposta de 5(cinco) milissegundos.    &lt;br /&gt;Ideal para seus jogos AAA, o monitor conta com alta definição em resolução Quad HD (2560x1440) que proporciona uma imagem rica em detalhes.    &lt;br /&gt;O monitor Bluecase BM2713GW é compatível com suportes VESA e também conta com conexões DisplayPort e HDMI.</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Samsung 27Pol, Full HD, 75Hz, IPS, HDMI, Vesa, Freesync - Lf27t350fhlmzd</t>
-  </si>
-  <si>
-    <t>Para compor a sua mesa e computador, precisa de um monitor de linha, não acha? Com o Monitor Gamer T350 Samsung você terá uma ótima visualização de tudo que fizer! Com a tela IPS, LED, em formato plano e de 27'' na horizontal, resolução Full HD 1920x1080. Possui conexões HDMI e VGA e tecnologia FreeSync da AMD, assim você pode assistir filmes e jogar tranquilamente sem interrupções na sua imagem. Além disso, possui o Game Mode, que ajusta qualquer jogo para preencher sua tela visualizando todos os detalhes, sendo possível detectar inimigos escondidos nas sombras através do contraste ideal, mais nitidez e cenas com cores mais vivas. Agora, a imagem é reproduzida sem falhas. A taxa de atualização de 75Hz oferece cenas mais fluidas. Seu momento de diversão não tem lag ou efeito fantasma, quer você esteja assistindo a um vídeo ou jogando um jogo. Vai deixar essa beleza passar? Garanta já seu Monitor Gamer T350 Samsung e aproveite com a melhor imagem!</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Curvo HQ 24 LED Full HD, 165 Hz, 1ms, HDMI, DisplayPort, FreeSync, Som Integrado, Preto - 24GHQ-Black</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;Monitor Gamer Curvo HQ 24 LED Full HD, 165 Hz, 1ms, HDMI, DisplayPort, FreeSync, Som Integrado, Preto&lt;/h2&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Tela Curva&lt;/h2&gt;
-&lt;p&gt;A curvatura da tela de R3000 oferece imers&amp;atilde;o total, voc&amp;ecirc; ser&amp;aacute; capaz de apreciar imagens panor&amp;acirc;micas grandes, em alta resolu&amp;ccedil;&amp;atilde;o e com todas as especifica&amp;ccedil;&amp;otilde;es que um monitor Gamer de ponta exige.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Baixo tempo de Resposta&lt;/h2&gt;
-&lt;p&gt;A HQ levou a s&amp;eacute;rio o desenvolvimento desta linha, trazendo ao p&amp;uacute;blico mais exigente um produto completo e de alto n&amp;iacute;vel. N&amp;atilde;o fique atras, reaja em tempo real e tenha os movimentos do teclado refletidos sem atrasos com o tempo de resposta de 1ms.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Atualiza&amp;ccedil;&amp;atilde;o de 165Hz&lt;/h2&gt;
-&lt;p&gt;Sem borr&amp;otilde;es e sem perda de imagem. A INCR&amp;Iacute;VEL taxa de atualiza&amp;ccedil;&amp;atilde;o de 165hz garante que voc&amp;ecirc; tenha uma experi&amp;ecirc;ncia acima dos seus advers&amp;aacute;rios.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Imagens em alta resolu&amp;ccedil;&amp;atilde;o + Visual incr&amp;iacute;vel&lt;/h2&gt;
-&lt;p&gt;A tela Full HD de alta resolu&amp;ccedil;&amp;atilde;o aliada ao design futurista e moderno do monitor garantem n&amp;atilde;o s&amp;oacute; imagens perfeitas como um visual incr&amp;iacute;vel de todo o seu conjunto.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Aproveite essa oportunidade e adquira seu Monitor Gamer Curvo no KaBuM!&lt;/h3&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Redragon, 23Pol, Full HD, 144Hz, 1MS, IPS, HDMI, DP, VGA, Freesync - M2444ph</t>
-  </si>
-  <si>
-    <t>O monitor Redragon Sapphire apresenta um design ultrafino, alinhado com o que há de mais moderno no mercado. Gamers de jogos competitivos podem obter vantagem sobre seus adversários ao utilizar uma tela com a alta taxa de atualização de 144 Hz. A tecnologia AMD FreeSync põe fim à jogabilidade travada e ao corte dos quadros com um desempenho fluido e livre de artefatos com praticamente qualquer taxa de quadros. Contemple a próxima inovação na experiência de jogos para PC e console. O Redragon Sapphire possui um visual moderno e elegante, que combina com qualquer setup, pela sua simplicidade e minimalismo.&lt;br /&gt;&lt;br /&gt;- Alta taxa de atualização até 144Hz auxiliando na fluidez da gameplay.&lt;br /&gt;- Design elegante e minimalista para se integrar a qualquer setup.&lt;br /&gt;- Painel do tipo IPS para maior fidelidade de cores.&lt;br /&gt;- Tecnologia Freesync integrada para eliminar as quebras de imagem.&lt;br /&gt;- Diversas opções de conexões de vídeo para maior praticidade e versatilidade.&lt;br /&gt;&lt;br /&gt;O monitor tem tela de 24 polegadas, um ótimo tamanho para o consumo de jogos e filmes, assim como navegar na internet e trabalhar.</t>
-  </si>
-  <si>
-    <t>Monitor Gamer LG LED 23.8 Polegadas FHD, 60Hz, 5Ms, IPS, VGA/HDMI/DP, Pivot - 24BL550J</t>
-  </si>
-  <si>
-    <t>Monitor Gamer LG LED 23.8 FHD IPS 60Hz 5ms VGA HDMI DP Pivot - 24BL550J CONTE COM SUA MELHOR EXIBIÇÃO A qualidade de imagem do LG 24BL550J é a melhor possível para um monitor Full HD, já que usa a elogiada tela IPS. Suas cores são vibrantes e nítidas, sem qualquer problema em replicar as cores reais em software e jogos. Sua tela de 23.9 faz com que ele esteja no tamanho ideal para a resolução Full HD (1920x1080p), apresentando ótimo nível de densidade de pixel (PPI 0,27 mm). Com isso, você não terá a impressão de imagem borrada ou com serrilhados, principalmente em jogos, vídeos e fotos. FLUIDEZ Tem baixo input lag e tempo de resposta de 5ms, suficiente para eliminar rastros. A taxa de atualização de 75hz da boa fluência aos jogos, ajudando ainda no conforto ocular. MELHOR RESOLUÇÃO Sua incrível tela em Full HD com tecnologia IPS e seu tratamento anti reflexivo conta com a exibição de imagens excepcionais cores mais realistas de qualquer ângulo, sem a interferência de qualquer luz. MODELO PIVOTANTE Permite ajuste de altura, inclinação, rotação e pivô. Esse monitor apresenta um design moderno, com bordas mais finas e base retangular com ótima estabilidade. Porém, seu grande trunfo é o ajuste de altura e giro em 90º (pivô), o que o torna ideal para trabalhar com o monitor na vertical (em pé)..</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Curvo Bright 27p, Full HD, 165Hz, 1Ms, HDMI/VGA, Preto</t>
-  </si>
-  <si>
-    <t>Monitor gamer curvo 27" polegadas 165hz full hd lcd/led preto mt007 bright&lt;br /&gt;  &lt;br /&gt; mergulhe no mundo dos games com estilo e velocidade!&lt;br /&gt;  &lt;br /&gt; ei, camarada gamer, já sentiu como se estivesse preso no passado com um monitor lento e sem graça? Deixe-me apresentar uma passagem direta para o futuro dos jogos: o monitor gamer curvo 27 polegadas 165 hz dp hdmi usb preto bright. Prepare-se para uma experiência visual de tirar o fôlego!&lt;br /&gt;  &lt;br /&gt; este monitor é como uma viagem ao paraíso dos gamers. Com suas 27 polegadas de tela imersiva e curva, ele envolve você em um abraço eletrizante de jogabilidade. E a taxa de atualização de 165 hz? É praticamente uma máquina do tempo para o futuro dos jogos!&lt;br /&gt;  &lt;br /&gt; e como se isso não fosse suficiente, este monitor oferece conectividade versátil com dp, hdmi e usb. Você pode se conectar facilmente aos seus dispositivos e mergulhar diretamente na ação. Sem complicações, apenas jogos de alta qualidade.&lt;br /&gt;  &lt;br /&gt; mas aqui está a cereja no topo do bolo: a resolução deslumbrante e as cores vibrantes. Este monitor faz com que cada detalhe dos seus jogos ganhe vida. Adeus a imagens borradas e cores apagadas. Prepare-se para gráficos que vão explodir sua mente!&lt;br /&gt;  &lt;br /&gt; ao comprar este monitor gamer curvo, você não está apenas adquirindo um pedaço de tecnologia. Você está se dando o presente de uma experiência de jogo que vai te levar a novos patamares de diversão e desempenho. É a sua passagem para o futuro dos jogos - uma jornada sem volta para a vitória!&lt;br /&gt;  &lt;br /&gt; então, o que você está esperando? Pegue seu ingresso para o futuro e adquira o monitor gamer curvo 27 polegadas 165 hz dp hdmi usb preto bright hoje. Jogue com estilo, velocidade e vitória garantida! Sua jornada começa agora!&lt;br /&gt;  &lt;br /&gt; especificações:&lt;br /&gt; dimensões(axlxp): 615 x 453 x 79 mm &lt;br /&gt; peso: 3,9&lt;br /&gt; área de visualização 683 × 128 × 445(mm2)&lt;br /&gt; ângulo de visão h:178°v:178°&lt;br /&gt; resolução(tip.) 1920x1080 60hz&lt;br /&gt; cores 16,7m&lt;br /&gt; brilho (tip.) 250cd/m2&lt;br /&gt; tela curva: 2800r&lt;br /&gt; frequência de resposta: 165 hz&lt;br /&gt; relação de contraste (tip.) 1000:1&lt;br /&gt; conector dp + hdmi + usb&lt;br /&gt;  &lt;br /&gt; conteúdo da embalagem: &lt;br /&gt; 01 monitor bright &lt;br /&gt; 01 cabo hdmi&lt;br /&gt; 01 manual&lt;br /&gt;  &lt;br /&gt; modelo:&lt;br /&gt; mt007&lt;br /&gt;  &lt;br /&gt; marca:&lt;br /&gt; bright&lt;br /&gt;  &lt;br /&gt; garantia 1 ano bright</t>
-  </si>
-  <si>
-    <t>Monitor Goldentec Gamer 27'' Led Full Hd, 75hz, 1ms</t>
-  </si>
-  <si>
-    <t>Monitor gamer 27´´ led full hd 75hz 1ms especificações técnicas  marcagoldentec  ean7899555687261  tamanho de tela27´´  framelesssim  resolução1920x1080 (full hd)  tempo de resposta1 ms  frequência75 hz  brilho250 cd/m²  contraste100 milhões: 1  ângulo de visão180° (h) 180° (v)  cores16,7 milhões  inclinação ajustável 20°  tecnologia freesyncelimina falhas e intermitências  tecnologia lowbluelightreduz a luz azul para mais conforto e segurança  100% flicker freesuaviza a ondulação do monitor  conexõeshdmi  conteúdo da embalagem1x monitor gamer 27´´ led full hd 75hz 1ms &lt;br&gt;cabos e fonte &lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;marca :&lt;/strong&gt; goldentec&lt;br&gt;&lt;strong&gt;tipo de uso :&lt;/strong&gt; gamer&lt;br&gt;&lt;strong&gt;tamanho da tela :&lt;/strong&gt; 27´´&lt;br&gt;&lt;strong&gt;tipo de tela :&lt;/strong&gt; led&lt;br&gt;&lt;strong&gt;resolução :&lt;/strong&gt; full hd&lt;br&gt;&lt;strong&gt;design de tela :&lt;/strong&gt; tela plana&lt;br&gt;&lt;strong&gt;tempo de resposta :&lt;/strong&gt; 1 ms&lt;br&gt;&lt;strong&gt;taxa de atualização :&lt;/strong&gt; 75 hz&lt;br&gt;&lt;strong&gt;estrutura :&lt;/strong&gt; padrão&lt;br&gt;&lt;strong&gt;voltagem :&lt;/strong&gt; bivolt&lt;br&gt;&lt;strong&gt;polegadas :&lt;/strong&gt; 27 ´´&lt;br&gt;&lt;br&gt;&lt;strong&gt;garantia : &lt;/strong&gt;12</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Redragon Azur, 23.8 Polegadas, 165hz, LED, FHD, HDMI - Gm24x5ips</t>
-  </si>
-  <si>
-    <t>Características:&lt;br /&gt; - marca: redragon&lt;br /&gt; - modelo: gm24x5ips&lt;br /&gt; especificações:&lt;br /&gt; - cor: preto&lt;br /&gt; - alta taxa de atualização até 165hz auxiliando na fluidez da gameplay.&lt;br /&gt; - design elegante e minimalista para se integrar a qualquer setup.&lt;br /&gt; - tecnologia freesync integrada para eliminar as quebras de imagem.&lt;br /&gt; - diversas opções de conexões de vídeo para maior praticidade e versatilidade.&lt;br /&gt; - tamanho: 23,8”&lt;br /&gt; - resolução: 1920 x 1080&lt;br /&gt; - tipo de painel: ips&lt;br /&gt; - taxa de atualização: 165 hz&lt;br /&gt; - número de cores: 16.7 m&lt;br /&gt; - brilho máximo: 250cd/m2 (typical)&lt;br /&gt; - taxa de contraste: 1000:1&lt;br /&gt; - conectividade: hdmi 1.4 x 2, dp 1.2  x1, dc x 1, 1x 3.5mm áudio.&lt;br /&gt; - power range: 100-240v 50/60hz&lt;br /&gt; - peso bruto(g): 4728&lt;br /&gt; - peso líquido(g): 3520&lt;br /&gt; conteúdo da embalagem:&lt;br /&gt; - monitor gamer redragon</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Cooler Master 23.8 Pol. Full HD (1920x1080), 0.5MS, 144Hz, IPS, HDMI, Hdr10, Vesa - Gm238-Ffs</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;b&gt;monitor gamer gm238-ffs cooler master full hd hdmi 1920x1080 vesa 144hz 23,8"&lt;/b&gt;&lt;/p&gt;&lt;p&gt;&lt;br /&gt;o monitor gamer gm238-ffs possui tela full hd de 144 hz e 23,8" combinada com uma ampla gama de cores dci-p3 de 90% oferece versatilidade not&amp;aacute;vel. Com recursos essenciais para jogos e produtividade, permite uma experi&amp;ecirc;ncia de jogo suave ou foco no trabalho diurno. A densidade de pixels de 92,6 por polegada (ppi) em um monitor de 23,8 polegadas e resolu&amp;ccedil;&amp;atilde;o full hd, o gm238-ffs equilibra de forma excelente a fidelidade visual e o desempenho. O monitor gamer fornece um display fhd de 23,8" com um painel ultraspeed ips de 144 hz, com recursos como dynamic overdrive, adaptive sync e uma cobertura dci-p3 de 90%, atende a todas as suas necessidades. &amp;eacute; ideal tanto para jogos quanto para produtividade, tornando-o uma adi&amp;ccedil;&amp;atilde;o valiosa &amp;agrave; sua configura&amp;ccedil;&amp;atilde;o de trabalho e entretenimento.&lt;/p&gt;&lt;p&gt;&lt;br /&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>USADO: Monitor Gamer 24 Polegadas Acer Nitro, 165Hz, 0.5ms, Freesync, HDMI, DisplayPort, Preto, Recertificado Prata - VG252Q</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Acer Nitro Vg252q, na cor preta com detalhes em vermelho, tela de 24 polegadas, taxa de atualização de 165hz, tempo de resposta de 0.5ms, amd freesync premium, 1 entrada hdmi e 1 entrada display port&lt;br /&gt;&lt;br /&gt;Atenção: este produto é recertificado.&lt;br /&gt;Os eletrônicos são originais e acompanham nota fiscal. Os produtos passam por uma avaliação de qualidade rigorosa, que certifica as condições técnicas e estéticas do aparelho, categorizadas de acordo com os selos ouro, prata ou bronze. Você ainda conta com garantia de três meses contra problemas e pode fazer a devolução do produto em até sete dias.</t>
-  </si>
-  <si>
-    <t>Monitor Gamer KBM! GAMING MG700 27' Led Full Hd, 240hz, 1ms, Hdmi E Displayport, 96% Srgb, Adaptive Sync, Ajuste De Altura - KGMG70027PT</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;Monitor Gamer KBM! GAMING MG700: Imers&amp;atilde;o e desempenho para seus jogos&lt;/h2&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;O Monitor Gamer KBM! GAMING MG700 &amp;eacute; a escolha perfeita para quem busca imers&amp;atilde;o e desempenho nos jogos. Com &lt;strong&gt;tela curva de 27 polegadas&lt;/strong&gt;, resolu&amp;ccedil;&amp;atilde;o &lt;strong&gt;Full HD&lt;/strong&gt; e taxa de atualiza&amp;ccedil;&amp;atilde;o de &lt;strong&gt;240 Hz,&lt;/strong&gt; o MG700 oferece uma experi&amp;ecirc;ncia visual incr&amp;iacute;vel.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;O tempo de resposta de &lt;strong&gt;1 ms&lt;/strong&gt; garante que voc&amp;ecirc; n&amp;atilde;o perca nenhum detalhe da a&amp;ccedil;&amp;atilde;o, mesmo nos jogos mais r&amp;aacute;pidos. Al&amp;eacute;m disso, o recurso &lt;strong&gt;AdaptiveSync&lt;/strong&gt; elimina o tearing e o stuttering, garantindo uma imagem suave e fluida.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;Para proteger a sua vis&amp;atilde;o, o MG700 conta com &lt;strong&gt;redu&amp;ccedil;&amp;atilde;o de luz azul&lt;/strong&gt; e &lt;strong&gt;Modo Game Plus&lt;/strong&gt;, que reduzem o cansa&amp;ccedil;o visual. O som integrado &amp;eacute; de alta qualidade, mas voc&amp;ecirc; tamb&amp;eacute;m pode conectar o seu headset atrav&amp;eacute;s das portas plug and play.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;Com o Monitor Gamer KBM! GAMING MG700, voc&amp;ecirc; ter&amp;aacute; tudo o que precisa para jogar seus games favoritos com o m&amp;aacute;ximo de desempenho e imers&amp;atilde;o.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;O Monitor Gamer KBM! GAMING MG700 &amp;eacute; a escolha perfeita para quem busca um monitor gamer de alta qualidade. Com recursos avan&amp;ccedil;ados e uma excelente rela&amp;ccedil;&amp;atilde;o custo-benef&amp;iacute;cio, o MG700 &amp;eacute; a garantia de uma experi&amp;ecirc;ncia de jogo inesquec&amp;iacute;vel.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Primetek, 27 Polegadas, 180hz Ips Qhd HDMI/dp</t>
-  </si>
-  <si>
-    <t>Caracteristicas: - marca: primetek - modelo: 27a2r  especificações técnicas: - tamanho do painel (diagonal) 27 - tipo de painel ips rápido - plana/ curva plana proporção 16:9 resolução 2560x1440 - tipo de moldura moldura sem moldura 3 - distância do pixel (h)*(v) (mm) 0,2331 (h) × 0,2331(v - brilho (cd/m2 )(tipo.) 250(min) 300(tipo) brilho (nits)(máx.)? 250(min) 300(tipo) - ângulo de visão (h/v) 178°(h)/178°(v) - profundidade de bits do painel verdadeiro 8 bits - cores da tela 16,7m - tempo de resposta do painel sem od 5ms tempo de resposta 1ms - taxa de atualização (máx.) 180 hz - hdmi 2.0 2 (máx. 144 hz) dp 1.4 2 (máx. 180 hz) saída de áudio 1 - design de suporte de exibição has inclinação (ângulo) 5°±2°,20°±2° giro (ângulo) 20°±2° - pivô (ângulo/direção) pviot: 90° ajuste de altura 120±5mm montagem vesa 75*75mm tecla do botão liga/desliga roker - tecla do botão osd roker contracapa design rgb - consumo de energia 48w modo de economia de energia ?0,5w modo de desligamento desligado &amp;lt,0,3 w tipo de energia adaptador de energia fonte de alimentação dc 12v, 4a - acessorios: cabo de alimentação (1,5m) 1,5m cabo dp versão 1.2 quantidade de cabo dp (1,5 m/1,8 m) 1,5 m - temperatura da cor (fria, quente, usuário) controle de luz azul baixa modo de cena dcr idiomas (23 idiomas) ajuste da luz de fundo sem oscilações freesync over drive fps/rts jogo mais modo de controle do efeito de iluminação (nenhum/mistura de cores rgb/seleção colorida) laranja - dimensão com suporte (l*a*p)(mm) 619x269,2x554,6 mm - dimensão sem suporte (lxaxp)(mm) 619x63,7x365,5 mm - dimensão da caixa (lxaxp)(mm) 715x213x471mm - peso líquido (kg) 6,3kg - peso bruto (kg) 8,3kg - garantia 1 ano &lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;tamanho da tela:&lt;/strong&gt; 27&lt;br&gt;&lt;strong&gt;marca:&lt;/strong&gt; primetek&lt;br&gt;&lt;strong&gt;modelo:&lt;/strong&gt; 27a2r</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Redragon Mirror, Tela de 27 Polegadas FHD, 165HZ, LED, HDMI - GM27X5IPS</t>
-  </si>
-  <si>
-    <t>Características:&lt;br /&gt; - marca: redragon&lt;br /&gt; - modelo: gm27x5ips&lt;br /&gt; especificações:&lt;br /&gt; - cor: preto&lt;br /&gt; - tamanho: 27”&lt;br /&gt; - resolução: 1920 x 1080 16:9&lt;br /&gt; - tipo de painel: ips&lt;br /&gt; - taxa de atualização: 165 hz&lt;br /&gt; - número de cores: 16.7 m&lt;br /&gt; - brilho máximo: 250cd/m2 (typical)&lt;br /&gt; - taxa de contraste: 1000:1&lt;br /&gt; - conectividade: dp 1.2 x1, hdmi 1.4 x2, dc in x1&lt;br /&gt; - power range: 100-240v 50/60hz&lt;br /&gt; - tempo de resposta: 1ms&lt;br /&gt; - peso bruto(g): 5900g&lt;br /&gt; - peso liquido(g): 4200g&lt;br /&gt; conteúdo da embalagem:&lt;br /&gt; - monitor gamer redragon</t>
-  </si>
-  <si>
-    <t>Monitor Gamer 27 Polegadas, 240hz Curvo FULL HD, HDMI/dp</t>
-  </si>
-  <si>
-    <t>Caracteristicas:  - marca: primetek  - modelo: 27c1h  se você está procurando um monitor para jogos, nossas ofertas primetek te oferece uma ótima opção de modelo e um bom preço. Monitor gamer 27curvo 240hz dp/hdmi fhd primetek 27c1h que entrega imagens mais nítidas, levando sua experiência visual e seu foco no jogo para um novo nível.  especificações técnicas:  - tamanho 27´´ painel tipo va  - fonte do painel csot curva plana/ curva  - suporte hdr n resolução 1920 x 1080  - tipo de moldura moldura sem moldura 3 área de visualização da tela (a*v) (mm) 597,888 (a) x 336,312 (v) tipo de luz de fundo do painel e-led  - distância do pixel (a)(v) (mm) 0,1038(a) x 0,3114(v) brilho (nits) (máx.) 280 nits (min)  - taxa de contraste (típico) 3000:1 taxa de contraste dinâmico milhões  - ângulo de visão (h/v) 178°(h)/178°(v)  - profundidade de bits do painel 8 bits cores da tela 16,7m  - tempo de resposta do painel sem od 21ms tempo de resposta 8 ms (alta) taxa de atualização do painel (máx.) 240 hz taxa de atualização da tela (máx.) 48hz-240hz scaler pn hdmi 1.4 n/a faixa freesync n/a hdmi 2.0 2 faixa freesync 48-240 hz  - saída de áudio  - botão liga/desliga cinco botão osd cinco  - contracapa design rgb  - consumo de energia 25w tipo.,54w máx. Modo de economia de energia?0,5w modo de desligamento ?0,3w  - tipo de energia adaptador de energia fonte de alimentação 12v 4a  - acessorios: cabo de alimentação (1,5 m) 1 (1,5 m) cabo dp versão 1.2 qtd de cabo dp (1,5 m/1,8 m) 1 (1,5 m)  - temperatura da cor (fria, quente, usuário) controle de baixa luz azul modos de cenários dcr menu de idiomas 23 idiomas  - nenhum ajuste de luz de fundo intermitente sincronização adaptável freesync  - over drive fps/rts jogo mais pip/pbp qp efeito de luz laranja  - dimensão com suporte (l/a/p)(mm) 616,2x453,1x195,7 mm  - dimensão sem suporte (lxaxp)(mm) 616,2x367,2x96,3 mm  - dimensão da caixa (lxaxp)(mm) 699x169x440mm  - peso líquido (kg) 4,85kg  - peso bruto (kg) 6,72kg  - garantia 1 ano &lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;marca:&lt;/strong&gt; primetek&lt;br&gt;&lt;strong&gt;modelo:&lt;/strong&gt; 25c1h&lt;br&gt;&lt;strong&gt;tamanho da tela:&lt;/strong&gt; 25</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Goldentec, 24 Polegadas, LED, Full HD, 144hz, 1ms</t>
-  </si>
-  <si>
-    <t>Monitor gamer goldentec 24´´ led full hd 144hz 1ms | gt gamer conta com tecnologia freesync, capaz de eliminar falhas e intermitências. Além disso, possui tecnologia lowbluelight, capaz de reduzir a luz azul do monitor proporcionando mais conforto e segurança. Conta também com 100% flicker free, suavizando a ondulação do monitor.   especificações técnicas  marcagoldentec  tamanho de tela24´´  framelesssim  resolução1920x1080 (full hd)  tempo de resposta 1ms  frequência 144hz  brilho250 cd/m²  contraste 100 milhões: 1  ângulo de visão180° (h) 180° (v)  cores16,7 milhões  inclinação ajustavel15°  tecnologia freesyncsim, elimina falhas e intermitências  tecnlogia lowbluelightsim, reduz a luz azul para mais conforto e segurança  100% flicker freesim, suaviza a ondulação do monitor  conexõeshdmi + vga  conteúdo da embalagemmonitor 24´´&lt;br&gt;fonte adaptadora&lt;br&gt;cabo hdmi&lt;br&gt;manual de instruções   &lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;marca :&lt;/strong&gt; goldentec&lt;br&gt;&lt;strong&gt;tipo :&lt;/strong&gt; gamer&lt;br&gt;&lt;strong&gt;polegadas :&lt;/strong&gt; 24 ´´&lt;br&gt;&lt;br&gt;&lt;strong&gt;garantia : &lt;/strong&gt;12</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Grasep 27 Polegadas Led, FHD, HDMI, Som Integrado - 1920P</t>
-  </si>
-  <si>
-    <t>PRONTA ENTREGA&lt;br /&gt;3 meses de garantia com o vendedor!&lt;br /&gt;6 meses de garantia com o fabricante!&lt;br /&gt;&lt;br /&gt;Monitor PC Gamer Led Full HD Som integrado 27 pol 75Hz&lt;br /&gt;&lt;br /&gt;Eleve a qualidade visual do seu computador com este incrível monitor PC de alta definição. Projetado para oferecer uma experiência visual imersiva e nítida, este monitor é perfeito para trabalhar, jogar, assistir a filmes e muito mais.&lt;br /&gt;&lt;br /&gt;Com uma tela de alta resolução, cada detalhe ganha vida, proporcionando imagens vibrantes e cores realistas. Seja para editar fotos e vídeos, jogar seus games favoritos ou assistir a filmes em alta definição, este monitor oferece uma qualidade de imagem impressionante, com alto contraste e brilho intenso.&lt;br /&gt;&lt;br /&gt;Além disso, o monitor possui um tamanho de 27 polegadas para acomodar várias janelas e facilitar a multitarefa. Você poderá abrir e trabalhar em diferentes aplicativos ao mesmo tempo, aumentando sua produtividade e tornando seu fluxo de trabalho mais eficiente.&lt;br /&gt;&lt;br /&gt;Dimensões: 4x56x33cm&lt;br /&gt;Peso: 3.6kg&lt;br /&gt;&lt;br /&gt;Especificações:&lt;br /&gt;Tela: 27"&lt;br /&gt;Tipo: LED&lt;br /&gt;Resolução: 1920x1080&lt;br /&gt;IPS&lt;br /&gt;Tempo de resposta: 1ms&lt;br /&gt;Brilho máxima: 250cd/m&lt;br /&gt;Interfaces: HDMI/VGA/AUDIO IN&lt;br /&gt;Frequência horizontal: 67.200KHz&lt;br /&gt;Frequência vertical: 75Hz&lt;br /&gt;Consumo de potência: 35W&lt;br /&gt;Consumo Potência em Standby: 0,5&lt;br /&gt;Não possui som integrado&lt;br /&gt;Visão expansiva&lt;br /&gt;&lt;br /&gt;Itens Inclusos:&lt;br /&gt;1 Monitor 27&lt;br /&gt;1 Cabo DisplayPort&lt;br /&gt;1 Fonte AC/DC&lt;br /&gt;1 Manual</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Acer VG240Y FHD 165hz FreeSync ZeroFrame 0,5ms.</t>
-  </si>
-  <si>
-    <t>A tecnologia AMDFreeSync Premium elimina a tela ?'rasgada', minimiza atrasos e latência durante os jogos, apresentando uma sincronização dos quadros do monitor muito mais eficiente. Sua experiência visual será mais suave, fluida e responsiva. O Nitro VG240Y conta com uma alta taxa de atualização de 144Hz até 165Hz. Prepare-se para ver imagens mais suaves, sem rastros e sem rasgos. Monitor é igual exp: quanto mais, melhor. Jogue com múltiplos monitores sem problemas, o design ZeroFrame praticamente elimina as bordas para que você tenha uma verdadeira imersão no jogo. Com Display Acer HDR, o VG240Y cria níveis mais profundos do contraste preto e branco. Nas cenas mais escuras, os pretos ricos são preservados e os detalhes aprimorados, gerando maior luminosidade. A tela de 23.8 polegadas IPS Full HD potencializa seu poder de imersão nas batalhas. A latência ultrabaixa deste monitor oferece respostas rápidas além das expectativas. Você terá controle total em jogos de corrida ou esporte, devido à redução do atraso de quadro. O tempo de resposta do Nitro é de 2ms até 0,5ms.</t>
-  </si>
-  <si>
-    <t>Monitor Gamer 27 Asus Vg279q1r Tuf Gaming - Full Hd Ips - 144hz - 1ms - Freesync - Hdmi/displayport</t>
-  </si>
-  <si>
-    <t>TUF Gaming VG279Q1RO TUF Gaming VG279Q1R é uma tela Full HD (1920x1080) de 27 polegadas com uma taxa de atualização ultrarrápida de 144 Hz projetada para jogadores profissionais e aqueles que buscam jogabilidade envolvente. Ele também possui a tecnologia Adaptive-Sync (FreeSync ™), para uma jogabilidade extremamente fluida sem tearing e stuttering.MONITOR GAMING ULTRA SLIM DE 27 POLEGADASO painel Full HD (1920 X 1080) de 27 polegadas do TUF Gaming VG279Q1R oferece visuais impressionantes de ângulos de visão amplos de 178 °. Também ocupa muito pouco espaço na área de trabalho e se encaixa bem em qualquer configuração. Seu perfil ultrafino mede apenas 7,5 mm em seu ponto mais fino, também apresenta o novo Turbo Rim baseado que combina com a configuração de jogo perfeita.Refresh rate de 144hzO TUF Gaming VG279Q1R tem uma taxa de atualização super rápida de 144 Hz, garantindo que mesmo os jogos mais rápidos, jogados nas configurações visuais mais altas, tenham uma aparência suave e completamente livre de atrasos. Obtenha a vantagem em jogos de tiro em primeira pessoa, corrida, estratégia em tempo real e títulos de esportes.EXTREME LOW MOTION BLURA tecnologia Extreme Low Motion Blur exclusiva da ASUS alcança 1 ms MPRT para eliminar manchas e desfoque de movimento. Também faz com que os objetos em movimento pareçam ainda mais nítidos, para que a jogabilidade seja mais fluida e ágil.Shadow BoostA tecnologia ASUS Shadow Boost esclarece as áreas escuras do jogo sem superexpor as áreas mais brilhantes, melhorando a visualização geral, ao mesmo tempo que torna mais fácil localizar inimigos escondidos em áreas escuras do mapa.</t>
-  </si>
-  <si>
-    <t>Monitor Goldentec, 24" Led Gt Gamer Fhd, Hdmi, 75hz</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Bluecase, 21.5" Full HD, 75Hz, Rako - BM221GW</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Husky Storm 27' LED, Curvo, 165 Hz, Full HD, 1ms, Adaptive Sync, HDMI/DisplayPort, Ajuste de Ângulo - HGMT001</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;Monitor Gamer Husky Storm 27' LED, Curvo, 165 Hz, Full HD, 1ms, Adaptive Sync, HDMI/DisplayPort, Ajuste de &amp;Acirc;ngulo&lt;/h2&gt;
-&lt;h3&gt;&lt;br /&gt;Esteja um passo &amp;agrave; frente!&lt;/h3&gt;
-&lt;p&gt;O Monitor Husky Storm conta com resposta de 1ms e taxa de atualiza&amp;ccedil;&amp;atilde;o de 165Hz, permitindo a mais alta performance durante suas gameplays. Sua curvatura amplia o campo de vis&amp;atilde;o relativo, concentrando toda a a&amp;ccedil;&amp;atilde;o ao alcance dos olhos do usu&amp;aacute;rio, sem perder resolu&amp;ccedil;&amp;atilde;o.&lt;/p&gt;
-&lt;h3&gt;&lt;br /&gt;Tecnologia Adaptive Sync&amp;nbsp;&lt;/h3&gt;
-&lt;p&gt;Compat&amp;iacute;vel com a tecnologia Adaptive Sync, permite a sincroniza&amp;ccedil;&amp;atilde;o dos frames da placa de v&amp;iacute;deo, decretando o fim do input lag, bem como do tearing.&lt;/p&gt;
-&lt;h3&gt;&lt;br /&gt;Monitor Curvo&amp;nbsp;&lt;/h3&gt;
-&lt;p&gt;Tenha mais imers&amp;atilde;o na sua gaming player com esse monitor curvo da Husky. Observe seus advers&amp;aacute;rios ainda mais de perto com essa imers&amp;atilde;o de 1500r de curvatura e um &amp;acirc;ngulo de vis&amp;atilde;o de 178&amp;ordm;.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Adaptive Sync&lt;/h3&gt;
-&lt;p&gt;Evita o imput lag e combate o problema da quebra de quadros durante a reprodu&amp;ccedil;&amp;atilde;o dos frames. Essa Tecnologia evita o travamento do jogo para uma jogabilidade mais suave poss&amp;iacute;vel. Explore novas paisagens e capture seus inimigos em movimentos suaves e cont&amp;iacute;nuos.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Inclin&amp;aacute;vel&lt;/h3&gt;
-&lt;p&gt;Ajuste de inclina&amp;ccedil;&amp;atilde;o da tela de 5&amp;deg; a 15&amp;deg;. Ajuste seu monitor da maneira que quiser deixando sua vis&amp;atilde;o ainda mais confort&amp;aacute;vel e ampla&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Monitor Husky &amp;eacute; no KaBuM!&amp;nbsp;&lt;/h3&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;&lt;strong&gt;&lt;a href="https://kabum.com.br/hotsite/manuais/115384-Monitor-Gamer-Husky-Storm-HGMT001.pdf" target="_blank"&gt;MANUAL DE INSTRU&amp;Ccedil;&amp;Otilde;ES&lt;/a&gt;&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Asus TUF Gaming 27 Full HD, 165Hz, 1ms, IPS, HDMI e DisplayPort, FreeSync Premium, VESA - VG279Q1A</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;TUF Gaming VG279Q1A Gaming Monitor Full HD de 27 polegadas (1920x1080), IPS, 165Hz (acima de 144Hz), Extreme Low Motion Blur, Adaptive-sync, FreeSync Premium, 1ms (MPRT)&lt;/h2&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;Monitor de jogos &lt;strong&gt;IPS Full HD (1920 x 1080)&lt;/strong&gt; de 27 polegadas com &lt;strong&gt;taxa de atualiza&amp;ccedil;&amp;atilde;o ultrarr&amp;aacute;pida de 165 Hz&lt;/strong&gt;, projetado para jogadores profissionais e jogabilidade envolvente.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;A tecnologia &lt;strong&gt;ASUS Extreme Low Motion Blur (ELMB)&lt;/strong&gt; permite um &lt;strong&gt;tempo de resposta de 1 ms (MPRT)&lt;/strong&gt; junto com a sincroniza&amp;ccedil;&amp;atilde;o adaptativa, eliminando fantasmas e rasgos para visuais de jogos n&amp;iacute;tidos com altas taxas de quadros.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;&lt;strong&gt;Tecnologia FreeSync Premium&lt;/strong&gt; para eliminar rasgos na tela e taxas de quadros inst&amp;aacute;veis.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;Suporta &lt;strong&gt;Adaptive-Sync&lt;/strong&gt; com placas gr&amp;aacute;ficas &lt;strong&gt;NVIDIA GeForce e FreeSync&lt;/strong&gt; com placas gr&amp;aacute;ficas AMD Radeon Compat&amp;iacute;vel com NVIDIA GeForce s&amp;eacute;rie GTX 10, s&amp;eacute;rie GTX 16, s&amp;eacute;rie RTX 20 e placas gr&amp;aacute;ficas mais recentes.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;O &lt;strong&gt;Shadow Boost aprimora os detalhes da imagem&lt;/strong&gt; em &amp;aacute;reas escuras, iluminando as cenas sem super expor as &amp;aacute;reas claras.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;Sa&amp;iacute;da &lt;strong&gt;Full HD (1920 x 1080) a 120 Hz no PS5 e Xbox&lt;/strong&gt; Series X/S.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Todos os elementos essenciais para jogos&lt;/h3&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;O TUF Gaming VG279Q1A &amp;eacute; um monitor IPS Full HD (1920 x 1080) de 27 polegadas com uma taxa de atualiza&amp;ccedil;&amp;atilde;o ultrarr&amp;aacute;pida de 165 Hz. Projetado para jogadores e outros que buscam uma jogabilidade envolvente, ele oferece algumas especifica&amp;ccedil;&amp;otilde;es s&amp;eacute;rias. Mas h&amp;aacute; mais...&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;Sua fun&amp;ccedil;&amp;atilde;o exclusiva ELMB apresenta um tempo de resposta MPRT de 1ms e tecnologia Adaptive-Sync (FreeSync Premium), para uma jogabilidade extremamente fluida sem tearing e gagueira.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Tela IPS de 27 polegadas para melhor reprodu&amp;ccedil;&amp;atilde;o de cores&lt;/h3&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;O painel IPS Full HD (1920 x 1080) de 27 polegadas do TUF Gaming VG279Q1A oferece visuais impressionantes de todos os &amp;acirc;ngulos com amplos &amp;acirc;ngulos de vis&amp;atilde;o de 178 graus, garantindo distor&amp;ccedil;&amp;atilde;o m&amp;iacute;nima e mudan&amp;ccedil;a de cor mesmo quando voc&amp;ecirc; est&amp;aacute; visualizando de posi&amp;ccedil;&amp;otilde;es extremas.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Taxa de atualiza&amp;ccedil;&amp;atilde;o super-r&amp;aacute;pida de 165 Hz&lt;/h3&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;Uma impressionante taxa de atualiza&amp;ccedil;&amp;atilde;o de 165 Hz elimina o atraso e o desfoque de movimento para dar a voc&amp;ecirc; vantagem em jogos de tiro em primeira pessoa, corrida, estrat&amp;eacute;gia em tempo real e t&amp;iacute;tulos esportivos. Essa taxa de atualiza&amp;ccedil;&amp;atilde;o ultrarr&amp;aacute;pida permite que voc&amp;ecirc; jogue nas configura&amp;ccedil;&amp;otilde;es visuais mais altas e reaja instantaneamente ao que est&amp;aacute; na tela.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Desfrute de uma jogabilidade super suave&lt;/h3&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;Apresenta a mais recente tecnologia Extreme Low Motion Blur exclusiva da ASUS, que atinge 1ms MPRT para eliminar manchas e desfoque de movimento, e torna os objetos em movimento mais n&amp;iacute;tidos, para que a jogabilidade seja mais fluida e responsiva.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Duex 27 Full HD Curvo, 240Hz, 1ms, IPS, HDMI e DisplayPort, 99% sRGB, VESA - 270ZG</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;Monitor Gamer Duex 27 Full HD&lt;/h2&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;Uma velocidade ultrarr&amp;aacute;pida de&amp;nbsp;&lt;strong&gt;240Hz e 1ms&lt;/strong&gt;&amp;nbsp;permite que os jogadores vejam o pr&amp;oacute;ximo quadro rapidamente e fazem com que a imagem apare&amp;ccedil;a suavemente. Os jogadores podem responder rapidamente aos oponentes e mirar no alvo facilmente.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Compre agora no KaBuM!&lt;/h3&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Husky 700  27 LED, Curvo Wide, WQHD, 165Hz, 1ms, HDMI e DisplayPort, Adaptive Sync, VESA - HGMT008</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;Monitor Gamer Husky Gaming Storm 700&lt;/h2&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;N&amp;atilde;o precisa mais se perguntar qual monitor gamer comprar! A Husky Gaming ajuda voc&amp;ecirc; a &lt;strong&gt;atualizar seu setup&lt;/strong&gt;, seja para partidas no PC ou v&amp;iacute;deo game. Sempre oferecemos &lt;strong&gt;o melhor para voc&amp;ecirc;!&lt;/strong&gt;&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;Monitor Gamer Husky Gaming Storm 700 tem uma alta &lt;strong&gt;taxa de atualiza&amp;ccedil;&amp;atilde;o de 165 Hz&lt;/strong&gt; com &lt;strong&gt;tempo de resposta de 1 ms&lt;/strong&gt;, que possibilita um tempo de rea&amp;ccedil;&amp;atilde;o mais r&amp;aacute;pido para suas partidas insanas.&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;Sua&lt;strong&gt; tela curva Quad HD de 27"&lt;/strong&gt;, com&lt;strong&gt; resolu&amp;ccedil;&amp;atilde;o de 2560 x 1440P&lt;/strong&gt; que garante imagem mais n&amp;iacute;tida e detalhada. Proporcionando&lt;strong&gt; jogabilidade fluida&lt;/strong&gt;, &lt;strong&gt;sem distor&amp;ccedil;&amp;otilde;es&lt;/strong&gt; e uma &lt;strong&gt;experi&amp;ecirc;ncia mais imersiva&lt;/strong&gt; para voc&amp;ecirc; n&amp;atilde;o perder nenhum detalhe importante, do seu programa de esporte, filme, s&amp;eacute;rie ou jogo preferido.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Aproveite e garanta j&amp;aacute; o seu Monitor Gamer Husky Gaming Storm 700! no KaBuM!&lt;/h3&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Gigabyte, 27 QHD, 170Hz, 1ms, DisplayPort e HDMI, 108% sRGB, HDR, Adaptive-Sync - GS27QC SA</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;Monitor Gamer Gigabyte 27 QHD&lt;/h2&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;A Mais Alta Qualidade&lt;/h2&gt;
-&lt;p&gt;Equipado com uma taxa de atualiza&amp;ccedil;&amp;atilde;o de &lt;strong&gt;165 Hz&lt;/strong&gt; que suporta a tecnologia &lt;strong&gt;Adaptive-Sync&lt;/strong&gt; (FreeSync Premium), que p&amp;otilde;e fim &amp;agrave; jogabilidade inst&amp;aacute;vel e aos frames quebrados e cria um desempenho fluido e livre de artefatos em qualquer taxa de quadros. GS27QC com um tempo de resposta extremamente r&amp;aacute;pido de &lt;strong&gt;1 ms&lt;/strong&gt; para eliminar totalmente o atraso e o rasgo da imagem.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Mais Curva e Mais Imers&amp;atilde;o&lt;/h2&gt;
-&lt;p&gt;Um painel VA nativo de &lt;strong&gt;1500 Raios&lt;/strong&gt; que apresenta uma vis&amp;atilde;o mais pr&amp;oacute;xima do olho humano do que um monitor plano, proporcionando uma sensa&amp;ccedil;&amp;atilde;o mais envolvente e ao mesmo tempo oferecendo mais conforto visual.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Milh&amp;otilde;es de Cores&lt;/h2&gt;
-&lt;p&gt;O GS27QC pode exibir &lt;strong&gt;16,7 milh&amp;otilde;es de cores&lt;/strong&gt; e possui uma taxa de contraste de &lt;strong&gt;4000:1&lt;/strong&gt;. Ele permite que voc&amp;ecirc; desfrute de uma experi&amp;ecirc;ncia de jogo fluente com cores reais e vibrantes. O GS27QC est&amp;aacute; pronto para &lt;strong&gt;HDR&lt;/strong&gt;, o que desperta interesse em uma ampla gama de aplica&amp;ccedil;&amp;otilde;es, incluindo jogos, entretenimento cinematogr&amp;aacute;fico e cria&amp;ccedil;&amp;atilde;o de conte&amp;uacute;do multim&amp;iacute;dia.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Compre j&amp;aacute; o seu no KaBuM!&lt;/h3&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Husky Hailstorm 31.5' LED, Curvo, 165 Hz, Full HD, 1ms, Adaptive Sync, HDMI/DisplayPort, Ajuste de Ângulo - HGMT002</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;Monitor Gamer Husky Hailstorm 31.5' LED, Curvo, 165 Hz, Full HD, 1ms, Adaptive Sync, HDMI/DisplayPort, Ajuste de &amp;Acirc;ngulo&amp;nbsp;&lt;/h2&gt;
-&lt;h2&gt;&amp;nbsp;&lt;/h2&gt;
-&lt;h3&gt;Esteja um passo &amp;agrave; frente!&amp;nbsp;&lt;/h3&gt;
-&lt;p&gt;O Monitor Husky Hail Storm conta com resposta de 1ms e taxa de atualiza&amp;ccedil;&amp;atilde;o de &lt;strong&gt;165Hz&lt;/strong&gt;, permitindo a mais alta performance durante suas gameplays. Sua &lt;strong&gt;curvatura&lt;/strong&gt; amplia o campo de vis&amp;atilde;o relativo, concentrando toda a a&amp;ccedil;&amp;atilde;o ao alcance dos olhos do usu&amp;aacute;rio, sem perder resolu&amp;ccedil;&amp;atilde;o.&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Melhor Entrega de Imagens para sua Gameplay&lt;/h3&gt;
-&lt;p&gt;Compat&amp;iacute;vel com a tecnologia &lt;strong&gt;Adaptive Sync&lt;/strong&gt;, permite a sincroniza&amp;ccedil;&amp;atilde;o dos frames da placa de v&amp;iacute;deo, decretando o fim do input lag, bem como do tearing.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Conectividade&lt;/h3&gt;
-&lt;p&gt;O monitor Husky Hailstorm acompanha um cabo &lt;strong&gt;DisplayPort&lt;/strong&gt; que garante a melhor qualidade de imagem para seu jogo. Al&amp;eacute;m da conex&amp;atilde;o DP, o monitor ainda possui duas conex&amp;otilde;es &lt;strong&gt;HDMI&lt;/strong&gt; e uma &lt;strong&gt;conex&amp;atilde;o P2&lt;/strong&gt; para ouvir seu jogo diretamente do seu monitor.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Maior Ergonomia e Conforto para Uso Prolongado&amp;nbsp;&amp;nbsp;&lt;/h3&gt;
-&lt;p&gt;O Husky Hailstorm possui ajuste de &lt;strong&gt;inclina&amp;ccedil;&amp;atilde;o de 5&amp;deg; a 15&amp;deg;&lt;/strong&gt; que se ajusta ergonomicamente para o seu uso. O monitor tamb&amp;eacute;m conta com &lt;strong&gt;Redu&amp;ccedil;&amp;atilde;o de Luz Azul&lt;/strong&gt;, se tornando uma &amp;oacute;tima op&amp;ccedil;&amp;atilde;o para Gameplays prolongadas.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Seu Monitor Husky voc&amp;ecirc; encontra aqui no KaBuM!&lt;/h3&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Gigabyte 27 IPS, QHD , 144Hz, 1ms, 120% sRGB, HDR 400, FreeSync Premium, Altura Ajustável - G27Q-SA</t>
-  </si>
-  <si>
-    <t>JUNTE-SE À LUTA com o Monitor Gamer de 27" G27Q-SA da Gigabyte com 1ms de tempo de resposta, freesync premium, 144 Hz e com uma taxa de cor de 8 bits, 92% DCI-P3 A ÚLTIMA MILHA PARA O SEU SISTEMA DE JOGO Como um jogador invisível, o monitor é frequentemente subestimado. A verdade é que os monitores se formam como um efeito sinérgico e trazem o melhor desempenho dos componentes do PC. Os monitores de jogos GIGABYTE oferecem as últimas especificações e qualidade, os usuários podem realmente desfrutar de um desempenho de alto nível sem a necessidade de extravagância. Tempo de Resposta de 1 ms Tempo de resposta super rápido de 1 ms para a experiência de jogo mais suave de todos os tempos! QHD e 144Hz Alta resolução e taxa de atualização rápida, proporcionando qualidade de exibição detalhada e experiência de jogo fluida! Cor de 8 bits, 92% DCI-P3 Fantástico visor colorido e 92% de cores DCI-P3 de gama super ampla. SIMPLES MAS ESTILOSO A aparência aerodinâmica representa a simplicidade da filosofia de design da série de jogos GIGABYTE, suporte robusto e acabamento fosco construído para características funcionais e estéticas adicionando mais características. ÂNGULO DE VISÃO PERFEITO O monitor de jogos GIGABYTE possui um suporte exclusivo ergonomicamente projetado para oferecer uma ampla gama de ajustes de altura e inclinação.</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Acer 31.5 LED Full HD, Curvo, 165 Hz, 1ms, HDMI e DisplayPort, FreeSync Premium, VESA - ED320QR</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;Monitor Gamer Acer 31.5 LED Full HD, Curvo, 165 Hz, 1ms, HDMI e DisplayPort, FreeSync Premium, VESA&lt;/h2&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Tela Curva e Imersiva&lt;/h2&gt;
-&lt;p&gt;Tenha uma experi&amp;ecirc;ncia visual imersiva e confort&amp;aacute;vel com uma&lt;strong&gt; tela curva&lt;/strong&gt; com raio de 1800 mm de visualiza&amp;ccedil;&amp;atilde;o. Essa tecnologia mant&amp;eacute;m os cantos da tela &amp;agrave; mesma dist&amp;acirc;ncia de seus olhos. S&amp;atilde;o &lt;strong&gt;31,5&amp;rdquo;&lt;/strong&gt; e resolu&amp;ccedil;&amp;atilde;o &lt;strong&gt;Full HD&lt;/strong&gt;, promovendo imagens n&amp;iacute;tidas, que levam seu foco no jogo a outro n&amp;iacute;vel.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Design ZeroFrame&lt;/h2&gt;
-&lt;p&gt;Monitor com tela &lt;strong&gt;LED VA&lt;/strong&gt; e design ZeroFrame, que praticamente elimina as bordas para que voc&amp;ecirc; tenha uma verdadeira imers&amp;atilde;o no jogo.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;De olho em cada Frame&lt;/h2&gt;
-&lt;p&gt;O Nitro Series ED0 conta com uma taxa de atualiza&amp;ccedil;&amp;atilde;o de at&amp;eacute; &lt;strong&gt;165Hz.&lt;/strong&gt; Prepare-se para ver imagens mais suaves, sem rastros e sem rasgos.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Foque no Movimento&lt;/h2&gt;
-&lt;p&gt;Com o Visual Response Boost (VRB) de 1 ms, o monitor reduz borr&amp;otilde;es, efeitos fantasmas e manchas nas imagens. Al&amp;eacute;m disso, elimina o desfoque em objetos em movimento r&amp;aacute;pido.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Jogue em Perfeita Sincronia&lt;/h2&gt;
-&lt;p&gt;A tecnologi&lt;strong&gt;a AMD FreeSync Premium&lt;/strong&gt; elimina a tela &amp;ldquo;rasgada&amp;rdquo;, minimiza atrasos e lat&amp;ecirc;ncia durante os jogos, apresentando uma sincroniza&amp;ccedil;&amp;atilde;o dos quadros do monitor muito mais eficiente. Sua experi&amp;ecirc;ncia visual ser&amp;aacute; mais&lt;strong&gt; suave, fluida e responsiva.&lt;/strong&gt;&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Contrastes Impressionantes&lt;/h2&gt;
-&lt;p&gt;O contraste de 100 milh&amp;otilde;es:1 &amp;eacute; alcan&amp;ccedil;ado atrav&amp;eacute;s da tecnologia Acer Adaptive Contrast Management. Ela proporciona um&lt;strong&gt; visual mais cristalino&lt;/strong&gt; e real&amp;ccedil;a a qualidade das cores do monitor.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Aproveite essa oportunidade e adquira seu Monitor Acer no KaBuM!&lt;/h3&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Samsung 22' IPS, 75 Hz, Full HD, FreeSync, HDMI/VGA, VESA -  LF22T350FHLMZD</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Monitor Gamer Samsung LED 22, IPS, Full HD, Vesa, Free Sync, Modo Gaming, Preto Vis&amp;atilde;o totalmente expansiva Design minimalista, concentra&amp;ccedil;&amp;atilde;o m&amp;aacute;xima. A tela com 3 lados sem borda traz uma est&amp;eacute;tica limpa e moderna para qualquer ambiente de trabalho. Em um setup com v&amp;aacute;rios monitores, se alinham perfeitamente para uma visualiza&amp;ccedil;&amp;atilde;o praticamente sem espa&amp;ccedil;os e sem distra&amp;ccedil;&amp;otilde;es. Imagens perfeitas e suaves Agora, a imagem &amp;eacute; reproduzida sem falhas. A taxa de atualiza&amp;ccedil;&amp;atilde;o de 75Hz oferece cenas mais fluidas. Seu momento de divers&amp;atilde;o n&amp;atilde;o tem lag ou efeito fantasma, quer voc&amp;ecirc; esteja acompanhando seu programa de TV favorito, assistindo a um v&amp;iacute;deo ou jogando um jogo. A&amp;ccedil;&amp;atilde;o Sincronizada Experi&amp;ecirc;ncia de entretenimento super fluida. AMD Radeon FreeSync mant&amp;eacute;m a taxa de atualiza&amp;ccedil;&amp;atilde;o do monitor e da placa gr&amp;aacute;fica em sincronia para reduzir a quebra de imagem. Assista a filmes e jogue sem interrup&amp;ccedil;&amp;otilde;es. At&amp;eacute; mesmo as cenas r&amp;aacute;pidas s&amp;atilde;o perfeitas e suaves. Veja de qualquer &amp;acirc;ngulo Sente-se em qualquer lugar e tenha uma experi&amp;ecirc;ncia completa sem distor&amp;ccedil;&amp;atilde;o de cores. O painel IPS preserva a nitidez e a vivacidade das cores em cada cent&amp;iacute;metro da tela. Mesmo em uma tela t&amp;atilde;o ampla, os tons e sombras s&amp;atilde;o completamente precisos de praticamente qualquer &amp;acirc;ngulo, sem altera&amp;ccedil;&amp;atilde;o de cor. Mais poder de jogo As configura&amp;ccedil;&amp;otilde;es de jogo ideais proporcionam uma vantagem instant&amp;acirc;nea. Detecte inimigos escondidos nas sombras atrav&amp;eacute;s do contraste ideal, mais nitidez e cenas com cores mais vivas. O Modo de Jogo ajusta qualquer jogo para preencher sua tela visualizando todos os detalhes. Mais conforto para os olhos Proteja seus olhos e fa&amp;ccedil;a mais. A avan&amp;ccedil;ada tecnologia de conforto visual reduz a fadiga ocular para uma experi&amp;ecirc;ncia prolongada menos cansativa. A tecnologia Flicker Free remove continuamente a tremula&amp;ccedil;&amp;atilde;o cansativa e irritante da tela, enquanto o Eye Saver Mode minimiza a emiss&amp;atilde;o de luz azul. Seus olhos ficam descansados por mais tempo. Versatilidade de verdade Conecte-se a mais. Com as portas HDMI e D-sub, v&amp;aacute;rios dispositivos podem ser conectados diretamente ao seu monitor para total flexibilidade. Agora, seu ambiente de computa&amp;ccedil;&amp;atilde;o &amp;eacute; ainda mais conveniente com possibilidades de entrada adicionais.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer AOC Agon 31.5' LED, Curvo, 165 Hz, Full HD, 1ms, FreeSync Premium, HDMI/DisplayPort, RGB Light FX - AG323FCXE</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Com tela de alta qualidade, amplo &amp;acirc;ngulo de vis&amp;atilde;o e comando em tempo real, prepare-se para obter uma experi&amp;ecirc;ncia muito mais imersiva em todos os g&amp;ecirc;neros de jogos. Projetado para gamers, o monitor Agon permite movimentos muito mais flu&amp;iacute;dos nos jogos devido a alt&amp;iacute;ssima taxa de atualiza&amp;ccedil;&amp;atilde;o de 165 Hz. O tempo de resposta de 1 ms proporciona movimentos instant&amp;acirc;neos e naturais para voc&amp;ecirc; ser o melhor, e com o painel VA, voc&amp;ecirc; tem mais brilho e contraste para enxergar onde os seus inimigos est&amp;atilde;o, mesmo em cenas com pouca ilumina&amp;ccedil;&amp;atilde;o. Al&amp;eacute;m disso, o design exclusivo com LEDs em diferentes configura&amp;ccedil;&amp;otilde;es de cores RGB deixam a sua maratona de jogos ainda mais emocionante.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer LG Ultra Gear 27 Full HD, 144 Hz, 1ms, IPS, HDMI e DisplayPort, sRGB 99%, HDR10, FreeSync, VESA, Altura Ajustável - 27GL650F-B</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;Monitor Gamer LG Ultra Gear 27 Full HD&lt;/h2&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Evolua o Jogo Antes do Seu Rival:&lt;/h2&gt;
-&lt;p&gt;Tenha incr&amp;iacute;vel qualidade de imagens e decis&amp;otilde;es imediatas aos seus jogos com o Monitor Gamer LG 27GL650F.&lt;br /&gt;Os &lt;strong&gt;frames ultra-r&amp;aacute;pidos&lt;/strong&gt; de &lt;strong&gt;144Hz&lt;/strong&gt; permite os jogadores a reagirem imediatamente aos seus advers&amp;aacute;rios e mudar a hist&amp;oacute;ria do jogo para a sua vit&amp;oacute;ria.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;1ms Motion Blur Reduction&lt;/h2&gt;
-&lt;p&gt;Tenha imagens sem rastros e a&amp;ccedil;&amp;otilde;es mais r&amp;aacute;pidos com o &lt;strong&gt;tempo de resposta de 1ms&lt;/strong&gt; com &lt;strong&gt;Motion Blur Reduction.&lt;br /&gt;&lt;/strong&gt;O LG 27GL650F exibe &lt;strong&gt;precis&amp;atilde;o de cores impec&amp;aacute;vel&lt;/strong&gt; com um &amp;acirc;ngulo de vis&amp;atilde;o ampliado de 178&amp;deg;.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Compat&amp;iacute;vel com G-SYNC certificado pela NVIDIA&lt;/h2&gt;
-&lt;p&gt;Ap&amp;oacute;s ser testado pela NVIDIA, o monitor LG 27GL650F &amp;eacute; oficialmente compat&amp;iacute;vel com &lt;strong&gt;G-SYNC&lt;/strong&gt;, eliminando cortes e minimizando as repeti&amp;ccedil;&amp;otilde;es de imagem para uma experi&amp;ecirc;ncia mais fluida nos seus jogos.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Incr&amp;iacute;vel qualidade de imagem&lt;/h2&gt;
-&lt;p&gt;Tenha&lt;strong&gt; imagens supreendentes&lt;/strong&gt; com &lt;strong&gt;HDR10&lt;/strong&gt;, que reproduz alto brilho e maior gama de cores quando comparado a monitores convencionais deixando as imagens com maior qualidade em situa&amp;ccedil;&amp;otilde;es mais brilhantes ou de maior contraste.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Imagens sem falhas&lt;/h2&gt;
-&lt;p&gt;A tecnologia &lt;strong&gt;AMD FreeSync&lt;/strong&gt; reduz corte e repeti&amp;ccedil;&amp;otilde;es de imagens que ocorrem devido a diferen&amp;ccedil;a entre os quadros gr&amp;aacute;ficos e a taxa de atualiza&amp;ccedil;&amp;atilde;o do monitor. Com o FreeSync, os jogadores podem experimentar &lt;strong&gt;movimentos perfeitos e fluidos durante os jogo&lt;/strong&gt; de altas configura&amp;ccedil;&amp;otilde;es visuais.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Compre agora no KaBuM!&lt;/h3&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Samsung Odyssey G3, 24 Full HD, 144Hz, 1ms, FreeSync Premium, HDMI/Displayport, Ajuste de altura, Preto - LF24G35TFWLXZD</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;Monitor Gamer Samsung Odyssey G3, 24 Full HD, 144Hz, 1ms, FreeSync Premium, HDMI/Displayport, Ajuste de altura, Preto&amp;nbsp;&lt;/h2&gt;
-&lt;p&gt;&lt;br /&gt;Monitor Gamer Samsung Odyssey G3 24&amp;rdquo;, FHD, 144 Hz, 1ms, com ajuste de altura, HDMI, DP, VGA, Freesync, Preto, S&amp;eacute;rie G3 Taxa de atualiza&amp;ccedil;&amp;atilde;o de 144Hz Domine todos os inimigos, mesmo em cenas muito r&amp;aacute;pidas. A taxa de atualiza&amp;ccedil;&amp;atilde;o de 144Hz elimina atrasos e desfoque de movimento para uma jogabilidade emocionante com a&amp;ccedil;&amp;atilde;o ultra suave.&lt;/p&gt;
-&lt;h3&gt;&lt;br /&gt;Tempo de resposta de 1ms&lt;/h3&gt;
-&lt;p&gt;Fa&amp;ccedil;a cada movimento contar com um tempo de resposta de 1ms. Ataque seus inimigos assim que os vir e fique &amp;agrave; frente com movimentos precisos do mouse. Seu desempenho na tela &amp;eacute; t&amp;atilde;o r&amp;aacute;pido quanto seus pr&amp;oacute;prios reflexos.&lt;/p&gt;
-&lt;h3&gt;&lt;br /&gt;AMD FreeSync Premium&lt;/h3&gt;
-&lt;p&gt;Jogabilidade suave sem esfor&amp;ccedil;o. O AMD FreeSync Premium apresenta tecnologia de sincroniza&amp;ccedil;&amp;atilde;o adapt&amp;aacute;vel, que reduz o travamento de tela, oscila&amp;ccedil;&amp;atilde;o e atrasos. Veja o jogo do seu jeito Gire, incline e ajuste seu monitor at&amp;eacute; que todos os inimigos estejam perfeitamente vis&amp;iacute;veis. Sua tela pode ser movida livremente para que voc&amp;ecirc; encontre conforto total no jogo. Design de tela cheia O design sem borda de 3 lados revela espa&amp;ccedil;o m&amp;aacute;ximo para uma jogabilidade maior e mais ousada. Alinhe dois monitores com precis&amp;atilde;o em uma configura&amp;ccedil;&amp;atilde;o de monitor duplo sem que nenhum inimigo fique escondido na jun&amp;ccedil;&amp;atilde;o.&lt;/p&gt;
-&lt;h3&gt;&lt;br /&gt;Mais conforto para os olhos&lt;/h3&gt;
-&lt;p&gt;Jogue por mais tempo sem incomodo visual. O Eye Saver Mode minimiza a emiss&amp;atilde;o de luz azul para manter seus olhos relaxados e confort&amp;aacute;veis enquanto joga por muitas horas. A tecnologia Flicker Free remove continuamente a tremula&amp;ccedil;&amp;atilde;o cansativa e irritante da tela para que voc&amp;ecirc; possa jogar por mais tempo sem distra&amp;ccedil;&amp;otilde;es ou fadiga ocular.&lt;/p&gt;
-&lt;h3&gt;&lt;br /&gt;Garanta o seu no KaBuM!&lt;/h3&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Concórdia 27" LED Full HD, 165Hz, 1ms, HDMI/DisplayPort, FreeSync, Preto - G5s</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;Monitor Conc&amp;oacute;rdia Gamer G5s 27" Led Full Hd 165hz Freesync Hdmi Display Port&lt;/h2&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;O Monitor Conc&amp;oacute;rdia Gamer G5s de 27" 144Hz/165Hz apresenta tecnologia para tornar sua experi&amp;ecirc;ncia com games ainda mais intensa. Sem rastros, sem atraso, sem imagens tremidas! Tudo isso possibilitado pela sua taxa de atualiza&amp;ccedil;&amp;atilde;o de 144Hz/165Hz e tecnologia Freesync que juntos tornam esse monitor a sua melhor escolha. Com som embutido, conex&amp;atilde;o para fones, ele ainda facilita a sua vida com duas&amp;nbsp; conex&amp;otilde;es HDMI.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Alto desempenho com conveni&amp;ecirc;ncia a um pre&amp;ccedil;o justo nesse excelente painel PVA.&lt;/h3&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer LG 25' IPS, Ultra Wide, 75 Hz, Full HD,  99% sRGB, HDMI, VESA - 25UM58-G</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;Monitor Gamer LG UltraWide&lt;/h2&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;1ms Motion Blur Reduction&lt;/h3&gt;
-&lt;p&gt;Tenha &lt;strong&gt;imagens sem rastros&lt;/strong&gt; e &lt;strong&gt;a&amp;ccedil;&amp;otilde;es mais r&amp;aacute;pidas&lt;/strong&gt; com o &lt;strong&gt;tempo de resposta de 1ms&lt;/strong&gt; com &lt;strong&gt;Motion Blur Reduction&lt;/strong&gt;.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;UltraWide&lt;/h3&gt;
-&lt;p&gt;A propor&amp;ccedil;&amp;atilde;o da imagem do monitor UltraWide torna os jogos e filmes mais envolventes do que nunca. A &lt;strong&gt;nitidez da resolu&amp;ccedil;&amp;atilde;o Full HD&lt;/strong&gt; de &lt;strong&gt;1080P com IPS&lt;/strong&gt; faz a diferen&amp;ccedil;a. Simplificando, de qualquer &amp;acirc;ngulo de vis&amp;atilde;o, tudo fica mais n&amp;iacute;tido e detalhado em FULL HD .&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Recursos Avan&amp;ccedil;ados para Jogos&lt;/h3&gt;
-&lt;p&gt;Ative o &lt;strong&gt;Dynamic Action Sync&lt;/strong&gt; para que o monitor acompanhe a velocidade das suas habilidades e veja os inimigos nos lugares mais escuros com o &lt;strong&gt;Black Stabilizer.&amp;nbsp;&lt;/strong&gt;Defina as condi&amp;ccedil;&amp;otilde;es ideais de jogo no Modo de Jogo. H&amp;aacute; &lt;strong&gt;3 modos&lt;/strong&gt; &lt;strong&gt;para jogadores&lt;/strong&gt;: &lt;strong&gt;2 modos de tiro&lt;/strong&gt; &lt;strong&gt;em primeira pessoa&lt;/strong&gt; e at&amp;eacute; mesmo um &lt;strong&gt;modo predefinido&lt;/strong&gt; &lt;strong&gt;de estrat&amp;eacute;gia em tempo real&lt;/strong&gt;.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;On-Screen Control&lt;/h3&gt;
-&lt;p&gt;O Controle On-Screen coloca uma s&amp;eacute;rie de &lt;strong&gt;configura&amp;ccedil;&amp;otilde;es essenciais em uma pr&amp;aacute;tica janela para acesso f&amp;aacute;cil&lt;/strong&gt;. As &lt;strong&gt;configura&amp;ccedil;&amp;otilde;es de volume, brilho, predefini&amp;ccedil;&amp;otilde;es de modo de imagem&lt;/strong&gt;, &lt;strong&gt;Screen Split 2.0 e Dual Controller&lt;/strong&gt;, al&amp;eacute;m de muitas outras, podem agora ser ajustadas com apenas alguns cliques do mouse, em vez dos bot&amp;otilde;es f&amp;iacute;sicos do monitor.&amp;nbsp;&lt;strong&gt;Personalize o layout de seu monitor&lt;/strong&gt; para multitarefas com a &amp;uacute;ltima vers&amp;atilde;o do LG Screen Split. &lt;strong&gt;Redimensione e exiba v&amp;aacute;rias janelas ao mesmo tempo&lt;/strong&gt;, com 14 op&amp;ccedil;&amp;otilde;es que incluem quatro escolhas diferentes de picture-in-picture (&lt;strong&gt;PIP&lt;/strong&gt;).&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;Compre no &lt;strong&gt;KaBuM!&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Asus TUF 27' IPS, 165 Hz, Full HD, 1ms, Adaptive Sync, HDMI/DisplayPort, Ajuste de Altura, Vesa, Som Integrado - VG279QR</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Monitor de jogos Full HD (1920 x 1080) de 27 polegadas com taxa de atualiza&amp;ccedil;&amp;atilde;o ultrarr&amp;aacute;pida de 165 Hz projetado para jogadores profissionais e jogabilidade envolvente. A tecnologia ASUS Extreme Low Motion Blur (ELMB ?) permite um tempo de resposta de 1 ms (MPRT), eliminando fantasmas para visuais n&amp;iacute;tidos de jogos. O Shadow Boost aprimora os detalhes da imagem em &amp;aacute;reas escuras, iluminando cenas sem expor demais as &amp;aacute;reas claras. Processamento compat&amp;iacute;vel com G-SYNC, proporcionando uma experi&amp;ecirc;ncia de jogo perfeita e sem problemas ao habilitar VRR (taxa de atualiza&amp;ccedil;&amp;atilde;o vari&amp;aacute;vel) por padr&amp;atilde;o. Apresenta um suporte ergonomicamente projetado para oferecer extensos ajustes de rota&amp;ccedil;&amp;atilde;o, inclina&amp;ccedil;&amp;atilde;o, rota&amp;ccedil;&amp;atilde;o e altura.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Concórdia C240 23.8, LED, HDMI, Full HD, Curvo, 75Hz, 2ms, Vermelho - 40511</t>
-  </si>
-  <si>
-    <t>Monitor Concórdia Gamer Curvo C240 23.8" Led Full HD HDMI VGA A tecnologia do novo C240 garante uma imersão total em seus jogos. Prepare-se para uma nova experiência com seus games! Agora você pode escolher ele em duas versões:todo preto ou preto com detalhe em vermelho.</t>
-  </si>
-  <si>
-    <t>Monitor Gamer LG Ultra Gear 23.8' IPS, 144 Hz, Full HD, 1ms, FreeSync, HDR 10, 99% sRGB, HDMI/DisplayPort, Ajuste de Ângulo - 24GN600-B</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;Monitor Gamer LG Ultra Gear 23.8 Full HD, 144Hz, 1ms, IPS, DMI, DisplayPort, 99% sRGB, Ajuste de &amp;Acirc;ngulo, FreeSync, HDR10, Preto&lt;/h2&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Inova&amp;ccedil;&amp;atilde;o sem fronteiras para jogos&lt;/h2&gt;
-&lt;p&gt;Complete seu setup Gamer com o monitor LG UltraGear premium. Desenvolvido para o Gamer, com os recursos mais avan&amp;ccedil;ados, aliados a ergonomia e &lt;strong&gt;design eletrizante&lt;/strong&gt;, entregando a experi&amp;ecirc;ncia imersiva! Seja o melhor com os melhores recursos feitos para apoiar sua vit&amp;oacute;ria, tempo de resposta de &lt;strong&gt;1ms Real&lt;/strong&gt; (GtG), em um painel com cores vislumbrantes IPS.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Jogabilidade fluida com frames instantaneos&lt;/h2&gt;
-&lt;p&gt;Os frames ultra-r&amp;aacute;pidos de 144Hz permite os jogadores a reagirem imediatamente aos seus advers&amp;aacute;rios e mudar a hist&amp;oacute;ria do jogo para a sua vit&amp;oacute;ria.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Aproveite os v&amp;iacute;deos e jogos HDR mais modernos&lt;/h2&gt;
-&lt;p&gt;O HDR10 melhora a qualidade da imagem com imers&amp;atilde;o visual mais din&amp;acirc;mica e cores aprimoradas do conte&amp;uacute;do HDR. &lt;strong&gt;HDR10&lt;/strong&gt; &amp;eacute; o padr&amp;atilde;o HDR digital baseado na gama de cores&lt;strong&gt; sRGB 99%&lt;/strong&gt;. Uma diferen&amp;ccedil;a real de cor e brilho.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Mais clara, suave e r&amp;aacute;pida&lt;/h2&gt;
-&lt;p&gt;Com a tecnologia &lt;strong&gt;FreeSync&lt;/strong&gt; os jogos t&amp;ecirc;m movimentos perfeitos e fluidos, balanceada com o processamento da placa de v&amp;iacute;deo, acabando com as imagens emba&amp;ccedil;adas e frames engasgados.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Design elegante&lt;/h2&gt;
-&lt;p&gt;Uma experi&amp;ecirc;ncia incr&amp;iacute;vel com imers&amp;atilde;o total. Design exuberante com&lt;strong&gt; bordas infinitas&lt;/strong&gt; (3-Side Bordeless) permitem uma imagem perfeita com incr&amp;iacute;vel imers&amp;atilde;o&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Aproveite essa oportunidade e adquira seu Monitor Gamer LG Ultra Gear no KaBuM!&lt;/h3&gt;</t>
+    <t>Monitor Gamer HQ Premium 25 Pol. Full HD, 1MS, 240Hz, IPS, AMD Freesync, HDMI, DP - Gp25i124</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;::: HQ Premium :::&lt;/b&gt;&lt;br /&gt;&lt;br /&gt;Revolucionário, assim é definido este monitor!&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Última geração:&lt;/b&gt; monitor de ponta, com uma vasta gama de tecnologias embarcadas. A melhor qualidade de imagem com um preço justo.&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Saia na frente: &lt;/b&gt;extraia o máximo de suas habilidades com uma tela pronta para qualquer tipo de desafio.&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Gamer de verdade: &lt;/b&gt;graças ao baixo tempo de resposta de 1ms, a alta taxa de atualização e a tecnologia amd freesync, jogue como um profissional!&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Longas jornadas: &lt;/b&gt;um grande diferencial: com as tecnologias flicker-free e low blue light, você pode encarar horas de jogatina sem cansar a vista.&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Alta resolução com alta definição: &lt;/b&gt;não basta apenas ser full hd. Você, merece mais! Viva momentos únicos com imagens de tirar o fôlego. Além de jogar em 1080p, você, perceberá, cada mínimo detalhe em qualquer tipo de cena. Saia na frente dos seus adversários, mesmo em situações de baixa luminosidade. Sinta-se dentro do jogo, a imersão é, total!&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Aproveitamento total: &lt;/b&gt;com a tela frameless, você, conta com bordas ultrafinas e aproveita todo o espaço da tela.&lt;br /&gt;&lt;br /&gt;&lt;b&gt;Sem reflexos: &lt;/b&gt;com a tela antireflexiva, você, pode embarcar nos seus desafios gamer em qualquer condição de luminosidade.</t>
   </si>
   <si>
     <t>Monitor Gamer Husky Snow 23.6 LED Full HD, Curvo, 165Hz, 1ms, HDMI e DisplayPort, Adaptive Sync, Ajuste de Ângulo - HGMT000</t>
@@ -1368,69 +880,99 @@
 &lt;p style="text-align: justify;"&gt;&lt;strong&gt;&lt;a href="https://kabum.com.br/hotsite/manuais/115383-Monitor-Gamer-Husky-Snow-HGMT000.pdf" target="_blank"&gt;MANUAL DE INSTRU&amp;Ccedil;&amp;Otilde;ES&lt;/a&gt;&lt;/strong&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>Monitor Gamer Acer 27 ZeroFrame Full HD, 165Hz, 0.5ms, IPS, HDMI e DisplayPort, FreeSync Premium, VESA, Preto - VG272 S</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;Monitor Gamer Acer 27 Full HD, 165Hz, 0.5ms, IPS, HDMI/DisplayPort, FreeSync Premium, VESA, Preto&lt;/h2&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;p&gt;Com tela de 27" FHD E2E (IPS) com resolu&amp;ccedil;&amp;atilde;o Full HD e uma taxa de atualiza&amp;ccedil;&amp;atilde;o no modo normal: 144Hz e modo de overclock 165Hz, com alta taxa de atualiza&amp;ccedil;&amp;atilde;o com 165Hz. Brilho 400 cd/m2 e um tempo de respostas baix&amp;iacute;ssimo de 2ms, ainda para aproveitar voc&amp;ecirc; poder&amp;aacute; desfrutar de uma conectividade HDMI (2.0), DisplayPort.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Bluecase 27 LED, 75 Hz, 2K QHD, 99%sRGB, HDMI/DisplayPort - BM2713GWCASE</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Explore um n&amp;iacute;vel superior de qualidade gr&amp;aacute;fica do seu gameplay com o monitor gamer Bluecase BM2713GW Esse monitor possui um painel TN ultrarr&amp;aacute;pido com frequ&amp;ecirc;ncia m&amp;aacute;xima de at&amp;eacute; 75 Hz e baix&amp;iacute;ssimo tempo de resposta de 5(cinco) milissegundos. Ideal para seus jogos AAA, o monitor conta com alta defini&amp;ccedil;&amp;atilde;o em resolu&amp;ccedil;&amp;atilde;o Quad HD (2560x1440) que proporciona uma imagem rica em detalhes. O monitor Bluecase BM2713GW &amp;eacute; compat&amp;iacute;vel com suportes VESA e tamb&amp;eacute;m conta com conex&amp;otilde;es DisplayPort e HDMI.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Acer Nitro 23.6 LED, Curvo, 165 Hz, Full HD, 1ms, FreeSync Premium, HDMI/DisplayPort - EI242QR</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;Monitor Gamer Acer Nitro 23.6 LED, Curvo, 165 Hz, Full HD, 1ms, FreeSync Premium, HDMI/DisplayPort&lt;/h2&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Tecnologia da Tela&lt;/h2&gt;
-&lt;p&gt;A Tela do Acer Nitro EI242QR possui campo de vis&amp;atilde;o de 23.6 Polegadas com um &lt;strong&gt;Resolu&amp;ccedil;&amp;atilde;o de 1920 x 1080 Full HD&lt;/strong&gt;, Painel VA de propor&amp;ccedil;&amp;atilde;o 16:9 com design &lt;strong&gt;curvo 1200R&lt;/strong&gt;, Taxa de atualiza&amp;ccedil;&amp;atilde;o de &lt;strong&gt;165Hz&lt;/strong&gt; (Utilizando Displayport), e Tempo de Resposta &lt;strong&gt;1ms&lt;/strong&gt; VRB (Visual Response Boost) para desempenhos profissionais nos seus gameplays.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;ZeroFrame&lt;/h2&gt;
-&lt;p&gt;Oferece um novo &lt;strong&gt;design de quadro zero&lt;/strong&gt;, remove virtualmente a caixa delimitadora da tela e oferece todas as imagens, prazer visual cont&amp;iacute;nuo.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Desing de tela curvo 1200 R&lt;/h2&gt;
-&lt;p&gt;Proporciona uma experi&amp;ecirc;ncia de visualiza&amp;ccedil;&amp;atilde;o uniforme e &lt;strong&gt;reduz o cansa&amp;ccedil;o visual&lt;/strong&gt; durante longos per&amp;iacute;odos de utiliza&amp;ccedil;&amp;atilde;o. Ele tamb&amp;eacute;m apresenta uma experi&amp;ecirc;ncia mais envolvente com um campo de vis&amp;atilde;o mais amplo e &amp;aacute;rea de vis&amp;atilde;o perif&amp;eacute;rica aumentada em compara&amp;ccedil;&amp;atilde;o com uma tela plana do mesmo&lt;/p&gt;
-&lt;p&gt;tamanho.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Tempo de resposta de 1ms&lt;/h2&gt;
-&lt;p&gt;O t&lt;strong&gt;empo de resposta r&amp;aacute;pido de 1 ms&lt;/strong&gt; melhora experi&amp;ecirc;ncia do jogador. N&amp;atilde;o importa a a&amp;ccedil;&amp;atilde;o em movimento r&amp;aacute;pido ou quaisquer transi&amp;ccedil;&amp;otilde;es dram&amp;aacute;ticas, tudo ser&amp;aacute; reproduzido suavemente, sem os efeitos irritantes de manchas ou fantasmas.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Taxa de atualiza&amp;ccedil;&amp;atilde;o de 165Hz&lt;/h2&gt;
-&lt;p&gt;Acelera os quadros por segundo para fornecer cenas de movimento ultra suaves. Com uma taxa de &lt;strong&gt;atualiza&amp;ccedil;&amp;atilde;o r&amp;aacute;pida de 165 Hz&lt;/strong&gt;, os monitores de jogos da Acer encurtam o tempo necess&amp;aacute;rio para a renderiza&amp;ccedil;&amp;atilde;o de quadros, diminuem o atraso de entrada e fornecem aos jogadores uma excelente experi&amp;ecirc;ncia no jogo.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Aproveite essa oportunidade e adquira seu Monitor Gamer Acer Nitro 23.6 no KaBuM!&lt;/h3&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Acer Nitro 23.8 LED Full HD, 165Hz, 1ms, HDMI/DisplayPort, FreeSync Premium, Preto - QG241Y</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;Monitor Gamer Acer Nitro 23.8 LED Full HD, 165Hz, 1ms, HDMI/DisplayPort, FreeSync Premium, Preto&lt;/h2&gt;
-&lt;p&gt;Com uma tela de&lt;strong&gt; 23,8&amp;rdquo; FHD&lt;/strong&gt;, o &lt;strong&gt;Nitro QG241Y&lt;/strong&gt; entrega imagens mais n&amp;iacute;tidas, levando sua experi&amp;ecirc;ncia visual e seu foco no jogo para um novo n&amp;iacute;vel.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;AMD FreeSync Premium&lt;/h2&gt;
-&lt;p&gt;Com o AMD FreeSync Premium, a taxa de quadros do jogo &amp;eacute; determinada pela sua placa de v&amp;iacute;deo, n&amp;atilde;o pela taxa de atualiza&amp;ccedil;&amp;atilde;o fixa do&amp;nbsp; monitor. Isso significa que os quadros do monitor s&amp;atilde;o sincronizados com os quadros da placa&amp;nbsp; gr&amp;aacute;fica, o que &lt;strong&gt;elimina a tela quebrada&lt;/strong&gt; e oferece &lt;strong&gt;experi&amp;ecirc;ncias de jogo muito suaves&lt;/strong&gt;.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Resolu&amp;ccedil;&amp;atilde;o FHD&lt;/h2&gt;
-&lt;p&gt;Traga os usu&amp;aacute;rios para um mundo colorido perfeito com &lt;strong&gt;FHD 1920 x 1080&lt;/strong&gt; e oferece a melhor qualidade original natural e n&amp;iacute;tida&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;1ms Visual Response Boost&lt;/h2&gt;
-&lt;p&gt;O &lt;strong&gt;Visual Response Boost (VRB)&lt;/strong&gt; de 1ms funciona desligando rapidamente a luz de fundo ou inserindo uma imagem em branco e preta entre os quadros, tamb&amp;eacute;m conhecida como &amp;ldquo;piscando&amp;rdquo;. Isso resulta em um &lt;strong&gt;desfoque menos percept&amp;iacute;vel&lt;/strong&gt; em imagens em movimento r&amp;aacute;pido porque os cristais l&amp;iacute;quidos n&amp;atilde;o precisam dobrar nos quadros &amp;agrave; medida que sobem e descem.&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h2&gt;Reduz a fadiga&lt;/h2&gt;
-&lt;p&gt;Fique na luta por horas com a tecnologia &lt;strong&gt;Flicker-less, Blue-light Filter.&lt;/strong&gt;&lt;/p&gt;
-&lt;p&gt;&amp;nbsp;&lt;/p&gt;
-&lt;h3&gt;Aproveite essa oportunidade e adquira seu Monitor Gamer Acer no KaBuM!&lt;/h3&gt;</t>
-  </si>
-  <si>
-    <t>Monitor Gamer Gigabyte 23.8 IPS, Full HD, 170Hz, 1ms, 120% sRGB, HDR, FreeSync Premium, Altura Ajustável - G24F-SA</t>
-  </si>
-  <si>
-    <t>JUNTE-SE À LUTA com o Monitor Gamer G24F da Gigabyte com 1ms de tempo de resposta, freesync premium, 165 Hz (170 Hz OC) e com uma taxa de cor de 8 bits, 90% DCI-P3 A ÚLTIMA MILHA PARA O SEU SISTEMA DE JOGO Como um jogador invisível, o monitor é frequentemente subestimado. A verdade é que os monitores se formam como um efeito sinérgico e trazem o melhor desempenho dos componentes do PC. Os monitores de jogos GIGABYTE oferecem as últimas especificações e qualidade, os usuários podem realmente desfrutar de um desempenho de alto nível sem a necessidade de extravagância. Tempo de resposta de 1 ms MPRT Tempo de resposta super rápido de 1 ms para a experiência de jogo mais suave de todos os tempos! FHD com 165 Hz (OC 170 Hz) Alta resolução e taxa de atualização rápida, proporcionando qualidade de exibição detalhada e experiência de jogo fluida! Cor de 8 bits, 90% DCI-P3 Fantástico visor a cores e 90% de cores DCI-P3 de gama super ampla. SIMPLES MAS ESTILOSO A aparência aerodinâmica representa a simplicidade da filosofia de design da série de jogos GIGABYTE, suporte robusto e acabamento fosco construído para características funcionais e estéticas adicionando mais características. OSD Sidekick GIGABYTE OSD Sidekick permite que você defina as opções de exibição com teclado e mouse, oferecendo a maneira mais fácil de ajustar as configurações do monitor. ÂNGULO DE VISÃO PERFEITO O monitor de jogos GIGABYTE possui um suporte exclusivo ergonomicamente projetado para oferecer uma ampla gama de ajustes de altura e inclinação.</t>
+    <t>Monitor Gamer Draxen 23.8'' resolução de 1920 x 1080 tempo de resposta de 1 MS 165HZ Full HD, Sem Borda</t>
+  </si>
+  <si>
+    <t>o monitor gamer draxen 165hz full hd é tudo o que você precisa para completar o seu setup. desenvolvido pensando no seu estilo de vida, oferecendo qualidade, desempenho e um design mais moderno do que nunca. a sua tela 23.8 lhe dará comodidade para estudar, trabalhar ou assistir sua série ou filme favoritos no seu tempo de lazer. além disso, sua alta resolução de 1920 x 1080 permite que você desfrute de momentos únicos graças a uma imagem nítida, cores realistas e contraste incrível. exibição de vídeo perfeita com tempo de resposta de 1 ms e mais de 16,7 milhões de cores que transformam as imagens em uma experiência muito fiel à realidade.&lt;br&gt;aprimore sua configuração com estilo. a furação padrão vesa 75x75 permite que você fixe o monitor em uma parede ou em um suporte.</t>
+  </si>
+  <si>
+    <t>Monitor Gamer KBM! GAMING MG330 31.5' Led, Curvo, 165 Hz, Full Hd, 1ms, Adaptive Sync, Hdmi/Displayport, Ajuste De Ângulo - KGMG33031PT</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Monitor Gamer KBM! GAMING MG330 31.5' LED, Curvo, 165 Hz, Full HD, 1ms, Adaptive Sync, HDMI/DisplayPort, Ajuste de&amp;nbsp; ngulo - KGMG330&lt;/h2&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Esteja um passo &amp;agrave; frente!&lt;/h2&gt;
+&lt;p&gt;O Monitor Gamer KBM! GAMING MG330 conta com resposta de &lt;strong&gt;1ms&lt;/strong&gt; e taxa de atualiza&amp;ccedil;&amp;atilde;o de &lt;strong&gt;165Hz&lt;/strong&gt;, permitindo a mais alta performance durante suas gameplays. Sua curvatura amplia o campo de vis&amp;atilde;o relativo, concentrando toda a a&amp;ccedil;&amp;atilde;o ao alcance dos olhos do usu&amp;aacute;rio, sem perder resolu&amp;ccedil;&amp;atilde;o.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Melhor Entrega de Imagens para sua Gameplay&lt;/h2&gt;
+&lt;p&gt;Compat&amp;iacute;vel com a tecnologia &lt;strong&gt;Adaptive Sync&lt;/strong&gt;, permite a sincroniza&amp;ccedil;&amp;atilde;o dos frames da placa de v&amp;iacute;deo, decretando o fim do input lag, bem como do tearing.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Conectividade&lt;/h2&gt;
+&lt;p&gt;O Monitor Gamer KBM! GAMING MG330 acompanha um cabo &lt;strong&gt;DisplayPort&lt;/strong&gt; que garante a melhor qualidade de imagem para seu jogo. Al&amp;eacute;m da conex&amp;atilde;o DP, o monitor ainda possui duas conex&amp;otilde;es &lt;strong&gt;HDMI&lt;/strong&gt; e uma conex&amp;atilde;o &lt;strong&gt;P2&lt;/strong&gt; para ouvir seu jogo diretamente do seu monitor.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Maior Ergonomia e Conforto para Uso Prolongado&lt;/h2&gt;
+&lt;p&gt;O Monitor Gamer KBM! GAMING MG330 possui ajuste de inclina&amp;ccedil;&amp;atilde;o &lt;strong&gt;de 5&amp;deg; a 15&amp;deg;&lt;/strong&gt; que se ajusta ergonomicamente para o seu uso. O monitor tamb&amp;eacute;m conta com &lt;strong&gt;Redu&amp;ccedil;&amp;atilde;o de Luz Azul&lt;/strong&gt;, se tornando uma &amp;oacute;tima op&amp;ccedil;&amp;atilde;o para Gameplays prolongadas.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Seu Monitor KBM! GAMING voc&amp;ecirc; encontra aqui no KaBuM!&lt;/h3&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Gigabyte 27 Full HD, 165Hz, 1ms, IPS, HDMI e DisplayPort, 130% sRGB, HDR, FreeSync, Altura Ajustável - G27F2BR</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Monitor Gamer Gigabyte 27 Full HD&lt;/h2&gt;
+&lt;h2&gt;&amp;nbsp;&lt;/h2&gt;
+&lt;h2&gt;A &amp;Uacute;ltima Milha para o seu Sistema de Jogo&lt;/h2&gt;
+&lt;p&gt;Como um jogador invis&amp;iacute;vel, o monitor costuma ser subestimado. A verdade &amp;eacute; que os monitores se formam como um efeito sin&amp;eacute;rgico e trazem o melhor desempenho dos componentes do PC. Os monitores de jogos GIGABYTE oferecem &lt;strong&gt;as especifica&amp;ccedil;&amp;otilde;es e qualidade mais recentes&lt;/strong&gt;, os usu&amp;aacute;rios podem realmente desfrutar de um &lt;strong&gt;desempenho de alto n&amp;iacute;vel&lt;/strong&gt; sem a necessidade de extravag&amp;acirc;ncia.&lt;/p&gt;
+&lt;p&gt;Suporta tecnologia&amp;nbsp;&lt;strong&gt;Adaptive-Sync&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Tempo de resposta MPRT de 1ms&lt;/h2&gt;
+&lt;p&gt;&lt;strong&gt;Tempo de resposta super r&amp;aacute;pido de 1ms&lt;/strong&gt;&amp;nbsp;para a experi&amp;ecirc;ncia de jogo mais suave de todos os tempos!&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;FHD com 165 Hz (OC 180 Hz)&lt;/h2&gt;
+&lt;p&gt;&lt;strong&gt;Alta resolu&amp;ccedil;&amp;atilde;o&lt;/strong&gt;&amp;nbsp;e taxa de atualiza&amp;ccedil;&amp;atilde;o r&amp;aacute;pida, oferecendo qualidade de exibi&amp;ccedil;&amp;atilde;o detalhada e experi&amp;ecirc;ncia de jogo fluida!&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;95% DCI-P3&lt;/h2&gt;
+&lt;p&gt;Fant&amp;aacute;stica&lt;strong&gt;&amp;nbsp;tela colorida e 130%&lt;/strong&gt;&amp;nbsp;DCI-P3 super ampla gama de cores.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Simples e Estiloso&lt;/h2&gt;
+&lt;p&gt;A&amp;nbsp;&lt;strong&gt;apar&amp;ecirc;ncia simplificada&lt;/strong&gt;&amp;nbsp;representa a simplicidade da filosofia de design da s&amp;eacute;rie de jogos GIGABYTE, &lt;strong&gt;suporte robusto e acabamento fosco&lt;/strong&gt; constru&amp;iacute;do para recursos funcionais e est&amp;eacute;ticos adicionando mais &amp;agrave;s caracter&amp;iacute;sticas.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;OSD Sidekick&lt;/h2&gt;
+&lt;p&gt;O GIGABYTE&amp;nbsp;&lt;strong&gt;OSD Sidekick&lt;/strong&gt;&amp;nbsp;permite que voc&amp;ecirc; defina as op&amp;ccedil;&amp;otilde;es de exibi&amp;ccedil;&amp;atilde;o com teclado e mouse, oferecendo a maneira mais &lt;strong&gt;f&amp;aacute;cil de ajustar&lt;/strong&gt; as configura&amp;ccedil;&amp;otilde;es do monitor.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Painel&lt;/h2&gt;
+&lt;p&gt;O painel revela suas&amp;nbsp;&lt;strong&gt;informa&amp;ccedil;&amp;otilde;es de hardware em tempo real&lt;/strong&gt;, incluindo&amp;nbsp;&lt;strong&gt;voltagens da CPU, velocidade do clock, temperaturas, etc.&lt;/strong&gt;&amp;nbsp;A melhor parte &amp;eacute; que n&amp;atilde;o ser&amp;aacute; bloqueado por nenhum jogo.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Equalizador Preto&lt;/h2&gt;
+&lt;p&gt;Esse recurso permite que voc&amp;ecirc; tenha mais&amp;nbsp;&lt;strong&gt;detalhes do lado escuro&lt;/strong&gt;&amp;nbsp;sem superexpor o lado claro ao mesmo tempo.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Atualiza&amp;ccedil;&amp;atilde;o autom&amp;aacute;tica&lt;/h2&gt;
+&lt;p&gt;Os usu&amp;aacute;rios podem &lt;strong&gt;desfrutar sem esfor&amp;ccedil;o da melhor experi&amp;ecirc;ncia de jogo&lt;/strong&gt; com recursos que a GIGABYTE continua a desenvolver e atualizar enquanto oferece&amp;nbsp;&lt;strong&gt;prote&amp;ccedil;&amp;atilde;o extra ao seu monitor&lt;/strong&gt;.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;&amp;Acirc;NGULO DE VIS&amp;Atilde;O PERFEITO&lt;/h2&gt;
+&lt;p&gt;O monitor Gaming GIGABYTE possui um suporte exclusivo projetado ergonomicamente para oferecer&amp;nbsp;&lt;strong&gt;ampla gama de ajustes de altura e inclina&amp;ccedil;&amp;atilde;o&lt;/strong&gt;.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Compre agora no KaBuM!&lt;/h3&gt;</t>
+  </si>
+  <si>
+    <t>Monitor 27" LED/IPS Acer Gamer Ultra Fino, 75Hz, 1Ms, HDMI + VGA - SA270</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Monitor Gamer Acer LCD 27 SA270 Bbix Full HD 75Hz 1ms IPS FreeSync HDMI Preto UM.HS0AA.B02&lt;/b&gt;&lt;br /&gt;&lt;br /&gt;NÃO PERCA NENHUM DETALHE DO SEU JOGO&lt;br /&gt;Veja tudo em alta definição com a resolução de 1920 x 1080 Full HD.&lt;br /&gt;E com as 27 da tela, seus jogos terão um campo de visão privilegiado.&lt;br /&gt;&lt;br /&gt;ENTRE NO UNIVERSO GAMER&lt;br /&gt;Garanta uma ótima performance de cor em seus jogos favoritos. O painel In Plane Switching (IPS) promove cores mais vibrantes e nítidas de qualquer ângulo, sem deixar rastros.&lt;br /&gt;&lt;br /&gt;ESTEJA PRONTO PARA JOGAR&lt;br /&gt;A taxa de atualização de 75Hz leva a renderização dos seus jogos a outro nível.&lt;br /&gt;E o tempo de resposta de 1ms acelera as transições e não trava durante a ação.</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Bluecase 23.6 Polegadas, Curvo, LED FULL HD, 180Hz, HDMI,VGA, Preto - Bm24ffd1gc</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;monitor gamer full hd curvo led 23,6" bluecase 180hz hdmi vga preto - bm24ffd1gc&lt;/b&gt;&lt;/p&gt;&lt;p&gt;&lt;br /&gt;o monitor gamer bm24ffd1gc possui um tamanho de 23,6", proporcionando uma resolu&amp;ccedil;&amp;atilde;o m&amp;aacute;xima de 1920x1080 pixels full hd. Sua taxa de atualiza&amp;ccedil;&amp;atilde;o m&amp;aacute;xima &amp;eacute; de 180 hz atrav&amp;eacute;s das conex&amp;otilde;es hdmi e dp, oferece imagens mais suaves e fluidas.&amp;nbsp;equipado com ilumina&amp;ccedil;&amp;atilde;o led, o monitor possui um brilho de 300 cd/m&amp;sup2; e um contraste t&amp;iacute;pico de 4.000:1, resultando em cores vibrantes e imagens detalhadas. O monitor gamer bm24ffd1gc &amp;eacute; uma &amp;oacute;tima escolha para jogos, trabalho e entretenimento, proporcionando uma experi&amp;ecirc;ncia visual envolvente e de alta qualidade.&lt;/p&gt;&lt;p&gt;&lt;br /&gt;&lt;b&gt;caracter&amp;iacute;sticas monitor gamer led full hd bluecase 23,6" 180hz - preto&lt;/b&gt;&lt;br /&gt;- marca: bluecase&lt;br /&gt;- modelo: bm24ffd1gcbx&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Bluecase 24 Polegadas Full HD,  144HZ, 1ms, HDMI e DisplayPort, FreeSync - BM242GW</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Full HD 144Hz de atualização para melhores gráficos. Com 1 conector DisplayPort e 1 conector HDMI. &lt;br /&gt;&lt;br /&gt;TAXA DE ATUALIZAÇÃO   &lt;br /&gt;Uma taxa de atualização de 144Hz deixa a sua tela sem nenhum borrão, serrilhado ou "ghosting". FLICKER-FREE   A função Flicker-Free regula o brilho para diminuir o cansaço dos olhos durante os jogos. &lt;br /&gt;&lt;br /&gt;APENAS 1MS TEMPO DE RESPOSTA (GTG)   &lt;br /&gt;Melhor desempenho e experiência de jogo nas ações de rápido movimento. &lt;br /&gt;&lt;br /&gt;TECNOLOGIA AMD FREESYNC   &lt;br /&gt;O AMD FREESYNC faz a sincronização entre a taxa de atualização de seu monitor e a taxa de quadros de sua placa de vídeo eliminando imagens quebradas.</t>
+  </si>
+  <si>
+    <t>Monitor Gamer HQ 27 Polegadas, FULL HD 144HZ A 240HZ 1MS HDMI Display Port, Curvo LED, Alto Falantes Iluminação RGB - Battle 27h240g</t>
+  </si>
+  <si>
+    <t>Monitor gamer hq battle&lt;br /&gt;&lt;br /&gt;A jogatina perfeita&lt;br /&gt;Com o monitor hq battle, os seus movimentos serão instantâneos e o seu tempo de reação ocorrerá em tempo real em qualquer tipo de jogo.&lt;br /&gt;Sem atrasos, você jogará com desempenho profissional.&lt;br /&gt;Graças a combinação de tempo de resposta ultrarápido + alta taxa de atualização, você sairá na frente dos seus oponentes:&lt;br /&gt;&lt;br /&gt;Tempo de resposta: 1ms&lt;br /&gt;Desempenho sem igual, imagens nítidas e sem espera. Enxergue toda a cena no milésimo de segundo em que ela acontece. Não desperdice nenhum movimento. O seu reflexo convertido em vitórias!&lt;br /&gt;&lt;br /&gt;Taxa de atualização: 240hz&lt;br /&gt;Nada de rastros nem imagens desfocadas. Tenha uma incrível vantagem sobre o seu adversário, principalmente em cenas rápidas. A altíssima taxa de atualização permitirá a você perceber cada sensível mudança no ambiente. E diferente dos demais modelos da linha battle, o 27h240g possui incríveis 240hz. É a garantia de uma experiência sublime.&lt;br /&gt;&lt;br /&gt;Amd freesync e nvidia g-sync&lt;br /&gt;E para completar o time, o monitor hq battle conta com as tecnologias amd freesync e nvidia g-sync. Incríveis ferramentas que impedem imagens serrilhadas e cortadas.&lt;br /&gt;Elas apresentam a tecnologia de sincronização adaptável, que reduz o travamento de tela, oscilação e atrasos.&lt;br /&gt;&lt;br /&gt;Enxergue no escuro&lt;br /&gt;Graças ao painel va utilizado nos monitores hq battle, você se dará bem em qualquer tipo de ambiente, mesmo em situações de baixa luminosidade.&lt;br /&gt;Encontre seus inimigos escondidos em qualquer lugar, mesmo os mais escuros.&lt;br /&gt;&lt;br /&gt;Mais sobre o painel va&lt;br /&gt;Quando falamos em tipo de painel para monitores gamer, existem três opções disponíveis no mercado.&lt;br /&gt;E por que a hq escolheu o tipo va para o monitor battle?&lt;br /&gt;A resposta é simples. Pois essa opção oferece a maior gama de vantagens para o jogador:&lt;br /&gt;1- ângulo de visão de 178x178 graus, enxergue bem em qualquer ângulo&lt;br /&gt;2- alto nível de contraste, imagens nítidas mesmo em cenas muito claras ou muito escuras&lt;br /&gt;3- tempo de resposta real de 1ms mprt&lt;br /&gt;4- cores vivas e nítidas&lt;br /&gt;5- permite as mais altas taxas de atualização&lt;br /&gt;&lt;br /&gt;Design único&lt;br /&gt;Além de todos os recursos apresentados, ainda temos o fato do monitor hq battle ter um visual sensacional.&lt;br /&gt;Desenvolvido com uma tela curva, isso já seria o bastante para deixar o seu setup gamer ainda mais moderno. Mas além disso, ele ainda possui a tecnologia ´´frameless´´, sem bordas, que garantirão a você uma imersão total. Aproveite 100% da tela.&lt;br /&gt;&lt;br /&gt;Conectividade e recursos&lt;br /&gt;Para garantir uma experiência perfeita, equipamos o battle com tudo o que você precisa.&lt;br /&gt;Dupla saída de vídeo hdmi e display port, além de uma conexão usb.&lt;br /&gt;E para deixar tudo ainda melhor, ele vem acompanhado com dois alto falantes surround e iluminação em rgb.</t>
+  </si>
+  <si>
+    <t>USADO: Monitor Gamer LG, Tela 29 Polegadas, 75Hz, 1ms, Dynamic Action Sync, AMD FreeSync - 29UM69G-B.AWZM - Bronze Recer</t>
+  </si>
+  <si>
+    <t>Monitor Gamer LG 29UM69G-B.AWZM, com tela de 29? polegadas com resolução Full HD (2560 x 1080), uma taxa de atualização de 75Hz, e um tempo de resposta de 1ms com tecnologia que todo gamer precisa como Dynamic action Sync e AMD FreeSync&lt;br /&gt;&lt;br /&gt;ATENÇÃO: este produto é RECERTIFICADO.&lt;br /&gt;Os eletrônicos são originais e acompanham Nota Fiscal. Os produtos passam por uma avaliação de qualidade rigorosa, que certifica as condições técnicas e estéticas do aparelho, categorizadas de acordo com os selos ouro, prata ou bronze. Você ainda conta com garantia de três meses contra problemas e pode fazer a devolução do produto em até sete dias.&lt;br /&gt;SAIBA O QUE É UM PRODUTO RECERTIFICADO (BRONZE)&lt;br /&gt;O produto recertificado em condições de fábrica é um produto que volta para o mercado, disponível para vendas, nas mesmas condições de um produto novo, com todas as funcionalidades e características originais, beneficiando o comprador e possibilitando economizar dinheiro na compra.&lt;br /&gt;O produto recertificado em condições de fábrica passa por um processo rigoroso de análise, onde todas as funcionalidades são testadas e após constatação de 100% de funcionamento o produto é liberado como recertificado.&lt;br /&gt;Depois de atingir 100% da certificação técnica de operação em suas funcionalidades, os produtos do Saldão da Informática são classificados em 3 certificações, de acordo com seu estado estético e superficial, sendo assim classificados como: Ouro, Prata e Bronze.&lt;br /&gt;Esse produto é recertificado Bronze: Produto têm alguns riscos. Estes riscos não alteram ao perfeito funcionamento do equipamento.</t>
   </si>
   <si>
     <t>Monitor Gamer Gigabyte 24 Full HD, 165Hz, 1ms, IPS, HDMI e DisplayPort, 125% sRGB, HDR, FreeSync, Altura Ajustável - G24F2BR</t>
@@ -1470,6 +1012,485 @@
 &lt;p&gt;O monitor Gaming GIGABYTE possui um suporte exclusivo projetado ergonomicamente para oferecer &lt;strong&gt;ampla gama de ajustes de altura e inclina&amp;ccedil;&amp;atilde;o&lt;/strong&gt;.&lt;/p&gt;
 &lt;p&gt;&amp;nbsp;&lt;/p&gt;
 &lt;h3&gt;Compre agora no KaBuM!&lt;/h3&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Duex 24´ Full HD (1920x1080), 144Hz, Preto - Dx 240zg</t>
+  </si>
+  <si>
+    <t>Marca: duex&lt;br /&gt;modelo: dx 240zg &lt;br /&gt;&lt;br /&gt;especificações: &lt;br /&gt;&lt;br /&gt;tamanho da tela: 24" &lt;br /&gt;área de display: 527.4 (h) x 296.4 (v) &lt;br /&gt;resolução: 1920x1080 (144hz) &lt;br /&gt;pixel pitch: 0.27mm &lt;br /&gt;ângulo de visão: h:178 / v:178 &lt;br /&gt;brilho: 250cd/m² &lt;br /&gt;tempo de resposta: 1ms &lt;br /&gt;número de cores: 16.7m &lt;br /&gt;&lt;br /&gt;conectores: &lt;br /&gt;1x hdmi &lt;br /&gt;1x displayport &lt;br /&gt;1x usb &lt;br /&gt;1x saída de áudio &lt;br /&gt;&lt;br /&gt;conteúdo da caixa: &lt;br /&gt;monitor &lt;br /&gt;base &lt;br /&gt;cabo hdmi &lt;br /&gt;cabo displayport &lt;br /&gt;fonte de energia &lt;br /&gt;guia do usuário&lt;br /&gt;&lt;br /&gt;garantia: 365 dias</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Curvo Duex Dx 270zg, 27 Polegadas, FULL HD (1920x1080), 240hz, Preto</t>
+  </si>
+  <si>
+    <t>Marca: duex&lt;br /&gt;modelo: dx 270zg &lt;br /&gt;&lt;br /&gt;especificações: &lt;br /&gt;&lt;br /&gt;tamanho da tela: 27" &lt;br /&gt;área de display: 527.4 (h) x 296.4 (v) &lt;br /&gt;resolução: 1920x1080 (240hz) &lt;br /&gt;pixel pitch: 0.27mm &lt;br /&gt;ângulo de visão: h:178 / v:178 &lt;br /&gt;brilho: 250cd/m² &lt;br /&gt;tempo de resposta: 1ms &lt;br /&gt;número de cores: 16.7m &lt;br /&gt;&lt;br /&gt;conectores: &lt;br /&gt;2x hdmi &lt;br /&gt;1x displayport &lt;br /&gt;1x usb &lt;br /&gt;1x áudio &lt;br /&gt;&lt;br /&gt;conteúdo da caixa: &lt;br /&gt;monitor &lt;br /&gt;base&lt;br /&gt;cabo hdmi&lt;br /&gt;fonte de energia&lt;br /&gt;&lt;br /&gt;garantia: 365 dias</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Redragon Amber, Tela de 27 Polegadas FHD, 165HZ, Curvo, LED, HDMI, Preto - GM27H10C</t>
+  </si>
+  <si>
+    <t>Características:&lt;br /&gt; - marca: redragon&lt;br /&gt; - modelo: gm27h10c&lt;br /&gt; especificações:&lt;br /&gt; - cor: preto&lt;br /&gt; - tamanho: 27”&lt;br /&gt; - resolução: 1920 x 1080 16:9&lt;br /&gt; - tipo de painel: va&lt;br /&gt; - taxa de atualização: 165 hz&lt;br /&gt; - número de cores: 16.7 m&lt;br /&gt; - brilho máximo: 250cd/m2 (typical)&lt;br /&gt; - taxa de contraste: 3000:1&lt;br /&gt; - conectividade: dp x1, hdmi x2, dc in x1&lt;br /&gt; - power range: 100-240v 50/60hz&lt;br /&gt; - tempo de resposta: 1ms&lt;br /&gt; - peso bruto(g): 5960g&lt;br /&gt; - peso liquido(g): 4830g&lt;br /&gt; conteúdo da embalagem:&lt;br /&gt; - monitor gamer redragon</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Bluecase 27" 2.5K, 75Hz, HDMI / Displayport, Vesa - BM2713GW</t>
+  </si>
+  <si>
+    <t>Explore um nível superior de qualidade gráfica do seu gameplay com o monitor gamer Bluecase - BM2713GW   &lt;br /&gt;&lt;br /&gt;Esse monitor possui um painel TN ultrarrápido com frequência máxima de até 75 Hz e baixíssimo tempo de resposta de 5(cinco) milissegundos.    &lt;br /&gt;Ideal para seus jogos AAA, o monitor conta com alta definição em resolução Quad HD (2560x1440) que proporciona uma imagem rica em detalhes.    &lt;br /&gt;O monitor Bluecase BM2713GW é compatível com suportes VESA e também conta com conexões DisplayPort e HDMI.</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Samsung 27Pol, Full HD, 75Hz, IPS, HDMI, Vesa, Freesync - Lf27t350fhlmzd</t>
+  </si>
+  <si>
+    <t>Para compor a sua mesa e computador, precisa de um monitor de linha, não acha? Com o Monitor Gamer T350 Samsung você terá uma ótima visualização de tudo que fizer! Com a tela IPS, LED, em formato plano e de 27'' na horizontal, resolução Full HD 1920x1080. Possui conexões HDMI e VGA e tecnologia FreeSync da AMD, assim você pode assistir filmes e jogar tranquilamente sem interrupções na sua imagem. Além disso, possui o Game Mode, que ajusta qualquer jogo para preencher sua tela visualizando todos os detalhes, sendo possível detectar inimigos escondidos nas sombras através do contraste ideal, mais nitidez e cenas com cores mais vivas. Agora, a imagem é reproduzida sem falhas. A taxa de atualização de 75Hz oferece cenas mais fluidas. Seu momento de diversão não tem lag ou efeito fantasma, quer você esteja assistindo a um vídeo ou jogando um jogo. Vai deixar essa beleza passar? Garanta já seu Monitor Gamer T350 Samsung e aproveite com a melhor imagem!</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Curvo HQ 24 LED Full HD, 165 Hz, 1ms, HDMI, DisplayPort, FreeSync, Som Integrado, Preto - 24GHQ-Black</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Monitor Gamer Curvo HQ 24 LED Full HD, 165 Hz, 1ms, HDMI, DisplayPort, FreeSync, Som Integrado, Preto&lt;/h2&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Tela Curva&lt;/h2&gt;
+&lt;p&gt;A curvatura da tela de R3000 oferece imers&amp;atilde;o total, voc&amp;ecirc; ser&amp;aacute; capaz de apreciar imagens panor&amp;acirc;micas grandes, em alta resolu&amp;ccedil;&amp;atilde;o e com todas as especifica&amp;ccedil;&amp;otilde;es que um monitor Gamer de ponta exige.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Baixo tempo de Resposta&lt;/h2&gt;
+&lt;p&gt;A HQ levou a s&amp;eacute;rio o desenvolvimento desta linha, trazendo ao p&amp;uacute;blico mais exigente um produto completo e de alto n&amp;iacute;vel. N&amp;atilde;o fique atras, reaja em tempo real e tenha os movimentos do teclado refletidos sem atrasos com o tempo de resposta de 1ms.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Atualiza&amp;ccedil;&amp;atilde;o de 165Hz&lt;/h2&gt;
+&lt;p&gt;Sem borr&amp;otilde;es e sem perda de imagem. A INCR&amp;Iacute;VEL taxa de atualiza&amp;ccedil;&amp;atilde;o de 165hz garante que voc&amp;ecirc; tenha uma experi&amp;ecirc;ncia acima dos seus advers&amp;aacute;rios.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Imagens em alta resolu&amp;ccedil;&amp;atilde;o + Visual incr&amp;iacute;vel&lt;/h2&gt;
+&lt;p&gt;A tela Full HD de alta resolu&amp;ccedil;&amp;atilde;o aliada ao design futurista e moderno do monitor garantem n&amp;atilde;o s&amp;oacute; imagens perfeitas como um visual incr&amp;iacute;vel de todo o seu conjunto.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Aproveite essa oportunidade e adquira seu Monitor Gamer Curvo no KaBuM!&lt;/h3&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Redragon, 23Pol, Full HD, 144Hz, 1MS, IPS, HDMI, DP, VGA, Freesync - M2444ph</t>
+  </si>
+  <si>
+    <t>O monitor Redragon Sapphire apresenta um design ultrafino, alinhado com o que há de mais moderno no mercado. Gamers de jogos competitivos podem obter vantagem sobre seus adversários ao utilizar uma tela com a alta taxa de atualização de 144 Hz. A tecnologia AMD FreeSync põe fim à jogabilidade travada e ao corte dos quadros com um desempenho fluido e livre de artefatos com praticamente qualquer taxa de quadros. Contemple a próxima inovação na experiência de jogos para PC e console. O Redragon Sapphire possui um visual moderno e elegante, que combina com qualquer setup, pela sua simplicidade e minimalismo.&lt;br /&gt;&lt;br /&gt;- Alta taxa de atualização até 144Hz auxiliando na fluidez da gameplay.&lt;br /&gt;- Design elegante e minimalista para se integrar a qualquer setup.&lt;br /&gt;- Painel do tipo IPS para maior fidelidade de cores.&lt;br /&gt;- Tecnologia Freesync integrada para eliminar as quebras de imagem.&lt;br /&gt;- Diversas opções de conexões de vídeo para maior praticidade e versatilidade.&lt;br /&gt;&lt;br /&gt;O monitor tem tela de 24 polegadas, um ótimo tamanho para o consumo de jogos e filmes, assim como navegar na internet e trabalhar.</t>
+  </si>
+  <si>
+    <t>Monitor Gamer LG LED 23.8 Polegadas FHD, 60Hz, 5Ms, IPS, VGA/HDMI/DP, Pivot - 24BL550J</t>
+  </si>
+  <si>
+    <t>Monitor Gamer LG LED 23.8 FHD IPS 60Hz 5ms VGA HDMI DP Pivot - 24BL550J CONTE COM SUA MELHOR EXIBIÇÃO A qualidade de imagem do LG 24BL550J é a melhor possível para um monitor Full HD, já que usa a elogiada tela IPS. Suas cores são vibrantes e nítidas, sem qualquer problema em replicar as cores reais em software e jogos. Sua tela de 23.9 faz com que ele esteja no tamanho ideal para a resolução Full HD (1920x1080p), apresentando ótimo nível de densidade de pixel (PPI 0,27 mm). Com isso, você não terá a impressão de imagem borrada ou com serrilhados, principalmente em jogos, vídeos e fotos. FLUIDEZ Tem baixo input lag e tempo de resposta de 5ms, suficiente para eliminar rastros. A taxa de atualização de 75hz da boa fluência aos jogos, ajudando ainda no conforto ocular. MELHOR RESOLUÇÃO Sua incrível tela em Full HD com tecnologia IPS e seu tratamento anti reflexivo conta com a exibição de imagens excepcionais cores mais realistas de qualquer ângulo, sem a interferência de qualquer luz. MODELO PIVOTANTE Permite ajuste de altura, inclinação, rotação e pivô. Esse monitor apresenta um design moderno, com bordas mais finas e base retangular com ótima estabilidade. Porém, seu grande trunfo é o ajuste de altura e giro em 90º (pivô), o que o torna ideal para trabalhar com o monitor na vertical (em pé)..</t>
+  </si>
+  <si>
+    <t>Monitor Goldentec Gamer 27'' Led Full Hd, 75hz, 1ms</t>
+  </si>
+  <si>
+    <t>Monitor gamer 27´´ led full hd 75hz 1ms especificações técnicas  marcagoldentec  ean7899555687261  tamanho de tela27´´  framelesssim  resolução1920x1080 (full hd)  tempo de resposta1 ms  frequência75 hz  brilho250 cd/m²  contraste100 milhões: 1  ângulo de visão180° (h) 180° (v)  cores16,7 milhões  inclinação ajustável 20°  tecnologia freesyncelimina falhas e intermitências  tecnologia lowbluelightreduz a luz azul para mais conforto e segurança  100% flicker freesuaviza a ondulação do monitor  conexõeshdmi  conteúdo da embalagem1x monitor gamer 27´´ led full hd 75hz 1ms &lt;br&gt;cabos e fonte &lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;marca :&lt;/strong&gt; goldentec&lt;br&gt;&lt;strong&gt;tipo de uso :&lt;/strong&gt; gamer&lt;br&gt;&lt;strong&gt;tamanho da tela :&lt;/strong&gt; 27´´&lt;br&gt;&lt;strong&gt;tipo de tela :&lt;/strong&gt; led&lt;br&gt;&lt;strong&gt;resolução :&lt;/strong&gt; full hd&lt;br&gt;&lt;strong&gt;design de tela :&lt;/strong&gt; tela plana&lt;br&gt;&lt;strong&gt;tempo de resposta :&lt;/strong&gt; 1 ms&lt;br&gt;&lt;strong&gt;taxa de atualização :&lt;/strong&gt; 75 hz&lt;br&gt;&lt;strong&gt;estrutura :&lt;/strong&gt; padrão&lt;br&gt;&lt;strong&gt;voltagem :&lt;/strong&gt; bivolt&lt;br&gt;&lt;strong&gt;polegadas :&lt;/strong&gt; 27 ´´&lt;br&gt;&lt;br&gt;&lt;strong&gt;garantia : &lt;/strong&gt;12</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Redragon Azur, 23.8 Polegadas, 165hz, LED, FHD, HDMI - Gm24x5ips</t>
+  </si>
+  <si>
+    <t>Características:&lt;br /&gt; - marca: redragon&lt;br /&gt; - modelo: gm24x5ips&lt;br /&gt; especificações:&lt;br /&gt; - cor: preto&lt;br /&gt; - alta taxa de atualização até 165hz auxiliando na fluidez da gameplay.&lt;br /&gt; - design elegante e minimalista para se integrar a qualquer setup.&lt;br /&gt; - tecnologia freesync integrada para eliminar as quebras de imagem.&lt;br /&gt; - diversas opções de conexões de vídeo para maior praticidade e versatilidade.&lt;br /&gt; - tamanho: 23,8”&lt;br /&gt; - resolução: 1920 x 1080&lt;br /&gt; - tipo de painel: ips&lt;br /&gt; - taxa de atualização: 165 hz&lt;br /&gt; - número de cores: 16.7 m&lt;br /&gt; - brilho máximo: 250cd/m2 (typical)&lt;br /&gt; - taxa de contraste: 1000:1&lt;br /&gt; - conectividade: hdmi 1.4 x 2, dp 1.2  x1, dc x 1, 1x 3.5mm áudio.&lt;br /&gt; - power range: 100-240v 50/60hz&lt;br /&gt; - peso bruto(g): 4728&lt;br /&gt; - peso líquido(g): 3520&lt;br /&gt; conteúdo da embalagem:&lt;br /&gt; - monitor gamer redragon</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Curvo Bright 27p, Full HD, 165Hz, 1Ms, HDMI/VGA, Preto</t>
+  </si>
+  <si>
+    <t>Monitor gamer curvo 27" polegadas 165hz full hd lcd/led preto mt007 bright&lt;br /&gt;  &lt;br /&gt; mergulhe no mundo dos games com estilo e velocidade!&lt;br /&gt;  &lt;br /&gt; ei, camarada gamer, já sentiu como se estivesse preso no passado com um monitor lento e sem graça? Deixe-me apresentar uma passagem direta para o futuro dos jogos: o monitor gamer curvo 27 polegadas 165 hz dp hdmi usb preto bright. Prepare-se para uma experiência visual de tirar o fôlego!&lt;br /&gt;  &lt;br /&gt; este monitor é como uma viagem ao paraíso dos gamers. Com suas 27 polegadas de tela imersiva e curva, ele envolve você em um abraço eletrizante de jogabilidade. E a taxa de atualização de 165 hz? É praticamente uma máquina do tempo para o futuro dos jogos!&lt;br /&gt;  &lt;br /&gt; e como se isso não fosse suficiente, este monitor oferece conectividade versátil com dp, hdmi e usb. Você pode se conectar facilmente aos seus dispositivos e mergulhar diretamente na ação. Sem complicações, apenas jogos de alta qualidade.&lt;br /&gt;  &lt;br /&gt; mas aqui está a cereja no topo do bolo: a resolução deslumbrante e as cores vibrantes. Este monitor faz com que cada detalhe dos seus jogos ganhe vida. Adeus a imagens borradas e cores apagadas. Prepare-se para gráficos que vão explodir sua mente!&lt;br /&gt;  &lt;br /&gt; ao comprar este monitor gamer curvo, você não está apenas adquirindo um pedaço de tecnologia. Você está se dando o presente de uma experiência de jogo que vai te levar a novos patamares de diversão e desempenho. É a sua passagem para o futuro dos jogos - uma jornada sem volta para a vitória!&lt;br /&gt;  &lt;br /&gt; então, o que você está esperando? Pegue seu ingresso para o futuro e adquira o monitor gamer curvo 27 polegadas 165 hz dp hdmi usb preto bright hoje. Jogue com estilo, velocidade e vitória garantida! Sua jornada começa agora!&lt;br /&gt;  &lt;br /&gt; especificações:&lt;br /&gt; dimensões(axlxp): 615 x 453 x 79 mm &lt;br /&gt; peso: 3,9&lt;br /&gt; área de visualização 683 × 128 × 445(mm2)&lt;br /&gt; ângulo de visão h:178°v:178°&lt;br /&gt; resolução(tip.) 1920x1080 60hz&lt;br /&gt; cores 16,7m&lt;br /&gt; brilho (tip.) 250cd/m2&lt;br /&gt; tela curva: 2800r&lt;br /&gt; frequência de resposta: 165 hz&lt;br /&gt; relação de contraste (tip.) 1000:1&lt;br /&gt; conector dp + hdmi + usb&lt;br /&gt;  &lt;br /&gt; conteúdo da embalagem: &lt;br /&gt; 01 monitor bright &lt;br /&gt; 01 cabo hdmi&lt;br /&gt; 01 manual&lt;br /&gt;  &lt;br /&gt; modelo:&lt;br /&gt; mt007&lt;br /&gt;  &lt;br /&gt; marca:&lt;br /&gt; bright&lt;br /&gt;  &lt;br /&gt; garantia 1 ano bright</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Cooler Master 23.8 Pol. Full HD (1920x1080), 0.5MS, 144Hz, IPS, HDMI, Hdr10, Vesa - Gm238-Ffs</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;b&gt;monitor gamer gm238-ffs cooler master full hd hdmi 1920x1080 vesa 144hz 23,8"&lt;/b&gt;&lt;/p&gt;&lt;p&gt;&lt;br /&gt;o monitor gamer gm238-ffs possui tela full hd de 144 hz e 23,8" combinada com uma ampla gama de cores dci-p3 de 90% oferece versatilidade not&amp;aacute;vel. Com recursos essenciais para jogos e produtividade, permite uma experi&amp;ecirc;ncia de jogo suave ou foco no trabalho diurno. A densidade de pixels de 92,6 por polegada (ppi) em um monitor de 23,8 polegadas e resolu&amp;ccedil;&amp;atilde;o full hd, o gm238-ffs equilibra de forma excelente a fidelidade visual e o desempenho. O monitor gamer fornece um display fhd de 23,8" com um painel ultraspeed ips de 144 hz, com recursos como dynamic overdrive, adaptive sync e uma cobertura dci-p3 de 90%, atende a todas as suas necessidades. &amp;eacute; ideal tanto para jogos quanto para produtividade, tornando-o uma adi&amp;ccedil;&amp;atilde;o valiosa &amp;agrave; sua configura&amp;ccedil;&amp;atilde;o de trabalho e entretenimento.&lt;/p&gt;&lt;p&gt;&lt;br /&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer KBM! GAMING MG700 27' Led Full Hd, 240hz, 1ms, Hdmi E Displayport, 96% Srgb, Adaptive Sync, Ajuste De Altura - KGMG70027PT</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Monitor Gamer KBM! GAMING MG700: Imers&amp;atilde;o e desempenho para seus jogos&lt;/h2&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;O Monitor Gamer KBM! GAMING MG700 &amp;eacute; a escolha perfeita para quem busca imers&amp;atilde;o e desempenho nos jogos. Com &lt;strong&gt;tela curva de 27 polegadas&lt;/strong&gt;, resolu&amp;ccedil;&amp;atilde;o &lt;strong&gt;Full HD&lt;/strong&gt; e taxa de atualiza&amp;ccedil;&amp;atilde;o de &lt;strong&gt;240 Hz,&lt;/strong&gt; o MG700 oferece uma experi&amp;ecirc;ncia visual incr&amp;iacute;vel.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;O tempo de resposta de &lt;strong&gt;1 ms&lt;/strong&gt; garante que voc&amp;ecirc; n&amp;atilde;o perca nenhum detalhe da a&amp;ccedil;&amp;atilde;o, mesmo nos jogos mais r&amp;aacute;pidos. Al&amp;eacute;m disso, o recurso &lt;strong&gt;AdaptiveSync&lt;/strong&gt; elimina o tearing e o stuttering, garantindo uma imagem suave e fluida.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;Para proteger a sua vis&amp;atilde;o, o MG700 conta com &lt;strong&gt;redu&amp;ccedil;&amp;atilde;o de luz azul&lt;/strong&gt; e &lt;strong&gt;Modo Game Plus&lt;/strong&gt;, que reduzem o cansa&amp;ccedil;o visual. O som integrado &amp;eacute; de alta qualidade, mas voc&amp;ecirc; tamb&amp;eacute;m pode conectar o seu headset atrav&amp;eacute;s das portas plug and play.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;Com o Monitor Gamer KBM! GAMING MG700, voc&amp;ecirc; ter&amp;aacute; tudo o que precisa para jogar seus games favoritos com o m&amp;aacute;ximo de desempenho e imers&amp;atilde;o.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;O Monitor Gamer KBM! GAMING MG700 &amp;eacute; a escolha perfeita para quem busca um monitor gamer de alta qualidade. Com recursos avan&amp;ccedil;ados e uma excelente rela&amp;ccedil;&amp;atilde;o custo-benef&amp;iacute;cio, o MG700 &amp;eacute; a garantia de uma experi&amp;ecirc;ncia de jogo inesquec&amp;iacute;vel.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>USADO: Monitor Gamer 24 Polegadas Acer Nitro, 165Hz, 0.5ms, Freesync, HDMI, DisplayPort, Preto, Recertificado Prata - VG252Q</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Acer Nitro Vg252q, na cor preta com detalhes em vermelho, tela de 24 polegadas, taxa de atualização de 165hz, tempo de resposta de 0.5ms, amd freesync premium, 1 entrada hdmi e 1 entrada display port&lt;br /&gt;&lt;br /&gt;Atenção: este produto é recertificado.&lt;br /&gt;Os eletrônicos são originais e acompanham nota fiscal. Os produtos passam por uma avaliação de qualidade rigorosa, que certifica as condições técnicas e estéticas do aparelho, categorizadas de acordo com os selos ouro, prata ou bronze. Você ainda conta com garantia de três meses contra problemas e pode fazer a devolução do produto em até sete dias.</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Primetek, 27 Polegadas, 180hz Ips Qhd HDMI/dp</t>
+  </si>
+  <si>
+    <t>Caracteristicas: - marca: primetek - modelo: 27a2r  especificações técnicas: - tamanho do painel (diagonal) 27 - tipo de painel ips rápido - plana/ curva plana proporção 16:9 resolução 2560x1440 - tipo de moldura moldura sem moldura 3 - distância do pixel (h)*(v) (mm) 0,2331 (h) × 0,2331(v - brilho (cd/m2 )(tipo.) 250(min) 300(tipo) brilho (nits)(máx.)? 250(min) 300(tipo) - ângulo de visão (h/v) 178°(h)/178°(v) - profundidade de bits do painel verdadeiro 8 bits - cores da tela 16,7m - tempo de resposta do painel sem od 5ms tempo de resposta 1ms - taxa de atualização (máx.) 180 hz - hdmi 2.0 2 (máx. 144 hz) dp 1.4 2 (máx. 180 hz) saída de áudio 1 - design de suporte de exibição has inclinação (ângulo) 5°±2°,20°±2° giro (ângulo) 20°±2° - pivô (ângulo/direção) pviot: 90° ajuste de altura 120±5mm montagem vesa 75*75mm tecla do botão liga/desliga roker - tecla do botão osd roker contracapa design rgb - consumo de energia 48w modo de economia de energia ?0,5w modo de desligamento desligado &amp;lt,0,3 w tipo de energia adaptador de energia fonte de alimentação dc 12v, 4a - acessorios: cabo de alimentação (1,5m) 1,5m cabo dp versão 1.2 quantidade de cabo dp (1,5 m/1,8 m) 1,5 m - temperatura da cor (fria, quente, usuário) controle de luz azul baixa modo de cena dcr idiomas (23 idiomas) ajuste da luz de fundo sem oscilações freesync over drive fps/rts jogo mais modo de controle do efeito de iluminação (nenhum/mistura de cores rgb/seleção colorida) laranja - dimensão com suporte (l*a*p)(mm) 619x269,2x554,6 mm - dimensão sem suporte (lxaxp)(mm) 619x63,7x365,5 mm - dimensão da caixa (lxaxp)(mm) 715x213x471mm - peso líquido (kg) 6,3kg - peso bruto (kg) 8,3kg - garantia 1 ano &lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;tamanho da tela:&lt;/strong&gt; 27&lt;br&gt;&lt;strong&gt;marca:&lt;/strong&gt; primetek&lt;br&gt;&lt;strong&gt;modelo:&lt;/strong&gt; 27a2r</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Redragon Mirror, Tela de 27 Polegadas FHD, 165HZ, LED, HDMI - GM27X5IPS</t>
+  </si>
+  <si>
+    <t>Características:&lt;br /&gt; - marca: redragon&lt;br /&gt; - modelo: gm27x5ips&lt;br /&gt; especificações:&lt;br /&gt; - cor: preto&lt;br /&gt; - tamanho: 27”&lt;br /&gt; - resolução: 1920 x 1080 16:9&lt;br /&gt; - tipo de painel: ips&lt;br /&gt; - taxa de atualização: 165 hz&lt;br /&gt; - número de cores: 16.7 m&lt;br /&gt; - brilho máximo: 250cd/m2 (typical)&lt;br /&gt; - taxa de contraste: 1000:1&lt;br /&gt; - conectividade: dp 1.2 x1, hdmi 1.4 x2, dc in x1&lt;br /&gt; - power range: 100-240v 50/60hz&lt;br /&gt; - tempo de resposta: 1ms&lt;br /&gt; - peso bruto(g): 5900g&lt;br /&gt; - peso liquido(g): 4200g&lt;br /&gt; conteúdo da embalagem:&lt;br /&gt; - monitor gamer redragon</t>
+  </si>
+  <si>
+    <t>Monitor Gamer 27 Polegadas, 240hz Curvo FULL HD, HDMI/dp</t>
+  </si>
+  <si>
+    <t>Caracteristicas:  - marca: primetek  - modelo: 27c1h  se você está procurando um monitor para jogos, nossas ofertas primetek te oferece uma ótima opção de modelo e um bom preço. Monitor gamer 27curvo 240hz dp/hdmi fhd primetek 27c1h que entrega imagens mais nítidas, levando sua experiência visual e seu foco no jogo para um novo nível.  especificações técnicas:  - tamanho 27´´ painel tipo va  - fonte do painel csot curva plana/ curva  - suporte hdr n resolução 1920 x 1080  - tipo de moldura moldura sem moldura 3 área de visualização da tela (a*v) (mm) 597,888 (a) x 336,312 (v) tipo de luz de fundo do painel e-led  - distância do pixel (a)(v) (mm) 0,1038(a) x 0,3114(v) brilho (nits) (máx.) 280 nits (min)  - taxa de contraste (típico) 3000:1 taxa de contraste dinâmico milhões  - ângulo de visão (h/v) 178°(h)/178°(v)  - profundidade de bits do painel 8 bits cores da tela 16,7m  - tempo de resposta do painel sem od 21ms tempo de resposta 8 ms (alta) taxa de atualização do painel (máx.) 240 hz taxa de atualização da tela (máx.) 48hz-240hz scaler pn hdmi 1.4 n/a faixa freesync n/a hdmi 2.0 2 faixa freesync 48-240 hz  - saída de áudio  - botão liga/desliga cinco botão osd cinco  - contracapa design rgb  - consumo de energia 25w tipo.,54w máx. Modo de economia de energia?0,5w modo de desligamento ?0,3w  - tipo de energia adaptador de energia fonte de alimentação 12v 4a  - acessorios: cabo de alimentação (1,5 m) 1 (1,5 m) cabo dp versão 1.2 qtd de cabo dp (1,5 m/1,8 m) 1 (1,5 m)  - temperatura da cor (fria, quente, usuário) controle de baixa luz azul modos de cenários dcr menu de idiomas 23 idiomas  - nenhum ajuste de luz de fundo intermitente sincronização adaptável freesync  - over drive fps/rts jogo mais pip/pbp qp efeito de luz laranja  - dimensão com suporte (l/a/p)(mm) 616,2x453,1x195,7 mm  - dimensão sem suporte (lxaxp)(mm) 616,2x367,2x96,3 mm  - dimensão da caixa (lxaxp)(mm) 699x169x440mm  - peso líquido (kg) 4,85kg  - peso bruto (kg) 6,72kg  - garantia 1 ano &lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;marca:&lt;/strong&gt; primetek&lt;br&gt;&lt;strong&gt;modelo:&lt;/strong&gt; 25c1h&lt;br&gt;&lt;strong&gt;tamanho da tela:&lt;/strong&gt; 25</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Goldentec, 24 Polegadas, LED, Full HD, 144hz, 1ms</t>
+  </si>
+  <si>
+    <t>Monitor gamer goldentec 24´´ led full hd 144hz 1ms | gt gamer conta com tecnologia freesync, capaz de eliminar falhas e intermitências. Além disso, possui tecnologia lowbluelight, capaz de reduzir a luz azul do monitor proporcionando mais conforto e segurança. Conta também com 100% flicker free, suavizando a ondulação do monitor.   especificações técnicas  marcagoldentec  tamanho de tela24´´  framelesssim  resolução1920x1080 (full hd)  tempo de resposta 1ms  frequência 144hz  brilho250 cd/m²  contraste 100 milhões: 1  ângulo de visão180° (h) 180° (v)  cores16,7 milhões  inclinação ajustavel15°  tecnologia freesyncsim, elimina falhas e intermitências  tecnlogia lowbluelightsim, reduz a luz azul para mais conforto e segurança  100% flicker freesim, suaviza a ondulação do monitor  conexõeshdmi + vga  conteúdo da embalagemmonitor 24´´&lt;br&gt;fonte adaptadora&lt;br&gt;cabo hdmi&lt;br&gt;manual de instruções   &lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;&lt;br&gt;&lt;strong&gt;marca :&lt;/strong&gt; goldentec&lt;br&gt;&lt;strong&gt;tipo :&lt;/strong&gt; gamer&lt;br&gt;&lt;strong&gt;polegadas :&lt;/strong&gt; 24 ´´&lt;br&gt;&lt;br&gt;&lt;strong&gt;garantia : &lt;/strong&gt;12</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Grasep 27 Polegadas Led, FHD, HDMI, Som Integrado - 1920P</t>
+  </si>
+  <si>
+    <t>PRONTA ENTREGA&lt;br /&gt;3 meses de garantia com o vendedor!&lt;br /&gt;6 meses de garantia com o fabricante!&lt;br /&gt;&lt;br /&gt;Monitor PC Gamer Led Full HD Som integrado 27 pol 75Hz&lt;br /&gt;&lt;br /&gt;Eleve a qualidade visual do seu computador com este incrível monitor PC de alta definição. Projetado para oferecer uma experiência visual imersiva e nítida, este monitor é perfeito para trabalhar, jogar, assistir a filmes e muito mais.&lt;br /&gt;&lt;br /&gt;Com uma tela de alta resolução, cada detalhe ganha vida, proporcionando imagens vibrantes e cores realistas. Seja para editar fotos e vídeos, jogar seus games favoritos ou assistir a filmes em alta definição, este monitor oferece uma qualidade de imagem impressionante, com alto contraste e brilho intenso.&lt;br /&gt;&lt;br /&gt;Além disso, o monitor possui um tamanho de 27 polegadas para acomodar várias janelas e facilitar a multitarefa. Você poderá abrir e trabalhar em diferentes aplicativos ao mesmo tempo, aumentando sua produtividade e tornando seu fluxo de trabalho mais eficiente.&lt;br /&gt;&lt;br /&gt;Dimensões: 4x56x33cm&lt;br /&gt;Peso: 3.6kg&lt;br /&gt;&lt;br /&gt;Especificações:&lt;br /&gt;Tela: 27"&lt;br /&gt;Tipo: LED&lt;br /&gt;Resolução: 1920x1080&lt;br /&gt;IPS&lt;br /&gt;Tempo de resposta: 1ms&lt;br /&gt;Brilho máxima: 250cd/m&lt;br /&gt;Interfaces: HDMI/VGA/AUDIO IN&lt;br /&gt;Frequência horizontal: 67.200KHz&lt;br /&gt;Frequência vertical: 75Hz&lt;br /&gt;Consumo de potência: 35W&lt;br /&gt;Consumo Potência em Standby: 0,5&lt;br /&gt;Não possui som integrado&lt;br /&gt;Visão expansiva&lt;br /&gt;&lt;br /&gt;Itens Inclusos:&lt;br /&gt;1 Monitor 27&lt;br /&gt;1 Cabo DisplayPort&lt;br /&gt;1 Fonte AC/DC&lt;br /&gt;1 Manual</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Acer VG240Y FHD 165hz FreeSync ZeroFrame 0,5ms.</t>
+  </si>
+  <si>
+    <t>A tecnologia AMDFreeSync Premium elimina a tela ?'rasgada', minimiza atrasos e latência durante os jogos, apresentando uma sincronização dos quadros do monitor muito mais eficiente. Sua experiência visual será mais suave, fluida e responsiva. O Nitro VG240Y conta com uma alta taxa de atualização de 144Hz até 165Hz. Prepare-se para ver imagens mais suaves, sem rastros e sem rasgos. Monitor é igual exp: quanto mais, melhor. Jogue com múltiplos monitores sem problemas, o design ZeroFrame praticamente elimina as bordas para que você tenha uma verdadeira imersão no jogo. Com Display Acer HDR, o VG240Y cria níveis mais profundos do contraste preto e branco. Nas cenas mais escuras, os pretos ricos são preservados e os detalhes aprimorados, gerando maior luminosidade. A tela de 23.8 polegadas IPS Full HD potencializa seu poder de imersão nas batalhas. A latência ultrabaixa deste monitor oferece respostas rápidas além das expectativas. Você terá controle total em jogos de corrida ou esporte, devido à redução do atraso de quadro. O tempo de resposta do Nitro é de 2ms até 0,5ms.</t>
+  </si>
+  <si>
+    <t>Monitor Gamer 27 Asus Vg279q1r Tuf Gaming - Full Hd Ips - 144hz - 1ms - Freesync - Hdmi/displayport</t>
+  </si>
+  <si>
+    <t>TUF Gaming VG279Q1RO TUF Gaming VG279Q1R é uma tela Full HD (1920x1080) de 27 polegadas com uma taxa de atualização ultrarrápida de 144 Hz projetada para jogadores profissionais e aqueles que buscam jogabilidade envolvente. Ele também possui a tecnologia Adaptive-Sync (FreeSync ™), para uma jogabilidade extremamente fluida sem tearing e stuttering.MONITOR GAMING ULTRA SLIM DE 27 POLEGADASO painel Full HD (1920 X 1080) de 27 polegadas do TUF Gaming VG279Q1R oferece visuais impressionantes de ângulos de visão amplos de 178 °. Também ocupa muito pouco espaço na área de trabalho e se encaixa bem em qualquer configuração. Seu perfil ultrafino mede apenas 7,5 mm em seu ponto mais fino, também apresenta o novo Turbo Rim baseado que combina com a configuração de jogo perfeita.Refresh rate de 144hzO TUF Gaming VG279Q1R tem uma taxa de atualização super rápida de 144 Hz, garantindo que mesmo os jogos mais rápidos, jogados nas configurações visuais mais altas, tenham uma aparência suave e completamente livre de atrasos. Obtenha a vantagem em jogos de tiro em primeira pessoa, corrida, estratégia em tempo real e títulos de esportes.EXTREME LOW MOTION BLURA tecnologia Extreme Low Motion Blur exclusiva da ASUS alcança 1 ms MPRT para eliminar manchas e desfoque de movimento. Também faz com que os objetos em movimento pareçam ainda mais nítidos, para que a jogabilidade seja mais fluida e ágil.Shadow BoostA tecnologia ASUS Shadow Boost esclarece as áreas escuras do jogo sem superexpor as áreas mais brilhantes, melhorando a visualização geral, ao mesmo tempo que torna mais fácil localizar inimigos escondidos em áreas escuras do mapa.</t>
+  </si>
+  <si>
+    <t>Monitor Goldentec, 24" Led Gt Gamer Fhd, Hdmi, 75hz</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Bluecase, 21.5" Full HD, 75Hz, Rako - BM221GW</t>
+  </si>
+  <si>
+    <t>Monitor Concórdia Gamer Curvo 27'', Led Full, Hd, 165hz, Freesync - Cz270f</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;você na vantagem sempre!&amp;nbsp &amp;nbsp&amp;nbsp&lt;/strong&gt;o&amp;nbsp&lt;strong&gt;monitor concórdia gamer curvo cz270f 27&amp;quot led full hd 165hz freesync&lt;/strong&gt;&amp;nbspconta com resposta de 1ms e taxa de atualização de 165hz, permitindo a mais alta performance durante suas gameplays. Sua curvatura amplia o campo de visão relativo, concentrando toda a ação ao alcance dos olhos do usuário, sem perder resolução.&lt;strong&gt;monitor curvo&amp;nbsp &amp;nbsp&lt;/strong&gt;tenha mais imersão na sua gameplay com esse monitor curvo da concórdia. Observe seus adversários ainda mais de perto com essa imersão de 1500r de curvatura e um ângulo de visão de 178º.&lt;strong&gt;inclinável&amp;nbsp&lt;/strong&gt;ajuste de inclinação da tela de 5&amp;deg a 15&amp;deg. Ajuste seu monitor da maneira que quiser deixando sua visão ainda mais confortável e ampla!&lt;strong&gt;especificações:&lt;/strong&gt;&lt;strong&gt;tela:&lt;/strong&gt;painel: vaárea ativa: 596.736 &amp;times 335.664 mmângulo de visão: 178/178&amp;nbspcurvatura: r1500&amp;nbspresolução: 1920*1080165hzdot pitch: 0,3108cores do painel: 16.7m&amp;nbsp&amp;nbspbrilho(máximo): 250cd/m2tempo de resposta: 1ms&amp;nbspcontraste: 3000: 1taxa de heartz: 165hz&amp;nbsp &amp;nbsp&lt;strong&gt;conectividade:&amp;nbsp&lt;/strong&gt;hdmidisplayport 1.4dvientrada earphonedc (energia)&lt;strong&gt;alimentação:&lt;/strong&gt;tipo: adaptador externovoltagem: 12v/3.5aconsumo: 38w | stand by: 0.5w&amp;nbsp&lt;strong&gt;recursos do monitor:&lt;/strong&gt;- base de fácil desmontagem- freesync/g-sync&amp;nbsp&amp;nbsp- filtro de luz azul- flicker free- baixo consumo em modo stand by- overdriver&amp;nbsp- base fixa- sem bordas- auto falante interno: sim.- vesa: 100*100mm.&amp;nbsp&lt;strong&gt;acompanha:&lt;/strong&gt;&amp;nbspcabo displayport,&amp;nbspmanual do usuário e parafusos.&amp;nbsp&amp;nbsp&lt;strong&gt;dimensões da tela (cm)(axlxp):&lt;/strong&gt;&amp;nbsp36 | 61 | 4,5 | peso(kg): 4,734.&lt;strong&gt;dimensões da tela com base&amp;nbsp(cm)(axlxp)&lt;/strong&gt;: 43 | 61 | 17 | peso(kg): 4,734.&lt;br&gt;&lt;br&gt;&lt;strong&gt;especificações técnicas&lt;/strong&gt;&lt;br&gt;monitor concórdia gamer curvo cz270f 27´´ led full hd 165hz freesync | entregue para todo o brasil |</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Husky Storm 27' LED, Curvo, 165 Hz, Full HD, 1ms, Adaptive Sync, HDMI/DisplayPort, Ajuste de Ângulo - HGMT001</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Monitor Gamer Husky Storm 27' LED, Curvo, 165 Hz, Full HD, 1ms, Adaptive Sync, HDMI/DisplayPort, Ajuste de &amp;Acirc;ngulo&lt;/h2&gt;
+&lt;h3&gt;&lt;br /&gt;Esteja um passo &amp;agrave; frente!&lt;/h3&gt;
+&lt;p&gt;O Monitor Husky Storm conta com resposta de 1ms e taxa de atualiza&amp;ccedil;&amp;atilde;o de 165Hz, permitindo a mais alta performance durante suas gameplays. Sua curvatura amplia o campo de vis&amp;atilde;o relativo, concentrando toda a a&amp;ccedil;&amp;atilde;o ao alcance dos olhos do usu&amp;aacute;rio, sem perder resolu&amp;ccedil;&amp;atilde;o.&lt;/p&gt;
+&lt;h3&gt;&lt;br /&gt;Tecnologia Adaptive Sync&amp;nbsp;&lt;/h3&gt;
+&lt;p&gt;Compat&amp;iacute;vel com a tecnologia Adaptive Sync, permite a sincroniza&amp;ccedil;&amp;atilde;o dos frames da placa de v&amp;iacute;deo, decretando o fim do input lag, bem como do tearing.&lt;/p&gt;
+&lt;h3&gt;&lt;br /&gt;Monitor Curvo&amp;nbsp;&lt;/h3&gt;
+&lt;p&gt;Tenha mais imers&amp;atilde;o na sua gaming player com esse monitor curvo da Husky. Observe seus advers&amp;aacute;rios ainda mais de perto com essa imers&amp;atilde;o de 1500r de curvatura e um &amp;acirc;ngulo de vis&amp;atilde;o de 178&amp;ordm;.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Adaptive Sync&lt;/h3&gt;
+&lt;p&gt;Evita o imput lag e combate o problema da quebra de quadros durante a reprodu&amp;ccedil;&amp;atilde;o dos frames. Essa Tecnologia evita o travamento do jogo para uma jogabilidade mais suave poss&amp;iacute;vel. Explore novas paisagens e capture seus inimigos em movimentos suaves e cont&amp;iacute;nuos.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Inclin&amp;aacute;vel&lt;/h3&gt;
+&lt;p&gt;Ajuste de inclina&amp;ccedil;&amp;atilde;o da tela de 5&amp;deg; a 15&amp;deg;. Ajuste seu monitor da maneira que quiser deixando sua vis&amp;atilde;o ainda mais confort&amp;aacute;vel e ampla&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Monitor Husky &amp;eacute; no KaBuM!&amp;nbsp;&lt;/h3&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;&lt;a href="https://kabum.com.br/hotsite/manuais/115384-Monitor-Gamer-Husky-Storm-HGMT001.pdf" target="_blank"&gt;MANUAL DE INSTRU&amp;Ccedil;&amp;Otilde;ES&lt;/a&gt;&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Asus TUF Gaming 27 Full HD, 165Hz, 1ms, IPS, HDMI e DisplayPort, FreeSync Premium, VESA - VG279Q1A</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;TUF Gaming VG279Q1A Gaming Monitor Full HD de 27 polegadas (1920x1080), IPS, 165Hz (acima de 144Hz), Extreme Low Motion Blur, Adaptive-sync, FreeSync Premium, 1ms (MPRT)&lt;/h2&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;Monitor de jogos &lt;strong&gt;IPS Full HD (1920 x 1080)&lt;/strong&gt; de 27 polegadas com &lt;strong&gt;taxa de atualiza&amp;ccedil;&amp;atilde;o ultrarr&amp;aacute;pida de 165 Hz&lt;/strong&gt;, projetado para jogadores profissionais e jogabilidade envolvente.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;A tecnologia &lt;strong&gt;ASUS Extreme Low Motion Blur (ELMB)&lt;/strong&gt; permite um &lt;strong&gt;tempo de resposta de 1 ms (MPRT)&lt;/strong&gt; junto com a sincroniza&amp;ccedil;&amp;atilde;o adaptativa, eliminando fantasmas e rasgos para visuais de jogos n&amp;iacute;tidos com altas taxas de quadros.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Tecnologia FreeSync Premium&lt;/strong&gt; para eliminar rasgos na tela e taxas de quadros inst&amp;aacute;veis.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;Suporta &lt;strong&gt;Adaptive-Sync&lt;/strong&gt; com placas gr&amp;aacute;ficas &lt;strong&gt;NVIDIA GeForce e FreeSync&lt;/strong&gt; com placas gr&amp;aacute;ficas AMD Radeon Compat&amp;iacute;vel com NVIDIA GeForce s&amp;eacute;rie GTX 10, s&amp;eacute;rie GTX 16, s&amp;eacute;rie RTX 20 e placas gr&amp;aacute;ficas mais recentes.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;O &lt;strong&gt;Shadow Boost aprimora os detalhes da imagem&lt;/strong&gt; em &amp;aacute;reas escuras, iluminando as cenas sem super expor as &amp;aacute;reas claras.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;Sa&amp;iacute;da &lt;strong&gt;Full HD (1920 x 1080) a 120 Hz no PS5 e Xbox&lt;/strong&gt; Series X/S.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Todos os elementos essenciais para jogos&lt;/h3&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;O TUF Gaming VG279Q1A &amp;eacute; um monitor IPS Full HD (1920 x 1080) de 27 polegadas com uma taxa de atualiza&amp;ccedil;&amp;atilde;o ultrarr&amp;aacute;pida de 165 Hz. Projetado para jogadores e outros que buscam uma jogabilidade envolvente, ele oferece algumas especifica&amp;ccedil;&amp;otilde;es s&amp;eacute;rias. Mas h&amp;aacute; mais...&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;Sua fun&amp;ccedil;&amp;atilde;o exclusiva ELMB apresenta um tempo de resposta MPRT de 1ms e tecnologia Adaptive-Sync (FreeSync Premium), para uma jogabilidade extremamente fluida sem tearing e gagueira.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Tela IPS de 27 polegadas para melhor reprodu&amp;ccedil;&amp;atilde;o de cores&lt;/h3&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;O painel IPS Full HD (1920 x 1080) de 27 polegadas do TUF Gaming VG279Q1A oferece visuais impressionantes de todos os &amp;acirc;ngulos com amplos &amp;acirc;ngulos de vis&amp;atilde;o de 178 graus, garantindo distor&amp;ccedil;&amp;atilde;o m&amp;iacute;nima e mudan&amp;ccedil;a de cor mesmo quando voc&amp;ecirc; est&amp;aacute; visualizando de posi&amp;ccedil;&amp;otilde;es extremas.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Taxa de atualiza&amp;ccedil;&amp;atilde;o super-r&amp;aacute;pida de 165 Hz&lt;/h3&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;Uma impressionante taxa de atualiza&amp;ccedil;&amp;atilde;o de 165 Hz elimina o atraso e o desfoque de movimento para dar a voc&amp;ecirc; vantagem em jogos de tiro em primeira pessoa, corrida, estrat&amp;eacute;gia em tempo real e t&amp;iacute;tulos esportivos. Essa taxa de atualiza&amp;ccedil;&amp;atilde;o ultrarr&amp;aacute;pida permite que voc&amp;ecirc; jogue nas configura&amp;ccedil;&amp;otilde;es visuais mais altas e reaja instantaneamente ao que est&amp;aacute; na tela.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Desfrute de uma jogabilidade super suave&lt;/h3&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;Apresenta a mais recente tecnologia Extreme Low Motion Blur exclusiva da ASUS, que atinge 1ms MPRT para eliminar manchas e desfoque de movimento, e torna os objetos em movimento mais n&amp;iacute;tidos, para que a jogabilidade seja mais fluida e responsiva.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Duex 27 Full HD Curvo, 240Hz, 1ms, IPS, HDMI e DisplayPort, 99% sRGB, VESA - 270ZG</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Monitor Gamer Duex 27 Full HD&lt;/h2&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;Uma velocidade ultrarr&amp;aacute;pida de&amp;nbsp;&lt;strong&gt;240Hz e 1ms&lt;/strong&gt;&amp;nbsp;permite que os jogadores vejam o pr&amp;oacute;ximo quadro rapidamente e fazem com que a imagem apare&amp;ccedil;a suavemente. Os jogadores podem responder rapidamente aos oponentes e mirar no alvo facilmente.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Compre agora no KaBuM!&lt;/h3&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Husky 700  27 LED, Curvo Wide, WQHD, 165Hz, 1ms, HDMI e DisplayPort, Adaptive Sync, VESA - HGMT008</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Monitor Gamer Husky Gaming Storm 700&lt;/h2&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;N&amp;atilde;o precisa mais se perguntar qual monitor gamer comprar! A Husky Gaming ajuda voc&amp;ecirc; a &lt;strong&gt;atualizar seu setup&lt;/strong&gt;, seja para partidas no PC ou v&amp;iacute;deo game. Sempre oferecemos &lt;strong&gt;o melhor para voc&amp;ecirc;!&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;Monitor Gamer Husky Gaming Storm 700 tem uma alta &lt;strong&gt;taxa de atualiza&amp;ccedil;&amp;atilde;o de 165 Hz&lt;/strong&gt; com &lt;strong&gt;tempo de resposta de 1 ms&lt;/strong&gt;, que possibilita um tempo de rea&amp;ccedil;&amp;atilde;o mais r&amp;aacute;pido para suas partidas insanas.&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;Sua&lt;strong&gt; tela curva Quad HD de 27"&lt;/strong&gt;, com&lt;strong&gt; resolu&amp;ccedil;&amp;atilde;o de 2560 x 1440P&lt;/strong&gt; que garante imagem mais n&amp;iacute;tida e detalhada. Proporcionando&lt;strong&gt; jogabilidade fluida&lt;/strong&gt;, &lt;strong&gt;sem distor&amp;ccedil;&amp;otilde;es&lt;/strong&gt; e uma &lt;strong&gt;experi&amp;ecirc;ncia mais imersiva&lt;/strong&gt; para voc&amp;ecirc; n&amp;atilde;o perder nenhum detalhe importante, do seu programa de esporte, filme, s&amp;eacute;rie ou jogo preferido.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Aproveite e garanta j&amp;aacute; o seu Monitor Gamer Husky Gaming Storm 700! no KaBuM!&lt;/h3&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Gigabyte, 27 QHD, 170Hz, 1ms, DisplayPort e HDMI, 108% sRGB, HDR, Adaptive-Sync - GS27QC SA</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Monitor Gamer Gigabyte 27 QHD&lt;/h2&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;A Mais Alta Qualidade&lt;/h2&gt;
+&lt;p&gt;Equipado com uma taxa de atualiza&amp;ccedil;&amp;atilde;o de &lt;strong&gt;165 Hz&lt;/strong&gt; que suporta a tecnologia &lt;strong&gt;Adaptive-Sync&lt;/strong&gt; (FreeSync Premium), que p&amp;otilde;e fim &amp;agrave; jogabilidade inst&amp;aacute;vel e aos frames quebrados e cria um desempenho fluido e livre de artefatos em qualquer taxa de quadros. GS27QC com um tempo de resposta extremamente r&amp;aacute;pido de &lt;strong&gt;1 ms&lt;/strong&gt; para eliminar totalmente o atraso e o rasgo da imagem.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Mais Curva e Mais Imers&amp;atilde;o&lt;/h2&gt;
+&lt;p&gt;Um painel VA nativo de &lt;strong&gt;1500 Raios&lt;/strong&gt; que apresenta uma vis&amp;atilde;o mais pr&amp;oacute;xima do olho humano do que um monitor plano, proporcionando uma sensa&amp;ccedil;&amp;atilde;o mais envolvente e ao mesmo tempo oferecendo mais conforto visual.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Milh&amp;otilde;es de Cores&lt;/h2&gt;
+&lt;p&gt;O GS27QC pode exibir &lt;strong&gt;16,7 milh&amp;otilde;es de cores&lt;/strong&gt; e possui uma taxa de contraste de &lt;strong&gt;4000:1&lt;/strong&gt;. Ele permite que voc&amp;ecirc; desfrute de uma experi&amp;ecirc;ncia de jogo fluente com cores reais e vibrantes. O GS27QC est&amp;aacute; pronto para &lt;strong&gt;HDR&lt;/strong&gt;, o que desperta interesse em uma ampla gama de aplica&amp;ccedil;&amp;otilde;es, incluindo jogos, entretenimento cinematogr&amp;aacute;fico e cria&amp;ccedil;&amp;atilde;o de conte&amp;uacute;do multim&amp;iacute;dia.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Compre j&amp;aacute; o seu no KaBuM!&lt;/h3&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Gigabyte 27 IPS, QHD , 144Hz, 1ms, 120% sRGB, HDR 400, FreeSync Premium, Altura Ajustável - G27Q-SA</t>
+  </si>
+  <si>
+    <t>JUNTE-SE À LUTA com o Monitor Gamer de 27" G27Q-SA da Gigabyte com 1ms de tempo de resposta, freesync premium, 144 Hz e com uma taxa de cor de 8 bits, 92% DCI-P3 A ÚLTIMA MILHA PARA O SEU SISTEMA DE JOGO Como um jogador invisível, o monitor é frequentemente subestimado. A verdade é que os monitores se formam como um efeito sinérgico e trazem o melhor desempenho dos componentes do PC. Os monitores de jogos GIGABYTE oferecem as últimas especificações e qualidade, os usuários podem realmente desfrutar de um desempenho de alto nível sem a necessidade de extravagância. Tempo de Resposta de 1 ms Tempo de resposta super rápido de 1 ms para a experiência de jogo mais suave de todos os tempos! QHD e 144Hz Alta resolução e taxa de atualização rápida, proporcionando qualidade de exibição detalhada e experiência de jogo fluida! Cor de 8 bits, 92% DCI-P3 Fantástico visor colorido e 92% de cores DCI-P3 de gama super ampla. SIMPLES MAS ESTILOSO A aparência aerodinâmica representa a simplicidade da filosofia de design da série de jogos GIGABYTE, suporte robusto e acabamento fosco construído para características funcionais e estéticas adicionando mais características. ÂNGULO DE VISÃO PERFEITO O monitor de jogos GIGABYTE possui um suporte exclusivo ergonomicamente projetado para oferecer uma ampla gama de ajustes de altura e inclinação.</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Acer 31.5 LED Full HD, Curvo, 165 Hz, 1ms, HDMI e DisplayPort, FreeSync Premium, VESA - ED320QR</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Monitor Gamer Acer 31.5 LED Full HD, Curvo, 165 Hz, 1ms, HDMI e DisplayPort, FreeSync Premium, VESA&lt;/h2&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Tela Curva e Imersiva&lt;/h2&gt;
+&lt;p&gt;Tenha uma experi&amp;ecirc;ncia visual imersiva e confort&amp;aacute;vel com uma&lt;strong&gt; tela curva&lt;/strong&gt; com raio de 1800 mm de visualiza&amp;ccedil;&amp;atilde;o. Essa tecnologia mant&amp;eacute;m os cantos da tela &amp;agrave; mesma dist&amp;acirc;ncia de seus olhos. S&amp;atilde;o &lt;strong&gt;31,5&amp;rdquo;&lt;/strong&gt; e resolu&amp;ccedil;&amp;atilde;o &lt;strong&gt;Full HD&lt;/strong&gt;, promovendo imagens n&amp;iacute;tidas, que levam seu foco no jogo a outro n&amp;iacute;vel.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Design ZeroFrame&lt;/h2&gt;
+&lt;p&gt;Monitor com tela &lt;strong&gt;LED VA&lt;/strong&gt; e design ZeroFrame, que praticamente elimina as bordas para que voc&amp;ecirc; tenha uma verdadeira imers&amp;atilde;o no jogo.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;De olho em cada Frame&lt;/h2&gt;
+&lt;p&gt;O Nitro Series ED0 conta com uma taxa de atualiza&amp;ccedil;&amp;atilde;o de at&amp;eacute; &lt;strong&gt;165Hz.&lt;/strong&gt; Prepare-se para ver imagens mais suaves, sem rastros e sem rasgos.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Foque no Movimento&lt;/h2&gt;
+&lt;p&gt;Com o Visual Response Boost (VRB) de 1 ms, o monitor reduz borr&amp;otilde;es, efeitos fantasmas e manchas nas imagens. Al&amp;eacute;m disso, elimina o desfoque em objetos em movimento r&amp;aacute;pido.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Jogue em Perfeita Sincronia&lt;/h2&gt;
+&lt;p&gt;A tecnologi&lt;strong&gt;a AMD FreeSync Premium&lt;/strong&gt; elimina a tela &amp;ldquo;rasgada&amp;rdquo;, minimiza atrasos e lat&amp;ecirc;ncia durante os jogos, apresentando uma sincroniza&amp;ccedil;&amp;atilde;o dos quadros do monitor muito mais eficiente. Sua experi&amp;ecirc;ncia visual ser&amp;aacute; mais&lt;strong&gt; suave, fluida e responsiva.&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Contrastes Impressionantes&lt;/h2&gt;
+&lt;p&gt;O contraste de 100 milh&amp;otilde;es:1 &amp;eacute; alcan&amp;ccedil;ado atrav&amp;eacute;s da tecnologia Acer Adaptive Contrast Management. Ela proporciona um&lt;strong&gt; visual mais cristalino&lt;/strong&gt; e real&amp;ccedil;a a qualidade das cores do monitor.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Aproveite essa oportunidade e adquira seu Monitor Acer no KaBuM!&lt;/h3&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Samsung 22' IPS, 75 Hz, Full HD, FreeSync, HDMI/VGA, VESA -  LF22T350FHLMZD</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Monitor Gamer Samsung LED 22, IPS, Full HD, Vesa, Free Sync, Modo Gaming, Preto Vis&amp;atilde;o totalmente expansiva Design minimalista, concentra&amp;ccedil;&amp;atilde;o m&amp;aacute;xima. A tela com 3 lados sem borda traz uma est&amp;eacute;tica limpa e moderna para qualquer ambiente de trabalho. Em um setup com v&amp;aacute;rios monitores, se alinham perfeitamente para uma visualiza&amp;ccedil;&amp;atilde;o praticamente sem espa&amp;ccedil;os e sem distra&amp;ccedil;&amp;otilde;es. Imagens perfeitas e suaves Agora, a imagem &amp;eacute; reproduzida sem falhas. A taxa de atualiza&amp;ccedil;&amp;atilde;o de 75Hz oferece cenas mais fluidas. Seu momento de divers&amp;atilde;o n&amp;atilde;o tem lag ou efeito fantasma, quer voc&amp;ecirc; esteja acompanhando seu programa de TV favorito, assistindo a um v&amp;iacute;deo ou jogando um jogo. A&amp;ccedil;&amp;atilde;o Sincronizada Experi&amp;ecirc;ncia de entretenimento super fluida. AMD Radeon FreeSync mant&amp;eacute;m a taxa de atualiza&amp;ccedil;&amp;atilde;o do monitor e da placa gr&amp;aacute;fica em sincronia para reduzir a quebra de imagem. Assista a filmes e jogue sem interrup&amp;ccedil;&amp;otilde;es. At&amp;eacute; mesmo as cenas r&amp;aacute;pidas s&amp;atilde;o perfeitas e suaves. Veja de qualquer &amp;acirc;ngulo Sente-se em qualquer lugar e tenha uma experi&amp;ecirc;ncia completa sem distor&amp;ccedil;&amp;atilde;o de cores. O painel IPS preserva a nitidez e a vivacidade das cores em cada cent&amp;iacute;metro da tela. Mesmo em uma tela t&amp;atilde;o ampla, os tons e sombras s&amp;atilde;o completamente precisos de praticamente qualquer &amp;acirc;ngulo, sem altera&amp;ccedil;&amp;atilde;o de cor. Mais poder de jogo As configura&amp;ccedil;&amp;otilde;es de jogo ideais proporcionam uma vantagem instant&amp;acirc;nea. Detecte inimigos escondidos nas sombras atrav&amp;eacute;s do contraste ideal, mais nitidez e cenas com cores mais vivas. O Modo de Jogo ajusta qualquer jogo para preencher sua tela visualizando todos os detalhes. Mais conforto para os olhos Proteja seus olhos e fa&amp;ccedil;a mais. A avan&amp;ccedil;ada tecnologia de conforto visual reduz a fadiga ocular para uma experi&amp;ecirc;ncia prolongada menos cansativa. A tecnologia Flicker Free remove continuamente a tremula&amp;ccedil;&amp;atilde;o cansativa e irritante da tela, enquanto o Eye Saver Mode minimiza a emiss&amp;atilde;o de luz azul. Seus olhos ficam descansados por mais tempo. Versatilidade de verdade Conecte-se a mais. Com as portas HDMI e D-sub, v&amp;aacute;rios dispositivos podem ser conectados diretamente ao seu monitor para total flexibilidade. Agora, seu ambiente de computa&amp;ccedil;&amp;atilde;o &amp;eacute; ainda mais conveniente com possibilidades de entrada adicionais.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer AOC Agon 31.5' LED, Curvo, 165 Hz, Full HD, 1ms, FreeSync Premium, HDMI/DisplayPort, RGB Light FX - AG323FCXE</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Com tela de alta qualidade, amplo &amp;acirc;ngulo de vis&amp;atilde;o e comando em tempo real, prepare-se para obter uma experi&amp;ecirc;ncia muito mais imersiva em todos os g&amp;ecirc;neros de jogos. Projetado para gamers, o monitor Agon permite movimentos muito mais flu&amp;iacute;dos nos jogos devido a alt&amp;iacute;ssima taxa de atualiza&amp;ccedil;&amp;atilde;o de 165 Hz. O tempo de resposta de 1 ms proporciona movimentos instant&amp;acirc;neos e naturais para voc&amp;ecirc; ser o melhor, e com o painel VA, voc&amp;ecirc; tem mais brilho e contraste para enxergar onde os seus inimigos est&amp;atilde;o, mesmo em cenas com pouca ilumina&amp;ccedil;&amp;atilde;o. Al&amp;eacute;m disso, o design exclusivo com LEDs em diferentes configura&amp;ccedil;&amp;otilde;es de cores RGB deixam a sua maratona de jogos ainda mais emocionante.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer LG Ultra Gear 27 Full HD, 144 Hz, 1ms, IPS, HDMI e DisplayPort, sRGB 99%, HDR10, FreeSync, VESA, Altura Ajustável - 27GL650F-B</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Monitor Gamer LG Ultra Gear 27 Full HD&lt;/h2&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Evolua o Jogo Antes do Seu Rival:&lt;/h2&gt;
+&lt;p&gt;Tenha incr&amp;iacute;vel qualidade de imagens e decis&amp;otilde;es imediatas aos seus jogos com o Monitor Gamer LG 27GL650F.&lt;br /&gt;Os &lt;strong&gt;frames ultra-r&amp;aacute;pidos&lt;/strong&gt; de &lt;strong&gt;144Hz&lt;/strong&gt; permite os jogadores a reagirem imediatamente aos seus advers&amp;aacute;rios e mudar a hist&amp;oacute;ria do jogo para a sua vit&amp;oacute;ria.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;1ms Motion Blur Reduction&lt;/h2&gt;
+&lt;p&gt;Tenha imagens sem rastros e a&amp;ccedil;&amp;otilde;es mais r&amp;aacute;pidos com o &lt;strong&gt;tempo de resposta de 1ms&lt;/strong&gt; com &lt;strong&gt;Motion Blur Reduction.&lt;br /&gt;&lt;/strong&gt;O LG 27GL650F exibe &lt;strong&gt;precis&amp;atilde;o de cores impec&amp;aacute;vel&lt;/strong&gt; com um &amp;acirc;ngulo de vis&amp;atilde;o ampliado de 178&amp;deg;.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Compat&amp;iacute;vel com G-SYNC certificado pela NVIDIA&lt;/h2&gt;
+&lt;p&gt;Ap&amp;oacute;s ser testado pela NVIDIA, o monitor LG 27GL650F &amp;eacute; oficialmente compat&amp;iacute;vel com &lt;strong&gt;G-SYNC&lt;/strong&gt;, eliminando cortes e minimizando as repeti&amp;ccedil;&amp;otilde;es de imagem para uma experi&amp;ecirc;ncia mais fluida nos seus jogos.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Incr&amp;iacute;vel qualidade de imagem&lt;/h2&gt;
+&lt;p&gt;Tenha&lt;strong&gt; imagens supreendentes&lt;/strong&gt; com &lt;strong&gt;HDR10&lt;/strong&gt;, que reproduz alto brilho e maior gama de cores quando comparado a monitores convencionais deixando as imagens com maior qualidade em situa&amp;ccedil;&amp;otilde;es mais brilhantes ou de maior contraste.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Imagens sem falhas&lt;/h2&gt;
+&lt;p&gt;A tecnologia &lt;strong&gt;AMD FreeSync&lt;/strong&gt; reduz corte e repeti&amp;ccedil;&amp;otilde;es de imagens que ocorrem devido a diferen&amp;ccedil;a entre os quadros gr&amp;aacute;ficos e a taxa de atualiza&amp;ccedil;&amp;atilde;o do monitor. Com o FreeSync, os jogadores podem experimentar &lt;strong&gt;movimentos perfeitos e fluidos durante os jogo&lt;/strong&gt; de altas configura&amp;ccedil;&amp;otilde;es visuais.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Compre agora no KaBuM!&lt;/h3&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Samsung Odyssey G3, 24 Full HD, 144Hz, 1ms, FreeSync Premium, HDMI/Displayport, Ajuste de altura, Preto - LF24G35TFWLXZD</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Monitor Gamer Samsung Odyssey G3, 24 Full HD, 144Hz, 1ms, FreeSync Premium, HDMI/Displayport, Ajuste de altura, Preto&amp;nbsp;&lt;/h2&gt;
+&lt;p&gt;&lt;br /&gt;Monitor Gamer Samsung Odyssey G3 24&amp;rdquo;, FHD, 144 Hz, 1ms, com ajuste de altura, HDMI, DP, VGA, Freesync, Preto, S&amp;eacute;rie G3 Taxa de atualiza&amp;ccedil;&amp;atilde;o de 144Hz Domine todos os inimigos, mesmo em cenas muito r&amp;aacute;pidas. A taxa de atualiza&amp;ccedil;&amp;atilde;o de 144Hz elimina atrasos e desfoque de movimento para uma jogabilidade emocionante com a&amp;ccedil;&amp;atilde;o ultra suave.&lt;/p&gt;
+&lt;h3&gt;&lt;br /&gt;Tempo de resposta de 1ms&lt;/h3&gt;
+&lt;p&gt;Fa&amp;ccedil;a cada movimento contar com um tempo de resposta de 1ms. Ataque seus inimigos assim que os vir e fique &amp;agrave; frente com movimentos precisos do mouse. Seu desempenho na tela &amp;eacute; t&amp;atilde;o r&amp;aacute;pido quanto seus pr&amp;oacute;prios reflexos.&lt;/p&gt;
+&lt;h3&gt;&lt;br /&gt;AMD FreeSync Premium&lt;/h3&gt;
+&lt;p&gt;Jogabilidade suave sem esfor&amp;ccedil;o. O AMD FreeSync Premium apresenta tecnologia de sincroniza&amp;ccedil;&amp;atilde;o adapt&amp;aacute;vel, que reduz o travamento de tela, oscila&amp;ccedil;&amp;atilde;o e atrasos. Veja o jogo do seu jeito Gire, incline e ajuste seu monitor at&amp;eacute; que todos os inimigos estejam perfeitamente vis&amp;iacute;veis. Sua tela pode ser movida livremente para que voc&amp;ecirc; encontre conforto total no jogo. Design de tela cheia O design sem borda de 3 lados revela espa&amp;ccedil;o m&amp;aacute;ximo para uma jogabilidade maior e mais ousada. Alinhe dois monitores com precis&amp;atilde;o em uma configura&amp;ccedil;&amp;atilde;o de monitor duplo sem que nenhum inimigo fique escondido na jun&amp;ccedil;&amp;atilde;o.&lt;/p&gt;
+&lt;h3&gt;&lt;br /&gt;Mais conforto para os olhos&lt;/h3&gt;
+&lt;p&gt;Jogue por mais tempo sem incomodo visual. O Eye Saver Mode minimiza a emiss&amp;atilde;o de luz azul para manter seus olhos relaxados e confort&amp;aacute;veis enquanto joga por muitas horas. A tecnologia Flicker Free remove continuamente a tremula&amp;ccedil;&amp;atilde;o cansativa e irritante da tela para que voc&amp;ecirc; possa jogar por mais tempo sem distra&amp;ccedil;&amp;otilde;es ou fadiga ocular.&lt;/p&gt;
+&lt;h3&gt;&lt;br /&gt;Garanta o seu no KaBuM!&lt;/h3&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Concórdia 27" LED Full HD, 165Hz, 1ms, HDMI/DisplayPort, FreeSync, Preto - G5s</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Monitor Conc&amp;oacute;rdia Gamer G5s 27" Led Full Hd 165hz Freesync Hdmi Display Port&lt;/h2&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;O Monitor Conc&amp;oacute;rdia Gamer G5s de 27" 144Hz/165Hz apresenta tecnologia para tornar sua experi&amp;ecirc;ncia com games ainda mais intensa. Sem rastros, sem atraso, sem imagens tremidas! Tudo isso possibilitado pela sua taxa de atualiza&amp;ccedil;&amp;atilde;o de 144Hz/165Hz e tecnologia Freesync que juntos tornam esse monitor a sua melhor escolha. Com som embutido, conex&amp;atilde;o para fones, ele ainda facilita a sua vida com duas&amp;nbsp; conex&amp;otilde;es HDMI.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Alto desempenho com conveni&amp;ecirc;ncia a um pre&amp;ccedil;o justo nesse excelente painel PVA.&lt;/h3&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer LG 25' IPS, Ultra Wide, 75 Hz, Full HD,  99% sRGB, HDMI, VESA - 25UM58-G</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Monitor Gamer LG UltraWide&lt;/h2&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;1ms Motion Blur Reduction&lt;/h3&gt;
+&lt;p&gt;Tenha &lt;strong&gt;imagens sem rastros&lt;/strong&gt; e &lt;strong&gt;a&amp;ccedil;&amp;otilde;es mais r&amp;aacute;pidas&lt;/strong&gt; com o &lt;strong&gt;tempo de resposta de 1ms&lt;/strong&gt; com &lt;strong&gt;Motion Blur Reduction&lt;/strong&gt;.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;UltraWide&lt;/h3&gt;
+&lt;p&gt;A propor&amp;ccedil;&amp;atilde;o da imagem do monitor UltraWide torna os jogos e filmes mais envolventes do que nunca. A &lt;strong&gt;nitidez da resolu&amp;ccedil;&amp;atilde;o Full HD&lt;/strong&gt; de &lt;strong&gt;1080P com IPS&lt;/strong&gt; faz a diferen&amp;ccedil;a. Simplificando, de qualquer &amp;acirc;ngulo de vis&amp;atilde;o, tudo fica mais n&amp;iacute;tido e detalhado em FULL HD .&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Recursos Avan&amp;ccedil;ados para Jogos&lt;/h3&gt;
+&lt;p&gt;Ative o &lt;strong&gt;Dynamic Action Sync&lt;/strong&gt; para que o monitor acompanhe a velocidade das suas habilidades e veja os inimigos nos lugares mais escuros com o &lt;strong&gt;Black Stabilizer.&amp;nbsp;&lt;/strong&gt;Defina as condi&amp;ccedil;&amp;otilde;es ideais de jogo no Modo de Jogo. H&amp;aacute; &lt;strong&gt;3 modos&lt;/strong&gt; &lt;strong&gt;para jogadores&lt;/strong&gt;: &lt;strong&gt;2 modos de tiro&lt;/strong&gt; &lt;strong&gt;em primeira pessoa&lt;/strong&gt; e at&amp;eacute; mesmo um &lt;strong&gt;modo predefinido&lt;/strong&gt; &lt;strong&gt;de estrat&amp;eacute;gia em tempo real&lt;/strong&gt;.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;On-Screen Control&lt;/h3&gt;
+&lt;p&gt;O Controle On-Screen coloca uma s&amp;eacute;rie de &lt;strong&gt;configura&amp;ccedil;&amp;otilde;es essenciais em uma pr&amp;aacute;tica janela para acesso f&amp;aacute;cil&lt;/strong&gt;. As &lt;strong&gt;configura&amp;ccedil;&amp;otilde;es de volume, brilho, predefini&amp;ccedil;&amp;otilde;es de modo de imagem&lt;/strong&gt;, &lt;strong&gt;Screen Split 2.0 e Dual Controller&lt;/strong&gt;, al&amp;eacute;m de muitas outras, podem agora ser ajustadas com apenas alguns cliques do mouse, em vez dos bot&amp;otilde;es f&amp;iacute;sicos do monitor.&amp;nbsp;&lt;strong&gt;Personalize o layout de seu monitor&lt;/strong&gt; para multitarefas com a &amp;uacute;ltima vers&amp;atilde;o do LG Screen Split. &lt;strong&gt;Redimensione e exiba v&amp;aacute;rias janelas ao mesmo tempo&lt;/strong&gt;, com 14 op&amp;ccedil;&amp;otilde;es que incluem quatro escolhas diferentes de picture-in-picture (&lt;strong&gt;PIP&lt;/strong&gt;).&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;Compre no &lt;strong&gt;KaBuM!&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Asus TUF 27' IPS, 165 Hz, Full HD, 1ms, Adaptive Sync, HDMI/DisplayPort, Ajuste de Altura, Vesa, Som Integrado - VG279QR</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Monitor de jogos Full HD (1920 x 1080) de 27 polegadas com taxa de atualiza&amp;ccedil;&amp;atilde;o ultrarr&amp;aacute;pida de 165 Hz projetado para jogadores profissionais e jogabilidade envolvente. A tecnologia ASUS Extreme Low Motion Blur (ELMB ?) permite um tempo de resposta de 1 ms (MPRT), eliminando fantasmas para visuais n&amp;iacute;tidos de jogos. O Shadow Boost aprimora os detalhes da imagem em &amp;aacute;reas escuras, iluminando cenas sem expor demais as &amp;aacute;reas claras. Processamento compat&amp;iacute;vel com G-SYNC, proporcionando uma experi&amp;ecirc;ncia de jogo perfeita e sem problemas ao habilitar VRR (taxa de atualiza&amp;ccedil;&amp;atilde;o vari&amp;aacute;vel) por padr&amp;atilde;o. Apresenta um suporte ergonomicamente projetado para oferecer extensos ajustes de rota&amp;ccedil;&amp;atilde;o, inclina&amp;ccedil;&amp;atilde;o, rota&amp;ccedil;&amp;atilde;o e altura.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Concórdia C240 23.8, LED, HDMI, Full HD, Curvo, 75Hz, 2ms, Vermelho - 40511</t>
+  </si>
+  <si>
+    <t>Monitor Concórdia Gamer Curvo C240 23.8" Led Full HD HDMI VGA A tecnologia do novo C240 garante uma imersão total em seus jogos. Prepare-se para uma nova experiência com seus games! Agora você pode escolher ele em duas versões:todo preto ou preto com detalhe em vermelho.</t>
+  </si>
+  <si>
+    <t>Monitor Gamer LG Ultra Gear 23.8' IPS, 144 Hz, Full HD, 1ms, FreeSync, HDR 10, 99% sRGB, HDMI/DisplayPort, Ajuste de Ângulo - 24GN600-B</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Monitor Gamer LG Ultra Gear 23.8 Full HD, 144Hz, 1ms, IPS, DMI, DisplayPort, 99% sRGB, Ajuste de &amp;Acirc;ngulo, FreeSync, HDR10, Preto&lt;/h2&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Inova&amp;ccedil;&amp;atilde;o sem fronteiras para jogos&lt;/h2&gt;
+&lt;p&gt;Complete seu setup Gamer com o monitor LG UltraGear premium. Desenvolvido para o Gamer, com os recursos mais avan&amp;ccedil;ados, aliados a ergonomia e &lt;strong&gt;design eletrizante&lt;/strong&gt;, entregando a experi&amp;ecirc;ncia imersiva! Seja o melhor com os melhores recursos feitos para apoiar sua vit&amp;oacute;ria, tempo de resposta de &lt;strong&gt;1ms Real&lt;/strong&gt; (GtG), em um painel com cores vislumbrantes IPS.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Jogabilidade fluida com frames instantaneos&lt;/h2&gt;
+&lt;p&gt;Os frames ultra-r&amp;aacute;pidos de 144Hz permite os jogadores a reagirem imediatamente aos seus advers&amp;aacute;rios e mudar a hist&amp;oacute;ria do jogo para a sua vit&amp;oacute;ria.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Aproveite os v&amp;iacute;deos e jogos HDR mais modernos&lt;/h2&gt;
+&lt;p&gt;O HDR10 melhora a qualidade da imagem com imers&amp;atilde;o visual mais din&amp;acirc;mica e cores aprimoradas do conte&amp;uacute;do HDR. &lt;strong&gt;HDR10&lt;/strong&gt; &amp;eacute; o padr&amp;atilde;o HDR digital baseado na gama de cores&lt;strong&gt; sRGB 99%&lt;/strong&gt;. Uma diferen&amp;ccedil;a real de cor e brilho.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Mais clara, suave e r&amp;aacute;pida&lt;/h2&gt;
+&lt;p&gt;Com a tecnologia &lt;strong&gt;FreeSync&lt;/strong&gt; os jogos t&amp;ecirc;m movimentos perfeitos e fluidos, balanceada com o processamento da placa de v&amp;iacute;deo, acabando com as imagens emba&amp;ccedil;adas e frames engasgados.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Design elegante&lt;/h2&gt;
+&lt;p&gt;Uma experi&amp;ecirc;ncia incr&amp;iacute;vel com imers&amp;atilde;o total. Design exuberante com&lt;strong&gt; bordas infinitas&lt;/strong&gt; (3-Side Bordeless) permitem uma imagem perfeita com incr&amp;iacute;vel imers&amp;atilde;o&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Aproveite essa oportunidade e adquira seu Monitor Gamer LG Ultra Gear no KaBuM!&lt;/h3&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Acer 27 ZeroFrame Full HD, 165Hz, 0.5ms, IPS, HDMI e DisplayPort, FreeSync Premium, VESA, Preto - VG272 S</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Monitor Gamer Acer 27 Full HD, 165Hz, 0.5ms, IPS, HDMI/DisplayPort, FreeSync Premium, VESA, Preto&lt;/h2&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;p&gt;Com tela de 27" FHD E2E (IPS) com resolu&amp;ccedil;&amp;atilde;o Full HD e uma taxa de atualiza&amp;ccedil;&amp;atilde;o no modo normal: 144Hz e modo de overclock 165Hz, com alta taxa de atualiza&amp;ccedil;&amp;atilde;o com 165Hz. Brilho 400 cd/m2 e um tempo de respostas baix&amp;iacute;ssimo de 2ms, ainda para aproveitar voc&amp;ecirc; poder&amp;aacute; desfrutar de uma conectividade HDMI (2.0), DisplayPort.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Bluecase 27 LED, 75 Hz, 2K QHD, 99%sRGB, HDMI/DisplayPort - BM2713GWCASE</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Explore um n&amp;iacute;vel superior de qualidade gr&amp;aacute;fica do seu gameplay com o monitor gamer Bluecase BM2713GW Esse monitor possui um painel TN ultrarr&amp;aacute;pido com frequ&amp;ecirc;ncia m&amp;aacute;xima de at&amp;eacute; 75 Hz e baix&amp;iacute;ssimo tempo de resposta de 5(cinco) milissegundos. Ideal para seus jogos AAA, o monitor conta com alta defini&amp;ccedil;&amp;atilde;o em resolu&amp;ccedil;&amp;atilde;o Quad HD (2560x1440) que proporciona uma imagem rica em detalhes. O monitor Bluecase BM2713GW &amp;eacute; compat&amp;iacute;vel com suportes VESA e tamb&amp;eacute;m conta com conex&amp;otilde;es DisplayPort e HDMI.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Acer Nitro 23.6 LED, Curvo, 165 Hz, Full HD, 1ms, FreeSync Premium, HDMI/DisplayPort - EI242QR</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Monitor Gamer Acer Nitro 23.6 LED, Curvo, 165 Hz, Full HD, 1ms, FreeSync Premium, HDMI/DisplayPort&lt;/h2&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Tecnologia da Tela&lt;/h2&gt;
+&lt;p&gt;A Tela do Acer Nitro EI242QR possui campo de vis&amp;atilde;o de 23.6 Polegadas com um &lt;strong&gt;Resolu&amp;ccedil;&amp;atilde;o de 1920 x 1080 Full HD&lt;/strong&gt;, Painel VA de propor&amp;ccedil;&amp;atilde;o 16:9 com design &lt;strong&gt;curvo 1200R&lt;/strong&gt;, Taxa de atualiza&amp;ccedil;&amp;atilde;o de &lt;strong&gt;165Hz&lt;/strong&gt; (Utilizando Displayport), e Tempo de Resposta &lt;strong&gt;1ms&lt;/strong&gt; VRB (Visual Response Boost) para desempenhos profissionais nos seus gameplays.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;ZeroFrame&lt;/h2&gt;
+&lt;p&gt;Oferece um novo &lt;strong&gt;design de quadro zero&lt;/strong&gt;, remove virtualmente a caixa delimitadora da tela e oferece todas as imagens, prazer visual cont&amp;iacute;nuo.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Desing de tela curvo 1200 R&lt;/h2&gt;
+&lt;p&gt;Proporciona uma experi&amp;ecirc;ncia de visualiza&amp;ccedil;&amp;atilde;o uniforme e &lt;strong&gt;reduz o cansa&amp;ccedil;o visual&lt;/strong&gt; durante longos per&amp;iacute;odos de utiliza&amp;ccedil;&amp;atilde;o. Ele tamb&amp;eacute;m apresenta uma experi&amp;ecirc;ncia mais envolvente com um campo de vis&amp;atilde;o mais amplo e &amp;aacute;rea de vis&amp;atilde;o perif&amp;eacute;rica aumentada em compara&amp;ccedil;&amp;atilde;o com uma tela plana do mesmo&lt;/p&gt;
+&lt;p&gt;tamanho.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Tempo de resposta de 1ms&lt;/h2&gt;
+&lt;p&gt;O t&lt;strong&gt;empo de resposta r&amp;aacute;pido de 1 ms&lt;/strong&gt; melhora experi&amp;ecirc;ncia do jogador. N&amp;atilde;o importa a a&amp;ccedil;&amp;atilde;o em movimento r&amp;aacute;pido ou quaisquer transi&amp;ccedil;&amp;otilde;es dram&amp;aacute;ticas, tudo ser&amp;aacute; reproduzido suavemente, sem os efeitos irritantes de manchas ou fantasmas.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Taxa de atualiza&amp;ccedil;&amp;atilde;o de 165Hz&lt;/h2&gt;
+&lt;p&gt;Acelera os quadros por segundo para fornecer cenas de movimento ultra suaves. Com uma taxa de &lt;strong&gt;atualiza&amp;ccedil;&amp;atilde;o r&amp;aacute;pida de 165 Hz&lt;/strong&gt;, os monitores de jogos da Acer encurtam o tempo necess&amp;aacute;rio para a renderiza&amp;ccedil;&amp;atilde;o de quadros, diminuem o atraso de entrada e fornecem aos jogadores uma excelente experi&amp;ecirc;ncia no jogo.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Aproveite essa oportunidade e adquira seu Monitor Gamer Acer Nitro 23.6 no KaBuM!&lt;/h3&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Acer Nitro 23.8 LED Full HD, 165Hz, 1ms, HDMI/DisplayPort, FreeSync Premium, Preto - QG241Y</t>
+  </si>
+  <si>
+    <t>&lt;h2&gt;Monitor Gamer Acer Nitro 23.8 LED Full HD, 165Hz, 1ms, HDMI/DisplayPort, FreeSync Premium, Preto&lt;/h2&gt;
+&lt;p&gt;Com uma tela de&lt;strong&gt; 23,8&amp;rdquo; FHD&lt;/strong&gt;, o &lt;strong&gt;Nitro QG241Y&lt;/strong&gt; entrega imagens mais n&amp;iacute;tidas, levando sua experi&amp;ecirc;ncia visual e seu foco no jogo para um novo n&amp;iacute;vel.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;AMD FreeSync Premium&lt;/h2&gt;
+&lt;p&gt;Com o AMD FreeSync Premium, a taxa de quadros do jogo &amp;eacute; determinada pela sua placa de v&amp;iacute;deo, n&amp;atilde;o pela taxa de atualiza&amp;ccedil;&amp;atilde;o fixa do&amp;nbsp; monitor. Isso significa que os quadros do monitor s&amp;atilde;o sincronizados com os quadros da placa&amp;nbsp; gr&amp;aacute;fica, o que &lt;strong&gt;elimina a tela quebrada&lt;/strong&gt; e oferece &lt;strong&gt;experi&amp;ecirc;ncias de jogo muito suaves&lt;/strong&gt;.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Resolu&amp;ccedil;&amp;atilde;o FHD&lt;/h2&gt;
+&lt;p&gt;Traga os usu&amp;aacute;rios para um mundo colorido perfeito com &lt;strong&gt;FHD 1920 x 1080&lt;/strong&gt; e oferece a melhor qualidade original natural e n&amp;iacute;tida&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;1ms Visual Response Boost&lt;/h2&gt;
+&lt;p&gt;O &lt;strong&gt;Visual Response Boost (VRB)&lt;/strong&gt; de 1ms funciona desligando rapidamente a luz de fundo ou inserindo uma imagem em branco e preta entre os quadros, tamb&amp;eacute;m conhecida como &amp;ldquo;piscando&amp;rdquo;. Isso resulta em um &lt;strong&gt;desfoque menos percept&amp;iacute;vel&lt;/strong&gt; em imagens em movimento r&amp;aacute;pido porque os cristais l&amp;iacute;quidos n&amp;atilde;o precisam dobrar nos quadros &amp;agrave; medida que sobem e descem.&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h2&gt;Reduz a fadiga&lt;/h2&gt;
+&lt;p&gt;Fique na luta por horas com a tecnologia &lt;strong&gt;Flicker-less, Blue-light Filter.&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;&amp;nbsp;&lt;/p&gt;
+&lt;h3&gt;Aproveite essa oportunidade e adquira seu Monitor Gamer Acer no KaBuM!&lt;/h3&gt;</t>
+  </si>
+  <si>
+    <t>Monitor Gamer 27" 144Hz, 1Ms, Bluecase, Full HD, Freesync, Borda Ultra Fina - BM2710GW</t>
+  </si>
+  <si>
+    <t>O Monitor Gamer BM2710GW entrega aos gamers uma experiência lisa, rápida e responsiva em todos os jogos. Experimente uma jogabilidade impecável com a taxa de atualização de tela 144 Hz que garante imagens rápidas, suaves e movimentos nítidos, para nenhum detalhe passar despercebido.</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Gigabyte 23.8 IPS, Full HD, 170Hz, 1ms, 120% sRGB, HDR, FreeSync Premium, Altura Ajustável - G24F-SA</t>
+  </si>
+  <si>
+    <t>JUNTE-SE À LUTA com o Monitor Gamer G24F da Gigabyte com 1ms de tempo de resposta, freesync premium, 165 Hz (170 Hz OC) e com uma taxa de cor de 8 bits, 90% DCI-P3 A ÚLTIMA MILHA PARA O SEU SISTEMA DE JOGO Como um jogador invisível, o monitor é frequentemente subestimado. A verdade é que os monitores se formam como um efeito sinérgico e trazem o melhor desempenho dos componentes do PC. Os monitores de jogos GIGABYTE oferecem as últimas especificações e qualidade, os usuários podem realmente desfrutar de um desempenho de alto nível sem a necessidade de extravagância. Tempo de resposta de 1 ms MPRT Tempo de resposta super rápido de 1 ms para a experiência de jogo mais suave de todos os tempos! FHD com 165 Hz (OC 170 Hz) Alta resolução e taxa de atualização rápida, proporcionando qualidade de exibição detalhada e experiência de jogo fluida! Cor de 8 bits, 90% DCI-P3 Fantástico visor a cores e 90% de cores DCI-P3 de gama super ampla. SIMPLES MAS ESTILOSO A aparência aerodinâmica representa a simplicidade da filosofia de design da série de jogos GIGABYTE, suporte robusto e acabamento fosco construído para características funcionais e estéticas adicionando mais características. OSD Sidekick GIGABYTE OSD Sidekick permite que você defina as opções de exibição com teclado e mouse, oferecendo a maneira mais fácil de ajustar as configurações do monitor. ÂNGULO DE VISÃO PERFEITO O monitor de jogos GIGABYTE possui um suporte exclusivo ergonomicamente projetado para oferecer uma ampla gama de ajustes de altura e inclinação.</t>
   </si>
   <si>
     <t>Monitor Gamer Ozone 24,5 LED, 144 Hz, Full HD, 1ms, FreeSync, HDMI/DisplayPort - OZDSP25FHD</t>
@@ -1644,6 +1665,12 @@
   </si>
   <si>
     <t>Monitor Gamer Full HD 165Hz de atualização para melhores gráficos. Curvatura R3000 para maior imersão. Com 1 conector DisplayPort e 1 conector HDMI. Monitor na cor branca para combinar com o estilo do seu setup.</t>
+  </si>
+  <si>
+    <t>Monitor Gamer Acer Aopen 25MH1Q, 24,5´, 144Hz, 1ms, Full HD, HDMI/ Display Port, AMD Radeon Freesync, Anti Reflexo, Preto - UM.KM1AA.P02</t>
+  </si>
+  <si>
+    <t>Embarque em uma nova realidade de visualização! O Monitor AOPEN 25MH1Q é ideal para jogos de tiros e aventuras, proporcionando imagens mais realistas e limpas. Sinta-se dentro do jogo!</t>
   </si>
 </sst>
 </file>
@@ -1990,7 +2017,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F146"/>
+  <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2064,7 +2091,10 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>1599</v>
+        <v>1947</v>
+      </c>
+      <c r="D4">
+        <v>1757</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2075,10 +2105,16 @@
         <v>13</v>
       </c>
       <c r="C5">
-        <v>1947</v>
+        <v>1055</v>
       </c>
       <c r="D5">
-        <v>1757</v>
+        <v>788</v>
+      </c>
+      <c r="E5">
+        <v>922</v>
+      </c>
+      <c r="F5">
+        <v>829</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2089,10 +2125,10 @@
         <v>15</v>
       </c>
       <c r="C6">
-        <v>1055</v>
+        <v>1736</v>
       </c>
       <c r="D6">
-        <v>902</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2103,10 +2139,16 @@
         <v>17</v>
       </c>
       <c r="C7">
-        <v>1631</v>
+        <v>1684</v>
       </c>
       <c r="D7">
-        <v>1472</v>
+        <v>1139</v>
+      </c>
+      <c r="E7">
+        <v>1263</v>
+      </c>
+      <c r="F7">
+        <v>1199</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2117,13 +2159,10 @@
         <v>19</v>
       </c>
       <c r="C8">
-        <v>1684</v>
-      </c>
-      <c r="E8">
-        <v>1368</v>
-      </c>
-      <c r="F8">
-        <v>1299</v>
+        <v>1221</v>
+      </c>
+      <c r="D8">
+        <v>1101</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2137,7 +2176,13 @@
         <v>1221</v>
       </c>
       <c r="D9">
-        <v>1101</v>
+        <v>1073</v>
+      </c>
+      <c r="E9">
+        <v>1189</v>
+      </c>
+      <c r="F9">
+        <v>1129</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2162,16 +2207,16 @@
         <v>25</v>
       </c>
       <c r="C11">
-        <v>1221</v>
+        <v>1789</v>
       </c>
       <c r="D11">
-        <v>1073</v>
+        <v>1519</v>
       </c>
       <c r="E11">
-        <v>1189</v>
+        <v>1684</v>
       </c>
       <c r="F11">
-        <v>1129</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2182,10 +2227,16 @@
         <v>27</v>
       </c>
       <c r="C12">
-        <v>1789</v>
+        <v>1177</v>
       </c>
       <c r="D12">
-        <v>1614</v>
+        <v>930</v>
+      </c>
+      <c r="E12">
+        <v>1088</v>
+      </c>
+      <c r="F12">
+        <v>979</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2196,16 +2247,10 @@
         <v>29</v>
       </c>
       <c r="C13">
-        <v>1177</v>
+        <v>1210</v>
       </c>
       <c r="D13">
-        <v>930</v>
-      </c>
-      <c r="E13">
-        <v>1088</v>
-      </c>
-      <c r="F13">
-        <v>979</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2216,10 +2261,13 @@
         <v>31</v>
       </c>
       <c r="C14">
-        <v>1111</v>
-      </c>
-      <c r="D14">
-        <v>949</v>
+        <v>1052</v>
+      </c>
+      <c r="E14">
+        <v>894</v>
+      </c>
+      <c r="F14">
+        <v>849</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2230,10 +2278,7 @@
         <v>33</v>
       </c>
       <c r="C15">
-        <v>1210</v>
-      </c>
-      <c r="D15">
-        <v>1092</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2244,7 +2289,16 @@
         <v>35</v>
       </c>
       <c r="C16">
-        <v>1198</v>
+        <v>1684</v>
+      </c>
+      <c r="D16">
+        <v>1329</v>
+      </c>
+      <c r="E16">
+        <v>1473</v>
+      </c>
+      <c r="F16">
+        <v>1399</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2255,10 +2309,13 @@
         <v>37</v>
       </c>
       <c r="C17">
-        <v>1684</v>
-      </c>
-      <c r="D17">
-        <v>1519</v>
+        <v>1199</v>
+      </c>
+      <c r="E17">
+        <v>1098</v>
+      </c>
+      <c r="F17">
+        <v>989</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2269,13 +2326,16 @@
         <v>39</v>
       </c>
       <c r="C18">
-        <v>1199</v>
+        <v>1578</v>
+      </c>
+      <c r="D18">
+        <v>1329</v>
       </c>
       <c r="E18">
-        <v>1098</v>
+        <v>1473</v>
       </c>
       <c r="F18">
-        <v>989</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2286,16 +2346,7 @@
         <v>41</v>
       </c>
       <c r="C19">
-        <v>1368</v>
-      </c>
-      <c r="D19">
-        <v>1158</v>
-      </c>
-      <c r="E19">
-        <v>1284</v>
-      </c>
-      <c r="F19">
-        <v>1219</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2306,7 +2357,16 @@
         <v>43</v>
       </c>
       <c r="C20">
-        <v>1776</v>
+        <v>1263</v>
+      </c>
+      <c r="D20">
+        <v>854</v>
+      </c>
+      <c r="E20">
+        <v>947</v>
+      </c>
+      <c r="F20">
+        <v>899</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2317,16 +2377,10 @@
         <v>45</v>
       </c>
       <c r="C21">
-        <v>1263</v>
+        <v>1974</v>
       </c>
       <c r="D21">
-        <v>892</v>
-      </c>
-      <c r="E21">
-        <v>989</v>
-      </c>
-      <c r="F21">
-        <v>939</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2337,10 +2391,7 @@
         <v>47</v>
       </c>
       <c r="C22">
-        <v>1974</v>
-      </c>
-      <c r="D22">
-        <v>1782</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2351,7 +2402,7 @@
         <v>49</v>
       </c>
       <c r="C23">
-        <v>1840</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2362,7 +2413,10 @@
         <v>51</v>
       </c>
       <c r="C24">
-        <v>1251</v>
+        <v>1968</v>
+      </c>
+      <c r="D24">
+        <v>1813</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2454,10 +2508,10 @@
         <v>65</v>
       </c>
       <c r="C31">
-        <v>1066</v>
+        <v>1368</v>
       </c>
       <c r="D31">
-        <v>912</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -2468,7 +2522,16 @@
         <v>67</v>
       </c>
       <c r="C32">
-        <v>1044</v>
+        <v>1066</v>
+      </c>
+      <c r="D32">
+        <v>760</v>
+      </c>
+      <c r="E32">
+        <v>888</v>
+      </c>
+      <c r="F32">
+        <v>799</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2479,10 +2542,7 @@
         <v>69</v>
       </c>
       <c r="C33">
-        <v>1349</v>
-      </c>
-      <c r="D33">
-        <v>1243</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -2493,10 +2553,10 @@
         <v>71</v>
       </c>
       <c r="C34">
-        <v>1193</v>
+        <v>1349</v>
       </c>
       <c r="D34">
-        <v>1099</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2507,10 +2567,10 @@
         <v>73</v>
       </c>
       <c r="C35">
-        <v>1424</v>
+        <v>1193</v>
       </c>
       <c r="D35">
-        <v>1312</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2521,7 +2581,10 @@
         <v>75</v>
       </c>
       <c r="C36">
-        <v>1233</v>
+        <v>1424</v>
+      </c>
+      <c r="D36">
+        <v>1312</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2552,10 +2615,7 @@
         <v>79</v>
       </c>
       <c r="C38">
-        <v>1894</v>
-      </c>
-      <c r="D38">
-        <v>1709</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2566,7 +2626,10 @@
         <v>81</v>
       </c>
       <c r="C39">
-        <v>1359</v>
+        <v>1894</v>
+      </c>
+      <c r="D39">
+        <v>1709</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2577,7 +2640,7 @@
         <v>83</v>
       </c>
       <c r="C40">
-        <v>1299</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2588,7 +2651,13 @@
         <v>85</v>
       </c>
       <c r="C41">
-        <v>1899</v>
+        <v>1079</v>
+      </c>
+      <c r="E41">
+        <v>1054</v>
+      </c>
+      <c r="F41">
+        <v>949</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2599,10 +2668,7 @@
         <v>87</v>
       </c>
       <c r="C42">
-        <v>1055</v>
-      </c>
-      <c r="D42">
-        <v>769</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2613,10 +2679,7 @@
         <v>89</v>
       </c>
       <c r="C43">
-        <v>1771</v>
-      </c>
-      <c r="D43">
-        <v>1598</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2627,13 +2690,16 @@
         <v>91</v>
       </c>
       <c r="C44">
-        <v>1122</v>
+        <v>1055</v>
+      </c>
+      <c r="D44">
+        <v>769</v>
       </c>
       <c r="E44">
-        <v>1054</v>
+        <v>899</v>
       </c>
       <c r="F44">
-        <v>949</v>
+        <v>809</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2644,7 +2710,10 @@
         <v>93</v>
       </c>
       <c r="C45">
-        <v>1548</v>
+        <v>1771</v>
+      </c>
+      <c r="D45">
+        <v>1598</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2655,38 +2724,35 @@
         <v>95</v>
       </c>
       <c r="C46">
-        <v>1052</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="B47" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C47">
-        <v>1155</v>
-      </c>
-      <c r="D47">
-        <v>1065</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="B48" t="s">
         <v>98</v>
       </c>
       <c r="C48">
-        <v>1111</v>
+        <v>1155</v>
       </c>
       <c r="D48">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>99</v>
       </c>
@@ -2694,13 +2760,16 @@
         <v>100</v>
       </c>
       <c r="C49">
-        <v>1252</v>
-      </c>
-      <c r="D49">
-        <v>1130</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>1111</v>
+      </c>
+      <c r="E49">
+        <v>888</v>
+      </c>
+      <c r="F49">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>101</v>
       </c>
@@ -2708,10 +2777,13 @@
         <v>102</v>
       </c>
       <c r="C50">
-        <v>1666</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+        <v>1031</v>
+      </c>
+      <c r="D50">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>103</v>
       </c>
@@ -2719,10 +2791,10 @@
         <v>104</v>
       </c>
       <c r="C51">
-        <v>1210</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>105</v>
       </c>
@@ -2730,13 +2802,10 @@
         <v>106</v>
       </c>
       <c r="C52">
-        <v>1594</v>
-      </c>
-      <c r="D52">
-        <v>1439</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>107</v>
       </c>
@@ -2744,10 +2813,13 @@
         <v>108</v>
       </c>
       <c r="C53">
-        <v>1433</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
+        <v>1594</v>
+      </c>
+      <c r="D53">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>109</v>
       </c>
@@ -2755,13 +2827,10 @@
         <v>110</v>
       </c>
       <c r="C54">
-        <v>1305</v>
-      </c>
-      <c r="D54">
-        <v>1177</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>111</v>
       </c>
@@ -2769,10 +2838,13 @@
         <v>112</v>
       </c>
       <c r="C55">
-        <v>1075</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
+        <v>1305</v>
+      </c>
+      <c r="D55">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>113</v>
       </c>
@@ -2783,7 +2855,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>115</v>
       </c>
@@ -2791,13 +2863,10 @@
         <v>116</v>
       </c>
       <c r="C57">
-        <v>1669</v>
-      </c>
-      <c r="D57">
-        <v>1506</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>117</v>
       </c>
@@ -2805,13 +2874,13 @@
         <v>118</v>
       </c>
       <c r="C58">
-        <v>1311</v>
+        <v>1669</v>
       </c>
       <c r="D58">
-        <v>1183</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+        <v>1506</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>119</v>
       </c>
@@ -2819,10 +2888,13 @@
         <v>120</v>
       </c>
       <c r="C59">
-        <v>1349</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+        <v>1311</v>
+      </c>
+      <c r="D59">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>121</v>
       </c>
@@ -2830,13 +2902,10 @@
         <v>122</v>
       </c>
       <c r="C60">
-        <v>1987</v>
-      </c>
-      <c r="D60">
-        <v>1793</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>123</v>
       </c>
@@ -2844,10 +2913,10 @@
         <v>124</v>
       </c>
       <c r="C61">
-        <v>1205</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>125</v>
       </c>
@@ -2855,29 +2924,32 @@
         <v>126</v>
       </c>
       <c r="C62">
-        <v>1129</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
+        <v>1987</v>
+      </c>
+      <c r="D62">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
         <v>127</v>
       </c>
       <c r="B63" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C63">
-        <v>1969</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B64" t="s">
         <v>129</v>
       </c>
       <c r="C64">
-        <v>1279</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2888,7 +2960,10 @@
         <v>131</v>
       </c>
       <c r="C65">
-        <v>1599</v>
+        <v>1976</v>
+      </c>
+      <c r="D65">
+        <v>1784</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2899,7 +2974,7 @@
         <v>133</v>
       </c>
       <c r="C66">
-        <v>1616</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2907,21 +2982,21 @@
         <v>134</v>
       </c>
       <c r="B67" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C67">
-        <v>1199</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B68" t="s">
         <v>136</v>
       </c>
       <c r="C68">
-        <v>1149</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2932,18 +3007,18 @@
         <v>138</v>
       </c>
       <c r="C69">
-        <v>1099</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>32</v>
+        <v>139</v>
       </c>
       <c r="B70" t="s">
         <v>139</v>
       </c>
       <c r="C70">
-        <v>1199</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2954,73 +3029,73 @@
         <v>141</v>
       </c>
       <c r="C71">
-        <v>1217</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
+        <v>28</v>
+      </c>
+      <c r="B72" t="s">
         <v>142</v>
       </c>
-      <c r="B72" t="s">
-        <v>143</v>
-      </c>
       <c r="C72">
-        <v>1799</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
+        <v>143</v>
+      </c>
+      <c r="B73" t="s">
         <v>144</v>
       </c>
-      <c r="B73" t="s">
-        <v>145</v>
-      </c>
       <c r="C73">
-        <v>1311</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
+        <v>145</v>
+      </c>
+      <c r="B74" t="s">
         <v>146</v>
       </c>
-      <c r="B74" t="s">
-        <v>147</v>
-      </c>
       <c r="C74">
-        <v>1649</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
+        <v>147</v>
+      </c>
+      <c r="B75" t="s">
         <v>148</v>
       </c>
-      <c r="B75" t="s">
-        <v>149</v>
-      </c>
       <c r="C75">
-        <v>1049</v>
+        <v>1263</v>
+      </c>
+      <c r="D75">
+        <v>1139</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
+        <v>149</v>
+      </c>
+      <c r="B76" t="s">
         <v>150</v>
       </c>
-      <c r="B76" t="s">
-        <v>151</v>
-      </c>
       <c r="C76">
-        <v>1971</v>
-      </c>
-      <c r="D76">
-        <v>1779</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
+        <v>151</v>
+      </c>
+      <c r="B77" t="s">
         <v>152</v>
-      </c>
-      <c r="B77" t="s">
-        <v>153</v>
       </c>
       <c r="C77">
         <v>1578</v>
@@ -3028,35 +3103,38 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
+        <v>153</v>
+      </c>
+      <c r="B78" t="s">
         <v>154</v>
       </c>
-      <c r="B78" t="s">
-        <v>155</v>
-      </c>
       <c r="C78">
-        <v>1083</v>
+        <v>1971</v>
+      </c>
+      <c r="D78">
+        <v>1779</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
+        <v>155</v>
+      </c>
+      <c r="B79" t="s">
         <v>156</v>
       </c>
-      <c r="B79" t="s">
-        <v>157</v>
-      </c>
       <c r="C79">
-        <v>1275</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B80" t="s">
         <v>158</v>
       </c>
       <c r="C80">
-        <v>1524</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -3067,10 +3145,7 @@
         <v>160</v>
       </c>
       <c r="C81">
-        <v>1976</v>
-      </c>
-      <c r="D81">
-        <v>1784</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -3092,7 +3167,7 @@
         <v>164</v>
       </c>
       <c r="C83">
-        <v>1196</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -3103,7 +3178,10 @@
         <v>166</v>
       </c>
       <c r="C84">
-        <v>1899</v>
+        <v>1649</v>
+      </c>
+      <c r="D84">
+        <v>1488</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -3114,7 +3192,7 @@
         <v>168</v>
       </c>
       <c r="C85">
-        <v>1279</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -3125,10 +3203,7 @@
         <v>170</v>
       </c>
       <c r="C86">
-        <v>1465</v>
-      </c>
-      <c r="D86">
-        <v>1322</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -3139,7 +3214,7 @@
         <v>172</v>
       </c>
       <c r="C87">
-        <v>1129</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -3150,7 +3225,7 @@
         <v>174</v>
       </c>
       <c r="C88">
-        <v>1150</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -3161,7 +3236,7 @@
         <v>176</v>
       </c>
       <c r="C89">
-        <v>1419</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -3172,7 +3247,10 @@
         <v>178</v>
       </c>
       <c r="C90">
-        <v>1190</v>
+        <v>1465</v>
+      </c>
+      <c r="D90">
+        <v>1322</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -3183,7 +3261,7 @@
         <v>180</v>
       </c>
       <c r="C91">
-        <v>1139</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -3194,7 +3272,7 @@
         <v>182</v>
       </c>
       <c r="C92">
-        <v>1514</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -3205,7 +3283,7 @@
         <v>184</v>
       </c>
       <c r="C93">
-        <v>1786</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -3216,7 +3294,7 @@
         <v>186</v>
       </c>
       <c r="C94">
-        <v>1473</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -3227,7 +3305,7 @@
         <v>188</v>
       </c>
       <c r="C95">
-        <v>1611</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -3238,7 +3316,7 @@
         <v>190</v>
       </c>
       <c r="C96">
-        <v>1275</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -3249,7 +3327,7 @@
         <v>192</v>
       </c>
       <c r="C97">
-        <v>1289</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -3260,7 +3338,7 @@
         <v>194</v>
       </c>
       <c r="C98">
-        <v>1011</v>
+        <v>1786</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -3271,7 +3349,7 @@
         <v>196</v>
       </c>
       <c r="C99">
-        <v>1049</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -3282,40 +3360,40 @@
         <v>198</v>
       </c>
       <c r="C100">
-        <v>1499</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B101" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C101">
-        <v>1989</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B102" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C102">
-        <v>1699</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B103" t="s">
         <v>202</v>
       </c>
       <c r="C103">
-        <v>1719</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -3326,10 +3404,7 @@
         <v>204</v>
       </c>
       <c r="C104">
-        <v>1088</v>
-      </c>
-      <c r="D104">
-        <v>931</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -3340,10 +3415,7 @@
         <v>206</v>
       </c>
       <c r="C105">
-        <v>1242</v>
-      </c>
-      <c r="D105">
-        <v>1120</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -3354,10 +3426,7 @@
         <v>208</v>
       </c>
       <c r="C106">
-        <v>1109</v>
-      </c>
-      <c r="D106">
-        <v>949</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -3365,80 +3434,71 @@
         <v>209</v>
       </c>
       <c r="B107" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C107">
-        <v>1473</v>
-      </c>
-      <c r="D107">
-        <v>1329</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B108" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C108">
-        <v>1446</v>
-      </c>
-      <c r="D108">
-        <v>1305</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B109" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C109">
-        <v>1368</v>
-      </c>
-      <c r="D109">
-        <v>1234</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B110" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C110">
-        <v>1953</v>
+        <v>1088</v>
       </c>
       <c r="D110">
-        <v>1763</v>
+        <v>931</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B111" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C111">
-        <v>1777</v>
+        <v>1242</v>
       </c>
       <c r="D111">
-        <v>1519</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B112" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C112">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="D112">
         <v>949</v>
@@ -3446,69 +3506,69 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B113" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C113">
-        <v>1831</v>
+        <v>1473</v>
       </c>
       <c r="D113">
-        <v>1687</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B114" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C114">
-        <v>1795</v>
+        <v>1446</v>
       </c>
       <c r="D114">
-        <v>1500</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B115" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C115">
-        <v>1635</v>
+        <v>1953</v>
       </c>
       <c r="D115">
-        <v>1398</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B116" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C116">
-        <v>1444</v>
+        <v>1777</v>
       </c>
       <c r="D116">
-        <v>1234</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B117" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C117">
-        <v>1136</v>
+        <v>1111</v>
       </c>
       <c r="D117">
         <v>949</v>
@@ -3516,346 +3576,343 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B118" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C118">
-        <v>1733</v>
+        <v>1831</v>
       </c>
       <c r="D118">
-        <v>1481</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B119" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C119">
-        <v>1372</v>
+        <v>1795</v>
       </c>
       <c r="D119">
-        <v>1173</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B120" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C120">
-        <v>1590</v>
+        <v>1635</v>
       </c>
       <c r="D120">
-        <v>1330</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B121" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C121">
-        <v>1263</v>
+        <v>1444</v>
       </c>
       <c r="D121">
-        <v>1139</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B122" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C122">
-        <v>1666</v>
+        <v>1136</v>
       </c>
       <c r="D122">
-        <v>1425</v>
+        <v>949</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B123" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C123">
-        <v>1555</v>
+        <v>1733</v>
       </c>
       <c r="D123">
-        <v>1329</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B124" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C124">
-        <v>1611</v>
+        <v>1372</v>
       </c>
       <c r="D124">
-        <v>1377</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B125" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C125">
-        <v>1402</v>
+        <v>1590</v>
       </c>
       <c r="D125">
-        <v>1198</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B126" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C126">
-        <v>1444</v>
+        <v>1666</v>
       </c>
       <c r="D126">
-        <v>1234</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B127" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C127">
-        <v>1649</v>
+        <v>1555</v>
       </c>
       <c r="D127">
-        <v>1488</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B128" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C128">
-        <v>1222</v>
+        <v>1611</v>
       </c>
       <c r="D128">
-        <v>1044</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B129" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C129">
-        <v>1868</v>
+        <v>1402</v>
       </c>
       <c r="D129">
-        <v>1597</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B130" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C130">
-        <v>1518</v>
-      </c>
-      <c r="D130">
-        <v>1298</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B131" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C131">
-        <v>1888</v>
+        <v>1444</v>
       </c>
       <c r="D131">
-        <v>1614</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B132" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C132">
-        <v>1635</v>
+        <v>1222</v>
       </c>
       <c r="D132">
-        <v>1398</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B133" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C133">
-        <v>1333</v>
+        <v>1868</v>
       </c>
       <c r="D133">
-        <v>1139</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B134" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C134">
-        <v>1285</v>
+        <v>1518</v>
       </c>
       <c r="D134">
-        <v>1099</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B135" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C135">
-        <v>1722</v>
+        <v>1888</v>
+      </c>
+      <c r="D135">
+        <v>1614</v>
       </c>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B136" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C136">
-        <v>1455</v>
+        <v>1635</v>
+      </c>
+      <c r="D136">
+        <v>1398</v>
       </c>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B137" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C137">
-        <v>1672</v>
+        <v>1333</v>
       </c>
       <c r="D137">
-        <v>1429</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B138" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C138">
-        <v>1815</v>
+        <v>1285</v>
       </c>
       <c r="D138">
-        <v>1552</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B139" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C139">
-        <v>1999</v>
-      </c>
-      <c r="D139">
-        <v>1614</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="140" spans="1:4">
       <c r="A140" t="s">
+        <v>273</v>
+      </c>
+      <c r="B140" t="s">
         <v>274</v>
       </c>
-      <c r="B140" t="s">
-        <v>275</v>
-      </c>
       <c r="C140">
-        <v>1999</v>
-      </c>
-      <c r="D140">
-        <v>1709</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" t="s">
+        <v>275</v>
+      </c>
+      <c r="B141" t="s">
         <v>276</v>
       </c>
-      <c r="B141" t="s">
-        <v>277</v>
-      </c>
       <c r="C141">
-        <v>1660</v>
+        <v>1672</v>
       </c>
       <c r="D141">
-        <v>1419</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B142" t="s">
         <v>278</v>
       </c>
       <c r="C142">
-        <v>1754</v>
+        <v>1815</v>
       </c>
       <c r="D142">
-        <v>1499</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -3863,55 +3920,125 @@
         <v>279</v>
       </c>
       <c r="B143" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C143">
-        <v>1604</v>
+        <v>1999</v>
       </c>
       <c r="D143">
-        <v>1371</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" t="s">
+        <v>280</v>
+      </c>
+      <c r="B144" t="s">
         <v>281</v>
       </c>
-      <c r="B144" t="s">
-        <v>282</v>
-      </c>
       <c r="C144">
-        <v>1777</v>
+        <v>1999</v>
       </c>
       <c r="D144">
-        <v>1519</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="145" spans="1:4">
       <c r="A145" t="s">
+        <v>282</v>
+      </c>
+      <c r="B145" t="s">
         <v>283</v>
       </c>
-      <c r="B145" t="s">
-        <v>284</v>
-      </c>
       <c r="C145">
-        <v>1999</v>
+        <v>1660</v>
       </c>
       <c r="D145">
-        <v>1709</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="146" spans="1:4">
       <c r="A146" t="s">
+        <v>284</v>
+      </c>
+      <c r="B146" t="s">
+        <v>284</v>
+      </c>
+      <c r="C146">
+        <v>1754</v>
+      </c>
+      <c r="D146">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" t="s">
         <v>285</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B147" t="s">
         <v>286</v>
       </c>
-      <c r="C146">
+      <c r="C147">
+        <v>1604</v>
+      </c>
+      <c r="D147">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" t="s">
+        <v>287</v>
+      </c>
+      <c r="B148" t="s">
+        <v>288</v>
+      </c>
+      <c r="C148">
+        <v>1777</v>
+      </c>
+      <c r="D148">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" t="s">
+        <v>289</v>
+      </c>
+      <c r="B149" t="s">
+        <v>290</v>
+      </c>
+      <c r="C149">
+        <v>1999</v>
+      </c>
+      <c r="D149">
+        <v>1709</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" t="s">
+        <v>291</v>
+      </c>
+      <c r="B150" t="s">
+        <v>292</v>
+      </c>
+      <c r="C150">
         <v>1888</v>
       </c>
-      <c r="D146">
+      <c r="D150">
         <v>1615</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" t="s">
+        <v>293</v>
+      </c>
+      <c r="B151" t="s">
+        <v>294</v>
+      </c>
+      <c r="C151">
+        <v>1625</v>
+      </c>
+      <c r="D151">
+        <v>1389</v>
       </c>
     </row>
   </sheetData>

</xml_diff>